<commit_message>
mergeSortedArray - moveZeroes - rotateArray
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView minimized="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1903,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2597,58 +2597,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="21">
-      <c r="A68" s="5" t="s">
+    <row r="68" spans="1:3" s="14" customFormat="1" ht="19.8">
+      <c r="A68" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="21">
-      <c r="A69" s="5" t="s">
+      <c r="C68" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="14" customFormat="1" ht="19.8">
+      <c r="A69" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="21">
-      <c r="A70" s="5" t="s">
+      <c r="C69" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="14" customFormat="1" ht="19.8">
+      <c r="A70" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="21">
-      <c r="A71" s="5" t="s">
+      <c r="C70" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="14" customFormat="1" ht="19.8">
+      <c r="A71" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="21">
-      <c r="A72" s="5" t="s">
+      <c r="C71" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="14" customFormat="1" ht="19.8">
+      <c r="A72" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LinkedList question from the sheet
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="492">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1497,6 +1497,9 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/is-it-a-circular-linked-list_981265?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/split-a-circular-linked-list_1071003?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1702,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1769,6 +1772,13 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
@@ -2090,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="18"/>
@@ -3744,7 +3754,10 @@
         <v>140</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>3</v>
+        <v>454</v>
+      </c>
+      <c r="D148" s="21" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="21">
@@ -3857,16 +3870,17 @@
         <v>480</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="21">
-      <c r="A158" s="5" t="s">
+    <row r="158" spans="1:4" s="32" customFormat="1" ht="21">
+      <c r="A158" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C158" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158" s="33"/>
     </row>
     <row r="159" spans="1:4" ht="21">
       <c r="A159" s="5" t="s">
@@ -7665,8 +7679,9 @@
     <hyperlink ref="D146" r:id="rId469"/>
     <hyperlink ref="D149" r:id="rId470"/>
     <hyperlink ref="D147" r:id="rId471"/>
+    <hyperlink ref="D148" r:id="rId472"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId472"/>
+  <pageSetup orientation="portrait" r:id="rId473"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zigzag traversal and preorderIterative
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="514">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1563,6 +1563,9 @@
   </si>
   <si>
     <t>Level order traversal V.V.IMP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-zigzag-level-order-traversal/</t>
   </si>
 </sst>
 </file>
@@ -2192,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="18"/>
@@ -4258,7 +4261,10 @@
         <v>164</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>3</v>
+        <v>446</v>
+      </c>
+      <c r="D181" s="21" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -7852,8 +7858,9 @@
     <hyperlink ref="D182" r:id="rId487"/>
     <hyperlink ref="D173" r:id="rId488"/>
     <hyperlink ref="D172" r:id="rId489"/>
+    <hyperlink ref="D181" r:id="rId490"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId490"/>
+  <pageSetup orientation="portrait" r:id="rId491"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BST Insertion, ceil deletion
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1596,6 +1596,21 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/construct-binary-tree-from-preorder-and-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>Ceil in a BST</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/ceil-from-bst_920464?source=youtube&amp;campaign=Striver_Tree_Videos&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Striver_Tree_Videos</t>
+  </si>
+  <si>
+    <t>Insertion in BST</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-into-a-binary-search-tree/submissions/</t>
   </si>
 </sst>
 </file>
@@ -2245,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F472"/>
+  <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F211" sqref="F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -4469,7 +4484,10 @@
         <v>174</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>3</v>
+        <v>441</v>
+      </c>
+      <c r="D193" s="21" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
@@ -4622,10 +4640,13 @@
         <v>182</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>184</v>
+        <v>525</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>3</v>
+        <v>441</v>
+      </c>
+      <c r="D207" s="21" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -4633,10 +4654,13 @@
         <v>182</v>
       </c>
       <c r="B208" s="14" t="s">
-        <v>185</v>
+        <v>527</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>3</v>
+        <v>441</v>
+      </c>
+      <c r="D208" s="21" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4644,7 +4668,7 @@
         <v>182</v>
       </c>
       <c r="B209" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>3</v>
@@ -4655,7 +4679,7 @@
         <v>182</v>
       </c>
       <c r="B210" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>3</v>
@@ -4666,7 +4690,7 @@
         <v>182</v>
       </c>
       <c r="B211" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>3</v>
@@ -4676,8 +4700,8 @@
       <c r="A212" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B212" s="16" t="s">
-        <v>189</v>
+      <c r="B212" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>3</v>
@@ -4688,7 +4712,7 @@
         <v>182</v>
       </c>
       <c r="B213" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>3</v>
@@ -4698,8 +4722,8 @@
       <c r="A214" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B214" s="14" t="s">
-        <v>191</v>
+      <c r="B214" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>3</v>
@@ -4710,52 +4734,52 @@
         <v>182</v>
       </c>
       <c r="B215" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A216" s="6" t="s">
+    <row r="216" spans="1:4" ht="21">
+      <c r="A216" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B216" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="C216" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D216" s="24"/>
+      <c r="B216" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="217" spans="1:4" ht="21">
       <c r="A217" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B217" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="21">
-      <c r="A218" s="3" t="s">
+    <row r="218" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A218" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B218" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B218" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D218" s="24"/>
     </row>
     <row r="219" spans="1:4" ht="21">
       <c r="A219" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B219" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>3</v>
@@ -4766,7 +4790,7 @@
         <v>182</v>
       </c>
       <c r="B220" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>3</v>
@@ -4777,7 +4801,7 @@
         <v>182</v>
       </c>
       <c r="B221" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>3</v>
@@ -4788,7 +4812,7 @@
         <v>182</v>
       </c>
       <c r="B222" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>3</v>
@@ -4799,7 +4823,7 @@
         <v>182</v>
       </c>
       <c r="B223" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>3</v>
@@ -4810,7 +4834,7 @@
         <v>182</v>
       </c>
       <c r="B224" s="14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>3</v>
@@ -4821,71 +4845,71 @@
         <v>182</v>
       </c>
       <c r="B225" s="14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A226" s="6" t="s">
+    <row r="226" spans="1:4" ht="21">
+      <c r="A226" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B226" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C226" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D226" s="24"/>
+      <c r="B226" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="227" spans="1:4" ht="21">
       <c r="A227" s="3" t="s">
         <v>182</v>
       </c>
       <c r="B227" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A228" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B228" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C228" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D228" s="24"/>
+    </row>
+    <row r="229" spans="1:4" ht="21">
+      <c r="A229" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B229" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C227" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" ht="21">
-      <c r="B228" s="4"/>
-      <c r="C228" s="2"/>
-    </row>
-    <row r="229" spans="1:4" ht="21">
-      <c r="B229" s="4"/>
-      <c r="C229" s="2"/>
+      <c r="C229" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="230" spans="1:4" ht="21">
-      <c r="A230" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B230" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B230" s="4"/>
+      <c r="C230" s="2"/>
     </row>
     <row r="231" spans="1:4" ht="21">
-      <c r="A231" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B231" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B231" s="4"/>
+      <c r="C231" s="2"/>
     </row>
     <row r="232" spans="1:4" ht="21">
       <c r="A232" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B232" s="14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>3</v>
@@ -4896,7 +4920,7 @@
         <v>204</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>3</v>
@@ -4907,7 +4931,7 @@
         <v>204</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>3</v>
@@ -4918,7 +4942,7 @@
         <v>204</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>3</v>
@@ -4929,7 +4953,7 @@
         <v>204</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>3</v>
@@ -4940,7 +4964,7 @@
         <v>204</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>3</v>
@@ -4951,7 +4975,7 @@
         <v>204</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>3</v>
@@ -4962,7 +4986,7 @@
         <v>204</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>3</v>
@@ -4973,7 +4997,7 @@
         <v>204</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>3</v>
@@ -4984,7 +5008,7 @@
         <v>204</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>3</v>
@@ -4995,7 +5019,7 @@
         <v>204</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>3</v>
@@ -5006,7 +5030,7 @@
         <v>204</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>3</v>
@@ -5017,7 +5041,7 @@
         <v>204</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>3</v>
@@ -5028,7 +5052,7 @@
         <v>204</v>
       </c>
       <c r="B245" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>3</v>
@@ -5039,7 +5063,7 @@
         <v>204</v>
       </c>
       <c r="B246" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>3</v>
@@ -5050,7 +5074,7 @@
         <v>204</v>
       </c>
       <c r="B247" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>3</v>
@@ -5061,7 +5085,7 @@
         <v>204</v>
       </c>
       <c r="B248" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>3</v>
@@ -5072,7 +5096,7 @@
         <v>204</v>
       </c>
       <c r="B249" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>3</v>
@@ -5083,7 +5107,7 @@
         <v>204</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>3</v>
@@ -5094,7 +5118,7 @@
         <v>204</v>
       </c>
       <c r="B251" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>3</v>
@@ -5105,7 +5129,7 @@
         <v>204</v>
       </c>
       <c r="B252" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>3</v>
@@ -5116,7 +5140,7 @@
         <v>204</v>
       </c>
       <c r="B253" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>3</v>
@@ -5127,7 +5151,7 @@
         <v>204</v>
       </c>
       <c r="B254" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>3</v>
@@ -5138,7 +5162,7 @@
         <v>204</v>
       </c>
       <c r="B255" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>3</v>
@@ -5149,7 +5173,7 @@
         <v>204</v>
       </c>
       <c r="B256" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>3</v>
@@ -5160,7 +5184,7 @@
         <v>204</v>
       </c>
       <c r="B257" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>3</v>
@@ -5171,7 +5195,7 @@
         <v>204</v>
       </c>
       <c r="B258" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>3</v>
@@ -5182,7 +5206,7 @@
         <v>204</v>
       </c>
       <c r="B259" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>3</v>
@@ -5193,7 +5217,7 @@
         <v>204</v>
       </c>
       <c r="B260" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>3</v>
@@ -5204,7 +5228,7 @@
         <v>204</v>
       </c>
       <c r="B261" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>3</v>
@@ -5215,7 +5239,7 @@
         <v>204</v>
       </c>
       <c r="B262" s="14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>3</v>
@@ -5226,7 +5250,7 @@
         <v>204</v>
       </c>
       <c r="B263" s="14" t="s">
-        <v>81</v>
+        <v>236</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>3</v>
@@ -5237,48 +5261,48 @@
         <v>204</v>
       </c>
       <c r="B264" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="21">
+      <c r="A265" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B265" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="21">
+      <c r="A266" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B266" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="C264" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" ht="21">
-      <c r="B265" s="4"/>
-      <c r="C265" s="2"/>
-    </row>
-    <row r="266" spans="1:3" ht="21">
-      <c r="B266" s="4"/>
-      <c r="C266" s="2"/>
+      <c r="C266" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="267" spans="1:3" ht="21">
-      <c r="A267" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B267" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B267" s="4"/>
+      <c r="C267" s="2"/>
     </row>
     <row r="268" spans="1:3" ht="21">
-      <c r="A268" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B268" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B268" s="4"/>
+      <c r="C268" s="2"/>
     </row>
     <row r="269" spans="1:3" ht="21">
       <c r="A269" s="3" t="s">
         <v>239</v>
       </c>
       <c r="B269" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>3</v>
@@ -5289,7 +5313,7 @@
         <v>239</v>
       </c>
       <c r="B270" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>3</v>
@@ -5300,7 +5324,7 @@
         <v>239</v>
       </c>
       <c r="B271" s="14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>3</v>
@@ -5311,7 +5335,7 @@
         <v>239</v>
       </c>
       <c r="B272" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>3</v>
@@ -5322,7 +5346,7 @@
         <v>239</v>
       </c>
       <c r="B273" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>3</v>
@@ -5333,7 +5357,7 @@
         <v>239</v>
       </c>
       <c r="B274" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>3</v>
@@ -5344,7 +5368,7 @@
         <v>239</v>
       </c>
       <c r="B275" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>3</v>
@@ -5355,7 +5379,7 @@
         <v>239</v>
       </c>
       <c r="B276" s="14" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>3</v>
@@ -5366,7 +5390,7 @@
         <v>239</v>
       </c>
       <c r="B277" s="14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>3</v>
@@ -5377,7 +5401,7 @@
         <v>239</v>
       </c>
       <c r="B278" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>3</v>
@@ -5388,7 +5412,7 @@
         <v>239</v>
       </c>
       <c r="B279" s="14" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>3</v>
@@ -5399,7 +5423,7 @@
         <v>239</v>
       </c>
       <c r="B280" s="14" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>3</v>
@@ -5410,7 +5434,7 @@
         <v>239</v>
       </c>
       <c r="B281" s="14" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>3</v>
@@ -5421,7 +5445,7 @@
         <v>239</v>
       </c>
       <c r="B282" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>3</v>
@@ -5432,7 +5456,7 @@
         <v>239</v>
       </c>
       <c r="B283" s="14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>3</v>
@@ -5443,7 +5467,7 @@
         <v>239</v>
       </c>
       <c r="B284" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>3</v>
@@ -5454,48 +5478,48 @@
         <v>239</v>
       </c>
       <c r="B285" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" ht="21">
+      <c r="A286" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B286" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" ht="21">
+      <c r="A287" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B287" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="C285" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" ht="21">
-      <c r="B286" s="4"/>
-      <c r="C286" s="2"/>
-    </row>
-    <row r="287" spans="1:3" ht="21">
-      <c r="B287" s="4"/>
-      <c r="C287" s="2"/>
+      <c r="C287" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="288" spans="1:3" ht="21">
-      <c r="A288" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B288" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B288" s="4"/>
+      <c r="C288" s="2"/>
     </row>
     <row r="289" spans="1:3" ht="21">
-      <c r="A289" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B289" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="C289" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B289" s="4"/>
+      <c r="C289" s="2"/>
     </row>
     <row r="290" spans="1:3" ht="21">
       <c r="A290" s="3" t="s">
         <v>259</v>
       </c>
       <c r="B290" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>3</v>
@@ -5506,7 +5530,7 @@
         <v>259</v>
       </c>
       <c r="B291" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>3</v>
@@ -5517,7 +5541,7 @@
         <v>259</v>
       </c>
       <c r="B292" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>3</v>
@@ -5528,7 +5552,7 @@
         <v>259</v>
       </c>
       <c r="B293" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>3</v>
@@ -5539,7 +5563,7 @@
         <v>259</v>
       </c>
       <c r="B294" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>3</v>
@@ -5550,7 +5574,7 @@
         <v>259</v>
       </c>
       <c r="B295" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>3</v>
@@ -5561,7 +5585,7 @@
         <v>259</v>
       </c>
       <c r="B296" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>3</v>
@@ -5572,7 +5596,7 @@
         <v>259</v>
       </c>
       <c r="B297" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>3</v>
@@ -5583,7 +5607,7 @@
         <v>259</v>
       </c>
       <c r="B298" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>3</v>
@@ -5594,7 +5618,7 @@
         <v>259</v>
       </c>
       <c r="B299" s="14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C299" s="2" t="s">
         <v>3</v>
@@ -5605,7 +5629,7 @@
         <v>259</v>
       </c>
       <c r="B300" s="14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>3</v>
@@ -5615,8 +5639,8 @@
       <c r="A301" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B301" s="16" t="s">
-        <v>273</v>
+      <c r="B301" s="14" t="s">
+        <v>271</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>3</v>
@@ -5627,7 +5651,7 @@
         <v>259</v>
       </c>
       <c r="B302" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C302" s="2" t="s">
         <v>3</v>
@@ -5637,8 +5661,8 @@
       <c r="A303" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B303" s="14" t="s">
-        <v>275</v>
+      <c r="B303" s="16" t="s">
+        <v>273</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>3</v>
@@ -5649,7 +5673,7 @@
         <v>259</v>
       </c>
       <c r="B304" s="14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>3</v>
@@ -5660,7 +5684,7 @@
         <v>259</v>
       </c>
       <c r="B305" s="14" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>3</v>
@@ -5671,7 +5695,7 @@
         <v>259</v>
       </c>
       <c r="B306" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>3</v>
@@ -5682,7 +5706,7 @@
         <v>259</v>
       </c>
       <c r="B307" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>3</v>
@@ -5693,7 +5717,7 @@
         <v>259</v>
       </c>
       <c r="B308" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>3</v>
@@ -5704,7 +5728,7 @@
         <v>259</v>
       </c>
       <c r="B309" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>3</v>
@@ -5715,7 +5739,7 @@
         <v>259</v>
       </c>
       <c r="B310" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>3</v>
@@ -5726,7 +5750,7 @@
         <v>259</v>
       </c>
       <c r="B311" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>3</v>
@@ -5737,7 +5761,7 @@
         <v>259</v>
       </c>
       <c r="B312" s="14" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>3</v>
@@ -5748,7 +5772,7 @@
         <v>259</v>
       </c>
       <c r="B313" s="14" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>3</v>
@@ -5759,7 +5783,7 @@
         <v>259</v>
       </c>
       <c r="B314" s="14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>3</v>
@@ -5770,7 +5794,7 @@
         <v>259</v>
       </c>
       <c r="B315" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>3</v>
@@ -5781,7 +5805,7 @@
         <v>259</v>
       </c>
       <c r="B316" s="14" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>3</v>
@@ -5792,7 +5816,7 @@
         <v>259</v>
       </c>
       <c r="B317" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>3</v>
@@ -5803,7 +5827,7 @@
         <v>259</v>
       </c>
       <c r="B318" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>3</v>
@@ -5814,7 +5838,7 @@
         <v>259</v>
       </c>
       <c r="B319" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>3</v>
@@ -5825,7 +5849,7 @@
         <v>259</v>
       </c>
       <c r="B320" s="14" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>3</v>
@@ -5836,7 +5860,7 @@
         <v>259</v>
       </c>
       <c r="B321" s="14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>3</v>
@@ -5847,7 +5871,7 @@
         <v>259</v>
       </c>
       <c r="B322" s="14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>3</v>
@@ -5858,7 +5882,7 @@
         <v>259</v>
       </c>
       <c r="B323" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>3</v>
@@ -5869,7 +5893,7 @@
         <v>259</v>
       </c>
       <c r="B324" s="14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>3</v>
@@ -5880,48 +5904,48 @@
         <v>259</v>
       </c>
       <c r="B325" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" ht="21">
+      <c r="A326" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B326" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" ht="21">
+      <c r="A327" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B327" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="C325" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="326" spans="1:3" ht="21">
-      <c r="B326" s="4"/>
-      <c r="C326" s="2"/>
-    </row>
-    <row r="327" spans="1:3" ht="21">
-      <c r="B327" s="4"/>
-      <c r="C327" s="2"/>
+      <c r="C327" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="328" spans="1:3" ht="21">
-      <c r="A328" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B328" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="C328" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B328" s="4"/>
+      <c r="C328" s="2"/>
     </row>
     <row r="329" spans="1:3" ht="21">
-      <c r="A329" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B329" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="C329" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B329" s="4"/>
+      <c r="C329" s="2"/>
     </row>
     <row r="330" spans="1:3" ht="21">
       <c r="A330" s="5" t="s">
         <v>298</v>
       </c>
       <c r="B330" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>3</v>
@@ -5932,7 +5956,7 @@
         <v>298</v>
       </c>
       <c r="B331" s="14" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C331" s="2" t="s">
         <v>3</v>
@@ -5943,7 +5967,7 @@
         <v>298</v>
       </c>
       <c r="B332" s="14" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C332" s="2" t="s">
         <v>3</v>
@@ -5954,7 +5978,7 @@
         <v>298</v>
       </c>
       <c r="B333" s="14" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>3</v>
@@ -5965,7 +5989,7 @@
         <v>298</v>
       </c>
       <c r="B334" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>3</v>
@@ -5976,7 +6000,7 @@
         <v>298</v>
       </c>
       <c r="B335" s="14" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>3</v>
@@ -5986,8 +6010,8 @@
       <c r="A336" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B336" s="16" t="s">
-        <v>307</v>
+      <c r="B336" s="14" t="s">
+        <v>305</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>3</v>
@@ -5998,7 +6022,7 @@
         <v>298</v>
       </c>
       <c r="B337" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>3</v>
@@ -6008,8 +6032,8 @@
       <c r="A338" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B338" s="14" t="s">
-        <v>309</v>
+      <c r="B338" s="16" t="s">
+        <v>307</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>3</v>
@@ -6020,7 +6044,7 @@
         <v>298</v>
       </c>
       <c r="B339" s="14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>3</v>
@@ -6031,7 +6055,7 @@
         <v>298</v>
       </c>
       <c r="B340" s="14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>3</v>
@@ -6042,7 +6066,7 @@
         <v>298</v>
       </c>
       <c r="B341" s="14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>3</v>
@@ -6053,7 +6077,7 @@
         <v>298</v>
       </c>
       <c r="B342" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>3</v>
@@ -6064,7 +6088,7 @@
         <v>298</v>
       </c>
       <c r="B343" s="14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C343" s="2" t="s">
         <v>3</v>
@@ -6075,7 +6099,7 @@
         <v>298</v>
       </c>
       <c r="B344" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>3</v>
@@ -6086,48 +6110,48 @@
         <v>298</v>
       </c>
       <c r="B345" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" ht="21">
+      <c r="A346" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B346" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" ht="21">
+      <c r="A347" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B347" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="C345" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" ht="21">
-      <c r="B346" s="4"/>
-      <c r="C346" s="2"/>
-    </row>
-    <row r="347" spans="1:3" ht="21">
-      <c r="B347" s="4"/>
-      <c r="C347" s="2"/>
+      <c r="C347" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="348" spans="1:3" ht="21">
-      <c r="A348" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B348" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C348" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B348" s="4"/>
+      <c r="C348" s="2"/>
     </row>
     <row r="349" spans="1:3" ht="21">
-      <c r="A349" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B349" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="C349" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B349" s="4"/>
+      <c r="C349" s="2"/>
     </row>
     <row r="350" spans="1:3" ht="21">
       <c r="A350" s="5" t="s">
         <v>317</v>
       </c>
       <c r="B350" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>3</v>
@@ -6138,7 +6162,7 @@
         <v>317</v>
       </c>
       <c r="B351" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>3</v>
@@ -6149,7 +6173,7 @@
         <v>317</v>
       </c>
       <c r="B352" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>3</v>
@@ -6160,7 +6184,7 @@
         <v>317</v>
       </c>
       <c r="B353" s="14" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>3</v>
@@ -6171,7 +6195,7 @@
         <v>317</v>
       </c>
       <c r="B354" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>3</v>
@@ -6182,7 +6206,7 @@
         <v>317</v>
       </c>
       <c r="B355" s="14" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>3</v>
@@ -6193,7 +6217,7 @@
         <v>317</v>
       </c>
       <c r="B356" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>3</v>
@@ -6204,7 +6228,7 @@
         <v>317</v>
       </c>
       <c r="B357" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>3</v>
@@ -6215,7 +6239,7 @@
         <v>317</v>
       </c>
       <c r="B358" s="14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>3</v>
@@ -6226,7 +6250,7 @@
         <v>317</v>
       </c>
       <c r="B359" s="14" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>3</v>
@@ -6237,7 +6261,7 @@
         <v>317</v>
       </c>
       <c r="B360" s="14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>3</v>
@@ -6248,7 +6272,7 @@
         <v>317</v>
       </c>
       <c r="B361" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>3</v>
@@ -6259,7 +6283,7 @@
         <v>317</v>
       </c>
       <c r="B362" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>3</v>
@@ -6270,7 +6294,7 @@
         <v>317</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>3</v>
@@ -6281,7 +6305,7 @@
         <v>317</v>
       </c>
       <c r="B364" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>3</v>
@@ -6292,7 +6316,7 @@
         <v>317</v>
       </c>
       <c r="B365" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>3</v>
@@ -6303,7 +6327,7 @@
         <v>317</v>
       </c>
       <c r="B366" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>3</v>
@@ -6314,7 +6338,7 @@
         <v>317</v>
       </c>
       <c r="B367" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>3</v>
@@ -6325,7 +6349,7 @@
         <v>317</v>
       </c>
       <c r="B368" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>3</v>
@@ -6336,7 +6360,7 @@
         <v>317</v>
       </c>
       <c r="B369" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>3</v>
@@ -6347,7 +6371,7 @@
         <v>317</v>
       </c>
       <c r="B370" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>3</v>
@@ -6358,7 +6382,7 @@
         <v>317</v>
       </c>
       <c r="B371" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>3</v>
@@ -6369,7 +6393,7 @@
         <v>317</v>
       </c>
       <c r="B372" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>3</v>
@@ -6380,52 +6404,52 @@
         <v>317</v>
       </c>
       <c r="B373" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="374" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A374" s="6" t="s">
+    <row r="374" spans="1:4" ht="21">
+      <c r="A374" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B374" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="C374" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D374" s="24"/>
+      <c r="B374" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="375" spans="1:4" ht="21">
       <c r="A375" s="5" t="s">
         <v>317</v>
       </c>
       <c r="B375" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="376" spans="1:4" ht="21">
-      <c r="A376" s="5" t="s">
+    <row r="376" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A376" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="B376" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="C376" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B376" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C376" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D376" s="24"/>
     </row>
     <row r="377" spans="1:4" ht="21">
       <c r="A377" s="5" t="s">
         <v>317</v>
       </c>
       <c r="B377" s="14" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>3</v>
@@ -6436,7 +6460,7 @@
         <v>317</v>
       </c>
       <c r="B378" s="14" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>3</v>
@@ -6447,7 +6471,7 @@
         <v>317</v>
       </c>
       <c r="B379" s="14" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>3</v>
@@ -6458,7 +6482,7 @@
         <v>317</v>
       </c>
       <c r="B380" s="14" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>3</v>
@@ -6469,7 +6493,7 @@
         <v>317</v>
       </c>
       <c r="B381" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>3</v>
@@ -6480,7 +6504,7 @@
         <v>317</v>
       </c>
       <c r="B382" s="14" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>3</v>
@@ -6491,7 +6515,7 @@
         <v>317</v>
       </c>
       <c r="B383" s="14" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>3</v>
@@ -6502,7 +6526,7 @@
         <v>317</v>
       </c>
       <c r="B384" s="14" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>3</v>
@@ -6513,7 +6537,7 @@
         <v>317</v>
       </c>
       <c r="B385" s="14" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>3</v>
@@ -6524,7 +6548,7 @@
         <v>317</v>
       </c>
       <c r="B386" s="14" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>3</v>
@@ -6535,7 +6559,7 @@
         <v>317</v>
       </c>
       <c r="B387" s="14" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>3</v>
@@ -6546,7 +6570,7 @@
         <v>317</v>
       </c>
       <c r="B388" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>3</v>
@@ -6557,7 +6581,7 @@
         <v>317</v>
       </c>
       <c r="B389" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>3</v>
@@ -6568,48 +6592,48 @@
         <v>317</v>
       </c>
       <c r="B390" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" ht="21">
+      <c r="A391" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B391" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" ht="21">
+      <c r="A392" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B392" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="C390" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="391" spans="1:3" ht="21">
-      <c r="B391" s="4"/>
-      <c r="C391" s="2"/>
-    </row>
-    <row r="392" spans="1:3" ht="21">
-      <c r="B392" s="4"/>
-      <c r="C392" s="2"/>
+      <c r="C392" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="393" spans="1:3" ht="21">
-      <c r="A393" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B393" s="14" t="s">
-        <v>362</v>
-      </c>
-      <c r="C393" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B393" s="4"/>
+      <c r="C393" s="2"/>
     </row>
     <row r="394" spans="1:3" ht="21">
-      <c r="A394" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B394" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="C394" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B394" s="4"/>
+      <c r="C394" s="2"/>
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
         <v>361</v>
       </c>
       <c r="B395" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>3</v>
@@ -6620,7 +6644,7 @@
         <v>361</v>
       </c>
       <c r="B396" s="14" t="s">
-        <v>83</v>
+        <v>363</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>3</v>
@@ -6631,7 +6655,7 @@
         <v>361</v>
       </c>
       <c r="B397" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>3</v>
@@ -6642,51 +6666,51 @@
         <v>361</v>
       </c>
       <c r="B398" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" ht="21">
+      <c r="A399" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B399" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" ht="21">
+      <c r="A400" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B400" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="C398" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="399" spans="1:3" ht="21">
-      <c r="B399" s="4"/>
-      <c r="C399" s="2"/>
-    </row>
-    <row r="400" spans="1:3" ht="21">
-      <c r="B400" s="4"/>
-      <c r="C400" s="2"/>
+      <c r="C400" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="401" spans="1:3" ht="21">
-      <c r="A401" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B401" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="C401" s="36" t="s">
-        <v>441</v>
-      </c>
+      <c r="B401" s="4"/>
+      <c r="C401" s="2"/>
     </row>
     <row r="402" spans="1:3" ht="21">
-      <c r="A402" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B402" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="C402" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B402" s="4"/>
+      <c r="C402" s="2"/>
     </row>
     <row r="403" spans="1:3" ht="21">
       <c r="A403" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B403" s="14" t="s">
-        <v>370</v>
-      </c>
-      <c r="C403" s="2" t="s">
-        <v>3</v>
+        <v>368</v>
+      </c>
+      <c r="C403" s="36" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
@@ -6694,7 +6718,7 @@
         <v>367</v>
       </c>
       <c r="B404" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>3</v>
@@ -6705,7 +6729,7 @@
         <v>367</v>
       </c>
       <c r="B405" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>3</v>
@@ -6716,10 +6740,10 @@
         <v>367</v>
       </c>
       <c r="B406" s="14" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>441</v>
+        <v>3</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">
@@ -6727,7 +6751,7 @@
         <v>367</v>
       </c>
       <c r="B407" s="14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>3</v>
@@ -6738,10 +6762,10 @@
         <v>367</v>
       </c>
       <c r="B408" s="14" t="s">
-        <v>247</v>
+        <v>373</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>3</v>
+        <v>441</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">
@@ -6749,7 +6773,7 @@
         <v>367</v>
       </c>
       <c r="B409" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>3</v>
@@ -6760,7 +6784,7 @@
         <v>367</v>
       </c>
       <c r="B410" s="14" t="s">
-        <v>376</v>
+        <v>247</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>3</v>
@@ -6771,7 +6795,7 @@
         <v>367</v>
       </c>
       <c r="B411" s="14" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>3</v>
@@ -6782,7 +6806,7 @@
         <v>367</v>
       </c>
       <c r="B412" s="14" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>3</v>
@@ -6793,7 +6817,7 @@
         <v>367</v>
       </c>
       <c r="B413" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>3</v>
@@ -6804,7 +6828,7 @@
         <v>367</v>
       </c>
       <c r="B414" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>3</v>
@@ -6815,7 +6839,7 @@
         <v>367</v>
       </c>
       <c r="B415" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>3</v>
@@ -6826,7 +6850,7 @@
         <v>367</v>
       </c>
       <c r="B416" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>3</v>
@@ -6837,7 +6861,7 @@
         <v>367</v>
       </c>
       <c r="B417" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>3</v>
@@ -6848,7 +6872,7 @@
         <v>367</v>
       </c>
       <c r="B418" s="14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>3</v>
@@ -6859,7 +6883,7 @@
         <v>367</v>
       </c>
       <c r="B419" s="14" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>3</v>
@@ -6870,7 +6894,7 @@
         <v>367</v>
       </c>
       <c r="B420" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>3</v>
@@ -6881,7 +6905,7 @@
         <v>367</v>
       </c>
       <c r="B421" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>3</v>
@@ -6892,7 +6916,7 @@
         <v>367</v>
       </c>
       <c r="B422" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>3</v>
@@ -6903,7 +6927,7 @@
         <v>367</v>
       </c>
       <c r="B423" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>3</v>
@@ -6914,7 +6938,7 @@
         <v>367</v>
       </c>
       <c r="B424" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>3</v>
@@ -6925,7 +6949,7 @@
         <v>367</v>
       </c>
       <c r="B425" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>3</v>
@@ -6936,7 +6960,7 @@
         <v>367</v>
       </c>
       <c r="B426" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>3</v>
@@ -6947,7 +6971,7 @@
         <v>367</v>
       </c>
       <c r="B427" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>3</v>
@@ -6958,7 +6982,7 @@
         <v>367</v>
       </c>
       <c r="B428" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>3</v>
@@ -6969,7 +6993,7 @@
         <v>367</v>
       </c>
       <c r="B429" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>3</v>
@@ -6980,7 +7004,7 @@
         <v>367</v>
       </c>
       <c r="B430" s="14" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>3</v>
@@ -6991,7 +7015,7 @@
         <v>367</v>
       </c>
       <c r="B431" s="14" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>3</v>
@@ -7002,7 +7026,7 @@
         <v>367</v>
       </c>
       <c r="B432" s="14" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>3</v>
@@ -7013,7 +7037,7 @@
         <v>367</v>
       </c>
       <c r="B433" s="14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>3</v>
@@ -7024,52 +7048,52 @@
         <v>367</v>
       </c>
       <c r="B434" s="14" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A435" s="6" t="s">
+    <row r="435" spans="1:4" ht="21">
+      <c r="A435" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="B435" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="C435" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D435" s="24"/>
+      <c r="B435" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="C435" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="436" spans="1:4" ht="21">
       <c r="A436" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B436" s="14" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="437" spans="1:4" ht="21">
-      <c r="A437" s="3" t="s">
+    <row r="437" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A437" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="B437" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="C437" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B437" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C437" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D437" s="24"/>
     </row>
     <row r="438" spans="1:4" ht="21">
       <c r="A438" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B438" s="14" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>3</v>
@@ -7080,7 +7104,7 @@
         <v>367</v>
       </c>
       <c r="B439" s="14" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>3</v>
@@ -7091,7 +7115,7 @@
         <v>367</v>
       </c>
       <c r="B440" s="14" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>3</v>
@@ -7102,7 +7126,7 @@
         <v>367</v>
       </c>
       <c r="B441" s="14" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>3</v>
@@ -7113,7 +7137,7 @@
         <v>367</v>
       </c>
       <c r="B442" s="14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>3</v>
@@ -7124,7 +7148,7 @@
         <v>367</v>
       </c>
       <c r="B443" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>3</v>
@@ -7135,7 +7159,7 @@
         <v>367</v>
       </c>
       <c r="B444" s="14" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>3</v>
@@ -7146,7 +7170,7 @@
         <v>367</v>
       </c>
       <c r="B445" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>3</v>
@@ -7157,64 +7181,64 @@
         <v>367</v>
       </c>
       <c r="B446" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" ht="21">
+      <c r="A447" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B447" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="C447" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" ht="21">
+      <c r="A448" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B448" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="C446" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="447" spans="1:4" s="26" customFormat="1" ht="21">
-      <c r="A447" s="25" t="s">
+      <c r="C448" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" s="26" customFormat="1" ht="21">
+      <c r="A449" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="B447" s="26" t="s">
+      <c r="B449" s="26" t="s">
         <v>413</v>
       </c>
-      <c r="C447" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D447" s="27"/>
-    </row>
-    <row r="448" spans="1:4" s="26" customFormat="1" ht="21">
-      <c r="A448" s="25" t="s">
+      <c r="C449" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D449" s="27"/>
+    </row>
+    <row r="450" spans="1:4" s="26" customFormat="1" ht="21">
+      <c r="A450" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="B448" s="26" t="s">
+      <c r="B450" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="C448" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D448" s="27"/>
-    </row>
-    <row r="449" spans="1:4" ht="21">
-      <c r="A449" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B449" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="C449" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="450" spans="1:4" ht="21">
-      <c r="A450" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B450" s="14" t="s">
-        <v>416</v>
-      </c>
-      <c r="C450" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C450" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D450" s="27"/>
     </row>
     <row r="451" spans="1:4" ht="21">
       <c r="A451" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B451" s="14" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>3</v>
@@ -7225,86 +7249,86 @@
         <v>367</v>
       </c>
       <c r="B452" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="453" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A453" s="6" t="s">
+    <row r="453" spans="1:4" ht="21">
+      <c r="A453" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="B453" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="C453" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D453" s="24"/>
+      <c r="B453" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="C453" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="454" spans="1:4" ht="21">
       <c r="A454" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B454" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="C454" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A455" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="B455" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C455" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D455" s="24"/>
+    </row>
+    <row r="456" spans="1:4" ht="21">
+      <c r="A456" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B456" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="C454" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="455" spans="1:4" ht="21">
-      <c r="A455" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B455" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="C455" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="456" spans="1:4" s="7" customFormat="1" ht="21">
-      <c r="A456" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="B456" s="7" t="s">
-        <v>422</v>
-      </c>
-      <c r="C456" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D456" s="24"/>
+      <c r="C456" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="457" spans="1:4" ht="21">
       <c r="A457" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B457" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="458" spans="1:4" ht="21">
-      <c r="A458" s="3" t="s">
+    <row r="458" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A458" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="B458" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="C458" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B458" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C458" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D458" s="24"/>
     </row>
     <row r="459" spans="1:4" ht="21">
       <c r="A459" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B459" s="14" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>3</v>
@@ -7315,49 +7339,49 @@
         <v>367</v>
       </c>
       <c r="B460" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C460" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" ht="21">
+      <c r="A461" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B461" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="C461" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" ht="21">
+      <c r="A462" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B462" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="C460" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="461" spans="1:4" ht="21">
-      <c r="B461" s="4"/>
-      <c r="C461" s="2"/>
-    </row>
-    <row r="462" spans="1:4" ht="21">
-      <c r="A462" s="5"/>
-      <c r="B462" s="4"/>
-      <c r="C462" s="2"/>
+      <c r="C462" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="463" spans="1:4" ht="21">
-      <c r="A463" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B463" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="C463" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B463" s="4"/>
+      <c r="C463" s="2"/>
     </row>
     <row r="464" spans="1:4" ht="21">
-      <c r="A464" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="B464" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="C464" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A464" s="5"/>
+      <c r="B464" s="4"/>
+      <c r="C464" s="2"/>
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="3" t="s">
         <v>427</v>
       </c>
       <c r="B465" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>3</v>
@@ -7368,7 +7392,7 @@
         <v>427</v>
       </c>
       <c r="B466" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>3</v>
@@ -7379,7 +7403,7 @@
         <v>427</v>
       </c>
       <c r="B467" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>3</v>
@@ -7390,10 +7414,10 @@
         <v>427</v>
       </c>
       <c r="B468" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>441</v>
+        <v>3</v>
       </c>
     </row>
     <row r="469" spans="1:3" ht="21">
@@ -7401,7 +7425,7 @@
         <v>427</v>
       </c>
       <c r="B469" s="14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>3</v>
@@ -7412,10 +7436,10 @@
         <v>427</v>
       </c>
       <c r="B470" s="14" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>3</v>
+        <v>441</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="21">
@@ -7423,7 +7447,7 @@
         <v>427</v>
       </c>
       <c r="B471" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>3</v>
@@ -7434,9 +7458,31 @@
         <v>427</v>
       </c>
       <c r="B472" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C472" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" ht="21">
+      <c r="A473" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B473" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="C473" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" ht="21">
+      <c r="A474" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B474" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="C472" s="2" t="s">
+      <c r="C474" s="2" t="s">
         <v>441</v>
       </c>
     </row>
@@ -7627,256 +7673,256 @@
     <hyperlink ref="B202" r:id="rId183"/>
     <hyperlink ref="B203" r:id="rId184"/>
     <hyperlink ref="B206" r:id="rId185"/>
-    <hyperlink ref="B207" r:id="rId186"/>
-    <hyperlink ref="B208" r:id="rId187"/>
-    <hyperlink ref="B209" r:id="rId188"/>
-    <hyperlink ref="B210" r:id="rId189"/>
-    <hyperlink ref="B211" r:id="rId190"/>
-    <hyperlink ref="B212" r:id="rId191"/>
-    <hyperlink ref="B213" r:id="rId192"/>
-    <hyperlink ref="B214" r:id="rId193"/>
-    <hyperlink ref="B215" r:id="rId194"/>
-    <hyperlink ref="B216" r:id="rId195" display="Merge two BST [ V.V.V&gt;IMP ]"/>
-    <hyperlink ref="B217" r:id="rId196"/>
-    <hyperlink ref="B218" r:id="rId197"/>
-    <hyperlink ref="B219" r:id="rId198"/>
-    <hyperlink ref="B220" r:id="rId199"/>
-    <hyperlink ref="B221" r:id="rId200"/>
-    <hyperlink ref="B222" r:id="rId201"/>
-    <hyperlink ref="B223" r:id="rId202"/>
-    <hyperlink ref="B224" r:id="rId203"/>
-    <hyperlink ref="B225" r:id="rId204"/>
-    <hyperlink ref="B226" r:id="rId205"/>
-    <hyperlink ref="B227" r:id="rId206"/>
-    <hyperlink ref="B230" r:id="rId207"/>
-    <hyperlink ref="B231" r:id="rId208"/>
-    <hyperlink ref="B232" r:id="rId209"/>
-    <hyperlink ref="B233" r:id="rId210"/>
-    <hyperlink ref="B234" r:id="rId211"/>
-    <hyperlink ref="B235" r:id="rId212"/>
-    <hyperlink ref="B236" r:id="rId213"/>
-    <hyperlink ref="B237" r:id="rId214"/>
-    <hyperlink ref="B238" r:id="rId215"/>
-    <hyperlink ref="B239" r:id="rId216"/>
-    <hyperlink ref="B240" r:id="rId217"/>
-    <hyperlink ref="B241" r:id="rId218"/>
-    <hyperlink ref="B242" r:id="rId219"/>
-    <hyperlink ref="B243" r:id="rId220"/>
-    <hyperlink ref="B244" r:id="rId221"/>
-    <hyperlink ref="B245" r:id="rId222"/>
-    <hyperlink ref="B246" r:id="rId223"/>
-    <hyperlink ref="B247" r:id="rId224"/>
-    <hyperlink ref="B248" r:id="rId225"/>
-    <hyperlink ref="B249" r:id="rId226" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B250" r:id="rId227"/>
-    <hyperlink ref="B251" r:id="rId228"/>
-    <hyperlink ref="B252" r:id="rId229"/>
-    <hyperlink ref="B253" r:id="rId230"/>
-    <hyperlink ref="B254" r:id="rId231"/>
-    <hyperlink ref="B255" r:id="rId232"/>
-    <hyperlink ref="B256" r:id="rId233"/>
-    <hyperlink ref="B257" r:id="rId234"/>
-    <hyperlink ref="B258" r:id="rId235"/>
-    <hyperlink ref="B259" r:id="rId236"/>
-    <hyperlink ref="B260" r:id="rId237"/>
-    <hyperlink ref="B261" r:id="rId238"/>
-    <hyperlink ref="B262" r:id="rId239"/>
-    <hyperlink ref="B263" r:id="rId240"/>
-    <hyperlink ref="B264" r:id="rId241"/>
-    <hyperlink ref="B267" r:id="rId242"/>
-    <hyperlink ref="B268" r:id="rId243"/>
-    <hyperlink ref="B269" r:id="rId244"/>
-    <hyperlink ref="B270" r:id="rId245"/>
-    <hyperlink ref="B271" r:id="rId246"/>
-    <hyperlink ref="B272" r:id="rId247"/>
-    <hyperlink ref="B273" r:id="rId248"/>
-    <hyperlink ref="B274" r:id="rId249"/>
-    <hyperlink ref="B275" r:id="rId250"/>
-    <hyperlink ref="B276" r:id="rId251"/>
-    <hyperlink ref="B277" r:id="rId252"/>
-    <hyperlink ref="B278" r:id="rId253"/>
-    <hyperlink ref="B279" r:id="rId254"/>
-    <hyperlink ref="B280" r:id="rId255"/>
-    <hyperlink ref="B281" r:id="rId256"/>
-    <hyperlink ref="B282" r:id="rId257"/>
-    <hyperlink ref="B283" r:id="rId258"/>
-    <hyperlink ref="B284" r:id="rId259"/>
-    <hyperlink ref="B285" r:id="rId260"/>
-    <hyperlink ref="B288" r:id="rId261"/>
-    <hyperlink ref="B289" r:id="rId262"/>
-    <hyperlink ref="B290" r:id="rId263"/>
-    <hyperlink ref="B291" r:id="rId264"/>
-    <hyperlink ref="B292" r:id="rId265"/>
-    <hyperlink ref="B293" r:id="rId266"/>
-    <hyperlink ref="B294" r:id="rId267"/>
-    <hyperlink ref="B295" r:id="rId268"/>
-    <hyperlink ref="B296" r:id="rId269"/>
-    <hyperlink ref="B297" r:id="rId270"/>
-    <hyperlink ref="B298" r:id="rId271" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B299" r:id="rId272"/>
-    <hyperlink ref="B300" r:id="rId273"/>
-    <hyperlink ref="B301" r:id="rId274"/>
-    <hyperlink ref="B302" r:id="rId275"/>
-    <hyperlink ref="B303" r:id="rId276"/>
-    <hyperlink ref="B304" r:id="rId277"/>
-    <hyperlink ref="B305" r:id="rId278"/>
-    <hyperlink ref="B306" r:id="rId279"/>
-    <hyperlink ref="B307" r:id="rId280"/>
-    <hyperlink ref="B308" r:id="rId281"/>
-    <hyperlink ref="B309" r:id="rId282"/>
-    <hyperlink ref="B310" r:id="rId283"/>
-    <hyperlink ref="B311" r:id="rId284"/>
-    <hyperlink ref="B312" r:id="rId285"/>
-    <hyperlink ref="B313" r:id="rId286"/>
-    <hyperlink ref="B314" r:id="rId287"/>
-    <hyperlink ref="B315" r:id="rId288"/>
-    <hyperlink ref="B316" r:id="rId289"/>
-    <hyperlink ref="B317" r:id="rId290"/>
-    <hyperlink ref="B318" r:id="rId291"/>
-    <hyperlink ref="B319" r:id="rId292"/>
-    <hyperlink ref="B320" r:id="rId293"/>
-    <hyperlink ref="B321" r:id="rId294"/>
-    <hyperlink ref="B322" r:id="rId295"/>
-    <hyperlink ref="B323" r:id="rId296"/>
-    <hyperlink ref="B324" r:id="rId297"/>
-    <hyperlink ref="B325" r:id="rId298"/>
-    <hyperlink ref="B328" r:id="rId299"/>
-    <hyperlink ref="B329" r:id="rId300"/>
-    <hyperlink ref="B330" r:id="rId301"/>
-    <hyperlink ref="B331" r:id="rId302"/>
-    <hyperlink ref="B332" r:id="rId303"/>
-    <hyperlink ref="B333" r:id="rId304"/>
-    <hyperlink ref="B334" r:id="rId305"/>
-    <hyperlink ref="B335" r:id="rId306"/>
-    <hyperlink ref="B336" r:id="rId307"/>
-    <hyperlink ref="B337" r:id="rId308"/>
-    <hyperlink ref="B338" r:id="rId309"/>
-    <hyperlink ref="B339" r:id="rId310"/>
-    <hyperlink ref="B340" r:id="rId311"/>
-    <hyperlink ref="B341" r:id="rId312"/>
-    <hyperlink ref="B342" r:id="rId313"/>
-    <hyperlink ref="B343" r:id="rId314"/>
-    <hyperlink ref="B344" r:id="rId315"/>
-    <hyperlink ref="B345" r:id="rId316"/>
-    <hyperlink ref="B349" r:id="rId317"/>
-    <hyperlink ref="B350" r:id="rId318"/>
-    <hyperlink ref="B351" r:id="rId319"/>
-    <hyperlink ref="B352" r:id="rId320"/>
-    <hyperlink ref="B353" r:id="rId321"/>
-    <hyperlink ref="B354" r:id="rId322"/>
-    <hyperlink ref="B355" r:id="rId323"/>
-    <hyperlink ref="B356" r:id="rId324"/>
-    <hyperlink ref="B357" r:id="rId325"/>
-    <hyperlink ref="B358" r:id="rId326"/>
-    <hyperlink ref="B359" r:id="rId327"/>
-    <hyperlink ref="B360" r:id="rId328"/>
-    <hyperlink ref="B361" r:id="rId329"/>
-    <hyperlink ref="B362" r:id="rId330"/>
-    <hyperlink ref="B363" r:id="rId331"/>
-    <hyperlink ref="B364" r:id="rId332"/>
-    <hyperlink ref="B365" r:id="rId333"/>
-    <hyperlink ref="B366" r:id="rId334"/>
-    <hyperlink ref="B367" r:id="rId335"/>
-    <hyperlink ref="B368" r:id="rId336"/>
-    <hyperlink ref="B369" r:id="rId337"/>
-    <hyperlink ref="B370" r:id="rId338"/>
-    <hyperlink ref="B371" r:id="rId339" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B372" r:id="rId340"/>
-    <hyperlink ref="B373" r:id="rId341"/>
-    <hyperlink ref="B374" r:id="rId342"/>
-    <hyperlink ref="B375" r:id="rId343"/>
-    <hyperlink ref="B376" r:id="rId344"/>
-    <hyperlink ref="B377" r:id="rId345"/>
-    <hyperlink ref="B378" r:id="rId346"/>
-    <hyperlink ref="B379" r:id="rId347"/>
-    <hyperlink ref="B380" r:id="rId348"/>
-    <hyperlink ref="B381" r:id="rId349"/>
-    <hyperlink ref="B382" r:id="rId350"/>
-    <hyperlink ref="B383" r:id="rId351"/>
-    <hyperlink ref="B384" r:id="rId352"/>
-    <hyperlink ref="B385" r:id="rId353"/>
-    <hyperlink ref="B387" r:id="rId354"/>
-    <hyperlink ref="B386" r:id="rId355"/>
-    <hyperlink ref="B388" r:id="rId356"/>
-    <hyperlink ref="B389" r:id="rId357"/>
-    <hyperlink ref="B390" r:id="rId358"/>
-    <hyperlink ref="B393" r:id="rId359"/>
-    <hyperlink ref="B394" r:id="rId360"/>
-    <hyperlink ref="B395" r:id="rId361"/>
-    <hyperlink ref="B396" r:id="rId362"/>
-    <hyperlink ref="B397" r:id="rId363"/>
-    <hyperlink ref="B398" r:id="rId364"/>
-    <hyperlink ref="B401" r:id="rId365"/>
-    <hyperlink ref="B402" r:id="rId366"/>
-    <hyperlink ref="B403" r:id="rId367"/>
-    <hyperlink ref="B404" r:id="rId368"/>
-    <hyperlink ref="B405" r:id="rId369"/>
-    <hyperlink ref="B406" r:id="rId370"/>
-    <hyperlink ref="B407" r:id="rId371"/>
-    <hyperlink ref="B408" r:id="rId372"/>
-    <hyperlink ref="B409" r:id="rId373"/>
-    <hyperlink ref="B410" r:id="rId374"/>
-    <hyperlink ref="B411" r:id="rId375"/>
-    <hyperlink ref="B412" r:id="rId376"/>
-    <hyperlink ref="B413" r:id="rId377"/>
-    <hyperlink ref="B414" r:id="rId378"/>
-    <hyperlink ref="B415" r:id="rId379"/>
-    <hyperlink ref="B416" r:id="rId380"/>
-    <hyperlink ref="B417" r:id="rId381"/>
-    <hyperlink ref="B418" r:id="rId382"/>
-    <hyperlink ref="B419" r:id="rId383"/>
-    <hyperlink ref="B420" r:id="rId384"/>
-    <hyperlink ref="B421" r:id="rId385"/>
-    <hyperlink ref="B422" r:id="rId386"/>
-    <hyperlink ref="B423" r:id="rId387"/>
-    <hyperlink ref="B424" r:id="rId388"/>
-    <hyperlink ref="B425" r:id="rId389"/>
-    <hyperlink ref="B426" r:id="rId390"/>
-    <hyperlink ref="B427" r:id="rId391"/>
-    <hyperlink ref="B428" r:id="rId392"/>
-    <hyperlink ref="B429" r:id="rId393"/>
-    <hyperlink ref="B430" r:id="rId394"/>
-    <hyperlink ref="B431" r:id="rId395"/>
-    <hyperlink ref="B432" r:id="rId396"/>
-    <hyperlink ref="B433" r:id="rId397"/>
-    <hyperlink ref="B434" r:id="rId398"/>
-    <hyperlink ref="B435" r:id="rId399"/>
-    <hyperlink ref="B436" r:id="rId400"/>
-    <hyperlink ref="B437" r:id="rId401"/>
-    <hyperlink ref="B438" r:id="rId402"/>
-    <hyperlink ref="B439" r:id="rId403"/>
-    <hyperlink ref="B440" r:id="rId404"/>
-    <hyperlink ref="B442" r:id="rId405"/>
-    <hyperlink ref="B441" r:id="rId406"/>
-    <hyperlink ref="B443" r:id="rId407"/>
-    <hyperlink ref="B444" r:id="rId408"/>
-    <hyperlink ref="B445" r:id="rId409"/>
-    <hyperlink ref="B446" r:id="rId410"/>
-    <hyperlink ref="B447" r:id="rId411"/>
-    <hyperlink ref="B448" r:id="rId412"/>
-    <hyperlink ref="B449" r:id="rId413"/>
-    <hyperlink ref="B450" r:id="rId414"/>
-    <hyperlink ref="B451" r:id="rId415"/>
-    <hyperlink ref="B452" r:id="rId416"/>
-    <hyperlink ref="B453" r:id="rId417"/>
-    <hyperlink ref="B460" r:id="rId418"/>
-    <hyperlink ref="B459" r:id="rId419"/>
-    <hyperlink ref="B458" r:id="rId420"/>
-    <hyperlink ref="B457" r:id="rId421"/>
-    <hyperlink ref="B456" r:id="rId422"/>
-    <hyperlink ref="B455" r:id="rId423"/>
-    <hyperlink ref="B454" r:id="rId424"/>
-    <hyperlink ref="B463" r:id="rId425"/>
-    <hyperlink ref="B464" r:id="rId426"/>
-    <hyperlink ref="B465" r:id="rId427"/>
-    <hyperlink ref="B466" r:id="rId428"/>
-    <hyperlink ref="B467" r:id="rId429"/>
-    <hyperlink ref="B468" r:id="rId430"/>
-    <hyperlink ref="B469" r:id="rId431"/>
-    <hyperlink ref="B472" r:id="rId432"/>
-    <hyperlink ref="B470" r:id="rId433"/>
-    <hyperlink ref="B471" r:id="rId434" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B348" r:id="rId435"/>
+    <hyperlink ref="B209" r:id="rId186"/>
+    <hyperlink ref="B210" r:id="rId187"/>
+    <hyperlink ref="B211" r:id="rId188"/>
+    <hyperlink ref="B212" r:id="rId189"/>
+    <hyperlink ref="B213" r:id="rId190"/>
+    <hyperlink ref="B214" r:id="rId191"/>
+    <hyperlink ref="B215" r:id="rId192"/>
+    <hyperlink ref="B216" r:id="rId193"/>
+    <hyperlink ref="B217" r:id="rId194"/>
+    <hyperlink ref="B218" r:id="rId195" display="Merge two BST [ V.V.V&gt;IMP ]"/>
+    <hyperlink ref="B219" r:id="rId196"/>
+    <hyperlink ref="B220" r:id="rId197"/>
+    <hyperlink ref="B221" r:id="rId198"/>
+    <hyperlink ref="B222" r:id="rId199"/>
+    <hyperlink ref="B223" r:id="rId200"/>
+    <hyperlink ref="B224" r:id="rId201"/>
+    <hyperlink ref="B225" r:id="rId202"/>
+    <hyperlink ref="B226" r:id="rId203"/>
+    <hyperlink ref="B227" r:id="rId204"/>
+    <hyperlink ref="B228" r:id="rId205"/>
+    <hyperlink ref="B229" r:id="rId206"/>
+    <hyperlink ref="B232" r:id="rId207"/>
+    <hyperlink ref="B233" r:id="rId208"/>
+    <hyperlink ref="B234" r:id="rId209"/>
+    <hyperlink ref="B235" r:id="rId210"/>
+    <hyperlink ref="B236" r:id="rId211"/>
+    <hyperlink ref="B237" r:id="rId212"/>
+    <hyperlink ref="B238" r:id="rId213"/>
+    <hyperlink ref="B239" r:id="rId214"/>
+    <hyperlink ref="B240" r:id="rId215"/>
+    <hyperlink ref="B241" r:id="rId216"/>
+    <hyperlink ref="B242" r:id="rId217"/>
+    <hyperlink ref="B243" r:id="rId218"/>
+    <hyperlink ref="B244" r:id="rId219"/>
+    <hyperlink ref="B245" r:id="rId220"/>
+    <hyperlink ref="B246" r:id="rId221"/>
+    <hyperlink ref="B247" r:id="rId222"/>
+    <hyperlink ref="B248" r:id="rId223"/>
+    <hyperlink ref="B249" r:id="rId224"/>
+    <hyperlink ref="B250" r:id="rId225"/>
+    <hyperlink ref="B251" r:id="rId226" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B252" r:id="rId227"/>
+    <hyperlink ref="B253" r:id="rId228"/>
+    <hyperlink ref="B254" r:id="rId229"/>
+    <hyperlink ref="B255" r:id="rId230"/>
+    <hyperlink ref="B256" r:id="rId231"/>
+    <hyperlink ref="B257" r:id="rId232"/>
+    <hyperlink ref="B258" r:id="rId233"/>
+    <hyperlink ref="B259" r:id="rId234"/>
+    <hyperlink ref="B260" r:id="rId235"/>
+    <hyperlink ref="B261" r:id="rId236"/>
+    <hyperlink ref="B262" r:id="rId237"/>
+    <hyperlink ref="B263" r:id="rId238"/>
+    <hyperlink ref="B264" r:id="rId239"/>
+    <hyperlink ref="B265" r:id="rId240"/>
+    <hyperlink ref="B266" r:id="rId241"/>
+    <hyperlink ref="B269" r:id="rId242"/>
+    <hyperlink ref="B270" r:id="rId243"/>
+    <hyperlink ref="B271" r:id="rId244"/>
+    <hyperlink ref="B272" r:id="rId245"/>
+    <hyperlink ref="B273" r:id="rId246"/>
+    <hyperlink ref="B274" r:id="rId247"/>
+    <hyperlink ref="B275" r:id="rId248"/>
+    <hyperlink ref="B276" r:id="rId249"/>
+    <hyperlink ref="B277" r:id="rId250"/>
+    <hyperlink ref="B278" r:id="rId251"/>
+    <hyperlink ref="B279" r:id="rId252"/>
+    <hyperlink ref="B280" r:id="rId253"/>
+    <hyperlink ref="B281" r:id="rId254"/>
+    <hyperlink ref="B282" r:id="rId255"/>
+    <hyperlink ref="B283" r:id="rId256"/>
+    <hyperlink ref="B284" r:id="rId257"/>
+    <hyperlink ref="B285" r:id="rId258"/>
+    <hyperlink ref="B286" r:id="rId259"/>
+    <hyperlink ref="B287" r:id="rId260"/>
+    <hyperlink ref="B290" r:id="rId261"/>
+    <hyperlink ref="B291" r:id="rId262"/>
+    <hyperlink ref="B292" r:id="rId263"/>
+    <hyperlink ref="B293" r:id="rId264"/>
+    <hyperlink ref="B294" r:id="rId265"/>
+    <hyperlink ref="B295" r:id="rId266"/>
+    <hyperlink ref="B296" r:id="rId267"/>
+    <hyperlink ref="B297" r:id="rId268"/>
+    <hyperlink ref="B298" r:id="rId269"/>
+    <hyperlink ref="B299" r:id="rId270"/>
+    <hyperlink ref="B300" r:id="rId271" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B301" r:id="rId272"/>
+    <hyperlink ref="B302" r:id="rId273"/>
+    <hyperlink ref="B303" r:id="rId274"/>
+    <hyperlink ref="B304" r:id="rId275"/>
+    <hyperlink ref="B305" r:id="rId276"/>
+    <hyperlink ref="B306" r:id="rId277"/>
+    <hyperlink ref="B307" r:id="rId278"/>
+    <hyperlink ref="B308" r:id="rId279"/>
+    <hyperlink ref="B309" r:id="rId280"/>
+    <hyperlink ref="B310" r:id="rId281"/>
+    <hyperlink ref="B311" r:id="rId282"/>
+    <hyperlink ref="B312" r:id="rId283"/>
+    <hyperlink ref="B313" r:id="rId284"/>
+    <hyperlink ref="B314" r:id="rId285"/>
+    <hyperlink ref="B315" r:id="rId286"/>
+    <hyperlink ref="B316" r:id="rId287"/>
+    <hyperlink ref="B317" r:id="rId288"/>
+    <hyperlink ref="B318" r:id="rId289"/>
+    <hyperlink ref="B319" r:id="rId290"/>
+    <hyperlink ref="B320" r:id="rId291"/>
+    <hyperlink ref="B321" r:id="rId292"/>
+    <hyperlink ref="B322" r:id="rId293"/>
+    <hyperlink ref="B323" r:id="rId294"/>
+    <hyperlink ref="B324" r:id="rId295"/>
+    <hyperlink ref="B325" r:id="rId296"/>
+    <hyperlink ref="B326" r:id="rId297"/>
+    <hyperlink ref="B327" r:id="rId298"/>
+    <hyperlink ref="B330" r:id="rId299"/>
+    <hyperlink ref="B331" r:id="rId300"/>
+    <hyperlink ref="B332" r:id="rId301"/>
+    <hyperlink ref="B333" r:id="rId302"/>
+    <hyperlink ref="B334" r:id="rId303"/>
+    <hyperlink ref="B335" r:id="rId304"/>
+    <hyperlink ref="B336" r:id="rId305"/>
+    <hyperlink ref="B337" r:id="rId306"/>
+    <hyperlink ref="B338" r:id="rId307"/>
+    <hyperlink ref="B339" r:id="rId308"/>
+    <hyperlink ref="B340" r:id="rId309"/>
+    <hyperlink ref="B341" r:id="rId310"/>
+    <hyperlink ref="B342" r:id="rId311"/>
+    <hyperlink ref="B343" r:id="rId312"/>
+    <hyperlink ref="B344" r:id="rId313"/>
+    <hyperlink ref="B345" r:id="rId314"/>
+    <hyperlink ref="B346" r:id="rId315"/>
+    <hyperlink ref="B347" r:id="rId316"/>
+    <hyperlink ref="B351" r:id="rId317"/>
+    <hyperlink ref="B352" r:id="rId318"/>
+    <hyperlink ref="B353" r:id="rId319"/>
+    <hyperlink ref="B354" r:id="rId320"/>
+    <hyperlink ref="B355" r:id="rId321"/>
+    <hyperlink ref="B356" r:id="rId322"/>
+    <hyperlink ref="B357" r:id="rId323"/>
+    <hyperlink ref="B358" r:id="rId324"/>
+    <hyperlink ref="B359" r:id="rId325"/>
+    <hyperlink ref="B360" r:id="rId326"/>
+    <hyperlink ref="B361" r:id="rId327"/>
+    <hyperlink ref="B362" r:id="rId328"/>
+    <hyperlink ref="B363" r:id="rId329"/>
+    <hyperlink ref="B364" r:id="rId330"/>
+    <hyperlink ref="B365" r:id="rId331"/>
+    <hyperlink ref="B366" r:id="rId332"/>
+    <hyperlink ref="B367" r:id="rId333"/>
+    <hyperlink ref="B368" r:id="rId334"/>
+    <hyperlink ref="B369" r:id="rId335"/>
+    <hyperlink ref="B370" r:id="rId336"/>
+    <hyperlink ref="B371" r:id="rId337"/>
+    <hyperlink ref="B372" r:id="rId338"/>
+    <hyperlink ref="B373" r:id="rId339" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B374" r:id="rId340"/>
+    <hyperlink ref="B375" r:id="rId341"/>
+    <hyperlink ref="B376" r:id="rId342"/>
+    <hyperlink ref="B377" r:id="rId343"/>
+    <hyperlink ref="B378" r:id="rId344"/>
+    <hyperlink ref="B379" r:id="rId345"/>
+    <hyperlink ref="B380" r:id="rId346"/>
+    <hyperlink ref="B381" r:id="rId347"/>
+    <hyperlink ref="B382" r:id="rId348"/>
+    <hyperlink ref="B383" r:id="rId349"/>
+    <hyperlink ref="B384" r:id="rId350"/>
+    <hyperlink ref="B385" r:id="rId351"/>
+    <hyperlink ref="B386" r:id="rId352"/>
+    <hyperlink ref="B387" r:id="rId353"/>
+    <hyperlink ref="B389" r:id="rId354"/>
+    <hyperlink ref="B388" r:id="rId355"/>
+    <hyperlink ref="B390" r:id="rId356"/>
+    <hyperlink ref="B391" r:id="rId357"/>
+    <hyperlink ref="B392" r:id="rId358"/>
+    <hyperlink ref="B395" r:id="rId359"/>
+    <hyperlink ref="B396" r:id="rId360"/>
+    <hyperlink ref="B397" r:id="rId361"/>
+    <hyperlink ref="B398" r:id="rId362"/>
+    <hyperlink ref="B399" r:id="rId363"/>
+    <hyperlink ref="B400" r:id="rId364"/>
+    <hyperlink ref="B403" r:id="rId365"/>
+    <hyperlink ref="B404" r:id="rId366"/>
+    <hyperlink ref="B405" r:id="rId367"/>
+    <hyperlink ref="B406" r:id="rId368"/>
+    <hyperlink ref="B407" r:id="rId369"/>
+    <hyperlink ref="B408" r:id="rId370"/>
+    <hyperlink ref="B409" r:id="rId371"/>
+    <hyperlink ref="B410" r:id="rId372"/>
+    <hyperlink ref="B411" r:id="rId373"/>
+    <hyperlink ref="B412" r:id="rId374"/>
+    <hyperlink ref="B413" r:id="rId375"/>
+    <hyperlink ref="B414" r:id="rId376"/>
+    <hyperlink ref="B415" r:id="rId377"/>
+    <hyperlink ref="B416" r:id="rId378"/>
+    <hyperlink ref="B417" r:id="rId379"/>
+    <hyperlink ref="B418" r:id="rId380"/>
+    <hyperlink ref="B419" r:id="rId381"/>
+    <hyperlink ref="B420" r:id="rId382"/>
+    <hyperlink ref="B421" r:id="rId383"/>
+    <hyperlink ref="B422" r:id="rId384"/>
+    <hyperlink ref="B423" r:id="rId385"/>
+    <hyperlink ref="B424" r:id="rId386"/>
+    <hyperlink ref="B425" r:id="rId387"/>
+    <hyperlink ref="B426" r:id="rId388"/>
+    <hyperlink ref="B427" r:id="rId389"/>
+    <hyperlink ref="B428" r:id="rId390"/>
+    <hyperlink ref="B429" r:id="rId391"/>
+    <hyperlink ref="B430" r:id="rId392"/>
+    <hyperlink ref="B431" r:id="rId393"/>
+    <hyperlink ref="B432" r:id="rId394"/>
+    <hyperlink ref="B433" r:id="rId395"/>
+    <hyperlink ref="B434" r:id="rId396"/>
+    <hyperlink ref="B435" r:id="rId397"/>
+    <hyperlink ref="B436" r:id="rId398"/>
+    <hyperlink ref="B437" r:id="rId399"/>
+    <hyperlink ref="B438" r:id="rId400"/>
+    <hyperlink ref="B439" r:id="rId401"/>
+    <hyperlink ref="B440" r:id="rId402"/>
+    <hyperlink ref="B441" r:id="rId403"/>
+    <hyperlink ref="B442" r:id="rId404"/>
+    <hyperlink ref="B444" r:id="rId405"/>
+    <hyperlink ref="B443" r:id="rId406"/>
+    <hyperlink ref="B445" r:id="rId407"/>
+    <hyperlink ref="B446" r:id="rId408"/>
+    <hyperlink ref="B447" r:id="rId409"/>
+    <hyperlink ref="B448" r:id="rId410"/>
+    <hyperlink ref="B449" r:id="rId411"/>
+    <hyperlink ref="B450" r:id="rId412"/>
+    <hyperlink ref="B451" r:id="rId413"/>
+    <hyperlink ref="B452" r:id="rId414"/>
+    <hyperlink ref="B453" r:id="rId415"/>
+    <hyperlink ref="B454" r:id="rId416"/>
+    <hyperlink ref="B455" r:id="rId417"/>
+    <hyperlink ref="B462" r:id="rId418"/>
+    <hyperlink ref="B461" r:id="rId419"/>
+    <hyperlink ref="B460" r:id="rId420"/>
+    <hyperlink ref="B459" r:id="rId421"/>
+    <hyperlink ref="B458" r:id="rId422"/>
+    <hyperlink ref="B457" r:id="rId423"/>
+    <hyperlink ref="B456" r:id="rId424"/>
+    <hyperlink ref="B465" r:id="rId425"/>
+    <hyperlink ref="B466" r:id="rId426"/>
+    <hyperlink ref="B467" r:id="rId427"/>
+    <hyperlink ref="B468" r:id="rId428"/>
+    <hyperlink ref="B469" r:id="rId429"/>
+    <hyperlink ref="B470" r:id="rId430"/>
+    <hyperlink ref="B471" r:id="rId431"/>
+    <hyperlink ref="B474" r:id="rId432"/>
+    <hyperlink ref="B472" r:id="rId433"/>
+    <hyperlink ref="B473" r:id="rId434" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B350" r:id="rId435"/>
     <hyperlink ref="B2" r:id="rId436"/>
     <hyperlink ref="D17" r:id="rId437"/>
     <hyperlink ref="D6" r:id="rId438"/>
@@ -7941,8 +7987,10 @@
     <hyperlink ref="D199" r:id="rId497"/>
     <hyperlink ref="D170" r:id="rId498"/>
     <hyperlink ref="D188" r:id="rId499"/>
+    <hyperlink ref="D193" r:id="rId500"/>
+    <hyperlink ref="D207" r:id="rId501"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId500"/>
+  <pageSetup orientation="portrait" r:id="rId502"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
factorial of large number
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="535">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1626,6 +1626,9 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/min-and-max-of-binary-tree_5673?leftPanelTab=2</t>
+  </si>
+  <si>
+    <t>https://www.hackerearth.com/practice/notes/factorial-of-large-number/</t>
   </si>
 </sst>
 </file>
@@ -2277,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D226" sqref="D226"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2586,7 +2589,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">
@@ -8030,8 +8036,9 @@
     <hyperlink ref="D221" r:id="rId502"/>
     <hyperlink ref="D190" r:id="rId503"/>
     <hyperlink ref="D211" r:id="rId504"/>
+    <hyperlink ref="D26" r:id="rId505"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId505"/>
+  <pageSetup orientation="portrait" r:id="rId506"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LCA , count NOdes , Valid or not BST
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="538">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1629,6 +1629,15 @@
   </si>
   <si>
     <t>https://www.hackerearth.com/practice/notes/factorial-of-large-number/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/submissions/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/library/count-bst-nodes-that-lie-in-a-given-range</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/submissions/</t>
   </si>
 </sst>
 </file>
@@ -2280,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -4742,7 +4751,10 @@
         <v>186</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D213" s="21" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="21">
@@ -4764,7 +4776,10 @@
         <v>188</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D215" s="21" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="21">
@@ -4870,7 +4885,10 @@
         <v>196</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D224" s="21" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="21">
@@ -8037,8 +8055,11 @@
     <hyperlink ref="D190" r:id="rId503"/>
     <hyperlink ref="D211" r:id="rId504"/>
     <hyperlink ref="D26" r:id="rId505"/>
+    <hyperlink ref="D213" r:id="rId506"/>
+    <hyperlink ref="D224" r:id="rId507"/>
+    <hyperlink ref="D215" r:id="rId508"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId506"/>
+  <pageSetup orientation="portrait" r:id="rId509"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rotate Image and miscellaneous questions on array(easy)
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="539">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1638,6 +1638,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/submissions/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rotate-image/submissions/</t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1876,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1970,6 +1973,9 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2289,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2672,7 +2678,7 @@
       <c r="C32" s="25" t="s">
         <v>440</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="42" t="s">
         <v>453</v>
       </c>
     </row>
@@ -2784,7 +2790,7 @@
       <c r="C43" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D43" s="23" t="s">
         <v>458</v>
       </c>
     </row>
@@ -2863,6 +2869,9 @@
       </c>
       <c r="C50" s="2" t="s">
         <v>440</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -8058,8 +8067,9 @@
     <hyperlink ref="D213" r:id="rId506"/>
     <hyperlink ref="D224" r:id="rId507"/>
     <hyperlink ref="D215" r:id="rId508"/>
+    <hyperlink ref="D50" r:id="rId509"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId509"/>
+  <pageSetup orientation="portrait" r:id="rId510"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inorder successor/predecessor in BST
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="541">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1641,6 +1641,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/rotate-image/submissions/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/predecessor-and-successor_920476?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>brute force would be to pass the value at each node to ValidateBST and check if it is valid or not and if valid count the total no. of nodes using any traversal</t>
   </si>
 </sst>
 </file>
@@ -1846,7 +1852,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1869,6 +1875,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1876,7 +1922,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1974,6 +2020,31 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
@@ -2295,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A208" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -4749,7 +4820,10 @@
         <v>185</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D212" s="21" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -4836,31 +4910,31 @@
       </c>
       <c r="D219" s="24"/>
     </row>
-    <row r="220" spans="1:4" ht="21">
-      <c r="A220" s="3" t="s">
+    <row r="220" spans="1:4" s="47" customFormat="1" ht="21">
+      <c r="A220" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="B220" s="14" t="s">
+      <c r="B220" s="44" t="s">
         <v>192</v>
       </c>
-      <c r="C220" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D220" s="17" t="s">
+      <c r="C220" s="45" t="s">
+        <v>440</v>
+      </c>
+      <c r="D220" s="46" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="21">
-      <c r="A221" s="3" t="s">
+    <row r="221" spans="1:4" s="52" customFormat="1" ht="21">
+      <c r="A221" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="B221" s="14" t="s">
+      <c r="B221" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C221" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D221" s="21" t="s">
+      <c r="C221" s="50" t="s">
+        <v>440</v>
+      </c>
+      <c r="D221" s="51" t="s">
         <v>528</v>
       </c>
     </row>
@@ -4900,7 +4974,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="21">
+    <row r="225" spans="1:6" ht="21">
       <c r="A225" s="3" t="s">
         <v>182</v>
       </c>
@@ -4911,7 +4985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="21">
+    <row r="226" spans="1:6" ht="21">
       <c r="A226" s="3" t="s">
         <v>182</v>
       </c>
@@ -4922,7 +4996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="21">
+    <row r="227" spans="1:6" ht="21">
       <c r="A227" s="3" t="s">
         <v>182</v>
       </c>
@@ -4932,8 +5006,9 @@
       <c r="C227" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" ht="21">
+      <c r="D227" s="53"/>
+    </row>
+    <row r="228" spans="1:6" ht="21">
       <c r="A228" s="3" t="s">
         <v>182</v>
       </c>
@@ -4944,7 +5019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="229" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="229" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A229" s="6" t="s">
         <v>182</v>
       </c>
@@ -4952,11 +5027,14 @@
         <v>201</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>3</v>
+        <v>440</v>
       </c>
       <c r="D229" s="24"/>
-    </row>
-    <row r="230" spans="1:4" ht="21">
+      <c r="F229" s="7" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="21">
       <c r="A230" s="3" t="s">
         <v>182</v>
       </c>
@@ -4967,15 +5045,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="21">
+    <row r="231" spans="1:6" ht="21">
       <c r="B231" s="4"/>
       <c r="C231" s="2"/>
     </row>
-    <row r="232" spans="1:4" ht="21">
+    <row r="232" spans="1:6" ht="21">
       <c r="B232" s="4"/>
       <c r="C232" s="2"/>
     </row>
-    <row r="233" spans="1:4" ht="21">
+    <row r="233" spans="1:6" ht="21">
       <c r="A233" s="3" t="s">
         <v>203</v>
       </c>
@@ -4986,7 +5064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="21">
+    <row r="234" spans="1:6" ht="21">
       <c r="A234" s="3" t="s">
         <v>203</v>
       </c>
@@ -4997,7 +5075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="21">
+    <row r="235" spans="1:6" ht="21">
       <c r="A235" s="3" t="s">
         <v>203</v>
       </c>
@@ -5008,7 +5086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="21">
+    <row r="236" spans="1:6" ht="21">
       <c r="A236" s="3" t="s">
         <v>203</v>
       </c>
@@ -5019,7 +5097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="21">
+    <row r="237" spans="1:6" ht="21">
       <c r="A237" s="3" t="s">
         <v>203</v>
       </c>
@@ -5030,7 +5108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="21">
+    <row r="238" spans="1:6" ht="21">
       <c r="A238" s="3" t="s">
         <v>203</v>
       </c>
@@ -5041,7 +5119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="21">
+    <row r="239" spans="1:6" ht="21">
       <c r="A239" s="3" t="s">
         <v>203</v>
       </c>
@@ -5052,7 +5130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="21">
+    <row r="240" spans="1:6" ht="21">
       <c r="A240" s="3" t="s">
         <v>203</v>
       </c>
@@ -8068,8 +8146,9 @@
     <hyperlink ref="D224" r:id="rId507"/>
     <hyperlink ref="D215" r:id="rId508"/>
     <hyperlink ref="D50" r:id="rId509"/>
+    <hyperlink ref="D212" r:id="rId510"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId510"/>
+  <pageSetup orientation="portrait" r:id="rId511"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kth largest and smallest element , merge n ropes
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="544">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1650,6 +1650,12 @@
   </si>
   <si>
     <t>folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same as above one </t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/connect-n-ropes-with-minimum-cost_630476?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2373,7 +2379,7 @@
   <dimension ref="A1:F475"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A330" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F334" sqref="F334"/>
+      <selection activeCell="F338" sqref="F338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6117,19 +6123,23 @@
         <v>299</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="333" spans="1:4" ht="21">
-      <c r="A333" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D332" s="17" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A333" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B333" s="14" t="s">
+      <c r="B333" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="C333" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C333" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D333" s="24"/>
     </row>
     <row r="334" spans="1:4" ht="21">
       <c r="A334" s="5" t="s">
@@ -6139,7 +6149,10 @@
         <v>301</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D334" s="21" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="21">
@@ -6150,7 +6163,10 @@
         <v>302</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D335" s="17" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="336" spans="1:4" s="7" customFormat="1" ht="21">
@@ -6251,7 +6267,10 @@
         <v>311</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>3</v>
+        <v>440</v>
+      </c>
+      <c r="D344" s="21" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="21">
@@ -8161,8 +8180,10 @@
     <hyperlink ref="D215" r:id="rId508"/>
     <hyperlink ref="D50" r:id="rId509"/>
     <hyperlink ref="D212" r:id="rId510"/>
+    <hyperlink ref="D334" r:id="rId511"/>
+    <hyperlink ref="D344" r:id="rId512"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId511"/>
+  <pageSetup orientation="portrait" r:id="rId513"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge k sorted linkedlist , minimum sum two numbers stored inform of array
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="548">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -947,9 +947,6 @@
     <t>Leetcode- reorganize strings</t>
   </si>
   <si>
-    <t>Merge “K” Sorted Linked Lists [V.IMP]</t>
-  </si>
-  <si>
     <t>Smallest range in “K” Lists</t>
   </si>
   <si>
@@ -1656,6 +1653,21 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/connect-n-ropes-with-minimum-cost_630476?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-k-sorted-lists/</t>
+  </si>
+  <si>
+    <t>Merge “K” Sorted Linked Lists [V.IMP]    [HARD YET EASY]</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/minimum-sum-of-two-numbers-formed-from-digits-of-an-array_1171162?leftPanelTab=3</t>
+  </si>
+  <si>
+    <t>failing on some edge test case</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reorganize-string/</t>
   </si>
 </sst>
 </file>
@@ -2378,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F338" sqref="F338"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2399,7 +2411,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21">
@@ -2410,10 +2422,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2427,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2441,10 +2453,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2455,10 +2467,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2469,10 +2481,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2483,10 +2495,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2508,10 +2520,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>440</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="9" customFormat="1" ht="19.8">
@@ -2537,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2548,10 +2560,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21">
@@ -2562,10 +2574,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="11" customFormat="1" ht="21">
@@ -2576,10 +2588,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21">
@@ -2604,7 +2616,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="21">
@@ -2626,10 +2638,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21">
@@ -2640,10 +2652,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21">
@@ -2687,10 +2699,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">
@@ -2701,10 +2713,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21">
@@ -2756,13 +2768,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="29" customFormat="1" ht="21">
@@ -2770,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>3</v>
@@ -2868,13 +2880,13 @@
         <v>38</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21">
@@ -2951,10 +2963,10 @@
         <v>45</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -2992,10 +3004,10 @@
         <v>49</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3006,10 +3018,10 @@
         <v>50</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3020,10 +3032,10 @@
         <v>51</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="21">
@@ -3473,10 +3485,10 @@
         <v>92</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="21">
@@ -3498,7 +3510,7 @@
         <v>94</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="21">
@@ -3509,10 +3521,10 @@
         <v>95</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="21">
@@ -3589,10 +3601,10 @@
         <v>102</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D109" s="24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="21">
@@ -3702,7 +3714,7 @@
         <v>112</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="21">
@@ -3841,10 +3853,10 @@
         <v>125</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D133" s="21" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="134" spans="1:4" s="7" customFormat="1" ht="21">
@@ -3855,10 +3867,10 @@
         <v>126</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D134" s="23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -3869,10 +3881,10 @@
         <v>127</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
@@ -3883,10 +3895,10 @@
         <v>128</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -3897,10 +3909,10 @@
         <v>129</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -3911,10 +3923,10 @@
         <v>130</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D138" s="21" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -3925,10 +3937,10 @@
         <v>131</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D139" s="21" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
@@ -3939,10 +3951,10 @@
         <v>132</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D140" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -3953,10 +3965,10 @@
         <v>133</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="21">
@@ -3989,7 +4001,7 @@
         <v>136</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D144" s="18"/>
     </row>
@@ -4013,10 +4025,10 @@
         <v>138</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D146" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4027,10 +4039,10 @@
         <v>139</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="21">
@@ -4041,10 +4053,10 @@
         <v>140</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="21">
@@ -4055,10 +4067,10 @@
         <v>141</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D149" s="21" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="21">
@@ -4069,10 +4081,10 @@
         <v>142</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D150" s="21" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="21">
@@ -4132,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="21">
@@ -4140,13 +4152,13 @@
         <v>124</v>
       </c>
       <c r="B156" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D156" s="21" t="s">
         <v>465</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D156" s="21" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="157" spans="1:6" s="32" customFormat="1" ht="21">
@@ -4154,10 +4166,10 @@
         <v>124</v>
       </c>
       <c r="B157" s="32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D157" s="33"/>
     </row>
@@ -4169,27 +4181,27 @@
         <v>148</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D158" s="21" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="159" spans="1:6" s="32" customFormat="1" ht="21">
       <c r="A159" s="31" t="s">
+        <v>488</v>
+      </c>
+      <c r="B159" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="B159" s="32" t="s">
+      <c r="C159" s="31" t="s">
         <v>490</v>
       </c>
-      <c r="C159" s="31" t="s">
+      <c r="D159" s="38" t="s">
         <v>491</v>
       </c>
-      <c r="D159" s="38" t="s">
+      <c r="F159" s="37" t="s">
         <v>492</v>
-      </c>
-      <c r="F159" s="37" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="160" spans="1:6" s="32" customFormat="1" ht="21">
@@ -4197,13 +4209,13 @@
         <v>124</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D160" s="38" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="21">
@@ -4211,13 +4223,13 @@
         <v>124</v>
       </c>
       <c r="B161" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D161" s="21" t="s">
         <v>485</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D161" s="21" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="21">
@@ -4247,13 +4259,13 @@
         <v>124</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C164" s="22" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D164" s="35" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4264,10 +4276,10 @@
         <v>151</v>
       </c>
       <c r="C165" s="36" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D165" s="21" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="21">
@@ -4278,10 +4290,10 @@
         <v>152</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D166" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="21">
@@ -4290,16 +4302,16 @@
     </row>
     <row r="169" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A169" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B169" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="B169" s="7" t="s">
-        <v>506</v>
-      </c>
       <c r="C169" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D169" s="24" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">
@@ -4310,10 +4322,10 @@
         <v>154</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D170" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">
@@ -4321,13 +4333,13 @@
         <v>153</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D171" s="21" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -4338,10 +4350,10 @@
         <v>155</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D172" s="21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4352,10 +4364,10 @@
         <v>156</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D173" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4366,10 +4378,10 @@
         <v>157</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D174" s="21" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">
@@ -4380,10 +4392,10 @@
         <v>158</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D175" s="21" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4394,10 +4406,10 @@
         <v>159</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D176" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
@@ -4408,10 +4420,10 @@
         <v>160</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D177" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4422,10 +4434,10 @@
         <v>161</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D178" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="21">
@@ -4458,10 +4470,10 @@
         <v>164</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D181" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -4472,10 +4484,10 @@
         <v>165</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D182" s="21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="21">
@@ -4494,13 +4506,13 @@
         <v>153</v>
       </c>
       <c r="B184" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D184" s="40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="21">
@@ -4519,13 +4531,13 @@
         <v>153</v>
       </c>
       <c r="B186" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D186" s="21" t="s">
         <v>516</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D186" s="21" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="21">
@@ -4547,10 +4559,10 @@
         <v>169</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D188" s="21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="21">
@@ -4569,13 +4581,13 @@
         <v>153</v>
       </c>
       <c r="B190" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D190" s="21" t="s">
         <v>531</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D190" s="21" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="21">
@@ -4620,10 +4632,10 @@
         <v>174</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D194" s="21" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="21">
@@ -4665,13 +4677,13 @@
         <v>153</v>
       </c>
       <c r="B198" s="39" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D198" s="33" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="21">
@@ -4690,13 +4702,13 @@
         <v>153</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D200" s="24" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">
@@ -4704,13 +4716,13 @@
         <v>153</v>
       </c>
       <c r="B201" s="41" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D201" s="21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="21">
@@ -4762,13 +4774,13 @@
         <v>182</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D207" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -4776,13 +4788,13 @@
         <v>182</v>
       </c>
       <c r="B208" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D208" s="21" t="s">
         <v>524</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D208" s="21" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4790,13 +4802,13 @@
         <v>182</v>
       </c>
       <c r="B209" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D209" s="21" t="s">
         <v>526</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D209" s="21" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="21">
@@ -4818,10 +4830,10 @@
         <v>184</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D211" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -4832,10 +4844,10 @@
         <v>185</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D212" s="21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -4846,10 +4858,10 @@
         <v>186</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D213" s="21" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="21">
@@ -4871,10 +4883,10 @@
         <v>188</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D215" s="21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="21">
@@ -4915,7 +4927,7 @@
         <v>182</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>3</v>
@@ -4930,10 +4942,10 @@
         <v>192</v>
       </c>
       <c r="C220" s="45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D220" s="46" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="221" spans="1:4" s="52" customFormat="1" ht="21">
@@ -4944,10 +4956,10 @@
         <v>193</v>
       </c>
       <c r="C221" s="50" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D221" s="51" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="21">
@@ -4980,10 +4992,10 @@
         <v>196</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D224" s="21" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="21">
@@ -5039,11 +5051,11 @@
         <v>201</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D229" s="24"/>
       <c r="F229" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="21">
@@ -6109,10 +6121,10 @@
         <v>298</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D331" s="22" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="21">
@@ -6123,10 +6135,10 @@
         <v>299</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D332" s="17" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="333" spans="1:4" s="7" customFormat="1" ht="21">
@@ -6149,10 +6161,10 @@
         <v>301</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D334" s="21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="21">
@@ -6163,10 +6175,10 @@
         <v>302</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D335" s="17" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="336" spans="1:4" s="7" customFormat="1" ht="21">
@@ -6181,7 +6193,7 @@
       </c>
       <c r="D336" s="24"/>
     </row>
-    <row r="337" spans="1:4" ht="21">
+    <row r="337" spans="1:6" ht="21">
       <c r="A337" s="5" t="s">
         <v>297</v>
       </c>
@@ -6192,7 +6204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="21">
+    <row r="338" spans="1:6" ht="21">
       <c r="A338" s="5" t="s">
         <v>297</v>
       </c>
@@ -6203,7 +6215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="21">
+    <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
         <v>297</v>
       </c>
@@ -6213,138 +6225,149 @@
       <c r="C339" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="340" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="D339" s="21" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A340" s="6" t="s">
         <v>297</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>307</v>
+        <v>544</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D340" s="24"/>
-    </row>
-    <row r="341" spans="1:4" ht="21">
+        <v>439</v>
+      </c>
+      <c r="D340" s="23" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" ht="21">
       <c r="A341" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B341" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="21">
+    <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B342" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="343" spans="1:4" ht="21">
+    <row r="343" spans="1:6" ht="21">
       <c r="A343" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B343" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C343" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="344" spans="1:4" ht="21">
+    <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B344" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D344" s="21" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="345" spans="1:4" ht="21">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" ht="21">
       <c r="A345" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B345" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C345" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="346" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="346" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A346" s="6" t="s">
         <v>297</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C346" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D346" s="54" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="347" spans="1:4" ht="21">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" ht="21">
       <c r="A347" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B347" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C347" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="21">
+    <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
         <v>297</v>
       </c>
       <c r="B348" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="349" spans="1:4" ht="21">
+        <v>439</v>
+      </c>
+      <c r="D348" s="21" t="s">
+        <v>545</v>
+      </c>
+      <c r="F348" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" ht="21">
       <c r="B349" s="4"/>
       <c r="C349" s="2"/>
     </row>
-    <row r="350" spans="1:4" ht="21">
+    <row r="350" spans="1:6" ht="21">
       <c r="B350" s="4"/>
       <c r="C350" s="2"/>
     </row>
-    <row r="351" spans="1:4" ht="21">
+    <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B351" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="B351" s="14" t="s">
+      <c r="C351" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" ht="21">
+      <c r="A352" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B352" s="14" t="s">
         <v>317</v>
-      </c>
-      <c r="C351" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="352" spans="1:4" ht="21">
-      <c r="A352" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B352" s="14" t="s">
-        <v>318</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>3</v>
@@ -6352,10 +6375,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B353" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>3</v>
@@ -6363,10 +6386,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B354" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>3</v>
@@ -6374,10 +6397,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B355" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>3</v>
@@ -6385,10 +6408,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B356" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>3</v>
@@ -6396,10 +6419,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B357" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>3</v>
@@ -6407,10 +6430,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B358" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>3</v>
@@ -6418,10 +6441,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B359" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>3</v>
@@ -6429,10 +6452,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B360" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>3</v>
@@ -6440,10 +6463,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B361" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>3</v>
@@ -6451,10 +6474,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B362" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>3</v>
@@ -6462,10 +6485,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>3</v>
@@ -6473,10 +6496,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B364" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>3</v>
@@ -6484,10 +6507,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B365" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>3</v>
@@ -6495,10 +6518,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B366" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>3</v>
@@ -6506,10 +6529,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B367" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>3</v>
@@ -6517,10 +6540,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B368" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>3</v>
@@ -6528,10 +6551,10 @@
     </row>
     <row r="369" spans="1:4" ht="21">
       <c r="A369" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B369" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>3</v>
@@ -6539,10 +6562,10 @@
     </row>
     <row r="370" spans="1:4" ht="21">
       <c r="A370" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B370" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>3</v>
@@ -6550,10 +6573,10 @@
     </row>
     <row r="371" spans="1:4" ht="21">
       <c r="A371" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B371" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>3</v>
@@ -6561,10 +6584,10 @@
     </row>
     <row r="372" spans="1:4" ht="21">
       <c r="A372" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B372" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>3</v>
@@ -6572,10 +6595,10 @@
     </row>
     <row r="373" spans="1:4" ht="21">
       <c r="A373" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B373" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>3</v>
@@ -6583,10 +6606,10 @@
     </row>
     <row r="374" spans="1:4" ht="21">
       <c r="A374" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B374" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>3</v>
@@ -6594,10 +6617,10 @@
     </row>
     <row r="375" spans="1:4" ht="21">
       <c r="A375" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B375" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>3</v>
@@ -6605,10 +6628,10 @@
     </row>
     <row r="376" spans="1:4" ht="21">
       <c r="A376" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B376" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>3</v>
@@ -6616,10 +6639,10 @@
     </row>
     <row r="377" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A377" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B377" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C377" s="6" t="s">
         <v>3</v>
@@ -6628,10 +6651,10 @@
     </row>
     <row r="378" spans="1:4" ht="21">
       <c r="A378" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B378" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>3</v>
@@ -6639,10 +6662,10 @@
     </row>
     <row r="379" spans="1:4" ht="21">
       <c r="A379" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B379" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>3</v>
@@ -6650,10 +6673,10 @@
     </row>
     <row r="380" spans="1:4" ht="21">
       <c r="A380" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B380" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>3</v>
@@ -6661,10 +6684,10 @@
     </row>
     <row r="381" spans="1:4" ht="21">
       <c r="A381" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B381" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>3</v>
@@ -6672,10 +6695,10 @@
     </row>
     <row r="382" spans="1:4" ht="21">
       <c r="A382" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B382" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>3</v>
@@ -6683,10 +6706,10 @@
     </row>
     <row r="383" spans="1:4" ht="21">
       <c r="A383" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B383" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>3</v>
@@ -6694,10 +6717,10 @@
     </row>
     <row r="384" spans="1:4" ht="21">
       <c r="A384" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B384" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>3</v>
@@ -6705,10 +6728,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B385" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>3</v>
@@ -6716,10 +6739,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B386" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>3</v>
@@ -6727,10 +6750,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B387" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>3</v>
@@ -6738,10 +6761,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B388" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>3</v>
@@ -6749,10 +6772,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B389" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>3</v>
@@ -6760,10 +6783,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B390" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>3</v>
@@ -6771,10 +6794,10 @@
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="A391" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B391" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>3</v>
@@ -6782,10 +6805,10 @@
     </row>
     <row r="392" spans="1:3" ht="21">
       <c r="A392" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B392" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>3</v>
@@ -6793,10 +6816,10 @@
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B393" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>3</v>
@@ -6812,10 +6835,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B396" s="14" t="s">
         <v>360</v>
-      </c>
-      <c r="B396" s="14" t="s">
-        <v>361</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>3</v>
@@ -6823,10 +6846,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B397" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>3</v>
@@ -6834,10 +6857,10 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B398" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>3</v>
@@ -6845,7 +6868,7 @@
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="A399" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B399" s="14" t="s">
         <v>83</v>
@@ -6856,10 +6879,10 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="A400" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B400" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>3</v>
@@ -6867,10 +6890,10 @@
     </row>
     <row r="401" spans="1:3" ht="21">
       <c r="A401" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B401" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C401" s="2" t="s">
         <v>3</v>
@@ -6886,21 +6909,21 @@
     </row>
     <row r="404" spans="1:3" ht="21">
       <c r="A404" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B404" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="B404" s="14" t="s">
-        <v>367</v>
-      </c>
       <c r="C404" s="36" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="21">
       <c r="A405" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B405" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>3</v>
@@ -6908,10 +6931,10 @@
     </row>
     <row r="406" spans="1:3" ht="21">
       <c r="A406" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B406" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>3</v>
@@ -6919,10 +6942,10 @@
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B407" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>3</v>
@@ -6930,10 +6953,10 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="A408" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B408" s="14" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>3</v>
@@ -6941,21 +6964,21 @@
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B409" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B410" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>3</v>
@@ -6963,7 +6986,7 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B411" s="14" t="s">
         <v>246</v>
@@ -6974,10 +6997,10 @@
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B412" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>3</v>
@@ -6985,10 +7008,10 @@
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B413" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>3</v>
@@ -6996,10 +7019,10 @@
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B414" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>3</v>
@@ -7007,10 +7030,10 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B415" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>3</v>
@@ -7018,10 +7041,10 @@
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B416" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>3</v>
@@ -7029,10 +7052,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B417" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>3</v>
@@ -7040,10 +7063,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B418" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>3</v>
@@ -7051,10 +7074,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B419" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>3</v>
@@ -7062,10 +7085,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B420" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>3</v>
@@ -7073,10 +7096,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B421" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>3</v>
@@ -7084,10 +7107,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B422" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>3</v>
@@ -7095,10 +7118,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B423" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>3</v>
@@ -7106,10 +7129,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B424" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>3</v>
@@ -7117,10 +7140,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B425" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>3</v>
@@ -7128,10 +7151,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B426" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>3</v>
@@ -7139,10 +7162,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B427" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>3</v>
@@ -7150,10 +7173,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B428" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>3</v>
@@ -7161,10 +7184,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B429" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>3</v>
@@ -7172,10 +7195,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B430" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>3</v>
@@ -7183,10 +7206,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B431" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>3</v>
@@ -7194,10 +7217,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B432" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>3</v>
@@ -7205,10 +7228,10 @@
     </row>
     <row r="433" spans="1:4" ht="21">
       <c r="A433" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B433" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>3</v>
@@ -7216,10 +7239,10 @@
     </row>
     <row r="434" spans="1:4" ht="21">
       <c r="A434" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B434" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>3</v>
@@ -7227,10 +7250,10 @@
     </row>
     <row r="435" spans="1:4" ht="21">
       <c r="A435" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B435" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>3</v>
@@ -7238,10 +7261,10 @@
     </row>
     <row r="436" spans="1:4" ht="21">
       <c r="A436" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B436" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>3</v>
@@ -7249,10 +7272,10 @@
     </row>
     <row r="437" spans="1:4" ht="21">
       <c r="A437" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B437" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>3</v>
@@ -7260,10 +7283,10 @@
     </row>
     <row r="438" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A438" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B438" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C438" s="6" t="s">
         <v>3</v>
@@ -7272,10 +7295,10 @@
     </row>
     <row r="439" spans="1:4" ht="21">
       <c r="A439" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B439" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>3</v>
@@ -7283,10 +7306,10 @@
     </row>
     <row r="440" spans="1:4" ht="21">
       <c r="A440" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B440" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>3</v>
@@ -7294,10 +7317,10 @@
     </row>
     <row r="441" spans="1:4" ht="21">
       <c r="A441" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B441" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>3</v>
@@ -7305,10 +7328,10 @@
     </row>
     <row r="442" spans="1:4" ht="21">
       <c r="A442" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B442" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>3</v>
@@ -7316,10 +7339,10 @@
     </row>
     <row r="443" spans="1:4" ht="21">
       <c r="A443" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B443" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>3</v>
@@ -7327,10 +7350,10 @@
     </row>
     <row r="444" spans="1:4" ht="21">
       <c r="A444" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B444" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>3</v>
@@ -7338,10 +7361,10 @@
     </row>
     <row r="445" spans="1:4" ht="21">
       <c r="A445" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B445" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>3</v>
@@ -7349,10 +7372,10 @@
     </row>
     <row r="446" spans="1:4" ht="21">
       <c r="A446" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B446" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>3</v>
@@ -7360,10 +7383,10 @@
     </row>
     <row r="447" spans="1:4" ht="21">
       <c r="A447" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B447" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>3</v>
@@ -7371,10 +7394,10 @@
     </row>
     <row r="448" spans="1:4" ht="21">
       <c r="A448" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B448" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>3</v>
@@ -7382,10 +7405,10 @@
     </row>
     <row r="449" spans="1:4" ht="21">
       <c r="A449" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B449" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>3</v>
@@ -7393,10 +7416,10 @@
     </row>
     <row r="450" spans="1:4" s="26" customFormat="1" ht="21">
       <c r="A450" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B450" s="26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C450" s="25" t="s">
         <v>3</v>
@@ -7405,10 +7428,10 @@
     </row>
     <row r="451" spans="1:4" s="26" customFormat="1" ht="21">
       <c r="A451" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B451" s="26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C451" s="25" t="s">
         <v>3</v>
@@ -7417,10 +7440,10 @@
     </row>
     <row r="452" spans="1:4" ht="21">
       <c r="A452" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B452" s="14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>3</v>
@@ -7428,10 +7451,10 @@
     </row>
     <row r="453" spans="1:4" ht="21">
       <c r="A453" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B453" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C453" s="2" t="s">
         <v>3</v>
@@ -7439,10 +7462,10 @@
     </row>
     <row r="454" spans="1:4" ht="21">
       <c r="A454" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B454" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>3</v>
@@ -7450,10 +7473,10 @@
     </row>
     <row r="455" spans="1:4" ht="21">
       <c r="A455" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B455" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C455" s="2" t="s">
         <v>3</v>
@@ -7461,22 +7484,22 @@
     </row>
     <row r="456" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A456" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C456" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D456" s="24"/>
     </row>
     <row r="457" spans="1:4" ht="21">
       <c r="A457" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B457" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>3</v>
@@ -7484,10 +7507,10 @@
     </row>
     <row r="458" spans="1:4" ht="21">
       <c r="A458" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B458" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>3</v>
@@ -7495,10 +7518,10 @@
     </row>
     <row r="459" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A459" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B459" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C459" s="6" t="s">
         <v>3</v>
@@ -7507,10 +7530,10 @@
     </row>
     <row r="460" spans="1:4" ht="21">
       <c r="A460" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B460" s="14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>3</v>
@@ -7518,10 +7541,10 @@
     </row>
     <row r="461" spans="1:4" ht="21">
       <c r="A461" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B461" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>3</v>
@@ -7529,10 +7552,10 @@
     </row>
     <row r="462" spans="1:4" ht="21">
       <c r="A462" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B462" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>3</v>
@@ -7540,10 +7563,10 @@
     </row>
     <row r="463" spans="1:4" ht="21">
       <c r="A463" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B463" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C463" s="2" t="s">
         <v>3</v>
@@ -7560,10 +7583,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B466" s="14" t="s">
         <v>426</v>
-      </c>
-      <c r="B466" s="14" t="s">
-        <v>427</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>3</v>
@@ -7571,10 +7594,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B467" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>3</v>
@@ -7582,10 +7605,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B468" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>3</v>
@@ -7593,10 +7616,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B469" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>3</v>
@@ -7604,10 +7627,10 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="A470" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B470" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>3</v>
@@ -7615,21 +7638,21 @@
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B471" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B472" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>3</v>
@@ -7637,10 +7660,10 @@
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B473" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>3</v>
@@ -7648,10 +7671,10 @@
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B474" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C474" s="2" t="s">
         <v>3</v>
@@ -7659,13 +7682,13 @@
     </row>
     <row r="475" spans="1:3" ht="21">
       <c r="A475" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B475" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -7977,7 +8000,7 @@
     <hyperlink ref="B337" r:id="rId305"/>
     <hyperlink ref="B338" r:id="rId306"/>
     <hyperlink ref="B339" r:id="rId307"/>
-    <hyperlink ref="B340" r:id="rId308"/>
+    <hyperlink ref="B340" r:id="rId308" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
     <hyperlink ref="B341" r:id="rId309"/>
     <hyperlink ref="B342" r:id="rId310"/>
     <hyperlink ref="B343" r:id="rId311"/>
@@ -8182,8 +8205,11 @@
     <hyperlink ref="D212" r:id="rId510"/>
     <hyperlink ref="D334" r:id="rId511"/>
     <hyperlink ref="D344" r:id="rId512"/>
+    <hyperlink ref="D340" r:id="rId513"/>
+    <hyperlink ref="D348" r:id="rId514"/>
+    <hyperlink ref="D339" r:id="rId515"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId513"/>
+  <pageSetup orientation="portrait" r:id="rId516"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
count inversion , sort even and odd indices
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -1364,9 +1364,6 @@
     <t>https://leetcode.com/problems/merge-sorted-array/</t>
   </si>
   <si>
-    <t>easy</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/find-the-duplicate-number/</t>
   </si>
   <si>
@@ -1668,6 +1665,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/reorganize-string/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/move-all-negative-numbers-to-beginning-and-positive-to-end_1112620?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2390,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B338" sqref="B338"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2422,7 +2422,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>437</v>
@@ -2497,8 +2497,8 @@
       <c r="C10" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>446</v>
+      <c r="D10" s="21" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2549,7 +2549,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2563,7 +2563,7 @@
         <v>439</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21">
@@ -2616,7 +2616,7 @@
         <v>3</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="21">
@@ -2641,7 +2641,7 @@
         <v>439</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21">
@@ -2655,7 +2655,7 @@
         <v>439</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21">
@@ -2702,7 +2702,7 @@
         <v>439</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">
@@ -2716,7 +2716,7 @@
         <v>439</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21">
@@ -2768,13 +2768,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C32" s="25" t="s">
         <v>439</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="29" customFormat="1" ht="21">
@@ -2782,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>3</v>
@@ -2880,13 +2880,13 @@
         <v>38</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>439</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21">
@@ -2966,7 +2966,7 @@
         <v>439</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3021,7 +3021,7 @@
         <v>439</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3035,7 +3035,7 @@
         <v>439</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="21">
@@ -3488,7 +3488,7 @@
         <v>439</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="21">
@@ -3524,7 +3524,7 @@
         <v>439</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="21">
@@ -3604,7 +3604,7 @@
         <v>439</v>
       </c>
       <c r="D109" s="24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="21">
@@ -3856,7 +3856,7 @@
         <v>439</v>
       </c>
       <c r="D133" s="21" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="134" spans="1:4" s="7" customFormat="1" ht="21">
@@ -3870,7 +3870,7 @@
         <v>439</v>
       </c>
       <c r="D134" s="23" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -3884,7 +3884,7 @@
         <v>439</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
@@ -3898,7 +3898,7 @@
         <v>439</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -3912,7 +3912,7 @@
         <v>439</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -3926,7 +3926,7 @@
         <v>439</v>
       </c>
       <c r="D138" s="21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -3940,7 +3940,7 @@
         <v>439</v>
       </c>
       <c r="D139" s="21" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
@@ -3954,7 +3954,7 @@
         <v>439</v>
       </c>
       <c r="D140" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -3968,7 +3968,7 @@
         <v>439</v>
       </c>
       <c r="D141" s="21" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="21">
@@ -4028,7 +4028,7 @@
         <v>439</v>
       </c>
       <c r="D146" s="21" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4042,7 +4042,7 @@
         <v>439</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="21">
@@ -4056,7 +4056,7 @@
         <v>439</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="21">
@@ -4070,7 +4070,7 @@
         <v>439</v>
       </c>
       <c r="D149" s="21" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="21">
@@ -4084,7 +4084,7 @@
         <v>439</v>
       </c>
       <c r="D150" s="21" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="21">
@@ -4144,7 +4144,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="21">
@@ -4152,13 +4152,13 @@
         <v>124</v>
       </c>
       <c r="B156" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D156" s="21" t="s">
         <v>464</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D156" s="21" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:6" s="32" customFormat="1" ht="21">
@@ -4166,7 +4166,7 @@
         <v>124</v>
       </c>
       <c r="B157" s="32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C157" s="31" t="s">
         <v>439</v>
@@ -4184,24 +4184,24 @@
         <v>439</v>
       </c>
       <c r="D158" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="159" spans="1:6" s="32" customFormat="1" ht="21">
       <c r="A159" s="31" t="s">
+        <v>487</v>
+      </c>
+      <c r="B159" s="32" t="s">
         <v>488</v>
       </c>
-      <c r="B159" s="32" t="s">
+      <c r="C159" s="31" t="s">
         <v>489</v>
       </c>
-      <c r="C159" s="31" t="s">
+      <c r="D159" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="D159" s="38" t="s">
+      <c r="F159" s="37" t="s">
         <v>491</v>
-      </c>
-      <c r="F159" s="37" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="160" spans="1:6" s="32" customFormat="1" ht="21">
@@ -4209,13 +4209,13 @@
         <v>124</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C160" s="31" t="s">
         <v>439</v>
       </c>
       <c r="D160" s="38" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="21">
@@ -4223,13 +4223,13 @@
         <v>124</v>
       </c>
       <c r="B161" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D161" s="21" t="s">
         <v>484</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D161" s="21" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="21">
@@ -4259,13 +4259,13 @@
         <v>124</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C164" s="22" t="s">
         <v>439</v>
       </c>
       <c r="D164" s="35" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4279,7 +4279,7 @@
         <v>439</v>
       </c>
       <c r="D165" s="21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="21">
@@ -4293,7 +4293,7 @@
         <v>439</v>
       </c>
       <c r="D166" s="21" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="21">
@@ -4302,16 +4302,16 @@
     </row>
     <row r="169" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A169" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B169" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="B169" s="7" t="s">
-        <v>505</v>
-      </c>
       <c r="C169" s="6" t="s">
         <v>439</v>
       </c>
       <c r="D169" s="24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">
@@ -4325,7 +4325,7 @@
         <v>439</v>
       </c>
       <c r="D170" s="21" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">
@@ -4333,13 +4333,13 @@
         <v>153</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>439</v>
       </c>
       <c r="D171" s="21" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -4353,7 +4353,7 @@
         <v>439</v>
       </c>
       <c r="D172" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4367,7 +4367,7 @@
         <v>439</v>
       </c>
       <c r="D173" s="21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4381,7 +4381,7 @@
         <v>439</v>
       </c>
       <c r="D174" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">
@@ -4395,7 +4395,7 @@
         <v>439</v>
       </c>
       <c r="D175" s="21" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4409,7 +4409,7 @@
         <v>439</v>
       </c>
       <c r="D176" s="21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
@@ -4423,7 +4423,7 @@
         <v>439</v>
       </c>
       <c r="D177" s="21" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4437,7 +4437,7 @@
         <v>439</v>
       </c>
       <c r="D178" s="21" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="21">
@@ -4473,7 +4473,7 @@
         <v>439</v>
       </c>
       <c r="D181" s="21" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -4487,7 +4487,7 @@
         <v>439</v>
       </c>
       <c r="D182" s="21" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="21">
@@ -4506,13 +4506,13 @@
         <v>153</v>
       </c>
       <c r="B184" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C184" s="31" t="s">
         <v>439</v>
       </c>
       <c r="D184" s="40" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="21">
@@ -4531,13 +4531,13 @@
         <v>153</v>
       </c>
       <c r="B186" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D186" s="21" t="s">
         <v>515</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D186" s="21" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="21">
@@ -4562,7 +4562,7 @@
         <v>439</v>
       </c>
       <c r="D188" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="21">
@@ -4581,13 +4581,13 @@
         <v>153</v>
       </c>
       <c r="B190" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D190" s="21" t="s">
         <v>530</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D190" s="21" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="21">
@@ -4635,7 +4635,7 @@
         <v>439</v>
       </c>
       <c r="D194" s="21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="21">
@@ -4677,13 +4677,13 @@
         <v>153</v>
       </c>
       <c r="B198" s="39" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C198" s="31" t="s">
         <v>439</v>
       </c>
       <c r="D198" s="33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="21">
@@ -4702,13 +4702,13 @@
         <v>153</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>439</v>
       </c>
       <c r="D200" s="24" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">
@@ -4716,13 +4716,13 @@
         <v>153</v>
       </c>
       <c r="B201" s="41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>439</v>
       </c>
       <c r="D201" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="21">
@@ -4774,13 +4774,13 @@
         <v>182</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>439</v>
       </c>
       <c r="D207" s="21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -4788,13 +4788,13 @@
         <v>182</v>
       </c>
       <c r="B208" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D208" s="21" t="s">
         <v>523</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D208" s="21" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4802,13 +4802,13 @@
         <v>182</v>
       </c>
       <c r="B209" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D209" s="21" t="s">
         <v>525</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D209" s="21" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="21">
@@ -4833,7 +4833,7 @@
         <v>439</v>
       </c>
       <c r="D211" s="21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -4847,7 +4847,7 @@
         <v>439</v>
       </c>
       <c r="D212" s="21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -4861,7 +4861,7 @@
         <v>439</v>
       </c>
       <c r="D213" s="21" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="21">
@@ -4886,7 +4886,7 @@
         <v>439</v>
       </c>
       <c r="D215" s="21" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="21">
@@ -4927,7 +4927,7 @@
         <v>182</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C219" s="6" t="s">
         <v>3</v>
@@ -4945,7 +4945,7 @@
         <v>439</v>
       </c>
       <c r="D220" s="46" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="221" spans="1:4" s="52" customFormat="1" ht="21">
@@ -4959,7 +4959,7 @@
         <v>439</v>
       </c>
       <c r="D221" s="51" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="21">
@@ -4995,7 +4995,7 @@
         <v>439</v>
       </c>
       <c r="D224" s="21" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="225" spans="1:6" ht="21">
@@ -5055,7 +5055,7 @@
       </c>
       <c r="D229" s="24"/>
       <c r="F229" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="230" spans="1:6" ht="21">
@@ -6124,7 +6124,7 @@
         <v>439</v>
       </c>
       <c r="D331" s="22" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="21">
@@ -6138,7 +6138,7 @@
         <v>439</v>
       </c>
       <c r="D332" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="333" spans="1:4" s="7" customFormat="1" ht="21">
@@ -6178,7 +6178,7 @@
         <v>439</v>
       </c>
       <c r="D335" s="17" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="336" spans="1:4" s="7" customFormat="1" ht="21">
@@ -6226,7 +6226,7 @@
         <v>3</v>
       </c>
       <c r="D339" s="21" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="340" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6234,13 +6234,13 @@
         <v>297</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C340" s="6" t="s">
         <v>439</v>
       </c>
       <c r="D340" s="23" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="341" spans="1:6" ht="21">
@@ -6287,7 +6287,7 @@
         <v>439</v>
       </c>
       <c r="D344" s="21" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="21">
@@ -6312,7 +6312,7 @@
         <v>439</v>
       </c>
       <c r="D346" s="54" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="347" spans="1:6" ht="21">
@@ -6337,10 +6337,10 @@
         <v>439</v>
       </c>
       <c r="D348" s="21" t="s">
+        <v>544</v>
+      </c>
+      <c r="F348" t="s">
         <v>545</v>
-      </c>
-      <c r="F348" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="349" spans="1:6" ht="21">
@@ -8208,8 +8208,9 @@
     <hyperlink ref="D340" r:id="rId513"/>
     <hyperlink ref="D348" r:id="rId514"/>
     <hyperlink ref="D339" r:id="rId515"/>
+    <hyperlink ref="D10" r:id="rId516"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId516"/>
+  <pageSetup orientation="portrait" r:id="rId517"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
defanging an IP Address , combinational Sum
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="556">
   <si>
     <t>Topic:</t>
   </si>
@@ -762,9 +762,6 @@
   </si>
   <si>
     <t>Find shortest safe route in a path with landmines</t>
-  </si>
-  <si>
-    <t>Combinational Sum</t>
   </si>
   <si>
     <t>Find Maximum number possible by doing at-most K swaps</t>
@@ -1702,6 +1699,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Questions by Love Babbar:</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum/submissions/</t>
+  </si>
+  <si>
+    <t>Combinational Sum [V.IMP]</t>
   </si>
 </sst>
 </file>
@@ -2427,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B280" sqref="B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2443,7 +2446,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21">
@@ -2454,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2471,10 +2474,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21">
@@ -2485,10 +2488,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2499,10 +2502,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2513,10 +2516,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2527,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2552,10 +2555,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>433</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1" ht="19.8">
@@ -2581,7 +2584,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
@@ -2592,10 +2595,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2606,10 +2609,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="11" customFormat="1" ht="21">
@@ -2620,10 +2623,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21">
@@ -2648,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21">
@@ -2670,10 +2673,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21">
@@ -2684,10 +2687,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21">
@@ -2709,10 +2712,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21">
@@ -2734,10 +2737,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21">
@@ -2748,10 +2751,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">
@@ -2803,13 +2806,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="28" customFormat="1" ht="21">
@@ -2817,7 +2820,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -2829,13 +2832,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21">
@@ -2887,13 +2890,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="28" customFormat="1" ht="21">
@@ -2901,13 +2904,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>545</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>432</v>
+      </c>
+      <c r="D39" s="54" t="s">
         <v>546</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>433</v>
-      </c>
-      <c r="D39" s="54" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="21">
@@ -2924,13 +2927,13 @@
         <v>34</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="21">
@@ -2941,10 +2944,10 @@
         <v>35</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21">
@@ -2966,10 +2969,10 @@
         <v>37</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="21">
@@ -2980,10 +2983,10 @@
         <v>38</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="21">
@@ -3016,10 +3019,10 @@
         <v>41</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3030,10 +3033,10 @@
         <v>42</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3060,10 +3063,10 @@
         <v>45</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3074,10 +3077,10 @@
         <v>46</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3088,10 +3091,10 @@
         <v>47</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3541,10 +3544,10 @@
         <v>88</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="21">
@@ -3566,7 +3569,7 @@
         <v>90</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="21">
@@ -3577,10 +3580,10 @@
         <v>91</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="21">
@@ -3657,10 +3660,10 @@
         <v>98</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="21">
@@ -3770,7 +3773,7 @@
         <v>108</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="21">
@@ -3792,7 +3795,7 @@
         <v>110</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D120" s="26"/>
     </row>
@@ -3804,7 +3807,7 @@
         <v>111</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D121" s="26"/>
     </row>
@@ -3849,7 +3852,7 @@
         <v>115</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D125" s="26"/>
     </row>
@@ -3909,10 +3912,10 @@
         <v>121</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="7" customFormat="1" ht="21">
@@ -3923,10 +3926,10 @@
         <v>122</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21">
@@ -3937,10 +3940,10 @@
         <v>123</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -3951,10 +3954,10 @@
         <v>124</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
@@ -3965,10 +3968,10 @@
         <v>125</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -3979,10 +3982,10 @@
         <v>126</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -3993,10 +3996,10 @@
         <v>127</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -4007,10 +4010,10 @@
         <v>128</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
@@ -4021,10 +4024,10 @@
         <v>129</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -4057,7 +4060,7 @@
         <v>132</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D143" s="17"/>
     </row>
@@ -4081,10 +4084,10 @@
         <v>134</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4095,10 +4098,10 @@
         <v>135</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4109,10 +4112,10 @@
         <v>136</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="21">
@@ -4123,10 +4126,10 @@
         <v>137</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="21">
@@ -4137,10 +4140,10 @@
         <v>138</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="21">
@@ -4200,7 +4203,7 @@
         <v>2</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="21">
@@ -4208,13 +4211,13 @@
         <v>120</v>
       </c>
       <c r="B155" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>457</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D155" s="20" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4222,10 +4225,10 @@
         <v>120</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D156" s="32"/>
     </row>
@@ -4237,27 +4240,27 @@
         <v>144</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="158" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A158" s="30" t="s">
+        <v>480</v>
+      </c>
+      <c r="B158" s="31" t="s">
         <v>481</v>
       </c>
-      <c r="B158" s="31" t="s">
+      <c r="C158" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="C158" s="30" t="s">
+      <c r="D158" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="D158" s="37" t="s">
+      <c r="F158" s="36" t="s">
         <v>484</v>
-      </c>
-      <c r="F158" s="36" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="159" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4265,13 +4268,13 @@
         <v>120</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D159" s="37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="21">
@@ -4279,13 +4282,13 @@
         <v>120</v>
       </c>
       <c r="B160" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D160" s="20" t="s">
         <v>477</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D160" s="20" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="21">
@@ -4315,13 +4318,13 @@
         <v>120</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C163" s="21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D163" s="34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="21">
@@ -4332,10 +4335,10 @@
         <v>147</v>
       </c>
       <c r="C164" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D164" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4346,10 +4349,10 @@
         <v>148</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D165" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="21">
@@ -4358,16 +4361,16 @@
     </row>
     <row r="168" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A168" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="B168" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>498</v>
-      </c>
       <c r="C168" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D168" s="23" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="21">
@@ -4378,10 +4381,10 @@
         <v>150</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">
@@ -4389,13 +4392,13 @@
         <v>149</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">
@@ -4406,10 +4409,10 @@
         <v>151</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -4420,10 +4423,10 @@
         <v>152</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4434,10 +4437,10 @@
         <v>153</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4448,10 +4451,10 @@
         <v>154</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">
@@ -4462,10 +4465,10 @@
         <v>155</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D175" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4476,10 +4479,10 @@
         <v>156</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
@@ -4490,10 +4493,10 @@
         <v>157</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4526,10 +4529,10 @@
         <v>160</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D180" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21">
@@ -4540,10 +4543,10 @@
         <v>161</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D181" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -4562,13 +4565,13 @@
         <v>149</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C183" s="30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D183" s="39" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">
@@ -4587,13 +4590,13 @@
         <v>149</v>
       </c>
       <c r="B185" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D185" s="20" t="s">
         <v>508</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D185" s="20" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="21">
@@ -4615,10 +4618,10 @@
         <v>165</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D187" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="21">
@@ -4637,13 +4640,13 @@
         <v>149</v>
       </c>
       <c r="B189" s="13" t="s">
+        <v>522</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D189" s="20" t="s">
         <v>523</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D189" s="20" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="21">
@@ -4688,10 +4691,10 @@
         <v>170</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D193" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
@@ -4733,13 +4736,13 @@
         <v>149</v>
       </c>
       <c r="B197" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C197" s="30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D197" s="32" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="21">
@@ -4758,13 +4761,13 @@
         <v>149</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D199" s="23" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">
@@ -4772,13 +4775,13 @@
         <v>149</v>
       </c>
       <c r="B200" s="40" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D200" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">
@@ -4830,13 +4833,13 @@
         <v>178</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D206" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="21">
@@ -4844,13 +4847,13 @@
         <v>178</v>
       </c>
       <c r="B207" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D207" s="20" t="s">
         <v>516</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D207" s="20" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -4858,13 +4861,13 @@
         <v>178</v>
       </c>
       <c r="B208" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D208" s="20" t="s">
         <v>518</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D208" s="20" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4886,10 +4889,10 @@
         <v>180</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D210" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="21">
@@ -4900,10 +4903,10 @@
         <v>181</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -4914,10 +4917,10 @@
         <v>182</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D212" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -4939,10 +4942,10 @@
         <v>184</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D214" s="20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="21">
@@ -4983,7 +4986,7 @@
         <v>178</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>2</v>
@@ -4998,10 +5001,10 @@
         <v>188</v>
       </c>
       <c r="C219" s="44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D219" s="45" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="220" spans="1:4" s="51" customFormat="1" ht="21">
@@ -5012,10 +5015,10 @@
         <v>189</v>
       </c>
       <c r="C220" s="49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D220" s="50" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="21">
@@ -5048,10 +5051,10 @@
         <v>192</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D223" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="21">
@@ -5107,11 +5110,11 @@
         <v>197</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D228" s="23"/>
       <c r="F228" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="21">
@@ -5570,7 +5573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="21">
+    <row r="273" spans="1:4" ht="21">
       <c r="A273" s="3" t="s">
         <v>234</v>
       </c>
@@ -5581,7 +5584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="21">
+    <row r="274" spans="1:4" ht="21">
       <c r="A274" s="3" t="s">
         <v>234</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:3" ht="21">
+    <row r="275" spans="1:4" ht="21">
       <c r="A275" s="3" t="s">
         <v>234</v>
       </c>
@@ -5603,7 +5606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="21">
+    <row r="276" spans="1:4" ht="21">
       <c r="A276" s="3" t="s">
         <v>234</v>
       </c>
@@ -5614,7 +5617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="21">
+    <row r="277" spans="1:4" ht="21">
       <c r="A277" s="3" t="s">
         <v>234</v>
       </c>
@@ -5625,7 +5628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="21">
+    <row r="278" spans="1:4" ht="21">
       <c r="A278" s="3" t="s">
         <v>234</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="21">
+    <row r="279" spans="1:4" ht="21">
       <c r="A279" s="3" t="s">
         <v>234</v>
       </c>
@@ -5647,95 +5650,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="21">
-      <c r="A280" s="3" t="s">
+    <row r="280" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A280" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B280" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="C280" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" ht="21">
+      <c r="B280" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="C280" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="D280" s="23" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" ht="21">
       <c r="A281" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="21">
+    <row r="282" spans="1:4" ht="21">
       <c r="A282" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="21">
+    <row r="283" spans="1:4" ht="21">
       <c r="A283" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="21">
+    <row r="284" spans="1:4" ht="21">
       <c r="A284" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="21">
+    <row r="285" spans="1:4" ht="21">
       <c r="A285" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="21">
+    <row r="286" spans="1:4" ht="21">
       <c r="A286" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="21">
+    <row r="287" spans="1:4" ht="21">
       <c r="A287" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="21">
+    <row r="288" spans="1:4" ht="21">
       <c r="B288" s="4"/>
       <c r="C288" s="2"/>
     </row>
@@ -5745,10 +5751,10 @@
     </row>
     <row r="290" spans="1:3" ht="21">
       <c r="A290" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B290" s="13" t="s">
         <v>254</v>
-      </c>
-      <c r="B290" s="13" t="s">
-        <v>255</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>2</v>
@@ -5756,10 +5762,10 @@
     </row>
     <row r="291" spans="1:3" ht="21">
       <c r="A291" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>2</v>
@@ -5767,10 +5773,10 @@
     </row>
     <row r="292" spans="1:3" ht="21">
       <c r="A292" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>2</v>
@@ -5778,10 +5784,10 @@
     </row>
     <row r="293" spans="1:3" ht="21">
       <c r="A293" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>2</v>
@@ -5789,10 +5795,10 @@
     </row>
     <row r="294" spans="1:3" ht="21">
       <c r="A294" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B294" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>2</v>
@@ -5800,10 +5806,10 @@
     </row>
     <row r="295" spans="1:3" ht="21">
       <c r="A295" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B295" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>2</v>
@@ -5811,10 +5817,10 @@
     </row>
     <row r="296" spans="1:3" ht="21">
       <c r="A296" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>2</v>
@@ -5822,10 +5828,10 @@
     </row>
     <row r="297" spans="1:3" ht="21">
       <c r="A297" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>2</v>
@@ -5833,10 +5839,10 @@
     </row>
     <row r="298" spans="1:3" ht="21">
       <c r="A298" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>2</v>
@@ -5844,10 +5850,10 @@
     </row>
     <row r="299" spans="1:3" ht="21">
       <c r="A299" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C299" s="2" t="s">
         <v>2</v>
@@ -5855,10 +5861,10 @@
     </row>
     <row r="300" spans="1:3" ht="21">
       <c r="A300" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>2</v>
@@ -5866,10 +5872,10 @@
     </row>
     <row r="301" spans="1:3" ht="21">
       <c r="A301" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>2</v>
@@ -5877,10 +5883,10 @@
     </row>
     <row r="302" spans="1:3" ht="21">
       <c r="A302" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C302" s="2" t="s">
         <v>2</v>
@@ -5888,10 +5894,10 @@
     </row>
     <row r="303" spans="1:3" ht="21">
       <c r="A303" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>2</v>
@@ -5899,10 +5905,10 @@
     </row>
     <row r="304" spans="1:3" ht="21">
       <c r="A304" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>2</v>
@@ -5910,10 +5916,10 @@
     </row>
     <row r="305" spans="1:3" ht="21">
       <c r="A305" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>2</v>
@@ -5921,10 +5927,10 @@
     </row>
     <row r="306" spans="1:3" ht="21">
       <c r="A306" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>2</v>
@@ -5932,10 +5938,10 @@
     </row>
     <row r="307" spans="1:3" ht="21">
       <c r="A307" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>2</v>
@@ -5943,10 +5949,10 @@
     </row>
     <row r="308" spans="1:3" ht="21">
       <c r="A308" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>2</v>
@@ -5954,10 +5960,10 @@
     </row>
     <row r="309" spans="1:3" ht="21">
       <c r="A309" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B309" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>2</v>
@@ -5965,10 +5971,10 @@
     </row>
     <row r="310" spans="1:3" ht="21">
       <c r="A310" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>2</v>
@@ -5976,10 +5982,10 @@
     </row>
     <row r="311" spans="1:3" ht="21">
       <c r="A311" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -5987,10 +5993,10 @@
     </row>
     <row r="312" spans="1:3" ht="21">
       <c r="A312" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -5998,10 +6004,10 @@
     </row>
     <row r="313" spans="1:3" ht="21">
       <c r="A313" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>2</v>
@@ -6009,10 +6015,10 @@
     </row>
     <row r="314" spans="1:3" ht="21">
       <c r="A314" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>2</v>
@@ -6020,10 +6026,10 @@
     </row>
     <row r="315" spans="1:3" ht="21">
       <c r="A315" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>2</v>
@@ -6031,10 +6037,10 @@
     </row>
     <row r="316" spans="1:3" ht="21">
       <c r="A316" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>2</v>
@@ -6042,10 +6048,10 @@
     </row>
     <row r="317" spans="1:3" ht="21">
       <c r="A317" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -6053,10 +6059,10 @@
     </row>
     <row r="318" spans="1:3" ht="21">
       <c r="A318" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -6064,10 +6070,10 @@
     </row>
     <row r="319" spans="1:3" ht="21">
       <c r="A319" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
@@ -6075,10 +6081,10 @@
     </row>
     <row r="320" spans="1:3" ht="21">
       <c r="A320" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6086,10 +6092,10 @@
     </row>
     <row r="321" spans="1:4" ht="21">
       <c r="A321" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -6097,10 +6103,10 @@
     </row>
     <row r="322" spans="1:4" ht="21">
       <c r="A322" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -6108,10 +6114,10 @@
     </row>
     <row r="323" spans="1:4" ht="21">
       <c r="A323" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>2</v>
@@ -6119,10 +6125,10 @@
     </row>
     <row r="324" spans="1:4" ht="21">
       <c r="A324" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>2</v>
@@ -6130,10 +6136,10 @@
     </row>
     <row r="325" spans="1:4" ht="21">
       <c r="A325" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>2</v>
@@ -6141,10 +6147,10 @@
     </row>
     <row r="326" spans="1:4" ht="21">
       <c r="A326" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>2</v>
@@ -6152,10 +6158,10 @@
     </row>
     <row r="327" spans="1:4" ht="21">
       <c r="A327" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>2</v>
@@ -6171,38 +6177,38 @@
     </row>
     <row r="330" spans="1:4" ht="21">
       <c r="A330" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D330" s="21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="21">
       <c r="A331" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D331" s="16" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="332" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A332" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C332" s="6" t="s">
         <v>2</v>
@@ -6211,38 +6217,38 @@
     </row>
     <row r="333" spans="1:4" ht="21">
       <c r="A333" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D333" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="21">
       <c r="A334" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="335" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A335" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B335" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C335" s="6" t="s">
         <v>2</v>
@@ -6251,10 +6257,10 @@
     </row>
     <row r="336" spans="1:4" ht="21">
       <c r="A336" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
@@ -6262,10 +6268,10 @@
     </row>
     <row r="337" spans="1:6" ht="21">
       <c r="A337" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>2</v>
@@ -6273,38 +6279,38 @@
     </row>
     <row r="338" spans="1:6" ht="21">
       <c r="A338" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D338" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="339" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A339" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B339" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D339" s="22" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -6312,10 +6318,10 @@
     </row>
     <row r="341" spans="1:6" ht="21">
       <c r="A341" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>2</v>
@@ -6323,10 +6329,10 @@
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6334,24 +6340,24 @@
     </row>
     <row r="343" spans="1:6" ht="21">
       <c r="A343" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D343" s="20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6359,24 +6365,24 @@
     </row>
     <row r="345" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A345" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D345" s="53" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
       <c r="A346" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>2</v>
@@ -6384,19 +6390,19 @@
     </row>
     <row r="347" spans="1:6" ht="21">
       <c r="A347" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D347" s="20" t="s">
+        <v>537</v>
+      </c>
+      <c r="F347" t="s">
         <v>538</v>
-      </c>
-      <c r="F347" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="21">
@@ -6409,10 +6415,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B350" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="B350" s="13" t="s">
-        <v>311</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6420,10 +6426,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6431,10 +6437,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6442,10 +6448,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6453,10 +6459,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6464,10 +6470,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -6475,10 +6481,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6486,10 +6492,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6497,10 +6503,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6508,10 +6514,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6519,10 +6525,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6530,10 +6536,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6541,10 +6547,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6552,10 +6558,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6563,10 +6569,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6574,10 +6580,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6585,10 +6591,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6596,10 +6602,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -6607,10 +6613,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -6618,10 +6624,10 @@
     </row>
     <row r="369" spans="1:4" ht="21">
       <c r="A369" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -6629,10 +6635,10 @@
     </row>
     <row r="370" spans="1:4" ht="21">
       <c r="A370" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -6640,10 +6646,10 @@
     </row>
     <row r="371" spans="1:4" ht="21">
       <c r="A371" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -6651,10 +6657,10 @@
     </row>
     <row r="372" spans="1:4" ht="21">
       <c r="A372" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -6662,10 +6668,10 @@
     </row>
     <row r="373" spans="1:4" ht="21">
       <c r="A373" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -6673,10 +6679,10 @@
     </row>
     <row r="374" spans="1:4" ht="21">
       <c r="A374" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>2</v>
@@ -6684,10 +6690,10 @@
     </row>
     <row r="375" spans="1:4" ht="21">
       <c r="A375" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -6695,10 +6701,10 @@
     </row>
     <row r="376" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A376" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C376" s="6" t="s">
         <v>2</v>
@@ -6707,10 +6713,10 @@
     </row>
     <row r="377" spans="1:4" ht="21">
       <c r="A377" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -6718,10 +6724,10 @@
     </row>
     <row r="378" spans="1:4" ht="21">
       <c r="A378" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -6729,10 +6735,10 @@
     </row>
     <row r="379" spans="1:4" ht="21">
       <c r="A379" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -6740,10 +6746,10 @@
     </row>
     <row r="380" spans="1:4" ht="21">
       <c r="A380" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -6751,10 +6757,10 @@
     </row>
     <row r="381" spans="1:4" ht="21">
       <c r="A381" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -6762,10 +6768,10 @@
     </row>
     <row r="382" spans="1:4" ht="21">
       <c r="A382" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -6773,10 +6779,10 @@
     </row>
     <row r="383" spans="1:4" ht="21">
       <c r="A383" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -6784,10 +6790,10 @@
     </row>
     <row r="384" spans="1:4" ht="21">
       <c r="A384" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -6795,10 +6801,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -6806,10 +6812,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -6817,10 +6823,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -6828,10 +6834,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -6839,10 +6845,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -6850,10 +6856,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -6861,10 +6867,10 @@
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="A391" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>2</v>
@@ -6872,10 +6878,10 @@
     </row>
     <row r="392" spans="1:3" ht="21">
       <c r="A392" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>2</v>
@@ -6891,10 +6897,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B395" s="13" t="s">
         <v>354</v>
-      </c>
-      <c r="B395" s="13" t="s">
-        <v>355</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -6902,10 +6908,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -6913,10 +6919,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -6924,7 +6930,7 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B398" s="13" t="s">
         <v>79</v>
@@ -6935,10 +6941,10 @@
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="A399" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>2</v>
@@ -6946,10 +6952,10 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="A400" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B400" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>2</v>
@@ -6965,21 +6971,21 @@
     </row>
     <row r="403" spans="1:3" ht="21">
       <c r="A403" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B403" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="B403" s="13" t="s">
-        <v>361</v>
-      </c>
       <c r="C403" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
       <c r="A404" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -6987,10 +6993,10 @@
     </row>
     <row r="405" spans="1:3" ht="21">
       <c r="A405" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -6998,10 +7004,10 @@
     </row>
     <row r="406" spans="1:3" ht="21">
       <c r="A406" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>2</v>
@@ -7009,10 +7015,10 @@
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7020,21 +7026,21 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="A408" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7042,7 +7048,7 @@
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B410" s="13" t="s">
         <v>242</v>
@@ -7053,10 +7059,10 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7064,10 +7070,10 @@
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7075,10 +7081,10 @@
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7086,10 +7092,10 @@
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>2</v>
@@ -7097,10 +7103,10 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>2</v>
@@ -7108,10 +7114,10 @@
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7119,10 +7125,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7130,10 +7136,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7141,10 +7147,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7152,10 +7158,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7163,10 +7169,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7174,10 +7180,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7185,10 +7191,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7196,10 +7202,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7207,10 +7213,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7218,10 +7224,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7229,10 +7235,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7240,10 +7246,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7251,10 +7257,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7262,10 +7268,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7273,10 +7279,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7284,10 +7290,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7295,10 +7301,10 @@
     </row>
     <row r="433" spans="1:4" ht="21">
       <c r="A433" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7306,10 +7312,10 @@
     </row>
     <row r="434" spans="1:4" ht="21">
       <c r="A434" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7317,10 +7323,10 @@
     </row>
     <row r="435" spans="1:4" ht="21">
       <c r="A435" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>2</v>
@@ -7328,10 +7334,10 @@
     </row>
     <row r="436" spans="1:4" ht="21">
       <c r="A436" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7339,10 +7345,10 @@
     </row>
     <row r="437" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A437" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B437" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>2</v>
@@ -7351,10 +7357,10 @@
     </row>
     <row r="438" spans="1:4" ht="21">
       <c r="A438" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7362,10 +7368,10 @@
     </row>
     <row r="439" spans="1:4" ht="21">
       <c r="A439" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7373,10 +7379,10 @@
     </row>
     <row r="440" spans="1:4" ht="21">
       <c r="A440" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7384,10 +7390,10 @@
     </row>
     <row r="441" spans="1:4" ht="21">
       <c r="A441" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7395,10 +7401,10 @@
     </row>
     <row r="442" spans="1:4" ht="21">
       <c r="A442" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7406,10 +7412,10 @@
     </row>
     <row r="443" spans="1:4" ht="21">
       <c r="A443" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7417,10 +7423,10 @@
     </row>
     <row r="444" spans="1:4" ht="21">
       <c r="A444" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7428,10 +7434,10 @@
     </row>
     <row r="445" spans="1:4" ht="21">
       <c r="A445" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7439,10 +7445,10 @@
     </row>
     <row r="446" spans="1:4" ht="21">
       <c r="A446" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7450,10 +7456,10 @@
     </row>
     <row r="447" spans="1:4" ht="21">
       <c r="A447" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>2</v>
@@ -7461,10 +7467,10 @@
     </row>
     <row r="448" spans="1:4" ht="21">
       <c r="A448" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>2</v>
@@ -7472,10 +7478,10 @@
     </row>
     <row r="449" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A449" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B449" s="25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C449" s="24" t="s">
         <v>2</v>
@@ -7484,10 +7490,10 @@
     </row>
     <row r="450" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A450" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B450" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C450" s="24" t="s">
         <v>2</v>
@@ -7496,10 +7502,10 @@
     </row>
     <row r="451" spans="1:4" ht="21">
       <c r="A451" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7507,10 +7513,10 @@
     </row>
     <row r="452" spans="1:4" ht="21">
       <c r="A452" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7518,10 +7524,10 @@
     </row>
     <row r="453" spans="1:4" ht="21">
       <c r="A453" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C453" s="2" t="s">
         <v>2</v>
@@ -7529,10 +7535,10 @@
     </row>
     <row r="454" spans="1:4" ht="21">
       <c r="A454" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7540,22 +7546,22 @@
     </row>
     <row r="455" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A455" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B455" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D455" s="23"/>
     </row>
     <row r="456" spans="1:4" ht="21">
       <c r="A456" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>2</v>
@@ -7563,10 +7569,10 @@
     </row>
     <row r="457" spans="1:4" ht="21">
       <c r="A457" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7574,10 +7580,10 @@
     </row>
     <row r="458" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A458" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>2</v>
@@ -7586,10 +7592,10 @@
     </row>
     <row r="459" spans="1:4" ht="21">
       <c r="A459" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -7597,10 +7603,10 @@
     </row>
     <row r="460" spans="1:4" ht="21">
       <c r="A460" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -7608,10 +7614,10 @@
     </row>
     <row r="461" spans="1:4" ht="21">
       <c r="A461" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>2</v>
@@ -7619,10 +7625,10 @@
     </row>
     <row r="462" spans="1:4" ht="21">
       <c r="A462" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>2</v>
@@ -7639,10 +7645,10 @@
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B465" s="13" t="s">
         <v>420</v>
-      </c>
-      <c r="B465" s="13" t="s">
-        <v>421</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>2</v>
@@ -7650,10 +7656,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>2</v>
@@ -7661,10 +7667,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>2</v>
@@ -7672,10 +7678,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>2</v>
@@ -7683,10 +7689,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -7694,21 +7700,21 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="A470" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>2</v>
@@ -7716,10 +7722,10 @@
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>2</v>
@@ -7727,10 +7733,10 @@
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>2</v>
@@ -7738,13 +7744,13 @@
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -8000,7 +8006,7 @@
     <hyperlink ref="B277" r:id="rId249"/>
     <hyperlink ref="B278" r:id="rId250"/>
     <hyperlink ref="B279" r:id="rId251"/>
-    <hyperlink ref="B280" r:id="rId252"/>
+    <hyperlink ref="B280" r:id="rId252" display="Combinational Sum"/>
     <hyperlink ref="B281" r:id="rId253"/>
     <hyperlink ref="B282" r:id="rId254"/>
     <hyperlink ref="B283" r:id="rId255"/>
@@ -8271,8 +8277,9 @@
     <hyperlink ref="D43" r:id="rId520"/>
     <hyperlink ref="D45" r:id="rId521"/>
     <hyperlink ref="D50" r:id="rId522"/>
+    <hyperlink ref="D280" r:id="rId523"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId523"/>
+  <pageSetup orientation="portrait" r:id="rId524"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
count inversion and minimize the difference between heights
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="562">
   <si>
     <t>Topic:</t>
   </si>
@@ -1714,6 +1714,15 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/find-minimum-number-of-merge-operations-to-make-an-array-palindrome/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/global-and-local-inversions/submissions/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/global-and-local-inversions/discuss/150991/From-intuition-to-optimization</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/minimize-the-maximum_696194?leftPanelTab=2</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +2007,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2135,6 +2144,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
@@ -2456,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2595,9 +2607,11 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="17"/>
+        <v>431</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="21">
       <c r="A13" s="3" t="s">
@@ -2655,7 +2669,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21">
+    <row r="17" spans="1:6" ht="21">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2666,7 +2680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="19.8">
+    <row r="18" spans="1:6" ht="19.8">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2680,7 +2694,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21">
+    <row r="19" spans="1:6" ht="21">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -2688,10 +2702,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="9" customFormat="1" ht="19.8">
+        <v>431</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>559</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A20" s="8" t="s">
         <v>3</v>
       </c>
@@ -2705,7 +2725,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21">
+    <row r="21" spans="1:6" ht="21">
       <c r="A21" s="3" t="s">
         <v>3</v>
       </c>
@@ -2719,7 +2739,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21">
+    <row r="22" spans="1:6" ht="21">
       <c r="A22" s="3" t="s">
         <v>3</v>
       </c>
@@ -2730,7 +2750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21">
+    <row r="23" spans="1:6" ht="21">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -2744,7 +2764,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21">
+    <row r="24" spans="1:6" ht="21">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -2758,7 +2778,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="21">
+    <row r="25" spans="1:6" ht="21">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2772,7 +2792,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21">
+    <row r="26" spans="1:6" ht="21">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -2786,7 +2806,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21">
+    <row r="27" spans="1:6" ht="21">
       <c r="A27" s="3" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2820,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21">
+    <row r="28" spans="1:6" ht="21">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
@@ -2811,7 +2831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="21">
+    <row r="29" spans="1:6" ht="21">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -2822,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21">
+    <row r="30" spans="1:6" ht="21">
       <c r="A30" s="3" t="s">
         <v>3</v>
       </c>
@@ -2833,7 +2853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="25" customFormat="1" ht="21">
+    <row r="31" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A31" s="24" t="s">
         <v>3</v>
       </c>
@@ -2847,7 +2867,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="28" customFormat="1" ht="21">
+    <row r="32" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A32" s="27" t="s">
         <v>3</v>
       </c>
@@ -8316,8 +8336,10 @@
     <hyperlink ref="D27" r:id="rId524"/>
     <hyperlink ref="D24" r:id="rId525"/>
     <hyperlink ref="D37" r:id="rId526"/>
+    <hyperlink ref="D19" r:id="rId527"/>
+    <hyperlink ref="D12" r:id="rId528"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId527"/>
+  <pageSetup orientation="portrait" r:id="rId529"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
intersection of 3 arrays
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="566">
   <si>
     <t>Topic:</t>
   </si>
@@ -1732,6 +1732,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/smallest-index-with-equal-value/submissions/</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/find-common-elements-three-sorted-arrays/</t>
   </si>
 </sst>
 </file>
@@ -2477,8 +2480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2759,7 +2762,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>2</v>
+        <v>430</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -8360,8 +8366,9 @@
     <hyperlink ref="D34" r:id="rId529"/>
     <hyperlink ref="D10" r:id="rId530"/>
     <hyperlink ref="D99" r:id="rId531"/>
+    <hyperlink ref="D22" r:id="rId532"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId532"/>
+  <pageSetup orientation="portrait" r:id="rId533"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
search in rotated array (binary Search)
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="567">
   <si>
     <t>Topic:</t>
   </si>
@@ -1735,6 +1735,9 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/find-common-elements-three-sorted-arrays/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array/</t>
   </si>
 </sst>
 </file>
@@ -2480,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -3650,6 +3653,9 @@
       </c>
       <c r="C100" s="2" t="s">
         <v>430</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="21">
@@ -8367,8 +8373,9 @@
     <hyperlink ref="D10" r:id="rId530"/>
     <hyperlink ref="D99" r:id="rId531"/>
     <hyperlink ref="D22" r:id="rId532"/>
+    <hyperlink ref="D100" r:id="rId533"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId533"/>
+  <pageSetup orientation="portrait" r:id="rId534"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2 stack in an array
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="569">
   <si>
     <t>Topic:</t>
   </si>
@@ -1741,6 +1741,9 @@
   </si>
   <si>
     <t>programs folder</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/two-stacks_983634?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2486,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D290" sqref="D290"/>
+    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F289" sqref="F289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5872,6 +5875,9 @@
       </c>
       <c r="C292" s="2" t="s">
         <v>430</v>
+      </c>
+      <c r="D292" s="20" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="21">
@@ -8380,8 +8386,9 @@
     <hyperlink ref="D99" r:id="rId531"/>
     <hyperlink ref="D22" r:id="rId532"/>
     <hyperlink ref="D100" r:id="rId533"/>
+    <hyperlink ref="D292" r:id="rId534"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId534"/>
+  <pageSetup orientation="portrait" r:id="rId535"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
find middle element in stack ans insert at bottom of stack
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="572">
   <si>
     <t>Topic:</t>
   </si>
@@ -795,9 +795,6 @@
   </si>
   <si>
     <t>Implement "N" stacks in an Array</t>
-  </si>
-  <si>
-    <t>Check the expression has valid or Balanced parenthesis or not.</t>
   </si>
   <si>
     <t>Reverse a String using Stack</t>
@@ -1744,6 +1741,18 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/two-stacks_983634?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-string/discuss/1307212/C%2B%2B-4-Different-Solutions-Recursion-Iterative-AND-Stacks..-Complete-Beginner</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/delete-middle-element-from-stack_985246?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>Check the expression has valid or Balanced parenthesis or not. V.V.V.IMP</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/insert-an-element-at-its-bottom-in-a-given-stack_1171166?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2489,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F289" sqref="F289"/>
+    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F302" sqref="F302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2505,7 +2514,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21">
@@ -2516,10 +2525,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2533,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21">
@@ -2547,10 +2556,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2561,10 +2570,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2575,10 +2584,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2589,10 +2598,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2603,10 +2612,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2617,10 +2626,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>430</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1" ht="19.8">
@@ -2631,10 +2640,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -2648,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
@@ -2659,10 +2668,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2673,10 +2682,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="11" customFormat="1" ht="21">
@@ -2687,10 +2696,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="21">
@@ -2698,7 +2707,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2712,10 +2721,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2726,13 +2735,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>557</v>
+      </c>
+      <c r="F19" s="58" t="s">
         <v>558</v>
-      </c>
-      <c r="F19" s="58" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2743,10 +2752,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="21">
@@ -2757,10 +2766,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2771,10 +2780,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2785,10 +2794,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2799,10 +2808,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2813,10 +2822,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2827,10 +2836,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2841,10 +2850,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -2885,13 +2894,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="28" customFormat="1" ht="21">
@@ -2899,7 +2908,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -2911,13 +2920,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="7" customFormat="1" ht="21">
@@ -2925,13 +2934,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21">
@@ -2964,10 +2973,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="28" customFormat="1" ht="21">
@@ -2975,13 +2984,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="28" customFormat="1" ht="21">
@@ -2989,13 +2998,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="D39" s="54" t="s">
         <v>543</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>430</v>
-      </c>
-      <c r="D39" s="54" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="21">
@@ -3012,13 +3021,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="21">
@@ -3029,10 +3038,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21">
@@ -3054,10 +3063,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="21">
@@ -3068,10 +3077,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="21">
@@ -3104,10 +3113,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3118,10 +3127,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3148,10 +3157,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3162,10 +3171,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3176,10 +3185,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3630,10 +3639,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="21">
@@ -3644,10 +3653,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="21">
@@ -3658,10 +3667,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="21">
@@ -3672,10 +3681,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="21">
@@ -3752,10 +3761,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="21">
@@ -3865,7 +3874,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="21">
@@ -3887,7 +3896,7 @@
         <v>108</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D120" s="26"/>
     </row>
@@ -3899,7 +3908,7 @@
         <v>109</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D121" s="26"/>
     </row>
@@ -3944,7 +3953,7 @@
         <v>113</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D125" s="26"/>
     </row>
@@ -4004,10 +4013,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="7" customFormat="1" ht="21">
@@ -4018,10 +4027,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21">
@@ -4032,10 +4041,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -4046,10 +4055,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
@@ -4060,10 +4069,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -4074,10 +4083,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -4088,10 +4097,10 @@
         <v>125</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -4102,10 +4111,10 @@
         <v>126</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
@@ -4116,10 +4125,10 @@
         <v>127</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -4152,7 +4161,7 @@
         <v>130</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D143" s="17"/>
     </row>
@@ -4176,10 +4185,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4190,10 +4199,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4204,10 +4213,10 @@
         <v>134</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="21">
@@ -4218,10 +4227,10 @@
         <v>135</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="21">
@@ -4232,10 +4241,10 @@
         <v>136</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="21">
@@ -4295,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="21">
@@ -4303,13 +4312,13 @@
         <v>118</v>
       </c>
       <c r="B155" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>454</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D155" s="20" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4317,10 +4326,10 @@
         <v>118</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D156" s="32"/>
     </row>
@@ -4332,27 +4341,27 @@
         <v>142</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A158" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="B158" s="31" t="s">
         <v>478</v>
       </c>
-      <c r="B158" s="31" t="s">
+      <c r="C158" s="30" t="s">
         <v>479</v>
       </c>
-      <c r="C158" s="30" t="s">
+      <c r="D158" s="37" t="s">
         <v>480</v>
       </c>
-      <c r="D158" s="37" t="s">
+      <c r="F158" s="36" t="s">
         <v>481</v>
-      </c>
-      <c r="F158" s="36" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="159" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4360,13 +4369,13 @@
         <v>118</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D159" s="37" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="21">
@@ -4374,13 +4383,13 @@
         <v>118</v>
       </c>
       <c r="B160" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D160" s="20" t="s">
         <v>474</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D160" s="20" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="21">
@@ -4410,13 +4419,13 @@
         <v>118</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C163" s="21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D163" s="34" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="21">
@@ -4427,10 +4436,10 @@
         <v>145</v>
       </c>
       <c r="C164" s="35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D164" s="20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4441,10 +4450,10 @@
         <v>146</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D165" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="21">
@@ -4453,16 +4462,16 @@
     </row>
     <row r="168" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A168" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="B168" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>495</v>
-      </c>
       <c r="C168" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D168" s="23" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="21">
@@ -4473,10 +4482,10 @@
         <v>148</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">
@@ -4484,13 +4493,13 @@
         <v>147</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">
@@ -4501,10 +4510,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -4515,10 +4524,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4529,10 +4538,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4543,10 +4552,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">
@@ -4557,10 +4566,10 @@
         <v>153</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D175" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4571,10 +4580,10 @@
         <v>154</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
@@ -4585,10 +4594,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4621,10 +4630,10 @@
         <v>158</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D180" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21">
@@ -4635,10 +4644,10 @@
         <v>159</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D181" s="20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -4657,13 +4666,13 @@
         <v>147</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C183" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D183" s="39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">
@@ -4682,13 +4691,13 @@
         <v>147</v>
       </c>
       <c r="B185" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D185" s="20" t="s">
         <v>505</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D185" s="20" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="21">
@@ -4710,10 +4719,10 @@
         <v>163</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D187" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="21">
@@ -4732,13 +4741,13 @@
         <v>147</v>
       </c>
       <c r="B189" s="13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D189" s="20" t="s">
         <v>520</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D189" s="20" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="21">
@@ -4783,10 +4792,10 @@
         <v>168</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D193" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
@@ -4828,13 +4837,13 @@
         <v>147</v>
       </c>
       <c r="B197" s="38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C197" s="30" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D197" s="32" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="21">
@@ -4853,13 +4862,13 @@
         <v>147</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D199" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">
@@ -4867,13 +4876,13 @@
         <v>147</v>
       </c>
       <c r="B200" s="40" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D200" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">
@@ -4925,13 +4934,13 @@
         <v>176</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D206" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="21">
@@ -4939,13 +4948,13 @@
         <v>176</v>
       </c>
       <c r="B207" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D207" s="20" t="s">
         <v>513</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D207" s="20" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -4953,13 +4962,13 @@
         <v>176</v>
       </c>
       <c r="B208" s="13" t="s">
+        <v>514</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D208" s="20" t="s">
         <v>515</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D208" s="20" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -4981,10 +4990,10 @@
         <v>178</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D210" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="21">
@@ -4995,10 +5004,10 @@
         <v>179</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -5009,10 +5018,10 @@
         <v>180</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D212" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -5034,10 +5043,10 @@
         <v>182</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D214" s="20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="21">
@@ -5078,7 +5087,7 @@
         <v>176</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>2</v>
@@ -5093,10 +5102,10 @@
         <v>186</v>
       </c>
       <c r="C219" s="44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D219" s="45" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="220" spans="1:4" s="51" customFormat="1" ht="21">
@@ -5107,10 +5116,10 @@
         <v>187</v>
       </c>
       <c r="C220" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D220" s="50" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="21">
@@ -5143,10 +5152,10 @@
         <v>190</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D223" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="21">
@@ -5202,11 +5211,11 @@
         <v>195</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D228" s="23"/>
       <c r="F228" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="21">
@@ -5747,13 +5756,13 @@
         <v>232</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D280" s="23" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="21">
@@ -5849,10 +5858,10 @@
         <v>252</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D290" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="21">
@@ -5874,10 +5883,10 @@
         <v>254</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D292" s="20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="21">
@@ -5888,7 +5897,10 @@
         <v>255</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="D293" s="20" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="21">
@@ -5902,26 +5914,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="21">
-      <c r="A295" s="3" t="s">
+    <row r="295" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A295" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B295" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B295" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="C295" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D295" s="23"/>
     </row>
     <row r="296" spans="1:4" ht="21">
       <c r="A296" s="3" t="s">
         <v>251</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="D296" s="20" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="21">
@@ -5929,7 +5945,7 @@
         <v>251</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>2</v>
@@ -5940,7 +5956,7 @@
         <v>251</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C298" s="2" t="s">
         <v>2</v>
@@ -5951,7 +5967,7 @@
         <v>251</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C299" s="2" t="s">
         <v>2</v>
@@ -5962,7 +5978,7 @@
         <v>251</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>2</v>
@@ -5973,7 +5989,7 @@
         <v>251</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>2</v>
@@ -5984,10 +6000,13 @@
         <v>251</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="D302" s="20" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="21">
@@ -5995,7 +6014,7 @@
         <v>251</v>
       </c>
       <c r="B303" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>2</v>
@@ -6006,7 +6025,7 @@
         <v>251</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>2</v>
@@ -6017,7 +6036,7 @@
         <v>251</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>2</v>
@@ -6028,7 +6047,7 @@
         <v>251</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>2</v>
@@ -6039,7 +6058,7 @@
         <v>251</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>2</v>
@@ -6050,7 +6069,7 @@
         <v>251</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>2</v>
@@ -6061,7 +6080,7 @@
         <v>251</v>
       </c>
       <c r="B309" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>2</v>
@@ -6072,7 +6091,7 @@
         <v>251</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>2</v>
@@ -6083,7 +6102,7 @@
         <v>251</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -6094,7 +6113,7 @@
         <v>251</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -6105,7 +6124,7 @@
         <v>251</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>2</v>
@@ -6116,7 +6135,7 @@
         <v>251</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>2</v>
@@ -6127,7 +6146,7 @@
         <v>251</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>2</v>
@@ -6138,7 +6157,7 @@
         <v>251</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>2</v>
@@ -6149,7 +6168,7 @@
         <v>251</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -6160,7 +6179,7 @@
         <v>251</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -6171,7 +6190,7 @@
         <v>251</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
@@ -6182,7 +6201,7 @@
         <v>251</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6193,7 +6212,7 @@
         <v>251</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -6204,7 +6223,7 @@
         <v>251</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -6215,7 +6234,7 @@
         <v>251</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>2</v>
@@ -6226,7 +6245,7 @@
         <v>251</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>2</v>
@@ -6237,7 +6256,7 @@
         <v>251</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>2</v>
@@ -6248,7 +6267,7 @@
         <v>251</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>2</v>
@@ -6259,7 +6278,7 @@
         <v>251</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>2</v>
@@ -6275,38 +6294,38 @@
     </row>
     <row r="330" spans="1:4" ht="21">
       <c r="A330" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D330" s="21" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="21">
       <c r="A331" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D331" s="16" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="332" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A332" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C332" s="6" t="s">
         <v>2</v>
@@ -6315,38 +6334,38 @@
     </row>
     <row r="333" spans="1:4" ht="21">
       <c r="A333" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D333" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="21">
       <c r="A334" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="335" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A335" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B335" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C335" s="6" t="s">
         <v>2</v>
@@ -6355,10 +6374,10 @@
     </row>
     <row r="336" spans="1:4" ht="21">
       <c r="A336" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
@@ -6366,10 +6385,10 @@
     </row>
     <row r="337" spans="1:6" ht="21">
       <c r="A337" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>2</v>
@@ -6377,38 +6396,38 @@
     </row>
     <row r="338" spans="1:6" ht="21">
       <c r="A338" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D338" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="339" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A339" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B339" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D339" s="22" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -6416,10 +6435,10 @@
     </row>
     <row r="341" spans="1:6" ht="21">
       <c r="A341" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>2</v>
@@ -6427,10 +6446,10 @@
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6438,24 +6457,24 @@
     </row>
     <row r="343" spans="1:6" ht="21">
       <c r="A343" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D343" s="20" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6463,24 +6482,24 @@
     </row>
     <row r="345" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A345" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D345" s="53" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
       <c r="A346" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>2</v>
@@ -6488,19 +6507,19 @@
     </row>
     <row r="347" spans="1:6" ht="21">
       <c r="A347" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D347" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F347" t="s">
         <v>535</v>
-      </c>
-      <c r="F347" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="21">
@@ -6513,10 +6532,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B350" s="13" t="s">
         <v>307</v>
-      </c>
-      <c r="B350" s="13" t="s">
-        <v>308</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6524,10 +6543,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6535,10 +6554,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6546,10 +6565,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6557,10 +6576,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6568,10 +6587,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -6579,10 +6598,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6590,10 +6609,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6601,10 +6620,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6612,10 +6631,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6623,10 +6642,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6634,10 +6653,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6645,10 +6664,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6656,10 +6675,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6667,10 +6686,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6678,10 +6697,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6689,10 +6708,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6700,10 +6719,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -6711,10 +6730,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -6722,10 +6741,10 @@
     </row>
     <row r="369" spans="1:4" ht="21">
       <c r="A369" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -6733,10 +6752,10 @@
     </row>
     <row r="370" spans="1:4" ht="21">
       <c r="A370" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -6744,10 +6763,10 @@
     </row>
     <row r="371" spans="1:4" ht="21">
       <c r="A371" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -6755,10 +6774,10 @@
     </row>
     <row r="372" spans="1:4" ht="21">
       <c r="A372" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -6766,10 +6785,10 @@
     </row>
     <row r="373" spans="1:4" ht="21">
       <c r="A373" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -6777,10 +6796,10 @@
     </row>
     <row r="374" spans="1:4" ht="21">
       <c r="A374" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>2</v>
@@ -6788,10 +6807,10 @@
     </row>
     <row r="375" spans="1:4" ht="21">
       <c r="A375" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -6799,10 +6818,10 @@
     </row>
     <row r="376" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A376" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C376" s="6" t="s">
         <v>2</v>
@@ -6811,10 +6830,10 @@
     </row>
     <row r="377" spans="1:4" ht="21">
       <c r="A377" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -6822,10 +6841,10 @@
     </row>
     <row r="378" spans="1:4" ht="21">
       <c r="A378" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -6833,10 +6852,10 @@
     </row>
     <row r="379" spans="1:4" ht="21">
       <c r="A379" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -6844,10 +6863,10 @@
     </row>
     <row r="380" spans="1:4" ht="21">
       <c r="A380" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -6855,10 +6874,10 @@
     </row>
     <row r="381" spans="1:4" ht="21">
       <c r="A381" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -6866,10 +6885,10 @@
     </row>
     <row r="382" spans="1:4" ht="21">
       <c r="A382" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -6877,10 +6896,10 @@
     </row>
     <row r="383" spans="1:4" ht="21">
       <c r="A383" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -6888,10 +6907,10 @@
     </row>
     <row r="384" spans="1:4" ht="21">
       <c r="A384" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -6899,10 +6918,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -6910,10 +6929,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -6921,10 +6940,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -6932,10 +6951,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -6943,10 +6962,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -6954,10 +6973,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -6965,10 +6984,10 @@
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="A391" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>2</v>
@@ -6976,10 +6995,10 @@
     </row>
     <row r="392" spans="1:3" ht="21">
       <c r="A392" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>2</v>
@@ -6995,10 +7014,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B395" s="13" t="s">
         <v>351</v>
-      </c>
-      <c r="B395" s="13" t="s">
-        <v>352</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7006,10 +7025,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -7017,10 +7036,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -7028,7 +7047,7 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B398" s="13" t="s">
         <v>77</v>
@@ -7039,10 +7058,10 @@
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="A399" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>2</v>
@@ -7050,10 +7069,10 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="A400" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B400" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>2</v>
@@ -7069,21 +7088,21 @@
     </row>
     <row r="403" spans="1:3" ht="21">
       <c r="A403" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B403" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="B403" s="13" t="s">
-        <v>358</v>
-      </c>
       <c r="C403" s="35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
       <c r="A404" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7091,10 +7110,10 @@
     </row>
     <row r="405" spans="1:3" ht="21">
       <c r="A405" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -7102,10 +7121,10 @@
     </row>
     <row r="406" spans="1:3" ht="21">
       <c r="A406" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>2</v>
@@ -7113,10 +7132,10 @@
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7124,21 +7143,21 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="A408" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7146,7 +7165,7 @@
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B410" s="13" t="s">
         <v>240</v>
@@ -7157,10 +7176,10 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7168,10 +7187,10 @@
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7179,10 +7198,10 @@
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7190,10 +7209,10 @@
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>2</v>
@@ -7201,10 +7220,10 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>2</v>
@@ -7212,10 +7231,10 @@
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7223,10 +7242,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7234,10 +7253,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7245,10 +7264,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7256,10 +7275,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7267,10 +7286,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7278,10 +7297,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7289,10 +7308,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7300,10 +7319,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7311,10 +7330,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7322,10 +7341,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7333,10 +7352,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7344,10 +7363,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7355,10 +7374,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7366,10 +7385,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7377,10 +7396,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7388,10 +7407,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7399,10 +7418,10 @@
     </row>
     <row r="433" spans="1:4" ht="21">
       <c r="A433" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7410,10 +7429,10 @@
     </row>
     <row r="434" spans="1:4" ht="21">
       <c r="A434" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7421,10 +7440,10 @@
     </row>
     <row r="435" spans="1:4" ht="21">
       <c r="A435" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>2</v>
@@ -7432,10 +7451,10 @@
     </row>
     <row r="436" spans="1:4" ht="21">
       <c r="A436" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7443,10 +7462,10 @@
     </row>
     <row r="437" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A437" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B437" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>2</v>
@@ -7455,10 +7474,10 @@
     </row>
     <row r="438" spans="1:4" ht="21">
       <c r="A438" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7466,10 +7485,10 @@
     </row>
     <row r="439" spans="1:4" ht="21">
       <c r="A439" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7477,10 +7496,10 @@
     </row>
     <row r="440" spans="1:4" ht="21">
       <c r="A440" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7488,10 +7507,10 @@
     </row>
     <row r="441" spans="1:4" ht="21">
       <c r="A441" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7499,10 +7518,10 @@
     </row>
     <row r="442" spans="1:4" ht="21">
       <c r="A442" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7510,10 +7529,10 @@
     </row>
     <row r="443" spans="1:4" ht="21">
       <c r="A443" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7521,10 +7540,10 @@
     </row>
     <row r="444" spans="1:4" ht="21">
       <c r="A444" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7532,10 +7551,10 @@
     </row>
     <row r="445" spans="1:4" ht="21">
       <c r="A445" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7543,10 +7562,10 @@
     </row>
     <row r="446" spans="1:4" ht="21">
       <c r="A446" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7554,10 +7573,10 @@
     </row>
     <row r="447" spans="1:4" ht="21">
       <c r="A447" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>2</v>
@@ -7565,10 +7584,10 @@
     </row>
     <row r="448" spans="1:4" ht="21">
       <c r="A448" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>2</v>
@@ -7576,10 +7595,10 @@
     </row>
     <row r="449" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A449" s="24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B449" s="25" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C449" s="24" t="s">
         <v>2</v>
@@ -7588,10 +7607,10 @@
     </row>
     <row r="450" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A450" s="24" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B450" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C450" s="24" t="s">
         <v>2</v>
@@ -7600,10 +7619,10 @@
     </row>
     <row r="451" spans="1:4" ht="21">
       <c r="A451" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7611,10 +7630,10 @@
     </row>
     <row r="452" spans="1:4" ht="21">
       <c r="A452" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7622,10 +7641,10 @@
     </row>
     <row r="453" spans="1:4" ht="21">
       <c r="A453" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C453" s="2" t="s">
         <v>2</v>
@@ -7633,10 +7652,10 @@
     </row>
     <row r="454" spans="1:4" ht="21">
       <c r="A454" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7644,22 +7663,22 @@
     </row>
     <row r="455" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A455" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B455" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D455" s="23"/>
     </row>
     <row r="456" spans="1:4" ht="21">
       <c r="A456" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>2</v>
@@ -7667,10 +7686,10 @@
     </row>
     <row r="457" spans="1:4" ht="21">
       <c r="A457" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7678,10 +7697,10 @@
     </row>
     <row r="458" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A458" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>2</v>
@@ -7690,10 +7709,10 @@
     </row>
     <row r="459" spans="1:4" ht="21">
       <c r="A459" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -7701,10 +7720,10 @@
     </row>
     <row r="460" spans="1:4" ht="21">
       <c r="A460" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -7712,10 +7731,10 @@
     </row>
     <row r="461" spans="1:4" ht="21">
       <c r="A461" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>2</v>
@@ -7723,10 +7742,10 @@
     </row>
     <row r="462" spans="1:4" ht="21">
       <c r="A462" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>2</v>
@@ -7743,10 +7762,10 @@
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B465" s="13" t="s">
         <v>417</v>
-      </c>
-      <c r="B465" s="13" t="s">
-        <v>418</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>2</v>
@@ -7754,10 +7773,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>2</v>
@@ -7765,10 +7784,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>2</v>
@@ -7776,10 +7795,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>2</v>
@@ -7787,10 +7806,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -7798,21 +7817,21 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="A470" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>2</v>
@@ -7820,10 +7839,10 @@
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>2</v>
@@ -7831,10 +7850,10 @@
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>2</v>
@@ -7842,13 +7861,13 @@
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -8117,7 +8136,7 @@
     <hyperlink ref="B292" r:id="rId262"/>
     <hyperlink ref="B293" r:id="rId263"/>
     <hyperlink ref="B294" r:id="rId264"/>
-    <hyperlink ref="B295" r:id="rId265"/>
+    <hyperlink ref="B295" r:id="rId265" display="Check the expression has valid or Balanced parenthesis or not."/>
     <hyperlink ref="B296" r:id="rId266"/>
     <hyperlink ref="B297" r:id="rId267"/>
     <hyperlink ref="B298" r:id="rId268"/>
@@ -8387,8 +8406,11 @@
     <hyperlink ref="D22" r:id="rId532"/>
     <hyperlink ref="D100" r:id="rId533"/>
     <hyperlink ref="D292" r:id="rId534"/>
+    <hyperlink ref="D296" r:id="rId535"/>
+    <hyperlink ref="D293" r:id="rId536"/>
+    <hyperlink ref="D302" r:id="rId537"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId535"/>
+  <pageSetup orientation="portrait" r:id="rId538"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minStack and sort a stack using temp. stack
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="574">
   <si>
     <t>Topic:</t>
   </si>
@@ -1753,6 +1753,12 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/insert-an-element-at-its-bottom-in-a-given-stack_1171166?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/blog/2021/09/14/sorting-a-stack-using-a-temporary-stack/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/min-stack/submissions/</t>
   </si>
 </sst>
 </file>
@@ -2498,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F302" sqref="F302"/>
+    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C303" sqref="C303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5948,7 +5954,10 @@
         <v>258</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="D297" s="20" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="21">
@@ -6028,7 +6037,10 @@
         <v>265</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>2</v>
+        <v>429</v>
+      </c>
+      <c r="D304" s="20" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">
@@ -8409,8 +8421,10 @@
     <hyperlink ref="D296" r:id="rId535"/>
     <hyperlink ref="D293" r:id="rId536"/>
     <hyperlink ref="D302" r:id="rId537"/>
+    <hyperlink ref="D304" r:id="rId538"/>
+    <hyperlink ref="D297" r:id="rId539"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId538"/>
+  <pageSetup orientation="portrait" r:id="rId540"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverse a stack using recursion
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="576">
   <si>
     <t>Topic:</t>
   </si>
@@ -1762,6 +1762,9 @@
   </si>
   <si>
     <t>The celebrity Problem [HARD]  [GRAPH]</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/reverse-stack-using-recursion_631875?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2046,7 +2049,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2187,6 +2190,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2508,7 +2514,7 @@
   <dimension ref="A1:F474"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A288" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F305" sqref="F305"/>
+      <selection activeCell="F294" sqref="F294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6024,15 +6030,18 @@
         <v>570</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="21">
-      <c r="A303" s="3" t="s">
+    <row r="303" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A303" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B303" s="15" t="s">
+      <c r="B303" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="C303" s="2" t="s">
-        <v>2</v>
+      <c r="C303" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="D303" s="22" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="21">
@@ -8430,8 +8439,9 @@
     <hyperlink ref="D304" r:id="rId538"/>
     <hyperlink ref="D297" r:id="rId539"/>
     <hyperlink ref="D295" r:id="rId540"/>
+    <hyperlink ref="D303" r:id="rId541"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId541"/>
+  <pageSetup orientation="portrait" r:id="rId542"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected the sort a stack using recursion
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -1752,9 +1752,6 @@
     <t>https://www.codingninjas.com/codestudio/problems/insert-an-element-at-its-bottom-in-a-given-stack_1171166?leftPanelTab=1</t>
   </si>
   <si>
-    <t>https://www.codingninjas.com/blog/2021/09/14/sorting-a-stack-using-a-temporary-stack/</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/min-stack/submissions/</t>
   </si>
   <si>
@@ -1765,6 +1762,9 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/reverse-stack-using-recursion_631875?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/sort-a-stack_985275?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2514,7 +2514,7 @@
   <dimension ref="A1:F474"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A288" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F294" sqref="F294"/>
+      <selection activeCell="B310" sqref="B310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5940,7 +5940,7 @@
         <v>428</v>
       </c>
       <c r="D295" s="22" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="21">
@@ -5968,7 +5968,7 @@
         <v>428</v>
       </c>
       <c r="D297" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="21">
@@ -5987,7 +5987,7 @@
         <v>251</v>
       </c>
       <c r="B299" s="31" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C299" s="30" t="s">
         <v>2</v>
@@ -6041,7 +6041,7 @@
         <v>428</v>
       </c>
       <c r="D303" s="22" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="21">
@@ -6055,7 +6055,7 @@
         <v>428</v>
       </c>
       <c r="D304" s="20" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">

</xml_diff>

<commit_message>
minimum cost to make string valid parenthesis
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="579">
   <si>
     <t>Topic:</t>
   </si>
@@ -1771,6 +1771,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/roman-to-integer/submissions/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/minimum-cost-to-make-string-valid_1115770?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2519,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -3402,6 +3405,9 @@
       </c>
       <c r="C73" s="2" t="s">
         <v>428</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="21">
@@ -8454,8 +8460,9 @@
     <hyperlink ref="D303" r:id="rId541"/>
     <hyperlink ref="D308" r:id="rId542"/>
     <hyperlink ref="D78" r:id="rId543"/>
+    <hyperlink ref="D73" r:id="rId544"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId544"/>
+  <pageSetup orientation="portrait" r:id="rId545"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
largest area in histrogram
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="582">
   <si>
     <t>Topic:</t>
   </si>
@@ -1780,6 +1780,9 @@
   </si>
   <si>
     <t>Largest rectangular Area in Histogram [HARD]</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/largest-rectangle-in-histogram/submissions/</t>
   </si>
 </sst>
 </file>
@@ -2528,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B466" sqref="B466"/>
+    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D306" sqref="D306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6103,7 +6106,9 @@
       <c r="C306" s="30" t="s">
         <v>427</v>
       </c>
-      <c r="D306" s="32"/>
+      <c r="D306" s="37" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="307" spans="1:4" ht="21">
       <c r="A307" s="3" t="s">
@@ -8476,8 +8481,9 @@
     <hyperlink ref="D73" r:id="rId544"/>
     <hyperlink ref="D327" r:id="rId545"/>
     <hyperlink ref="D298" r:id="rId546"/>
+    <hyperlink ref="D306" r:id="rId547"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId547"/>
+  <pageSetup orientation="portrait" r:id="rId548"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
getMin in O(1) space and maxRectangle in binary matrix tried
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="586">
   <si>
     <t>Topic:</t>
   </si>
@@ -1789,6 +1789,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximal-rectangle/</t>
+  </si>
+  <si>
+    <t>babbar solution of gfg not working on leetcode</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/design-a-stack-that-supports-getmin-in-o-1-time-and-o-1-extra-space_842465?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2537,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G296" sqref="G296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2954,7 +2960,7 @@
       </c>
       <c r="D32" s="29"/>
     </row>
-    <row r="33" spans="1:4" ht="21">
+    <row r="33" spans="1:6" ht="21">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A34" s="6" t="s">
         <v>3</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="21">
+    <row r="35" spans="1:6" ht="21">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="21">
+    <row r="36" spans="1:6" ht="21">
       <c r="A36" s="3" t="s">
         <v>3</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" ht="21">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="21">
       <c r="A37" s="55" t="s">
         <v>3</v>
       </c>
@@ -3018,7 +3024,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="28" customFormat="1" ht="21">
+    <row r="38" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A38" s="27" t="s">
         <v>3</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="28" customFormat="1" ht="21">
+    <row r="39" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A39" s="27" t="s">
         <v>3</v>
       </c>
@@ -3046,16 +3052,16 @@
         <v>541</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="21">
+    <row r="40" spans="1:6" ht="21">
       <c r="B40" s="4"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="21">
+    <row r="41" spans="1:6" ht="21">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="42" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
@@ -3069,7 +3075,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="21">
+    <row r="43" spans="1:6" ht="21">
       <c r="A43" s="5" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="21">
+    <row r="44" spans="1:6" ht="21">
       <c r="A44" s="5" t="s">
         <v>32</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="21">
+    <row r="45" spans="1:6" ht="21">
       <c r="A45" s="5" t="s">
         <v>32</v>
       </c>
@@ -3108,7 +3114,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="21">
+    <row r="46" spans="1:6" ht="21">
       <c r="A46" s="5" t="s">
         <v>32</v>
       </c>
@@ -3122,7 +3128,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A47" s="30" t="s">
         <v>32</v>
       </c>
@@ -3135,8 +3141,11 @@
       <c r="D47" s="37" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="21">
+      <c r="F47" s="31" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="21">
       <c r="A48" s="5" t="s">
         <v>32</v>
       </c>
@@ -5894,11 +5903,11 @@
       <c r="B288" s="4"/>
       <c r="C288" s="2"/>
     </row>
-    <row r="289" spans="1:4" ht="21">
+    <row r="289" spans="1:6" ht="21">
       <c r="B289" s="4"/>
       <c r="C289" s="2"/>
     </row>
-    <row r="290" spans="1:4" ht="21">
+    <row r="290" spans="1:6" ht="21">
       <c r="A290" s="3" t="s">
         <v>251</v>
       </c>
@@ -5912,7 +5921,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="21">
+    <row r="291" spans="1:6" ht="21">
       <c r="A291" s="3" t="s">
         <v>251</v>
       </c>
@@ -5923,7 +5932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="21">
+    <row r="292" spans="1:6" ht="21">
       <c r="A292" s="3" t="s">
         <v>251</v>
       </c>
@@ -5937,7 +5946,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="21">
+    <row r="293" spans="1:6" ht="21">
       <c r="A293" s="3" t="s">
         <v>251</v>
       </c>
@@ -5951,7 +5960,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="21">
+    <row r="294" spans="1:6" ht="21">
       <c r="A294" s="3" t="s">
         <v>251</v>
       </c>
@@ -5962,7 +5971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="295" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A295" s="6" t="s">
         <v>251</v>
       </c>
@@ -5976,7 +5985,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="21">
+    <row r="296" spans="1:6" ht="21">
       <c r="A296" s="3" t="s">
         <v>251</v>
       </c>
@@ -5990,7 +5999,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="21">
+    <row r="297" spans="1:6" ht="21">
       <c r="A297" s="3" t="s">
         <v>251</v>
       </c>
@@ -6003,8 +6012,11 @@
       <c r="D297" s="20" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" ht="21">
+      <c r="F297" s="20" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="21">
       <c r="A298" s="3" t="s">
         <v>251</v>
       </c>
@@ -6018,7 +6030,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="299" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="299" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A299" s="30" t="s">
         <v>251</v>
       </c>
@@ -6032,7 +6044,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="21">
+    <row r="300" spans="1:6" ht="21">
       <c r="A300" s="3" t="s">
         <v>251</v>
       </c>
@@ -6043,7 +6055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="21">
+    <row r="301" spans="1:6" ht="21">
       <c r="A301" s="3" t="s">
         <v>251</v>
       </c>
@@ -6054,7 +6066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="21">
+    <row r="302" spans="1:6" ht="21">
       <c r="A302" s="3" t="s">
         <v>251</v>
       </c>
@@ -6068,7 +6080,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="303" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="303" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A303" s="6" t="s">
         <v>251</v>
       </c>
@@ -6082,7 +6094,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="21">
+    <row r="304" spans="1:6" ht="21">
       <c r="A304" s="3" t="s">
         <v>251</v>
       </c>
@@ -8495,8 +8507,9 @@
     <hyperlink ref="D306" r:id="rId547"/>
     <hyperlink ref="D299" r:id="rId548"/>
     <hyperlink ref="D47" r:id="rId549"/>
+    <hyperlink ref="F297" r:id="rId550"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId550"/>
+  <pageSetup orientation="portrait" r:id="rId551"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first negative number in window of size K
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="589">
   <si>
     <t>Topic:</t>
   </si>
@@ -867,9 +867,6 @@
   </si>
   <si>
     <t>Distance of nearest cell having 1 in a binary matrix</t>
-  </si>
-  <si>
-    <t>First negative integer in every window of size “k”</t>
   </si>
   <si>
     <t>Check if all levels of two trees are anagrams or not.</t>
@@ -1798,6 +1795,15 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/circular-queue_1170058?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/reversing-a-queue_982934?leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/first-negative-in-every-window_759333?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>First negative integer in every window of size “k”  [IMP]</t>
   </si>
 </sst>
 </file>
@@ -2546,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F474"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F321" sqref="F321"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B322" sqref="B322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2562,7 +2568,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21">
@@ -2573,10 +2579,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2590,10 +2596,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21">
@@ -2604,10 +2610,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21">
@@ -2618,10 +2624,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21">
@@ -2632,10 +2638,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21">
@@ -2646,10 +2652,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">
@@ -2660,10 +2666,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">
@@ -2674,10 +2680,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>427</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1" ht="19.8">
@@ -2688,10 +2694,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -2705,7 +2711,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">
@@ -2716,10 +2722,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">
@@ -2730,10 +2736,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="11" customFormat="1" ht="21">
@@ -2744,10 +2750,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="21">
@@ -2755,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2769,10 +2775,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2783,13 +2789,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>554</v>
+      </c>
+      <c r="F19" s="58" t="s">
         <v>555</v>
-      </c>
-      <c r="F19" s="58" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2800,10 +2806,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="21">
@@ -2814,10 +2820,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2828,10 +2834,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2842,10 +2848,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2856,10 +2862,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2870,10 +2876,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2884,10 +2890,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2898,10 +2904,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -2942,13 +2948,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="28" customFormat="1" ht="21">
@@ -2956,7 +2962,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -2968,13 +2974,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
@@ -2982,13 +2988,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="21">
@@ -3021,10 +3027,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="56" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D37" s="57" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="28" customFormat="1" ht="21">
@@ -3032,13 +3038,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="28" customFormat="1" ht="21">
@@ -3046,13 +3052,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>426</v>
+      </c>
+      <c r="D39" s="54" t="s">
         <v>540</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>427</v>
-      </c>
-      <c r="D39" s="54" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="21">
@@ -3069,13 +3075,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="21">
@@ -3086,10 +3092,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21">
@@ -3111,10 +3117,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -3125,10 +3131,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
@@ -3139,13 +3145,13 @@
         <v>37</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D47" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="F47" s="31" t="s">
         <v>583</v>
-      </c>
-      <c r="F47" s="31" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -3167,10 +3173,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3181,10 +3187,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3211,10 +3217,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3225,10 +3231,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3239,10 +3245,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3423,7 +3429,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="21">
@@ -3434,10 +3440,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="21">
@@ -3493,10 +3499,10 @@
         <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="21">
@@ -3699,10 +3705,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="21">
@@ -3713,10 +3719,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="21">
@@ -3727,10 +3733,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="21">
@@ -3741,10 +3747,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="21">
@@ -3821,10 +3827,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="21">
@@ -3934,7 +3940,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="21">
@@ -3956,7 +3962,7 @@
         <v>108</v>
       </c>
       <c r="C120" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D120" s="26"/>
     </row>
@@ -3968,7 +3974,7 @@
         <v>109</v>
       </c>
       <c r="C121" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D121" s="26"/>
     </row>
@@ -4013,7 +4019,7 @@
         <v>113</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D125" s="26"/>
     </row>
@@ -4073,10 +4079,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D132" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="7" customFormat="1" ht="21">
@@ -4087,10 +4093,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D133" s="22" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21">
@@ -4101,10 +4107,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">
@@ -4115,10 +4121,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">
@@ -4129,10 +4135,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">
@@ -4143,10 +4149,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -4157,10 +4163,10 @@
         <v>125</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -4171,10 +4177,10 @@
         <v>126</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D139" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">
@@ -4185,10 +4191,10 @@
         <v>127</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D140" s="20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">
@@ -4221,7 +4227,7 @@
         <v>130</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D143" s="17"/>
     </row>
@@ -4245,10 +4251,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4259,10 +4265,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4273,10 +4279,10 @@
         <v>134</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D147" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="21">
@@ -4287,10 +4293,10 @@
         <v>135</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D148" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="149" spans="1:6" ht="21">
@@ -4301,10 +4307,10 @@
         <v>136</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D149" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="150" spans="1:6" ht="21">
@@ -4364,7 +4370,7 @@
         <v>2</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="21">
@@ -4372,13 +4378,13 @@
         <v>118</v>
       </c>
       <c r="B155" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>451</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D155" s="20" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4386,10 +4392,10 @@
         <v>118</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D156" s="32"/>
     </row>
@@ -4401,27 +4407,27 @@
         <v>142</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="158" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A158" s="30" t="s">
+        <v>474</v>
+      </c>
+      <c r="B158" s="31" t="s">
         <v>475</v>
       </c>
-      <c r="B158" s="31" t="s">
+      <c r="C158" s="30" t="s">
         <v>476</v>
       </c>
-      <c r="C158" s="30" t="s">
+      <c r="D158" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="D158" s="37" t="s">
+      <c r="F158" s="36" t="s">
         <v>478</v>
-      </c>
-      <c r="F158" s="36" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="159" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4429,13 +4435,13 @@
         <v>118</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C159" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D159" s="37" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="21">
@@ -4443,13 +4449,13 @@
         <v>118</v>
       </c>
       <c r="B160" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D160" s="20" t="s">
         <v>471</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D160" s="20" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="21">
@@ -4479,13 +4485,13 @@
         <v>118</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C163" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D163" s="34" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="21">
@@ -4496,10 +4502,10 @@
         <v>145</v>
       </c>
       <c r="C164" s="35" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D164" s="20" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4510,10 +4516,10 @@
         <v>146</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D165" s="20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="21">
@@ -4522,16 +4528,16 @@
     </row>
     <row r="168" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A168" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B168" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>492</v>
-      </c>
       <c r="C168" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D168" s="23" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="21">
@@ -4542,10 +4548,10 @@
         <v>148</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">
@@ -4553,13 +4559,13 @@
         <v>147</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">
@@ -4570,10 +4576,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">
@@ -4584,10 +4590,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4598,10 +4604,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4612,10 +4618,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">
@@ -4626,10 +4632,10 @@
         <v>153</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D175" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4640,10 +4646,10 @@
         <v>154</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">
@@ -4654,10 +4660,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4690,10 +4696,10 @@
         <v>158</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D180" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21">
@@ -4704,10 +4710,10 @@
         <v>159</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D181" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">
@@ -4726,13 +4732,13 @@
         <v>147</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C183" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D183" s="39" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">
@@ -4751,13 +4757,13 @@
         <v>147</v>
       </c>
       <c r="B185" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D185" s="20" t="s">
         <v>502</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D185" s="20" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="21">
@@ -4779,10 +4785,10 @@
         <v>163</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D187" s="20" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="21">
@@ -4801,13 +4807,13 @@
         <v>147</v>
       </c>
       <c r="B189" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D189" s="20" t="s">
         <v>517</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D189" s="20" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="21">
@@ -4852,10 +4858,10 @@
         <v>168</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D193" s="20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
@@ -4897,13 +4903,13 @@
         <v>147</v>
       </c>
       <c r="B197" s="38" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C197" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D197" s="32" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="21">
@@ -4922,13 +4928,13 @@
         <v>147</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D199" s="23" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">
@@ -4936,13 +4942,13 @@
         <v>147</v>
       </c>
       <c r="B200" s="40" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D200" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">
@@ -4994,13 +5000,13 @@
         <v>176</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D206" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="21">
@@ -5008,13 +5014,13 @@
         <v>176</v>
       </c>
       <c r="B207" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D207" s="20" t="s">
         <v>510</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D207" s="20" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="21">
@@ -5022,13 +5028,13 @@
         <v>176</v>
       </c>
       <c r="B208" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D208" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D208" s="20" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="21">
@@ -5050,10 +5056,10 @@
         <v>178</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D210" s="20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="21">
@@ -5064,10 +5070,10 @@
         <v>179</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="21">
@@ -5078,10 +5084,10 @@
         <v>180</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D212" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="21">
@@ -5103,10 +5109,10 @@
         <v>182</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D214" s="20" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="21">
@@ -5147,7 +5153,7 @@
         <v>176</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C218" s="6" t="s">
         <v>2</v>
@@ -5162,10 +5168,10 @@
         <v>186</v>
       </c>
       <c r="C219" s="44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D219" s="45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="220" spans="1:4" s="51" customFormat="1" ht="21">
@@ -5176,10 +5182,10 @@
         <v>187</v>
       </c>
       <c r="C220" s="49" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D220" s="50" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="21">
@@ -5212,10 +5218,10 @@
         <v>190</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D223" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="21">
@@ -5271,11 +5277,11 @@
         <v>195</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D228" s="23"/>
       <c r="F228" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="21">
@@ -5816,13 +5822,13 @@
         <v>232</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D280" s="23" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="21">
@@ -5918,10 +5924,10 @@
         <v>252</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D290" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="21">
@@ -5932,10 +5938,10 @@
         <v>253</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D291" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="292" spans="1:6" ht="21">
@@ -5946,10 +5952,10 @@
         <v>254</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D292" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="293" spans="1:6" ht="21">
@@ -5960,10 +5966,10 @@
         <v>255</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="21">
@@ -5982,13 +5988,13 @@
         <v>251</v>
       </c>
       <c r="B295" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C295" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D295" s="22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="21">
@@ -5999,10 +6005,10 @@
         <v>257</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D296" s="20" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="297" spans="1:6" ht="21">
@@ -6013,13 +6019,13 @@
         <v>258</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D297" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F297" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="21">
@@ -6030,10 +6036,10 @@
         <v>259</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D298" s="20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="299" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6041,13 +6047,13 @@
         <v>251</v>
       </c>
       <c r="B299" s="31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C299" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D299" s="37" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="21">
@@ -6080,10 +6086,10 @@
         <v>262</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D302" s="20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="303" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6094,10 +6100,10 @@
         <v>263</v>
       </c>
       <c r="C303" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D303" s="22" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="304" spans="1:6" ht="21">
@@ -6108,10 +6114,10 @@
         <v>264</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D304" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="21">
@@ -6130,13 +6136,13 @@
         <v>251</v>
       </c>
       <c r="B306" s="31" t="s">
+        <v>578</v>
+      </c>
+      <c r="C306" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="D306" s="37" t="s">
         <v>579</v>
-      </c>
-      <c r="C306" s="30" t="s">
-        <v>427</v>
-      </c>
-      <c r="D306" s="37" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="307" spans="1:4" ht="21">
@@ -6158,10 +6164,10 @@
         <v>267</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D308" s="20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="21">
@@ -6227,10 +6233,10 @@
         <v>273</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="21">
@@ -6252,7 +6258,10 @@
         <v>275</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>2</v>
+        <v>426</v>
+      </c>
+      <c r="D316" s="20" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="21">
@@ -6310,15 +6319,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:4" ht="21">
-      <c r="A322" s="3" t="s">
+    <row r="322" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="A322" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B322" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="C322" s="2" t="s">
-        <v>2</v>
+      <c r="B322" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="C322" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="D322" s="23" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="21">
@@ -6326,7 +6338,7 @@
         <v>251</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>2</v>
@@ -6337,7 +6349,7 @@
         <v>251</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>2</v>
@@ -6348,7 +6360,7 @@
         <v>251</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>2</v>
@@ -6359,7 +6371,7 @@
         <v>251</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>2</v>
@@ -6370,13 +6382,13 @@
         <v>251</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D327" s="20" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="21">
@@ -6389,38 +6401,38 @@
     </row>
     <row r="330" spans="1:4" ht="21">
       <c r="A330" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C330" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D330" s="21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="331" spans="1:4" ht="21">
       <c r="A331" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D331" s="16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="332" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A332" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C332" s="6" t="s">
         <v>2</v>
@@ -6429,38 +6441,38 @@
     </row>
     <row r="333" spans="1:4" ht="21">
       <c r="A333" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B333" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D333" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="334" spans="1:4" ht="21">
       <c r="A334" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="335" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A335" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B335" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C335" s="6" t="s">
         <v>2</v>
@@ -6469,10 +6481,10 @@
     </row>
     <row r="336" spans="1:4" ht="21">
       <c r="A336" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B336" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
@@ -6480,10 +6492,10 @@
     </row>
     <row r="337" spans="1:6" ht="21">
       <c r="A337" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B337" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>2</v>
@@ -6491,38 +6503,38 @@
     </row>
     <row r="338" spans="1:6" ht="21">
       <c r="A338" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B338" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D338" s="20" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="339" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A339" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B339" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D339" s="22" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -6530,10 +6542,10 @@
     </row>
     <row r="341" spans="1:6" ht="21">
       <c r="A341" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>2</v>
@@ -6541,10 +6553,10 @@
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6552,24 +6564,24 @@
     </row>
     <row r="343" spans="1:6" ht="21">
       <c r="A343" s="6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B343" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D343" s="20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6577,24 +6589,24 @@
     </row>
     <row r="345" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A345" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D345" s="53" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
       <c r="A346" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B346" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>2</v>
@@ -6602,19 +6614,19 @@
     </row>
     <row r="347" spans="1:6" ht="21">
       <c r="A347" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B347" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D347" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="F347" t="s">
         <v>532</v>
-      </c>
-      <c r="F347" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="21">
@@ -6627,10 +6639,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B350" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="B350" s="13" t="s">
-        <v>305</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6638,10 +6650,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6649,10 +6661,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6660,10 +6672,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6671,10 +6683,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6682,10 +6694,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -6693,10 +6705,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6704,10 +6716,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6715,10 +6727,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6726,10 +6738,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6737,10 +6749,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6748,10 +6760,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6759,10 +6771,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6770,10 +6782,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6781,10 +6793,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6792,10 +6804,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6803,10 +6815,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6814,10 +6826,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -6825,10 +6837,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -6836,10 +6848,10 @@
     </row>
     <row r="369" spans="1:4" ht="21">
       <c r="A369" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -6847,10 +6859,10 @@
     </row>
     <row r="370" spans="1:4" ht="21">
       <c r="A370" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -6858,10 +6870,10 @@
     </row>
     <row r="371" spans="1:4" ht="21">
       <c r="A371" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -6869,10 +6881,10 @@
     </row>
     <row r="372" spans="1:4" ht="21">
       <c r="A372" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -6880,10 +6892,10 @@
     </row>
     <row r="373" spans="1:4" ht="21">
       <c r="A373" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -6891,10 +6903,10 @@
     </row>
     <row r="374" spans="1:4" ht="21">
       <c r="A374" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>2</v>
@@ -6902,10 +6914,10 @@
     </row>
     <row r="375" spans="1:4" ht="21">
       <c r="A375" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -6913,10 +6925,10 @@
     </row>
     <row r="376" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A376" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C376" s="6" t="s">
         <v>2</v>
@@ -6925,10 +6937,10 @@
     </row>
     <row r="377" spans="1:4" ht="21">
       <c r="A377" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -6936,10 +6948,10 @@
     </row>
     <row r="378" spans="1:4" ht="21">
       <c r="A378" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -6947,10 +6959,10 @@
     </row>
     <row r="379" spans="1:4" ht="21">
       <c r="A379" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -6958,10 +6970,10 @@
     </row>
     <row r="380" spans="1:4" ht="21">
       <c r="A380" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -6969,10 +6981,10 @@
     </row>
     <row r="381" spans="1:4" ht="21">
       <c r="A381" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -6980,10 +6992,10 @@
     </row>
     <row r="382" spans="1:4" ht="21">
       <c r="A382" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -6991,10 +7003,10 @@
     </row>
     <row r="383" spans="1:4" ht="21">
       <c r="A383" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -7002,10 +7014,10 @@
     </row>
     <row r="384" spans="1:4" ht="21">
       <c r="A384" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -7013,10 +7025,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -7024,10 +7036,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -7035,10 +7047,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -7046,10 +7058,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -7057,10 +7069,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -7068,10 +7080,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -7079,10 +7091,10 @@
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="A391" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>2</v>
@@ -7090,10 +7102,10 @@
     </row>
     <row r="392" spans="1:3" ht="21">
       <c r="A392" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>2</v>
@@ -7109,10 +7121,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B395" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="B395" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7120,10 +7132,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -7131,10 +7143,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -7142,7 +7154,7 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B398" s="13" t="s">
         <v>77</v>
@@ -7153,10 +7165,10 @@
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="A399" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>2</v>
@@ -7164,10 +7176,10 @@
     </row>
     <row r="400" spans="1:3" ht="21">
       <c r="A400" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B400" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>2</v>
@@ -7183,21 +7195,21 @@
     </row>
     <row r="403" spans="1:3" ht="21">
       <c r="A403" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B403" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="B403" s="13" t="s">
-        <v>355</v>
-      </c>
       <c r="C403" s="35" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
       <c r="A404" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7205,10 +7217,10 @@
     </row>
     <row r="405" spans="1:3" ht="21">
       <c r="A405" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -7216,10 +7228,10 @@
     </row>
     <row r="406" spans="1:3" ht="21">
       <c r="A406" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>2</v>
@@ -7227,10 +7239,10 @@
     </row>
     <row r="407" spans="1:3" ht="21">
       <c r="A407" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7238,21 +7250,21 @@
     </row>
     <row r="408" spans="1:3" ht="21">
       <c r="A408" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="21">
       <c r="A409" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7260,7 +7272,7 @@
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B410" s="13" t="s">
         <v>240</v>
@@ -7271,10 +7283,10 @@
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7282,10 +7294,10 @@
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7293,10 +7305,10 @@
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7304,10 +7316,10 @@
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>2</v>
@@ -7315,10 +7327,10 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>2</v>
@@ -7326,10 +7338,10 @@
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7337,10 +7349,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7348,10 +7360,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7359,10 +7371,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7370,10 +7382,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7381,10 +7393,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7392,10 +7404,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7403,10 +7415,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7414,10 +7426,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7425,10 +7437,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7436,10 +7448,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7447,10 +7459,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7458,10 +7470,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7469,10 +7481,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7480,10 +7492,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7491,10 +7503,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7502,10 +7514,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7513,10 +7525,10 @@
     </row>
     <row r="433" spans="1:4" ht="21">
       <c r="A433" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7524,10 +7536,10 @@
     </row>
     <row r="434" spans="1:4" ht="21">
       <c r="A434" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7535,10 +7547,10 @@
     </row>
     <row r="435" spans="1:4" ht="21">
       <c r="A435" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>2</v>
@@ -7546,10 +7558,10 @@
     </row>
     <row r="436" spans="1:4" ht="21">
       <c r="A436" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7557,10 +7569,10 @@
     </row>
     <row r="437" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A437" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B437" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>2</v>
@@ -7569,10 +7581,10 @@
     </row>
     <row r="438" spans="1:4" ht="21">
       <c r="A438" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7580,10 +7592,10 @@
     </row>
     <row r="439" spans="1:4" ht="21">
       <c r="A439" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7591,10 +7603,10 @@
     </row>
     <row r="440" spans="1:4" ht="21">
       <c r="A440" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7602,10 +7614,10 @@
     </row>
     <row r="441" spans="1:4" ht="21">
       <c r="A441" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7613,10 +7625,10 @@
     </row>
     <row r="442" spans="1:4" ht="21">
       <c r="A442" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7624,10 +7636,10 @@
     </row>
     <row r="443" spans="1:4" ht="21">
       <c r="A443" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7635,10 +7647,10 @@
     </row>
     <row r="444" spans="1:4" ht="21">
       <c r="A444" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7646,10 +7658,10 @@
     </row>
     <row r="445" spans="1:4" ht="21">
       <c r="A445" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7657,10 +7669,10 @@
     </row>
     <row r="446" spans="1:4" ht="21">
       <c r="A446" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7668,10 +7680,10 @@
     </row>
     <row r="447" spans="1:4" ht="21">
       <c r="A447" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>2</v>
@@ -7679,10 +7691,10 @@
     </row>
     <row r="448" spans="1:4" ht="21">
       <c r="A448" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>2</v>
@@ -7690,10 +7702,10 @@
     </row>
     <row r="449" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A449" s="24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B449" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C449" s="24" t="s">
         <v>2</v>
@@ -7702,10 +7714,10 @@
     </row>
     <row r="450" spans="1:4" s="25" customFormat="1" ht="21">
       <c r="A450" s="24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B450" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C450" s="24" t="s">
         <v>2</v>
@@ -7714,10 +7726,10 @@
     </row>
     <row r="451" spans="1:4" ht="21">
       <c r="A451" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7725,10 +7737,10 @@
     </row>
     <row r="452" spans="1:4" ht="21">
       <c r="A452" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7736,10 +7748,10 @@
     </row>
     <row r="453" spans="1:4" ht="21">
       <c r="A453" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C453" s="2" t="s">
         <v>2</v>
@@ -7747,10 +7759,10 @@
     </row>
     <row r="454" spans="1:4" ht="21">
       <c r="A454" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7758,22 +7770,22 @@
     </row>
     <row r="455" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A455" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B455" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D455" s="23"/>
     </row>
     <row r="456" spans="1:4" ht="21">
       <c r="A456" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>2</v>
@@ -7781,10 +7793,10 @@
     </row>
     <row r="457" spans="1:4" ht="21">
       <c r="A457" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7792,10 +7804,10 @@
     </row>
     <row r="458" spans="1:4" s="7" customFormat="1" ht="21">
       <c r="A458" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>2</v>
@@ -7804,10 +7816,10 @@
     </row>
     <row r="459" spans="1:4" ht="21">
       <c r="A459" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -7815,10 +7827,10 @@
     </row>
     <row r="460" spans="1:4" ht="21">
       <c r="A460" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -7826,10 +7838,10 @@
     </row>
     <row r="461" spans="1:4" ht="21">
       <c r="A461" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>2</v>
@@ -7837,10 +7849,10 @@
     </row>
     <row r="462" spans="1:4" ht="21">
       <c r="A462" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>2</v>
@@ -7857,10 +7869,10 @@
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B465" s="13" t="s">
         <v>414</v>
-      </c>
-      <c r="B465" s="13" t="s">
-        <v>415</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>2</v>
@@ -7868,10 +7880,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>2</v>
@@ -7879,10 +7891,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>2</v>
@@ -7890,10 +7902,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>2</v>
@@ -7901,10 +7913,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -7912,21 +7924,21 @@
     </row>
     <row r="470" spans="1:3" ht="21">
       <c r="A470" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="471" spans="1:3" ht="21">
       <c r="A471" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>2</v>
@@ -7934,10 +7946,10 @@
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>2</v>
@@ -7945,10 +7957,10 @@
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>2</v>
@@ -7956,13 +7968,13 @@
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -8258,7 +8270,7 @@
     <hyperlink ref="B319" r:id="rId289"/>
     <hyperlink ref="B320" r:id="rId290"/>
     <hyperlink ref="B321" r:id="rId291"/>
-    <hyperlink ref="B322" r:id="rId292"/>
+    <hyperlink ref="B322" r:id="rId292" display="First negative integer in every window of size “k”"/>
     <hyperlink ref="B323" r:id="rId293"/>
     <hyperlink ref="B324" r:id="rId294"/>
     <hyperlink ref="B325" r:id="rId295"/>
@@ -8518,8 +8530,10 @@
     <hyperlink ref="D47" r:id="rId549"/>
     <hyperlink ref="F297" r:id="rId550"/>
     <hyperlink ref="D314" r:id="rId551"/>
+    <hyperlink ref="D316" r:id="rId552"/>
+    <hyperlink ref="D322" r:id="rId553"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId552"/>
+  <pageSetup orientation="portrait" r:id="rId554"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
count bits to be flipped and find two non repeating using bit manipulation
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="598">
   <si>
     <t>Topic:</t>
   </si>
@@ -1819,6 +1819,18 @@
   </si>
   <si>
     <t>Power Set  V.V.V.IMP</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/find-the-lone-set-bit_1062725?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/unique-pair-using-bits_972997?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>isko normally sort karke b O(nlogn) mein kar sakte h</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/number-of-flips_3125902?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2115,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2190,7 +2202,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
@@ -2247,6 +2258,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2567,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A468" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F477" sqref="F477"/>
+    <sheetView tabSelected="1" topLeftCell="A462" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D473" sqref="D473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2578,15 +2604,15 @@
     <col min="3" max="3" width="12.296875" customWidth="1"/>
     <col min="4" max="4" width="36.296875" style="16" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="31.3984375" customWidth="1"/>
+    <col min="6" max="6" width="31.3984375" style="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6">
+    <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="10" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21">
+    <row r="3" spans="1:6" ht="21">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2600,10 +2626,10 @@
         <v>423</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="21">
+    <row r="5" spans="1:6" ht="21">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2617,7 +2643,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21">
+    <row r="6" spans="1:6" ht="21">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2631,7 +2657,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21">
+    <row r="7" spans="1:6" ht="21">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2645,7 +2671,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21">
+    <row r="8" spans="1:6" ht="21">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2659,7 +2685,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21">
+    <row r="9" spans="1:6" ht="21">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -2673,7 +2699,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21">
+    <row r="10" spans="1:6" ht="21">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2687,7 +2713,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21">
+    <row r="11" spans="1:6" ht="21">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2701,7 +2727,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="19.8">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A12" s="8" t="s">
         <v>3</v>
       </c>
@@ -2714,8 +2740,9 @@
       <c r="D12" s="22" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="21">
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="1:6" ht="21">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -2729,7 +2756,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21">
+    <row r="14" spans="1:6" ht="21">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -2743,7 +2770,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21">
+    <row r="15" spans="1:6" ht="21">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
@@ -2757,7 +2784,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="11" customFormat="1" ht="21">
+    <row r="16" spans="1:6" s="11" customFormat="1" ht="21">
       <c r="A16" s="18" t="s">
         <v>3</v>
       </c>
@@ -2770,6 +2797,7 @@
       <c r="D16" s="19" t="s">
         <v>424</v>
       </c>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" ht="21">
       <c r="A17" s="3" t="s">
@@ -2809,7 +2837,7 @@
       <c r="D19" s="20" t="s">
         <v>553</v>
       </c>
-      <c r="F19" s="58" t="s">
+      <c r="F19" s="57" t="s">
         <v>554</v>
       </c>
     </row>
@@ -2826,6 +2854,7 @@
       <c r="D20" s="22" t="s">
         <v>433</v>
       </c>
+      <c r="F20" s="59"/>
     </row>
     <row r="21" spans="1:6" ht="21">
       <c r="A21" s="3" t="s">
@@ -2968,9 +2997,10 @@
       <c r="C31" s="24" t="s">
         <v>425</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="40" t="s">
         <v>437</v>
       </c>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A32" s="27" t="s">
@@ -2983,6 +3013,7 @@
         <v>2</v>
       </c>
       <c r="D32" s="29"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" ht="21">
       <c r="A33" s="3" t="s">
@@ -3011,6 +3042,7 @@
       <c r="D34" s="23" t="s">
         <v>556</v>
       </c>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" ht="21">
       <c r="A35" s="3" t="s">
@@ -3035,18 +3067,19 @@
       </c>
     </row>
     <row r="37" spans="1:6" s="4" customFormat="1" ht="21">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="56" t="s">
-        <v>425</v>
-      </c>
-      <c r="D37" s="57" t="s">
+      <c r="C37" s="55" t="s">
+        <v>425</v>
+      </c>
+      <c r="D37" s="56" t="s">
         <v>552</v>
       </c>
+      <c r="F37" s="61"/>
     </row>
     <row r="38" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A38" s="27" t="s">
@@ -3061,6 +3094,7 @@
       <c r="D38" s="29" t="s">
         <v>534</v>
       </c>
+      <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:6" s="28" customFormat="1" ht="21">
       <c r="A39" s="27" t="s">
@@ -3072,9 +3106,10 @@
       <c r="C39" s="27" t="s">
         <v>425</v>
       </c>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="53" t="s">
         <v>539</v>
       </c>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:6" ht="21">
       <c r="B40" s="4"/>
@@ -3098,6 +3133,7 @@
       <c r="D42" s="22" t="s">
         <v>442</v>
       </c>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" ht="21">
       <c r="A43" s="5" t="s">
@@ -3162,10 +3198,10 @@
       <c r="C47" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="36" t="s">
         <v>581</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="32" t="s">
         <v>582</v>
       </c>
     </row>
@@ -3354,7 +3390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="9" customFormat="1" ht="19.8">
+    <row r="65" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A65" s="8" t="s">
         <v>42</v>
       </c>
@@ -3365,8 +3401,9 @@
         <v>2</v>
       </c>
       <c r="D65" s="17"/>
-    </row>
-    <row r="66" spans="1:4" s="9" customFormat="1" ht="19.8">
+      <c r="F65" s="59"/>
+    </row>
+    <row r="66" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A66" s="8" t="s">
         <v>42</v>
       </c>
@@ -3377,8 +3414,9 @@
         <v>2</v>
       </c>
       <c r="D66" s="17"/>
-    </row>
-    <row r="67" spans="1:4" s="9" customFormat="1" ht="19.8">
+      <c r="F66" s="59"/>
+    </row>
+    <row r="67" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A67" s="8" t="s">
         <v>42</v>
       </c>
@@ -3389,8 +3427,9 @@
         <v>2</v>
       </c>
       <c r="D67" s="17"/>
-    </row>
-    <row r="68" spans="1:4" s="9" customFormat="1" ht="19.8">
+      <c r="F67" s="59"/>
+    </row>
+    <row r="68" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A68" s="8" t="s">
         <v>42</v>
       </c>
@@ -3401,8 +3440,9 @@
         <v>2</v>
       </c>
       <c r="D68" s="17"/>
-    </row>
-    <row r="69" spans="1:4" s="9" customFormat="1" ht="19.8">
+      <c r="F68" s="59"/>
+    </row>
+    <row r="69" spans="1:6" s="9" customFormat="1" ht="19.8">
       <c r="A69" s="8" t="s">
         <v>42</v>
       </c>
@@ -3413,8 +3453,9 @@
         <v>2</v>
       </c>
       <c r="D69" s="17"/>
-    </row>
-    <row r="70" spans="1:4" ht="21">
+      <c r="F69" s="59"/>
+    </row>
+    <row r="70" spans="1:6" ht="21">
       <c r="A70" s="3" t="s">
         <v>42</v>
       </c>
@@ -3425,7 +3466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="21">
+    <row r="71" spans="1:6" ht="21">
       <c r="A71" s="3" t="s">
         <v>42</v>
       </c>
@@ -3436,7 +3477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="21">
+    <row r="72" spans="1:6" ht="21">
       <c r="A72" s="3" t="s">
         <v>42</v>
       </c>
@@ -3447,7 +3488,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="21">
+    <row r="73" spans="1:6" ht="21">
       <c r="A73" s="3" t="s">
         <v>42</v>
       </c>
@@ -3461,7 +3502,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="21">
+    <row r="74" spans="1:6" ht="21">
       <c r="A74" s="3" t="s">
         <v>42</v>
       </c>
@@ -3472,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="21">
+    <row r="75" spans="1:6" ht="21">
       <c r="A75" s="3" t="s">
         <v>42</v>
       </c>
@@ -3483,7 +3524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="21">
+    <row r="76" spans="1:6" ht="21">
       <c r="A76" s="3" t="s">
         <v>42</v>
       </c>
@@ -3494,7 +3535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="77" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A77" s="6" t="s">
         <v>42</v>
       </c>
@@ -3505,8 +3546,9 @@
         <v>2</v>
       </c>
       <c r="D77" s="23"/>
-    </row>
-    <row r="78" spans="1:4" ht="21">
+      <c r="F77" s="23"/>
+    </row>
+    <row r="78" spans="1:6" ht="21">
       <c r="A78" s="3" t="s">
         <v>42</v>
       </c>
@@ -3520,7 +3562,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="21">
+    <row r="79" spans="1:6" ht="21">
       <c r="A79" s="3" t="s">
         <v>42</v>
       </c>
@@ -3531,7 +3573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="21">
+    <row r="80" spans="1:6" ht="21">
       <c r="A80" s="3" t="s">
         <v>42</v>
       </c>
@@ -3707,12 +3749,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="21">
+    <row r="97" spans="1:6" ht="21">
       <c r="A97" s="5"/>
       <c r="B97" s="4"/>
       <c r="C97" s="2"/>
     </row>
-    <row r="98" spans="1:4" ht="21">
+    <row r="98" spans="1:6" ht="21">
       <c r="A98" s="3" t="s">
         <v>85</v>
       </c>
@@ -3726,7 +3768,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="21">
+    <row r="99" spans="1:6" ht="21">
       <c r="A99" s="3" t="s">
         <v>85</v>
       </c>
@@ -3740,7 +3782,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="21">
+    <row r="100" spans="1:6" ht="21">
       <c r="A100" s="3" t="s">
         <v>85</v>
       </c>
@@ -3754,7 +3796,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="21">
+    <row r="101" spans="1:6" ht="21">
       <c r="A101" s="3" t="s">
         <v>85</v>
       </c>
@@ -3768,7 +3810,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="21">
+    <row r="102" spans="1:6" ht="21">
       <c r="A102" s="3" t="s">
         <v>85</v>
       </c>
@@ -3779,7 +3821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="21">
+    <row r="103" spans="1:6" ht="21">
       <c r="A103" s="3" t="s">
         <v>85</v>
       </c>
@@ -3790,7 +3832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="21">
+    <row r="104" spans="1:6" ht="21">
       <c r="A104" s="3" t="s">
         <v>85</v>
       </c>
@@ -3801,7 +3843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="21">
+    <row r="105" spans="1:6" ht="21">
       <c r="A105" s="3" t="s">
         <v>85</v>
       </c>
@@ -3812,7 +3854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="21">
+    <row r="106" spans="1:6" ht="21">
       <c r="A106" s="3" t="s">
         <v>85</v>
       </c>
@@ -3823,7 +3865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="21">
+    <row r="107" spans="1:6" ht="21">
       <c r="A107" s="3" t="s">
         <v>85</v>
       </c>
@@ -3834,7 +3876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A108" s="6" t="s">
         <v>85</v>
       </c>
@@ -3847,8 +3889,9 @@
       <c r="D108" s="23" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="21">
+      <c r="F108" s="23"/>
+    </row>
+    <row r="109" spans="1:6" ht="21">
       <c r="A109" s="3" t="s">
         <v>85</v>
       </c>
@@ -3859,7 +3902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="21">
+    <row r="110" spans="1:6" ht="21">
       <c r="A110" s="3" t="s">
         <v>85</v>
       </c>
@@ -3870,7 +3913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="21">
+    <row r="111" spans="1:6" ht="21">
       <c r="A111" s="3" t="s">
         <v>85</v>
       </c>
@@ -3881,7 +3924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="21">
+    <row r="112" spans="1:6" ht="21">
       <c r="A112" s="3" t="s">
         <v>85</v>
       </c>
@@ -3892,7 +3935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="21">
+    <row r="113" spans="1:6" ht="21">
       <c r="A113" s="3" t="s">
         <v>85</v>
       </c>
@@ -3903,7 +3946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="21">
+    <row r="114" spans="1:6" ht="21">
       <c r="A114" s="3" t="s">
         <v>85</v>
       </c>
@@ -3914,7 +3957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="21">
+    <row r="115" spans="1:6" ht="21">
       <c r="A115" s="3" t="s">
         <v>85</v>
       </c>
@@ -3925,7 +3968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="21">
+    <row r="116" spans="1:6" ht="21">
       <c r="A116" s="3" t="s">
         <v>85</v>
       </c>
@@ -3936,7 +3979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="21">
+    <row r="117" spans="1:6" ht="21">
       <c r="A117" s="3" t="s">
         <v>85</v>
       </c>
@@ -3947,7 +3990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="21">
+    <row r="118" spans="1:6" ht="21">
       <c r="A118" s="3" t="s">
         <v>85</v>
       </c>
@@ -3958,7 +4001,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="21">
+    <row r="119" spans="1:6" ht="21">
       <c r="A119" s="3" t="s">
         <v>85</v>
       </c>
@@ -3969,7 +4012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:4" s="25" customFormat="1" ht="21">
+    <row r="120" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A120" s="24" t="s">
         <v>85</v>
       </c>
@@ -3980,8 +4023,9 @@
         <v>425</v>
       </c>
       <c r="D120" s="26"/>
-    </row>
-    <row r="121" spans="1:4" s="25" customFormat="1" ht="21">
+      <c r="F120" s="26"/>
+    </row>
+    <row r="121" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A121" s="24" t="s">
         <v>85</v>
       </c>
@@ -3992,8 +4036,9 @@
         <v>425</v>
       </c>
       <c r="D121" s="26"/>
-    </row>
-    <row r="122" spans="1:4" ht="21">
+      <c r="F121" s="26"/>
+    </row>
+    <row r="122" spans="1:6" ht="21">
       <c r="A122" s="3" t="s">
         <v>85</v>
       </c>
@@ -4004,7 +4049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="21">
+    <row r="123" spans="1:6" ht="21">
       <c r="A123" s="3" t="s">
         <v>85</v>
       </c>
@@ -4015,7 +4060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="21">
+    <row r="124" spans="1:6" ht="21">
       <c r="A124" s="3" t="s">
         <v>85</v>
       </c>
@@ -4026,7 +4071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:4" s="25" customFormat="1" ht="21">
+    <row r="125" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A125" s="24" t="s">
         <v>85</v>
       </c>
@@ -4037,8 +4082,9 @@
         <v>425</v>
       </c>
       <c r="D125" s="26"/>
-    </row>
-    <row r="126" spans="1:4" ht="21">
+      <c r="F125" s="26"/>
+    </row>
+    <row r="126" spans="1:6" ht="21">
       <c r="A126" s="3" t="s">
         <v>85</v>
       </c>
@@ -4049,7 +4095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="21">
+    <row r="127" spans="1:6" ht="21">
       <c r="A127" s="3" t="s">
         <v>85</v>
       </c>
@@ -4060,7 +4106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="21">
+    <row r="128" spans="1:6" ht="21">
       <c r="A128" s="3" t="s">
         <v>85</v>
       </c>
@@ -4071,7 +4117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="21">
+    <row r="129" spans="1:6" ht="21">
       <c r="A129" s="3" t="s">
         <v>85</v>
       </c>
@@ -4082,11 +4128,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="21">
+    <row r="131" spans="1:6" ht="21">
       <c r="B131" s="4"/>
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="1:4" ht="21">
+    <row r="132" spans="1:6" ht="21">
       <c r="A132" s="5" t="s">
         <v>118</v>
       </c>
@@ -4100,7 +4146,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="133" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="133" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A133" s="6" t="s">
         <v>118</v>
       </c>
@@ -4113,8 +4159,9 @@
       <c r="D133" s="22" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="21">
+      <c r="F133" s="23"/>
+    </row>
+    <row r="134" spans="1:6" ht="21">
       <c r="A134" s="5" t="s">
         <v>118</v>
       </c>
@@ -4128,7 +4175,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="21">
+    <row r="135" spans="1:6" ht="21">
       <c r="A135" s="5" t="s">
         <v>118</v>
       </c>
@@ -4142,7 +4189,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="21">
+    <row r="136" spans="1:6" ht="21">
       <c r="A136" s="5" t="s">
         <v>118</v>
       </c>
@@ -4156,7 +4203,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="21">
+    <row r="137" spans="1:6" ht="21">
       <c r="A137" s="5" t="s">
         <v>118</v>
       </c>
@@ -4170,7 +4217,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="21">
+    <row r="138" spans="1:6" ht="21">
       <c r="A138" s="5" t="s">
         <v>118</v>
       </c>
@@ -4184,7 +4231,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="21">
+    <row r="139" spans="1:6" ht="21">
       <c r="A139" s="5" t="s">
         <v>118</v>
       </c>
@@ -4198,7 +4245,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="21">
+    <row r="140" spans="1:6" ht="21">
       <c r="A140" s="5" t="s">
         <v>118</v>
       </c>
@@ -4212,7 +4259,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="21">
+    <row r="141" spans="1:6" ht="21">
       <c r="A141" s="5" t="s">
         <v>118</v>
       </c>
@@ -4223,7 +4270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="21">
+    <row r="142" spans="1:6" ht="21">
       <c r="A142" s="5" t="s">
         <v>118</v>
       </c>
@@ -4234,7 +4281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="143" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A143" s="6" t="s">
         <v>118</v>
       </c>
@@ -4245,8 +4292,9 @@
         <v>425</v>
       </c>
       <c r="D143" s="17"/>
-    </row>
-    <row r="144" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="F143" s="23"/>
+    </row>
+    <row r="144" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A144" s="6" t="s">
         <v>118</v>
       </c>
@@ -4257,6 +4305,7 @@
         <v>2</v>
       </c>
       <c r="D144" s="17"/>
+      <c r="F144" s="23"/>
     </row>
     <row r="145" spans="1:6" ht="21">
       <c r="A145" s="5" t="s">
@@ -4361,6 +4410,7 @@
         <v>2</v>
       </c>
       <c r="D152" s="23"/>
+      <c r="F152" s="23"/>
     </row>
     <row r="153" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A153" s="6" t="s">
@@ -4373,6 +4423,7 @@
         <v>2</v>
       </c>
       <c r="D153" s="23"/>
+      <c r="F153" s="23"/>
     </row>
     <row r="154" spans="1:6" ht="21">
       <c r="A154" s="5" t="s">
@@ -4413,6 +4464,7 @@
         <v>425</v>
       </c>
       <c r="D156" s="32"/>
+      <c r="F156" s="32"/>
     </row>
     <row r="157" spans="1:6" ht="21">
       <c r="A157" s="5" t="s">
@@ -4438,10 +4490,10 @@
       <c r="C158" s="30" t="s">
         <v>475</v>
       </c>
-      <c r="D158" s="37" t="s">
+      <c r="D158" s="36" t="s">
         <v>476</v>
       </c>
-      <c r="F158" s="36" t="s">
+      <c r="F158" s="38" t="s">
         <v>477</v>
       </c>
     </row>
@@ -4455,9 +4507,10 @@
       <c r="C159" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D159" s="37" t="s">
+      <c r="D159" s="36" t="s">
         <v>471</v>
       </c>
+      <c r="F159" s="32"/>
     </row>
     <row r="160" spans="1:6" ht="21">
       <c r="A160" s="5" t="s">
@@ -4473,7 +4526,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="21">
+    <row r="161" spans="1:6" ht="21">
       <c r="A161" s="5" t="s">
         <v>118</v>
       </c>
@@ -4484,7 +4537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="21">
+    <row r="162" spans="1:6" ht="21">
       <c r="A162" s="5" t="s">
         <v>118</v>
       </c>
@@ -4495,7 +4548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:4" s="4" customFormat="1" ht="21">
+    <row r="163" spans="1:6" s="4" customFormat="1" ht="21">
       <c r="A163" s="33" t="s">
         <v>118</v>
       </c>
@@ -4508,8 +4561,9 @@
       <c r="D163" s="34" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="21">
+      <c r="F163" s="61"/>
+    </row>
+    <row r="164" spans="1:6" ht="21">
       <c r="A164" s="5" t="s">
         <v>118</v>
       </c>
@@ -4523,7 +4577,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="21">
+    <row r="165" spans="1:6" ht="21">
       <c r="A165" s="5" t="s">
         <v>118</v>
       </c>
@@ -4537,11 +4591,11 @@
         <v>467</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="21">
+    <row r="167" spans="1:6" ht="21">
       <c r="B167" s="4"/>
       <c r="C167" s="2"/>
     </row>
-    <row r="168" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="168" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A168" s="6" t="s">
         <v>489</v>
       </c>
@@ -4554,8 +4608,9 @@
       <c r="D168" s="23" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="21">
+      <c r="F168" s="23"/>
+    </row>
+    <row r="169" spans="1:6" ht="21">
       <c r="A169" s="3" t="s">
         <v>147</v>
       </c>
@@ -4569,7 +4624,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="21">
+    <row r="170" spans="1:6" ht="21">
       <c r="A170" s="3" t="s">
         <v>147</v>
       </c>
@@ -4583,7 +4638,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="21">
+    <row r="171" spans="1:6" ht="21">
       <c r="A171" s="3" t="s">
         <v>147</v>
       </c>
@@ -4597,7 +4652,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="21">
+    <row r="172" spans="1:6" ht="21">
       <c r="A172" s="3" t="s">
         <v>147</v>
       </c>
@@ -4611,7 +4666,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="21">
+    <row r="173" spans="1:6" ht="21">
       <c r="A173" s="3" t="s">
         <v>147</v>
       </c>
@@ -4625,7 +4680,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="21">
+    <row r="174" spans="1:6" ht="21">
       <c r="A174" s="3" t="s">
         <v>147</v>
       </c>
@@ -4639,7 +4694,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="21">
+    <row r="175" spans="1:6" ht="21">
       <c r="A175" s="3" t="s">
         <v>147</v>
       </c>
@@ -4653,7 +4708,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="21">
+    <row r="176" spans="1:6" ht="21">
       <c r="A176" s="3" t="s">
         <v>147</v>
       </c>
@@ -4667,7 +4722,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="21">
+    <row r="177" spans="1:6" ht="21">
       <c r="A177" s="3" t="s">
         <v>147</v>
       </c>
@@ -4681,7 +4736,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="21">
+    <row r="178" spans="1:6" ht="21">
       <c r="A178" s="3" t="s">
         <v>147</v>
       </c>
@@ -4692,7 +4747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="21">
+    <row r="179" spans="1:6" ht="21">
       <c r="A179" s="3" t="s">
         <v>147</v>
       </c>
@@ -4703,7 +4758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="21">
+    <row r="180" spans="1:6" ht="21">
       <c r="A180" s="3" t="s">
         <v>147</v>
       </c>
@@ -4717,7 +4772,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="21">
+    <row r="181" spans="1:6" ht="21">
       <c r="A181" s="3" t="s">
         <v>147</v>
       </c>
@@ -4731,7 +4786,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="21">
+    <row r="182" spans="1:6" ht="21">
       <c r="A182" s="3" t="s">
         <v>147</v>
       </c>
@@ -4742,7 +4797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="183" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A183" s="30" t="s">
         <v>147</v>
       </c>
@@ -4752,11 +4807,12 @@
       <c r="C183" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D183" s="39" t="s">
+      <c r="D183" s="38" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" ht="21">
+      <c r="F183" s="32"/>
+    </row>
+    <row r="184" spans="1:6" ht="21">
       <c r="A184" s="3" t="s">
         <v>147</v>
       </c>
@@ -4767,7 +4823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="21">
+    <row r="185" spans="1:6" ht="21">
       <c r="A185" s="3" t="s">
         <v>147</v>
       </c>
@@ -4781,7 +4837,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="21">
+    <row r="186" spans="1:6" ht="21">
       <c r="A186" s="3" t="s">
         <v>147</v>
       </c>
@@ -4792,7 +4848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="21">
+    <row r="187" spans="1:6" ht="21">
       <c r="A187" s="3" t="s">
         <v>147</v>
       </c>
@@ -4806,7 +4862,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="21">
+    <row r="188" spans="1:6" ht="21">
       <c r="A188" s="3" t="s">
         <v>147</v>
       </c>
@@ -4817,7 +4873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="21">
+    <row r="189" spans="1:6" ht="21">
       <c r="A189" s="3" t="s">
         <v>147</v>
       </c>
@@ -4831,7 +4887,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="21">
+    <row r="190" spans="1:6" ht="21">
       <c r="A190" s="3" t="s">
         <v>147</v>
       </c>
@@ -4842,7 +4898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="21">
+    <row r="191" spans="1:6" ht="21">
       <c r="A191" s="3" t="s">
         <v>147</v>
       </c>
@@ -4853,7 +4909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="192" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A192" s="6" t="s">
         <v>147</v>
       </c>
@@ -4864,8 +4920,9 @@
         <v>2</v>
       </c>
       <c r="D192" s="23"/>
-    </row>
-    <row r="193" spans="1:4" ht="21">
+      <c r="F192" s="23"/>
+    </row>
+    <row r="193" spans="1:6" ht="21">
       <c r="A193" s="3" t="s">
         <v>147</v>
       </c>
@@ -4879,7 +4936,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="21">
+    <row r="194" spans="1:6" ht="21">
       <c r="A194" s="3" t="s">
         <v>147</v>
       </c>
@@ -4890,7 +4947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="195" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A195" s="6" t="s">
         <v>147</v>
       </c>
@@ -4901,8 +4958,9 @@
         <v>2</v>
       </c>
       <c r="D195" s="23"/>
-    </row>
-    <row r="196" spans="1:4" ht="21">
+      <c r="F195" s="23"/>
+    </row>
+    <row r="196" spans="1:6" ht="21">
       <c r="A196" s="3" t="s">
         <v>147</v>
       </c>
@@ -4913,11 +4971,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="197" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A197" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B197" s="38" t="s">
+      <c r="B197" s="37" t="s">
         <v>493</v>
       </c>
       <c r="C197" s="30" t="s">
@@ -4926,8 +4984,9 @@
       <c r="D197" s="32" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" ht="21">
+      <c r="F197" s="32"/>
+    </row>
+    <row r="198" spans="1:6" ht="21">
       <c r="A198" s="3" t="s">
         <v>147</v>
       </c>
@@ -4938,7 +4997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="199" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A199" s="6" t="s">
         <v>147</v>
       </c>
@@ -4951,12 +5010,13 @@
       <c r="D199" s="23" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" ht="21">
+      <c r="F199" s="23"/>
+    </row>
+    <row r="200" spans="1:6" ht="21">
       <c r="A200" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B200" s="40" t="s">
+      <c r="B200" s="39" t="s">
         <v>499</v>
       </c>
       <c r="C200" s="2" t="s">
@@ -4966,7 +5026,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="21">
+    <row r="201" spans="1:6" ht="21">
       <c r="A201" s="3" t="s">
         <v>147</v>
       </c>
@@ -4977,7 +5037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="202" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="202" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A202" s="6" t="s">
         <v>147</v>
       </c>
@@ -4988,8 +5048,9 @@
         <v>2</v>
       </c>
       <c r="D202" s="23"/>
-    </row>
-    <row r="203" spans="1:4" ht="21">
+      <c r="F202" s="23"/>
+    </row>
+    <row r="203" spans="1:6" ht="21">
       <c r="A203" s="3" t="s">
         <v>147</v>
       </c>
@@ -5000,17 +5061,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="21">
+    <row r="204" spans="1:6" ht="21">
       <c r="A204" s="5"/>
       <c r="B204" s="4"/>
       <c r="C204" s="2"/>
     </row>
-    <row r="205" spans="1:4" ht="21">
+    <row r="205" spans="1:6" ht="21">
       <c r="A205" s="5"/>
       <c r="B205" s="4"/>
       <c r="C205" s="2"/>
     </row>
-    <row r="206" spans="1:4" ht="21">
+    <row r="206" spans="1:6" ht="21">
       <c r="A206" s="3" t="s">
         <v>176</v>
       </c>
@@ -5024,7 +5085,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="21">
+    <row r="207" spans="1:6" ht="21">
       <c r="A207" s="3" t="s">
         <v>176</v>
       </c>
@@ -5038,7 +5099,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="21">
+    <row r="208" spans="1:6" ht="21">
       <c r="A208" s="3" t="s">
         <v>176</v>
       </c>
@@ -5052,7 +5113,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="21">
+    <row r="209" spans="1:6" ht="21">
       <c r="A209" s="3" t="s">
         <v>176</v>
       </c>
@@ -5063,7 +5124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="21">
+    <row r="210" spans="1:6" ht="21">
       <c r="A210" s="3" t="s">
         <v>176</v>
       </c>
@@ -5077,7 +5138,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="21">
+    <row r="211" spans="1:6" ht="21">
       <c r="A211" s="3" t="s">
         <v>176</v>
       </c>
@@ -5091,7 +5152,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="21">
+    <row r="212" spans="1:6" ht="21">
       <c r="A212" s="3" t="s">
         <v>176</v>
       </c>
@@ -5105,7 +5166,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="21">
+    <row r="213" spans="1:6" ht="21">
       <c r="A213" s="3" t="s">
         <v>176</v>
       </c>
@@ -5116,7 +5177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="21">
+    <row r="214" spans="1:6" ht="21">
       <c r="A214" s="3" t="s">
         <v>176</v>
       </c>
@@ -5130,7 +5191,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="21">
+    <row r="215" spans="1:6" ht="21">
       <c r="A215" s="3" t="s">
         <v>176</v>
       </c>
@@ -5141,7 +5202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="21">
+    <row r="216" spans="1:6" ht="21">
       <c r="A216" s="3" t="s">
         <v>176</v>
       </c>
@@ -5152,7 +5213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="21">
+    <row r="217" spans="1:6" ht="21">
       <c r="A217" s="3" t="s">
         <v>176</v>
       </c>
@@ -5163,7 +5224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="218" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A218" s="6" t="s">
         <v>176</v>
       </c>
@@ -5174,36 +5235,39 @@
         <v>2</v>
       </c>
       <c r="D218" s="23"/>
-    </row>
-    <row r="219" spans="1:4" s="46" customFormat="1" ht="21">
-      <c r="A219" s="42" t="s">
+      <c r="F218" s="23"/>
+    </row>
+    <row r="219" spans="1:6" s="45" customFormat="1" ht="21">
+      <c r="A219" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="B219" s="43" t="s">
+      <c r="B219" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="C219" s="44" t="s">
-        <v>425</v>
-      </c>
-      <c r="D219" s="45" t="s">
+      <c r="C219" s="43" t="s">
+        <v>425</v>
+      </c>
+      <c r="D219" s="44" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" s="51" customFormat="1" ht="21">
-      <c r="A220" s="47" t="s">
+      <c r="F219" s="62"/>
+    </row>
+    <row r="220" spans="1:6" s="50" customFormat="1" ht="21">
+      <c r="A220" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="B220" s="48" t="s">
+      <c r="B220" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="C220" s="49" t="s">
-        <v>425</v>
-      </c>
-      <c r="D220" s="50" t="s">
+      <c r="C220" s="48" t="s">
+        <v>425</v>
+      </c>
+      <c r="D220" s="49" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" ht="21">
+      <c r="F220" s="63"/>
+    </row>
+    <row r="221" spans="1:6" ht="21">
       <c r="A221" s="3" t="s">
         <v>176</v>
       </c>
@@ -5214,7 +5278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="21">
+    <row r="222" spans="1:6" ht="21">
       <c r="A222" s="3" t="s">
         <v>176</v>
       </c>
@@ -5225,7 +5289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="21">
+    <row r="223" spans="1:6" ht="21">
       <c r="A223" s="3" t="s">
         <v>176</v>
       </c>
@@ -5239,7 +5303,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="21">
+    <row r="224" spans="1:6" ht="21">
       <c r="A224" s="3" t="s">
         <v>176</v>
       </c>
@@ -5271,7 +5335,7 @@
       <c r="C226" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D226" s="52"/>
+      <c r="D226" s="51"/>
     </row>
     <row r="227" spans="1:6" ht="21">
       <c r="A227" s="3" t="s">
@@ -5295,7 +5359,7 @@
         <v>425</v>
       </c>
       <c r="D228" s="23"/>
-      <c r="F228" s="7" t="s">
+      <c r="F228" s="23" t="s">
         <v>524</v>
       </c>
     </row>
@@ -5755,7 +5819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="21">
+    <row r="273" spans="1:6" ht="21">
       <c r="A273" s="3" t="s">
         <v>232</v>
       </c>
@@ -5766,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="21">
+    <row r="274" spans="1:6" ht="21">
       <c r="A274" s="3" t="s">
         <v>232</v>
       </c>
@@ -5777,7 +5841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="21">
+    <row r="275" spans="1:6" ht="21">
       <c r="A275" s="3" t="s">
         <v>232</v>
       </c>
@@ -5788,7 +5852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="21">
+    <row r="276" spans="1:6" ht="21">
       <c r="A276" s="3" t="s">
         <v>232</v>
       </c>
@@ -5799,7 +5863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="21">
+    <row r="277" spans="1:6" ht="21">
       <c r="A277" s="3" t="s">
         <v>232</v>
       </c>
@@ -5810,7 +5874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="21">
+    <row r="278" spans="1:6" ht="21">
       <c r="A278" s="3" t="s">
         <v>232</v>
       </c>
@@ -5821,7 +5885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="21">
+    <row r="279" spans="1:6" ht="21">
       <c r="A279" s="3" t="s">
         <v>232</v>
       </c>
@@ -5832,7 +5896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="280" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A280" s="6" t="s">
         <v>232</v>
       </c>
@@ -5845,8 +5909,9 @@
       <c r="D280" s="23" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" ht="21">
+      <c r="F280" s="23"/>
+    </row>
+    <row r="281" spans="1:6" ht="21">
       <c r="A281" s="3" t="s">
         <v>232</v>
       </c>
@@ -5857,7 +5922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="21">
+    <row r="282" spans="1:6" ht="21">
       <c r="A282" s="3" t="s">
         <v>232</v>
       </c>
@@ -5868,7 +5933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="21">
+    <row r="283" spans="1:6" ht="21">
       <c r="A283" s="3" t="s">
         <v>232</v>
       </c>
@@ -5879,7 +5944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="21">
+    <row r="284" spans="1:6" ht="21">
       <c r="A284" s="3" t="s">
         <v>232</v>
       </c>
@@ -5890,7 +5955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="21">
+    <row r="285" spans="1:6" ht="21">
       <c r="A285" s="3" t="s">
         <v>232</v>
       </c>
@@ -5901,7 +5966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="21">
+    <row r="286" spans="1:6" ht="21">
       <c r="A286" s="3" t="s">
         <v>232</v>
       </c>
@@ -5912,7 +5977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="21">
+    <row r="287" spans="1:6" ht="21">
       <c r="A287" s="3" t="s">
         <v>232</v>
       </c>
@@ -5923,7 +5988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="21">
+    <row r="288" spans="1:6" ht="21">
       <c r="B288" s="4"/>
       <c r="C288" s="2"/>
     </row>
@@ -6011,6 +6076,7 @@
       <c r="D295" s="22" t="s">
         <v>569</v>
       </c>
+      <c r="F295" s="23"/>
     </row>
     <row r="296" spans="1:6" ht="21">
       <c r="A296" s="3" t="s">
@@ -6067,9 +6133,10 @@
       <c r="C299" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D299" s="37" t="s">
+      <c r="D299" s="36" t="s">
         <v>579</v>
       </c>
+      <c r="F299" s="32"/>
     </row>
     <row r="300" spans="1:6" ht="21">
       <c r="A300" s="3" t="s">
@@ -6111,7 +6178,7 @@
       <c r="A303" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B303" s="59" t="s">
+      <c r="B303" s="58" t="s">
         <v>263</v>
       </c>
       <c r="C303" s="6" t="s">
@@ -6120,6 +6187,7 @@
       <c r="D303" s="22" t="s">
         <v>570</v>
       </c>
+      <c r="F303" s="23"/>
     </row>
     <row r="304" spans="1:6" ht="21">
       <c r="A304" s="3" t="s">
@@ -6135,7 +6203,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="21">
+    <row r="305" spans="1:6" ht="21">
       <c r="A305" s="3" t="s">
         <v>251</v>
       </c>
@@ -6146,7 +6214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="306" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="306" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A306" s="30" t="s">
         <v>251</v>
       </c>
@@ -6156,11 +6224,12 @@
       <c r="C306" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D306" s="37" t="s">
+      <c r="D306" s="36" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="307" spans="1:4" ht="21">
+      <c r="F306" s="32"/>
+    </row>
+    <row r="307" spans="1:6" ht="21">
       <c r="A307" s="3" t="s">
         <v>251</v>
       </c>
@@ -6171,7 +6240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="21">
+    <row r="308" spans="1:6" ht="21">
       <c r="A308" s="3" t="s">
         <v>251</v>
       </c>
@@ -6185,7 +6254,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="21">
+    <row r="309" spans="1:6" ht="21">
       <c r="A309" s="3" t="s">
         <v>251</v>
       </c>
@@ -6196,7 +6265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="21">
+    <row r="310" spans="1:6" ht="21">
       <c r="A310" s="3" t="s">
         <v>251</v>
       </c>
@@ -6207,7 +6276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="21">
+    <row r="311" spans="1:6" ht="21">
       <c r="A311" s="3" t="s">
         <v>251</v>
       </c>
@@ -6218,7 +6287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="21">
+    <row r="312" spans="1:6" ht="21">
       <c r="A312" s="3" t="s">
         <v>251</v>
       </c>
@@ -6229,7 +6298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="21">
+    <row r="313" spans="1:6" ht="21">
       <c r="A313" s="3" t="s">
         <v>251</v>
       </c>
@@ -6240,7 +6309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="21">
+    <row r="314" spans="1:6" ht="21">
       <c r="A314" s="3" t="s">
         <v>251</v>
       </c>
@@ -6254,7 +6323,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="21">
+    <row r="315" spans="1:6" ht="21">
       <c r="A315" s="3" t="s">
         <v>251</v>
       </c>
@@ -6265,7 +6334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="21">
+    <row r="316" spans="1:6" ht="21">
       <c r="A316" s="3" t="s">
         <v>251</v>
       </c>
@@ -6279,7 +6348,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="21">
+    <row r="317" spans="1:6" ht="21">
       <c r="A317" s="3" t="s">
         <v>251</v>
       </c>
@@ -6290,7 +6359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="21">
+    <row r="318" spans="1:6" ht="21">
       <c r="A318" s="3" t="s">
         <v>251</v>
       </c>
@@ -6301,7 +6370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="21">
+    <row r="319" spans="1:6" ht="21">
       <c r="A319" s="3" t="s">
         <v>251</v>
       </c>
@@ -6312,7 +6381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="21">
+    <row r="320" spans="1:6" ht="21">
       <c r="A320" s="3" t="s">
         <v>251</v>
       </c>
@@ -6323,7 +6392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="21">
+    <row r="321" spans="1:6" ht="21">
       <c r="A321" s="3" t="s">
         <v>251</v>
       </c>
@@ -6334,7 +6403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="322" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A322" s="6" t="s">
         <v>251</v>
       </c>
@@ -6347,8 +6416,9 @@
       <c r="D322" s="23" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="323" spans="1:4" ht="21">
+      <c r="F322" s="23"/>
+    </row>
+    <row r="323" spans="1:6" ht="21">
       <c r="A323" s="3" t="s">
         <v>251</v>
       </c>
@@ -6359,7 +6429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="21">
+    <row r="324" spans="1:6" ht="21">
       <c r="A324" s="3" t="s">
         <v>251</v>
       </c>
@@ -6370,7 +6440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="21">
+    <row r="325" spans="1:6" ht="21">
       <c r="A325" s="3" t="s">
         <v>251</v>
       </c>
@@ -6381,7 +6451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:4" ht="21">
+    <row r="326" spans="1:6" ht="21">
       <c r="A326" s="3" t="s">
         <v>251</v>
       </c>
@@ -6392,7 +6462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="21">
+    <row r="327" spans="1:6" ht="21">
       <c r="A327" s="3" t="s">
         <v>251</v>
       </c>
@@ -6406,7 +6476,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="328" spans="1:4" s="31" customFormat="1" ht="21">
+    <row r="328" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A328" s="30" t="s">
         <v>251</v>
       </c>
@@ -6416,19 +6486,20 @@
       <c r="C328" s="30" t="s">
         <v>425</v>
       </c>
-      <c r="D328" s="37" t="s">
+      <c r="D328" s="36" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="329" spans="1:4" ht="21">
+      <c r="F328" s="32"/>
+    </row>
+    <row r="329" spans="1:6" ht="21">
       <c r="B329" s="4"/>
       <c r="C329" s="2"/>
     </row>
-    <row r="330" spans="1:4" ht="21">
+    <row r="330" spans="1:6" ht="21">
       <c r="B330" s="4"/>
       <c r="C330" s="2"/>
     </row>
-    <row r="331" spans="1:4" ht="21">
+    <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
         <v>537</v>
       </c>
@@ -6442,7 +6513,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="21">
+    <row r="332" spans="1:6" ht="21">
       <c r="A332" s="5" t="s">
         <v>537</v>
       </c>
@@ -6456,7 +6527,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="333" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A333" s="6" t="s">
         <v>537</v>
       </c>
@@ -6467,8 +6538,9 @@
         <v>2</v>
       </c>
       <c r="D333" s="23"/>
-    </row>
-    <row r="334" spans="1:4" ht="21">
+      <c r="F333" s="23"/>
+    </row>
+    <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
         <v>537</v>
       </c>
@@ -6482,7 +6554,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="21">
+    <row r="335" spans="1:6" ht="21">
       <c r="A335" s="5" t="s">
         <v>537</v>
       </c>
@@ -6496,7 +6568,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="336" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="336" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A336" s="6" t="s">
         <v>537</v>
       </c>
@@ -6507,6 +6579,7 @@
         <v>2</v>
       </c>
       <c r="D336" s="23"/>
+      <c r="F336" s="23"/>
     </row>
     <row r="337" spans="1:6" ht="21">
       <c r="A337" s="5" t="s">
@@ -6557,6 +6630,7 @@
       <c r="D340" s="22" t="s">
         <v>528</v>
       </c>
+      <c r="F340" s="23"/>
     </row>
     <row r="341" spans="1:6" ht="21">
       <c r="A341" s="6" t="s">
@@ -6626,9 +6700,10 @@
       <c r="C346" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="D346" s="53" t="s">
+      <c r="D346" s="52" t="s">
         <v>525</v>
       </c>
+      <c r="F346" s="23"/>
     </row>
     <row r="347" spans="1:6" ht="21">
       <c r="A347" s="5" t="s">
@@ -6654,7 +6729,7 @@
       <c r="D348" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="F348" t="s">
+      <c r="F348" s="57" t="s">
         <v>531</v>
       </c>
     </row>
@@ -6864,7 +6939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="369" spans="1:4" ht="21">
+    <row r="369" spans="1:6" ht="21">
       <c r="A369" s="5" t="s">
         <v>303</v>
       </c>
@@ -6875,7 +6950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="370" spans="1:4" ht="21">
+    <row r="370" spans="1:6" ht="21">
       <c r="A370" s="5" t="s">
         <v>303</v>
       </c>
@@ -6886,7 +6961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="371" spans="1:4" ht="21">
+    <row r="371" spans="1:6" ht="21">
       <c r="A371" s="5" t="s">
         <v>303</v>
       </c>
@@ -6897,7 +6972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="21">
+    <row r="372" spans="1:6" ht="21">
       <c r="A372" s="5" t="s">
         <v>303</v>
       </c>
@@ -6908,7 +6983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="373" spans="1:4" ht="21">
+    <row r="373" spans="1:6" ht="21">
       <c r="A373" s="5" t="s">
         <v>303</v>
       </c>
@@ -6919,7 +6994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="374" spans="1:4" ht="21">
+    <row r="374" spans="1:6" ht="21">
       <c r="A374" s="5" t="s">
         <v>303</v>
       </c>
@@ -6930,7 +7005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:4" ht="21">
+    <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
         <v>303</v>
       </c>
@@ -6941,7 +7016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="376" spans="1:4" ht="21">
+    <row r="376" spans="1:6" ht="21">
       <c r="A376" s="5" t="s">
         <v>303</v>
       </c>
@@ -6952,7 +7027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="377" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="377" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A377" s="6" t="s">
         <v>303</v>
       </c>
@@ -6963,8 +7038,9 @@
         <v>2</v>
       </c>
       <c r="D377" s="23"/>
-    </row>
-    <row r="378" spans="1:4" ht="21">
+      <c r="F377" s="23"/>
+    </row>
+    <row r="378" spans="1:6" ht="21">
       <c r="A378" s="5" t="s">
         <v>303</v>
       </c>
@@ -6975,7 +7051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="379" spans="1:4" ht="21">
+    <row r="379" spans="1:6" ht="21">
       <c r="A379" s="5" t="s">
         <v>303</v>
       </c>
@@ -6986,7 +7062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="380" spans="1:4" ht="21">
+    <row r="380" spans="1:6" ht="21">
       <c r="A380" s="5" t="s">
         <v>303</v>
       </c>
@@ -6997,7 +7073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="381" spans="1:4" ht="21">
+    <row r="381" spans="1:6" ht="21">
       <c r="A381" s="5" t="s">
         <v>303</v>
       </c>
@@ -7008,7 +7084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="382" spans="1:4" ht="21">
+    <row r="382" spans="1:6" ht="21">
       <c r="A382" s="5" t="s">
         <v>303</v>
       </c>
@@ -7019,7 +7095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="383" spans="1:4" ht="21">
+    <row r="383" spans="1:6" ht="21">
       <c r="A383" s="5" t="s">
         <v>303</v>
       </c>
@@ -7030,7 +7106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:4" ht="21">
+    <row r="384" spans="1:6" ht="21">
       <c r="A384" s="5" t="s">
         <v>303</v>
       </c>
@@ -7365,7 +7441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="417" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="417" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A417" s="6" t="s">
         <v>353</v>
       </c>
@@ -7376,8 +7452,9 @@
         <v>2</v>
       </c>
       <c r="D417" s="23"/>
-    </row>
-    <row r="418" spans="1:4" s="7" customFormat="1" ht="21">
+      <c r="F417" s="23"/>
+    </row>
+    <row r="418" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A418" s="6" t="s">
         <v>353</v>
       </c>
@@ -7388,8 +7465,9 @@
         <v>2</v>
       </c>
       <c r="D418" s="23"/>
-    </row>
-    <row r="419" spans="1:4" ht="21">
+      <c r="F418" s="23"/>
+    </row>
+    <row r="419" spans="1:6" ht="21">
       <c r="A419" s="3" t="s">
         <v>353</v>
       </c>
@@ -7400,7 +7478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="420" spans="1:4" ht="21">
+    <row r="420" spans="1:6" ht="21">
       <c r="A420" s="3" t="s">
         <v>353</v>
       </c>
@@ -7411,7 +7489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="421" spans="1:4" ht="21">
+    <row r="421" spans="1:6" ht="21">
       <c r="A421" s="3" t="s">
         <v>353</v>
       </c>
@@ -7422,7 +7500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="422" spans="1:4" ht="21">
+    <row r="422" spans="1:6" ht="21">
       <c r="A422" s="3" t="s">
         <v>353</v>
       </c>
@@ -7433,7 +7511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:4" ht="21">
+    <row r="423" spans="1:6" ht="21">
       <c r="A423" s="3" t="s">
         <v>353</v>
       </c>
@@ -7444,7 +7522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="424" spans="1:4" ht="21">
+    <row r="424" spans="1:6" ht="21">
       <c r="A424" s="3" t="s">
         <v>353</v>
       </c>
@@ -7455,7 +7533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="425" spans="1:4" ht="21">
+    <row r="425" spans="1:6" ht="21">
       <c r="A425" s="3" t="s">
         <v>353</v>
       </c>
@@ -7466,7 +7544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="426" spans="1:4" ht="21">
+    <row r="426" spans="1:6" ht="21">
       <c r="A426" s="3" t="s">
         <v>353</v>
       </c>
@@ -7477,7 +7555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="427" spans="1:4" ht="21">
+    <row r="427" spans="1:6" ht="21">
       <c r="A427" s="3" t="s">
         <v>353</v>
       </c>
@@ -7488,7 +7566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="428" spans="1:4" ht="21">
+    <row r="428" spans="1:6" ht="21">
       <c r="A428" s="3" t="s">
         <v>353</v>
       </c>
@@ -7499,7 +7577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="429" spans="1:4" ht="21">
+    <row r="429" spans="1:6" ht="21">
       <c r="A429" s="3" t="s">
         <v>353</v>
       </c>
@@ -7510,7 +7588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="430" spans="1:4" ht="21">
+    <row r="430" spans="1:6" ht="21">
       <c r="A430" s="3" t="s">
         <v>353</v>
       </c>
@@ -7521,7 +7599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="431" spans="1:4" ht="21">
+    <row r="431" spans="1:6" ht="21">
       <c r="A431" s="3" t="s">
         <v>353</v>
       </c>
@@ -7532,7 +7610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="432" spans="1:4" ht="21">
+    <row r="432" spans="1:6" ht="21">
       <c r="A432" s="3" t="s">
         <v>353</v>
       </c>
@@ -7543,7 +7621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="433" spans="1:4" ht="21">
+    <row r="433" spans="1:6" ht="21">
       <c r="A433" s="3" t="s">
         <v>353</v>
       </c>
@@ -7554,7 +7632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="434" spans="1:4" ht="21">
+    <row r="434" spans="1:6" ht="21">
       <c r="A434" s="3" t="s">
         <v>353</v>
       </c>
@@ -7565,7 +7643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="435" spans="1:4" ht="21">
+    <row r="435" spans="1:6" ht="21">
       <c r="A435" s="3" t="s">
         <v>353</v>
       </c>
@@ -7576,7 +7654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="436" spans="1:4" ht="21">
+    <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
         <v>353</v>
       </c>
@@ -7587,7 +7665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="437" spans="1:4" ht="21">
+    <row r="437" spans="1:6" ht="21">
       <c r="A437" s="3" t="s">
         <v>353</v>
       </c>
@@ -7598,7 +7676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="438" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="438" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A438" s="6" t="s">
         <v>353</v>
       </c>
@@ -7609,8 +7687,9 @@
         <v>2</v>
       </c>
       <c r="D438" s="23"/>
-    </row>
-    <row r="439" spans="1:4" ht="21">
+      <c r="F438" s="23"/>
+    </row>
+    <row r="439" spans="1:6" ht="21">
       <c r="A439" s="3" t="s">
         <v>353</v>
       </c>
@@ -7621,7 +7700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="440" spans="1:4" ht="21">
+    <row r="440" spans="1:6" ht="21">
       <c r="A440" s="3" t="s">
         <v>353</v>
       </c>
@@ -7632,7 +7711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="441" spans="1:4" ht="21">
+    <row r="441" spans="1:6" ht="21">
       <c r="A441" s="3" t="s">
         <v>353</v>
       </c>
@@ -7643,7 +7722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="442" spans="1:4" ht="21">
+    <row r="442" spans="1:6" ht="21">
       <c r="A442" s="3" t="s">
         <v>353</v>
       </c>
@@ -7654,7 +7733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="443" spans="1:4" ht="21">
+    <row r="443" spans="1:6" ht="21">
       <c r="A443" s="3" t="s">
         <v>353</v>
       </c>
@@ -7665,7 +7744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="444" spans="1:4" ht="21">
+    <row r="444" spans="1:6" ht="21">
       <c r="A444" s="3" t="s">
         <v>353</v>
       </c>
@@ -7676,7 +7755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="445" spans="1:4" ht="21">
+    <row r="445" spans="1:6" ht="21">
       <c r="A445" s="3" t="s">
         <v>353</v>
       </c>
@@ -7687,7 +7766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="446" spans="1:4" ht="21">
+    <row r="446" spans="1:6" ht="21">
       <c r="A446" s="3" t="s">
         <v>353</v>
       </c>
@@ -7698,7 +7777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="447" spans="1:4" ht="21">
+    <row r="447" spans="1:6" ht="21">
       <c r="A447" s="3" t="s">
         <v>353</v>
       </c>
@@ -7709,7 +7788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="448" spans="1:4" ht="21">
+    <row r="448" spans="1:6" ht="21">
       <c r="A448" s="3" t="s">
         <v>353</v>
       </c>
@@ -7720,7 +7799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="449" spans="1:4" ht="21">
+    <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
         <v>353</v>
       </c>
@@ -7731,7 +7810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="450" spans="1:4" s="25" customFormat="1" ht="21">
+    <row r="450" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A450" s="24" t="s">
         <v>353</v>
       </c>
@@ -7742,8 +7821,9 @@
         <v>2</v>
       </c>
       <c r="D450" s="26"/>
-    </row>
-    <row r="451" spans="1:4" s="25" customFormat="1" ht="21">
+      <c r="F450" s="26"/>
+    </row>
+    <row r="451" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A451" s="24" t="s">
         <v>353</v>
       </c>
@@ -7754,8 +7834,9 @@
         <v>2</v>
       </c>
       <c r="D451" s="26"/>
-    </row>
-    <row r="452" spans="1:4" ht="21">
+      <c r="F451" s="26"/>
+    </row>
+    <row r="452" spans="1:6" ht="21">
       <c r="A452" s="3" t="s">
         <v>353</v>
       </c>
@@ -7766,7 +7847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="453" spans="1:4" ht="21">
+    <row r="453" spans="1:6" ht="21">
       <c r="A453" s="3" t="s">
         <v>353</v>
       </c>
@@ -7777,7 +7858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="454" spans="1:4" ht="21">
+    <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
         <v>353</v>
       </c>
@@ -7788,7 +7869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="455" spans="1:4" ht="21">
+    <row r="455" spans="1:6" ht="21">
       <c r="A455" s="3" t="s">
         <v>353</v>
       </c>
@@ -7799,7 +7880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="456" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A456" s="6" t="s">
         <v>353</v>
       </c>
@@ -7810,8 +7891,9 @@
         <v>425</v>
       </c>
       <c r="D456" s="23"/>
-    </row>
-    <row r="457" spans="1:4" ht="21">
+      <c r="F456" s="23"/>
+    </row>
+    <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
         <v>353</v>
       </c>
@@ -7822,7 +7904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="458" spans="1:4" ht="21">
+    <row r="458" spans="1:6" ht="21">
       <c r="A458" s="3" t="s">
         <v>353</v>
       </c>
@@ -7833,7 +7915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="459" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="459" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A459" s="6" t="s">
         <v>353</v>
       </c>
@@ -7844,8 +7926,9 @@
         <v>2</v>
       </c>
       <c r="D459" s="23"/>
-    </row>
-    <row r="460" spans="1:4" ht="21">
+      <c r="F459" s="23"/>
+    </row>
+    <row r="460" spans="1:6" ht="21">
       <c r="A460" s="3" t="s">
         <v>353</v>
       </c>
@@ -7856,7 +7939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="461" spans="1:4" ht="21">
+    <row r="461" spans="1:6" ht="21">
       <c r="A461" s="3" t="s">
         <v>353</v>
       </c>
@@ -7867,7 +7950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="462" spans="1:4" ht="21">
+    <row r="462" spans="1:6" ht="21">
       <c r="A462" s="3" t="s">
         <v>353</v>
       </c>
@@ -7878,7 +7961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="463" spans="1:4" ht="21">
+    <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
         <v>353</v>
       </c>
@@ -7889,16 +7972,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="464" spans="1:4" ht="21">
+    <row r="464" spans="1:6" ht="21">
       <c r="B464" s="4"/>
       <c r="C464" s="2"/>
     </row>
-    <row r="465" spans="1:4" ht="21">
+    <row r="465" spans="1:6" ht="21">
       <c r="A465" s="5"/>
       <c r="B465" s="4"/>
       <c r="C465" s="2"/>
     </row>
-    <row r="466" spans="1:4" ht="21">
+    <row r="466" spans="1:6" ht="21">
       <c r="A466" s="3" t="s">
         <v>413</v>
       </c>
@@ -7912,7 +7995,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="467" spans="1:4" ht="21">
+    <row r="467" spans="1:6" ht="21">
       <c r="A467" s="3" t="s">
         <v>413</v>
       </c>
@@ -7920,10 +8003,16 @@
         <v>415</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="468" spans="1:4" ht="21">
+        <v>425</v>
+      </c>
+      <c r="D467" s="20" t="s">
+        <v>595</v>
+      </c>
+      <c r="F467" s="57" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" ht="21">
       <c r="A468" s="3" t="s">
         <v>413</v>
       </c>
@@ -7931,10 +8020,13 @@
         <v>416</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="469" spans="1:4" ht="21">
+        <v>425</v>
+      </c>
+      <c r="D468" s="20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" ht="21">
       <c r="A469" s="3" t="s">
         <v>413</v>
       </c>
@@ -7948,7 +8040,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="470" spans="1:4" ht="21">
+    <row r="470" spans="1:6" ht="21">
       <c r="A470" s="3" t="s">
         <v>413</v>
       </c>
@@ -7962,7 +8054,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="471" spans="1:4" ht="21">
+    <row r="471" spans="1:6" ht="21">
       <c r="A471" s="3" t="s">
         <v>413</v>
       </c>
@@ -7972,8 +8064,11 @@
       <c r="C471" s="2" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="472" spans="1:4" ht="21">
+      <c r="D471" s="20" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" ht="21">
       <c r="A472" s="3" t="s">
         <v>413</v>
       </c>
@@ -7984,7 +8079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="473" spans="1:4" ht="21">
+    <row r="473" spans="1:6" ht="21">
       <c r="A473" s="3" t="s">
         <v>413</v>
       </c>
@@ -7995,7 +8090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="474" spans="1:4" ht="21">
+    <row r="474" spans="1:6" ht="21">
       <c r="A474" s="3" t="s">
         <v>413</v>
       </c>
@@ -8006,7 +8101,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="475" spans="1:4" s="7" customFormat="1" ht="21">
+    <row r="475" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A475" s="6" t="s">
         <v>413</v>
       </c>
@@ -8019,6 +8114,7 @@
       <c r="D475" s="22" t="s">
         <v>592</v>
       </c>
+      <c r="F475" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8580,8 +8676,11 @@
     <hyperlink ref="D469" r:id="rId556"/>
     <hyperlink ref="D470" r:id="rId557"/>
     <hyperlink ref="D475" r:id="rId558"/>
+    <hyperlink ref="D471" r:id="rId559"/>
+    <hyperlink ref="D467" r:id="rId560"/>
+    <hyperlink ref="D468" r:id="rId561"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId559"/>
+  <pageSetup orientation="portrait" r:id="rId562"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calculate square of a number without using *, / and pow()
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="599">
   <si>
     <t>Topic:</t>
   </si>
@@ -1831,6 +1831,9 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/number-of-flips_3125902?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/calculate-square-of-a-number_1112623?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2594,7 +2597,7 @@
   <dimension ref="A1:F475"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A462" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D473" sqref="D473"/>
+      <selection activeCell="F479" sqref="F479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -8098,7 +8101,10 @@
         <v>422</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>2</v>
+        <v>425</v>
+      </c>
+      <c r="D474" s="20" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="475" spans="1:6" s="7" customFormat="1" ht="21">
@@ -8679,8 +8685,9 @@
     <hyperlink ref="D471" r:id="rId559"/>
     <hyperlink ref="D467" r:id="rId560"/>
     <hyperlink ref="D468" r:id="rId561"/>
+    <hyperlink ref="D474" r:id="rId562"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId562"/>
+  <pageSetup orientation="portrait" r:id="rId563"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
find pair with difference k
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="601">
   <si>
     <t>Topic:</t>
   </si>
@@ -1837,6 +1837,9 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/find-the-repeating-and-missing-number_1062727?leftPanelTab=3</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-number-of-pairs-with-absolute-difference-k/submissions/</t>
   </si>
 </sst>
 </file>
@@ -2599,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115:XFD116"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -3885,7 +3888,10 @@
         <v>95</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>2</v>
+        <v>423</v>
+      </c>
+      <c r="D107" s="20" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
@@ -8677,8 +8683,9 @@
     <hyperlink ref="D471" r:id="rId561"/>
     <hyperlink ref="D105" r:id="rId562"/>
     <hyperlink ref="D104" r:id="rId563"/>
+    <hyperlink ref="D107" r:id="rId564"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId564"/>
+  <pageSetup orientation="portrait" r:id="rId565"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverse first k elements of queue
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="602">
   <si>
     <t>Topic:</t>
   </si>
@@ -1840,6 +1840,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/product-of-array-except-self/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/reverse-first-k-elements-of-queue_982771?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F314" sqref="F314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6350,7 +6353,10 @@
         <v>273</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>2</v>
+        <v>422</v>
+      </c>
+      <c r="D314" s="20" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="21">
@@ -8682,8 +8688,9 @@
     <hyperlink ref="D104" r:id="rId562"/>
     <hyperlink ref="D107" r:id="rId563"/>
     <hyperlink ref="D112" r:id="rId564"/>
+    <hyperlink ref="D314" r:id="rId565"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId565"/>
+  <pageSetup orientation="portrait" r:id="rId566"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first non repeating character in a stream
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="604">
   <si>
     <t>Topic:</t>
   </si>
@@ -849,9 +849,6 @@
   </si>
   <si>
     <t>Interleave the first half of the queue with second half</t>
-  </si>
-  <si>
-    <t>Find the first circular tour that visits all Petrol Pumps</t>
   </si>
   <si>
     <t>Minimum time required to rot all oranges</t>
@@ -1843,6 +1840,15 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/reverse-first-k-elements-of-queue_982771?leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/library/first-non-repeating-character-in-a-stream</t>
+  </si>
+  <si>
+    <t>(FOLDER FIRST) https://www.interviewbit.com/problems/first-non-repeating-character-in-a-stream-of-characters/</t>
+  </si>
+  <si>
+    <t>Find the first circular tour that visits all Petrol Pumps [V.V.V.IMP]</t>
   </si>
 </sst>
 </file>
@@ -2605,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F314" sqref="F314"/>
+    <sheetView tabSelected="1" topLeftCell="A302" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B316" sqref="B316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2621,7 +2627,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21">
@@ -2632,10 +2638,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2649,10 +2655,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21">
@@ -2663,10 +2669,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21">
@@ -2677,10 +2683,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21">
@@ -2691,10 +2697,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21">
@@ -2705,10 +2711,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21">
@@ -2719,10 +2725,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
@@ -2733,10 +2739,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>422</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2747,10 +2753,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F12" s="59"/>
     </row>
@@ -2765,7 +2771,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
@@ -2776,10 +2782,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21">
@@ -2790,10 +2796,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="21">
@@ -2804,10 +2810,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F16" s="60"/>
     </row>
@@ -2816,7 +2822,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2830,10 +2836,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2844,13 +2850,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="F19" s="57" t="s">
         <v>550</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2861,10 +2867,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F20" s="59"/>
     </row>
@@ -2876,10 +2882,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2890,10 +2896,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2904,10 +2910,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2918,10 +2924,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2932,10 +2938,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2946,10 +2952,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2960,10 +2966,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -3004,13 +3010,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F31" s="26"/>
     </row>
@@ -3019,7 +3025,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -3032,13 +3038,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3046,13 +3052,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F34" s="23"/>
     </row>
@@ -3086,10 +3092,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F37" s="61"/>
     </row>
@@ -3098,13 +3104,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F38" s="29"/>
     </row>
@@ -3113,13 +3119,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>421</v>
+      </c>
+      <c r="D39" s="53" t="s">
         <v>535</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>422</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>536</v>
       </c>
       <c r="F39" s="29"/>
     </row>
@@ -3137,13 +3143,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F42" s="23"/>
     </row>
@@ -3155,10 +3161,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21">
@@ -3180,10 +3186,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -3194,10 +3200,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
@@ -3208,13 +3214,13 @@
         <v>37</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D47" s="36" t="s">
+        <v>577</v>
+      </c>
+      <c r="F47" s="32" t="s">
         <v>578</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -3236,10 +3242,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3250,10 +3256,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3280,10 +3286,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3294,10 +3300,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3308,10 +3314,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3497,7 +3503,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="21">
@@ -3508,10 +3514,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="21">
@@ -3568,10 +3574,10 @@
         <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="21">
@@ -3774,10 +3780,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="21">
@@ -3788,10 +3794,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="21">
@@ -3802,10 +3808,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="21">
@@ -3816,10 +3822,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="21">
@@ -3852,10 +3858,10 @@
         <v>92</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="21">
@@ -3866,10 +3872,10 @@
         <v>93</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="21">
@@ -3891,10 +3897,10 @@
         <v>95</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3905,10 +3911,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F108" s="23"/>
     </row>
@@ -3953,10 +3959,10 @@
         <v>100</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="21">
@@ -4000,7 +4006,7 @@
         <v>104</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="21">
@@ -4022,7 +4028,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D118" s="26"/>
       <c r="F118" s="26"/>
@@ -4035,7 +4041,7 @@
         <v>107</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D119" s="26"/>
       <c r="F119" s="26"/>
@@ -4081,7 +4087,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D123" s="26"/>
       <c r="F123" s="26"/>
@@ -4131,10 +4137,10 @@
         <v>116</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="7" customFormat="1" ht="21">
@@ -4145,10 +4151,10 @@
         <v>117</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F130" s="23"/>
     </row>
@@ -4160,10 +4166,10 @@
         <v>118</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="21">
@@ -4174,10 +4180,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="21">
@@ -4188,10 +4194,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="21">
@@ -4202,10 +4208,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="21">
@@ -4216,10 +4222,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="21">
@@ -4230,10 +4236,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="21">
@@ -4244,10 +4250,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="21">
@@ -4280,7 +4286,7 @@
         <v>127</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D140" s="17"/>
       <c r="F140" s="23"/>
@@ -4306,10 +4312,10 @@
         <v>129</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="21">
@@ -4320,10 +4326,10 @@
         <v>130</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="21">
@@ -4334,10 +4340,10 @@
         <v>131</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="21">
@@ -4348,10 +4354,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4362,10 +4368,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4427,7 +4433,7 @@
         <v>2</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="21">
@@ -4435,13 +4441,13 @@
         <v>115</v>
       </c>
       <c r="B152" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D152" s="20" t="s">
         <v>446</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D152" s="20" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="153" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4449,10 +4455,10 @@
         <v>115</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C153" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D153" s="32"/>
       <c r="F153" s="32"/>
@@ -4465,27 +4471,27 @@
         <v>139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A155" s="30" t="s">
+        <v>469</v>
+      </c>
+      <c r="B155" s="31" t="s">
         <v>470</v>
       </c>
-      <c r="B155" s="31" t="s">
+      <c r="C155" s="30" t="s">
         <v>471</v>
       </c>
-      <c r="C155" s="30" t="s">
+      <c r="D155" s="36" t="s">
         <v>472</v>
       </c>
-      <c r="D155" s="36" t="s">
+      <c r="F155" s="38" t="s">
         <v>473</v>
-      </c>
-      <c r="F155" s="38" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4493,13 +4499,13 @@
         <v>115</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F156" s="32"/>
     </row>
@@ -4508,13 +4514,13 @@
         <v>115</v>
       </c>
       <c r="B157" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D157" s="20" t="s">
         <v>466</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D157" s="20" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="21">
@@ -4544,13 +4550,13 @@
         <v>115</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D160" s="34" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F160" s="61"/>
     </row>
@@ -4562,10 +4568,10 @@
         <v>142</v>
       </c>
       <c r="C161" s="35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D161" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="21">
@@ -4576,10 +4582,10 @@
         <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="21">
@@ -4588,16 +4594,16 @@
     </row>
     <row r="165" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A165" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B165" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="B165" s="7" t="s">
-        <v>487</v>
-      </c>
       <c r="C165" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F165" s="23"/>
     </row>
@@ -4609,10 +4615,10 @@
         <v>145</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="21">
@@ -4620,13 +4626,13 @@
         <v>144</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="21">
@@ -4637,10 +4643,10 @@
         <v>146</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="21">
@@ -4651,10 +4657,10 @@
         <v>147</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="21">
@@ -4665,10 +4671,10 @@
         <v>148</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="21">
@@ -4679,10 +4685,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="21">
@@ -4693,10 +4699,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="21">
@@ -4707,10 +4713,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="21">
@@ -4721,10 +4727,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="21">
@@ -4757,10 +4763,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="21">
@@ -4771,10 +4777,10 @@
         <v>156</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="21">
@@ -4793,13 +4799,13 @@
         <v>144</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F180" s="32"/>
     </row>
@@ -4819,13 +4825,13 @@
         <v>144</v>
       </c>
       <c r="B182" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D182" s="20" t="s">
         <v>497</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D182" s="20" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="21">
@@ -4847,10 +4853,10 @@
         <v>160</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="21">
@@ -4869,13 +4875,13 @@
         <v>144</v>
       </c>
       <c r="B186" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D186" s="20" t="s">
         <v>512</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D186" s="20" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="21">
@@ -4921,10 +4927,10 @@
         <v>165</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D190" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="21">
@@ -4967,13 +4973,13 @@
         <v>144</v>
       </c>
       <c r="B194" s="37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C194" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D194" s="32" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F194" s="32"/>
     </row>
@@ -4993,13 +4999,13 @@
         <v>144</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D196" s="23" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F196" s="23"/>
     </row>
@@ -5008,13 +5014,13 @@
         <v>144</v>
       </c>
       <c r="B197" s="39" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="21">
@@ -5067,13 +5073,13 @@
         <v>173</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D203" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="21">
@@ -5081,13 +5087,13 @@
         <v>173</v>
       </c>
       <c r="B204" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D204" s="20" t="s">
         <v>505</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D204" s="20" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="21">
@@ -5095,13 +5101,13 @@
         <v>173</v>
       </c>
       <c r="B205" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D205" s="20" t="s">
         <v>507</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D205" s="20" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="21">
@@ -5123,10 +5129,10 @@
         <v>175</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D207" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="21">
@@ -5137,10 +5143,10 @@
         <v>176</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D208" s="20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="21">
@@ -5151,10 +5157,10 @@
         <v>177</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D209" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="21">
@@ -5176,10 +5182,10 @@
         <v>179</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="21">
@@ -5220,7 +5226,7 @@
         <v>173</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>2</v>
@@ -5236,10 +5242,10 @@
         <v>183</v>
       </c>
       <c r="C216" s="43" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D216" s="44" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F216" s="62"/>
     </row>
@@ -5251,10 +5257,10 @@
         <v>184</v>
       </c>
       <c r="C217" s="48" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D217" s="49" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F217" s="63"/>
     </row>
@@ -5288,10 +5294,10 @@
         <v>187</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D220" s="20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="21">
@@ -5347,11 +5353,11 @@
         <v>192</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D225" s="23"/>
       <c r="F225" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="21">
@@ -5898,13 +5904,13 @@
         <v>229</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D277" s="22" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F277" s="23"/>
     </row>
@@ -6001,10 +6007,10 @@
         <v>249</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D287" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="21">
@@ -6015,10 +6021,10 @@
         <v>250</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D288" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="21">
@@ -6029,10 +6035,10 @@
         <v>251</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D289" s="20" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="21">
@@ -6043,10 +6049,10 @@
         <v>252</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="21">
@@ -6065,13 +6071,13 @@
         <v>248</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C292" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D292" s="22" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F292" s="23"/>
     </row>
@@ -6083,10 +6089,10 @@
         <v>254</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="21">
@@ -6097,13 +6103,13 @@
         <v>255</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F294" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="21">
@@ -6114,10 +6120,10 @@
         <v>256</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D295" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="296" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6125,13 +6131,13 @@
         <v>248</v>
       </c>
       <c r="B296" s="31" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C296" s="30" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D296" s="36" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F296" s="32"/>
     </row>
@@ -6165,10 +6171,10 @@
         <v>259</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D299" s="20" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="300" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6179,10 +6185,10 @@
         <v>260</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D300" s="22" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F300" s="23"/>
     </row>
@@ -6194,10 +6200,10 @@
         <v>261</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D301" s="20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="21">
@@ -6216,13 +6222,13 @@
         <v>248</v>
       </c>
       <c r="B303" s="31" t="s">
+        <v>573</v>
+      </c>
+      <c r="C303" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D303" s="36" t="s">
         <v>574</v>
-      </c>
-      <c r="C303" s="30" t="s">
-        <v>422</v>
-      </c>
-      <c r="D303" s="36" t="s">
-        <v>575</v>
       </c>
       <c r="F303" s="32"/>
     </row>
@@ -6245,10 +6251,10 @@
         <v>264</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D305" s="20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="21">
@@ -6314,10 +6320,10 @@
         <v>270</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D311" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6339,10 +6345,10 @@
         <v>272</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D313" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="21">
@@ -6353,10 +6359,10 @@
         <v>273</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="21">
@@ -6370,23 +6376,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="21">
-      <c r="A316" s="3" t="s">
+    <row r="316" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A316" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B316" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B316" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="C316" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D316" s="23"/>
+      <c r="F316" s="23"/>
     </row>
     <row r="317" spans="1:6" ht="21">
       <c r="A317" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -6397,7 +6405,7 @@
         <v>248</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -6408,13 +6416,13 @@
         <v>248</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D319" s="23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F319" s="23"/>
     </row>
@@ -6423,7 +6431,7 @@
         <v>248</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6434,7 +6442,7 @@
         <v>248</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -6445,7 +6453,7 @@
         <v>248</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -6456,10 +6464,16 @@
         <v>248</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>2</v>
+        <v>421</v>
+      </c>
+      <c r="D323" s="16" t="s">
+        <v>602</v>
+      </c>
+      <c r="F323" s="57" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="21">
@@ -6467,13 +6481,13 @@
         <v>248</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D324" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6481,13 +6495,13 @@
         <v>248</v>
       </c>
       <c r="B325" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="C325" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="D325" s="36" t="s">
         <v>585</v>
-      </c>
-      <c r="C325" s="30" t="s">
-        <v>422</v>
-      </c>
-      <c r="D325" s="36" t="s">
-        <v>586</v>
       </c>
       <c r="F325" s="32"/>
     </row>
@@ -6501,38 +6515,38 @@
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D328" s="21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="21">
       <c r="A329" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D329" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A330" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C330" s="6" t="s">
         <v>2</v>
@@ -6542,38 +6556,38 @@
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D331" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="21">
       <c r="A332" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D332" s="16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A333" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C333" s="6" t="s">
         <v>2</v>
@@ -6583,10 +6597,10 @@
     </row>
     <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>2</v>
@@ -6594,10 +6608,10 @@
     </row>
     <row r="335" spans="1:6" ht="21">
       <c r="A335" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>2</v>
@@ -6605,39 +6619,39 @@
     </row>
     <row r="336" spans="1:6" ht="21">
       <c r="A336" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D336" s="20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="337" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A337" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D337" s="22" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F337" s="23"/>
     </row>
     <row r="338" spans="1:6" ht="21">
       <c r="A338" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B338" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>2</v>
@@ -6645,10 +6659,10 @@
     </row>
     <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>2</v>
@@ -6656,10 +6670,10 @@
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -6667,24 +6681,24 @@
     </row>
     <row r="341" spans="1:6" ht="21">
       <c r="A341" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B341" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D341" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6692,25 +6706,25 @@
     </row>
     <row r="343" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A343" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C343" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D343" s="52" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F343" s="23"/>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6718,19 +6732,19 @@
     </row>
     <row r="345" spans="1:6" ht="21">
       <c r="A345" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D345" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="F345" s="57" t="s">
         <v>527</v>
-      </c>
-      <c r="F345" s="57" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
@@ -6743,10 +6757,10 @@
     </row>
     <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B348" s="13" t="s">
         <v>300</v>
-      </c>
-      <c r="B348" s="13" t="s">
-        <v>301</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>2</v>
@@ -6754,10 +6768,10 @@
     </row>
     <row r="349" spans="1:6" ht="21">
       <c r="A349" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>2</v>
@@ -6765,10 +6779,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6776,10 +6790,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6787,10 +6801,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6798,10 +6812,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6809,10 +6823,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6820,10 +6834,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -6831,10 +6845,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6842,10 +6856,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6853,10 +6867,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6864,10 +6878,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6875,10 +6889,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6886,10 +6900,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6897,10 +6911,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6908,10 +6922,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6919,10 +6933,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6930,10 +6944,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6941,10 +6955,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6952,10 +6966,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -6963,10 +6977,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -6974,10 +6988,10 @@
     </row>
     <row r="369" spans="1:6" ht="21">
       <c r="A369" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -6985,10 +6999,10 @@
     </row>
     <row r="370" spans="1:6" ht="21">
       <c r="A370" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -6996,10 +7010,10 @@
     </row>
     <row r="371" spans="1:6" ht="21">
       <c r="A371" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -7007,10 +7021,10 @@
     </row>
     <row r="372" spans="1:6" ht="21">
       <c r="A372" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -7018,10 +7032,10 @@
     </row>
     <row r="373" spans="1:6" ht="21">
       <c r="A373" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -7029,10 +7043,10 @@
     </row>
     <row r="374" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A374" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C374" s="6" t="s">
         <v>2</v>
@@ -7042,10 +7056,10 @@
     </row>
     <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -7053,10 +7067,10 @@
     </row>
     <row r="376" spans="1:6" ht="21">
       <c r="A376" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>2</v>
@@ -7064,10 +7078,10 @@
     </row>
     <row r="377" spans="1:6" ht="21">
       <c r="A377" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -7075,10 +7089,10 @@
     </row>
     <row r="378" spans="1:6" ht="21">
       <c r="A378" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -7086,10 +7100,10 @@
     </row>
     <row r="379" spans="1:6" ht="21">
       <c r="A379" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -7097,10 +7111,10 @@
     </row>
     <row r="380" spans="1:6" ht="21">
       <c r="A380" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -7108,10 +7122,10 @@
     </row>
     <row r="381" spans="1:6" ht="21">
       <c r="A381" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -7119,10 +7133,10 @@
     </row>
     <row r="382" spans="1:6" ht="21">
       <c r="A382" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -7130,10 +7144,10 @@
     </row>
     <row r="383" spans="1:6" ht="21">
       <c r="A383" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -7141,10 +7155,10 @@
     </row>
     <row r="384" spans="1:6" ht="21">
       <c r="A384" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -7152,10 +7166,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -7163,10 +7177,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -7174,10 +7188,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -7185,10 +7199,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -7196,10 +7210,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -7207,10 +7221,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -7226,10 +7240,10 @@
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B393" s="13" t="s">
         <v>344</v>
-      </c>
-      <c r="B393" s="13" t="s">
-        <v>345</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>2</v>
@@ -7237,10 +7251,10 @@
     </row>
     <row r="394" spans="1:3" ht="21">
       <c r="A394" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>2</v>
@@ -7248,10 +7262,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7259,7 +7273,7 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B396" s="13" t="s">
         <v>77</v>
@@ -7270,10 +7284,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -7281,10 +7295,10 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>2</v>
@@ -7300,21 +7314,21 @@
     </row>
     <row r="401" spans="1:6" ht="21">
       <c r="A401" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B401" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="B401" s="13" t="s">
-        <v>351</v>
-      </c>
       <c r="C401" s="35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="21">
       <c r="A402" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>2</v>
@@ -7322,10 +7336,10 @@
     </row>
     <row r="403" spans="1:6" ht="21">
       <c r="A403" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>2</v>
@@ -7333,10 +7347,10 @@
     </row>
     <row r="404" spans="1:6" ht="21">
       <c r="A404" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7344,10 +7358,10 @@
     </row>
     <row r="405" spans="1:6" ht="21">
       <c r="A405" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -7355,21 +7369,21 @@
     </row>
     <row r="406" spans="1:6" ht="21">
       <c r="A406" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="21">
       <c r="A407" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7377,7 +7391,7 @@
     </row>
     <row r="408" spans="1:6" ht="21">
       <c r="A408" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B408" s="13" t="s">
         <v>237</v>
@@ -7388,10 +7402,10 @@
     </row>
     <row r="409" spans="1:6" ht="21">
       <c r="A409" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7399,10 +7413,10 @@
     </row>
     <row r="410" spans="1:6" ht="21">
       <c r="A410" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>2</v>
@@ -7410,10 +7424,10 @@
     </row>
     <row r="411" spans="1:6" ht="21">
       <c r="A411" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7421,10 +7435,10 @@
     </row>
     <row r="412" spans="1:6" ht="21">
       <c r="A412" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7432,10 +7446,10 @@
     </row>
     <row r="413" spans="1:6" ht="21">
       <c r="A413" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7443,10 +7457,10 @@
     </row>
     <row r="414" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A414" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>2</v>
@@ -7456,10 +7470,10 @@
     </row>
     <row r="415" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A415" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B415" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>2</v>
@@ -7469,10 +7483,10 @@
     </row>
     <row r="416" spans="1:6" ht="21">
       <c r="A416" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7480,10 +7494,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7491,10 +7505,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7502,10 +7516,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7513,10 +7527,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7524,10 +7538,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7535,10 +7549,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7546,10 +7560,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7557,10 +7571,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7568,10 +7582,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7579,10 +7593,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7590,10 +7604,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7601,10 +7615,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7612,10 +7626,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7623,10 +7637,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7634,10 +7648,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7645,10 +7659,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7656,10 +7670,10 @@
     </row>
     <row r="433" spans="1:6" ht="21">
       <c r="A433" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7667,10 +7681,10 @@
     </row>
     <row r="434" spans="1:6" ht="21">
       <c r="A434" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7678,10 +7692,10 @@
     </row>
     <row r="435" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A435" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B435" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>2</v>
@@ -7691,10 +7705,10 @@
     </row>
     <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7702,10 +7716,10 @@
     </row>
     <row r="437" spans="1:6" ht="21">
       <c r="A437" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>2</v>
@@ -7713,10 +7727,10 @@
     </row>
     <row r="438" spans="1:6" ht="21">
       <c r="A438" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7724,10 +7738,10 @@
     </row>
     <row r="439" spans="1:6" ht="21">
       <c r="A439" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7735,10 +7749,10 @@
     </row>
     <row r="440" spans="1:6" ht="21">
       <c r="A440" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7746,10 +7760,10 @@
     </row>
     <row r="441" spans="1:6" ht="21">
       <c r="A441" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7757,10 +7771,10 @@
     </row>
     <row r="442" spans="1:6" ht="21">
       <c r="A442" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7768,10 +7782,10 @@
     </row>
     <row r="443" spans="1:6" ht="21">
       <c r="A443" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7779,10 +7793,10 @@
     </row>
     <row r="444" spans="1:6" ht="21">
       <c r="A444" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7790,10 +7804,10 @@
     </row>
     <row r="445" spans="1:6" ht="21">
       <c r="A445" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7801,10 +7815,10 @@
     </row>
     <row r="446" spans="1:6" ht="21">
       <c r="A446" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7812,10 +7826,10 @@
     </row>
     <row r="447" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A447" s="24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B447" s="25" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C447" s="24" t="s">
         <v>2</v>
@@ -7825,10 +7839,10 @@
     </row>
     <row r="448" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A448" s="24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B448" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C448" s="24" t="s">
         <v>2</v>
@@ -7838,10 +7852,10 @@
     </row>
     <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>2</v>
@@ -7849,10 +7863,10 @@
     </row>
     <row r="450" spans="1:6" ht="21">
       <c r="A450" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>2</v>
@@ -7860,10 +7874,10 @@
     </row>
     <row r="451" spans="1:6" ht="21">
       <c r="A451" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7871,10 +7885,10 @@
     </row>
     <row r="452" spans="1:6" ht="21">
       <c r="A452" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7882,23 +7896,23 @@
     </row>
     <row r="453" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A453" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D453" s="23"/>
       <c r="F453" s="23"/>
     </row>
     <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7906,10 +7920,10 @@
     </row>
     <row r="455" spans="1:6" ht="21">
       <c r="A455" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C455" s="2" t="s">
         <v>2</v>
@@ -7917,10 +7931,10 @@
     </row>
     <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A456" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>2</v>
@@ -7930,10 +7944,10 @@
     </row>
     <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7941,10 +7955,10 @@
     </row>
     <row r="458" spans="1:6" ht="21">
       <c r="A458" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>2</v>
@@ -7952,10 +7966,10 @@
     </row>
     <row r="459" spans="1:6" ht="21">
       <c r="A459" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -7963,10 +7977,10 @@
     </row>
     <row r="460" spans="1:6" ht="21">
       <c r="A460" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -7983,97 +7997,97 @@
     </row>
     <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B463" s="13" t="s">
         <v>410</v>
       </c>
-      <c r="B463" s="13" t="s">
-        <v>411</v>
-      </c>
       <c r="C463" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D463" s="16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="21">
       <c r="A464" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C464" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D464" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="F464" s="57" t="s">
         <v>592</v>
-      </c>
-      <c r="F464" s="57" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="21">
       <c r="A465" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="21">
       <c r="A466" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="21">
       <c r="A467" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="21">
       <c r="A468" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="21">
       <c r="A469" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -8081,44 +8095,44 @@
     </row>
     <row r="470" spans="1:6" ht="21">
       <c r="A470" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D470" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="471" spans="1:6" ht="21">
       <c r="A471" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D471" s="20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="472" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A472" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D472" s="22" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F472" s="23"/>
     </row>
@@ -8409,7 +8423,7 @@
     <hyperlink ref="B313" r:id="rId283"/>
     <hyperlink ref="B314" r:id="rId284"/>
     <hyperlink ref="B315" r:id="rId285"/>
-    <hyperlink ref="B316" r:id="rId286"/>
+    <hyperlink ref="B316" r:id="rId286" display="Find the first circular tour that visits all Petrol Pumps"/>
     <hyperlink ref="B317" r:id="rId287"/>
     <hyperlink ref="B318" r:id="rId288"/>
     <hyperlink ref="B319" r:id="rId289" display="First negative integer in every window of size “k”"/>

</xml_diff>

<commit_message>
interleave first and second half of queuee
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="605">
   <si>
     <t>Topic:</t>
   </si>
@@ -821,16 +821,10 @@
     <t>Expression contains redundant bracket or not</t>
   </si>
   <si>
-    <t>Implement Stack using Queue</t>
-  </si>
-  <si>
     <t>Implement Stack using Deque</t>
   </si>
   <si>
     <t>Stack Permutations (Check if an array is stack permutation of other)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implement Queue using Stack  </t>
   </si>
   <si>
     <t>Implement "n" queue in an array</t>
@@ -1758,9 +1752,6 @@
     <t>https://leetcode.com/problems/next-greater-element-i/submissions/</t>
   </si>
   <si>
-    <t>Largest rectangular Area in Histogram [HARD]</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/largest-rectangle-in-histogram/submissions/</t>
   </si>
   <si>
@@ -1849,6 +1840,18 @@
   </si>
   <si>
     <t>Find the first circular tour that visits all Petrol Pumps [V.V.V.IMP]</t>
+  </si>
+  <si>
+    <t>Implement Queue using Stack   [IMP]</t>
+  </si>
+  <si>
+    <t>Implement Stack using Queue [IMP]</t>
+  </si>
+  <si>
+    <t>Largest rectangular Area in Histogram [HARD]  V.V.V.V.IMP</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/interleave-the-first-half-of-the-queue-with-the-second-half_1169450?leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2136,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2290,6 +2293,13 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
@@ -2611,8 +2621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B316" sqref="B316"/>
+    <sheetView tabSelected="1" topLeftCell="A329" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F335" sqref="F335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2627,7 +2637,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21">
@@ -2638,10 +2648,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2655,10 +2665,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>421</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21">
@@ -2669,10 +2679,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21">
@@ -2683,10 +2693,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21">
@@ -2697,10 +2707,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21">
@@ -2711,10 +2721,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21">
@@ -2725,10 +2735,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
@@ -2739,10 +2749,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2753,10 +2763,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F12" s="59"/>
     </row>
@@ -2771,7 +2781,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
@@ -2782,10 +2792,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21">
@@ -2796,10 +2806,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="21">
@@ -2810,10 +2820,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F16" s="60"/>
     </row>
@@ -2822,7 +2832,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2836,10 +2846,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2850,13 +2860,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2867,10 +2877,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F20" s="59"/>
     </row>
@@ -2882,10 +2892,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2896,10 +2906,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2910,10 +2920,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2924,10 +2934,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2938,10 +2948,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2952,10 +2962,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2966,10 +2976,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -3010,13 +3020,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F31" s="26"/>
     </row>
@@ -3025,7 +3035,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -3038,13 +3048,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3052,13 +3062,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F34" s="23"/>
     </row>
@@ -3092,10 +3102,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F37" s="61"/>
     </row>
@@ -3104,13 +3114,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F38" s="29"/>
     </row>
@@ -3119,13 +3129,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F39" s="29"/>
     </row>
@@ -3143,13 +3153,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F42" s="23"/>
     </row>
@@ -3161,10 +3171,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21">
@@ -3186,10 +3196,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -3200,10 +3210,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
@@ -3214,13 +3224,13 @@
         <v>37</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -3242,10 +3252,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3256,10 +3266,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3286,10 +3296,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>421</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3300,10 +3310,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3314,10 +3324,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3503,7 +3513,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="21">
@@ -3514,10 +3524,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="21">
@@ -3574,10 +3584,10 @@
         <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="21">
@@ -3780,10 +3790,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="21">
@@ -3794,10 +3804,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="21">
@@ -3808,10 +3818,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="21">
@@ -3822,10 +3832,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="21">
@@ -3858,10 +3868,10 @@
         <v>92</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="21">
@@ -3872,10 +3882,10 @@
         <v>93</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="21">
@@ -3897,10 +3907,10 @@
         <v>95</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3911,10 +3921,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F108" s="23"/>
     </row>
@@ -3959,10 +3969,10 @@
         <v>100</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="21">
@@ -4006,7 +4016,7 @@
         <v>104</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="21">
@@ -4028,7 +4038,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D118" s="26"/>
       <c r="F118" s="26"/>
@@ -4041,7 +4051,7 @@
         <v>107</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D119" s="26"/>
       <c r="F119" s="26"/>
@@ -4087,7 +4097,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D123" s="26"/>
       <c r="F123" s="26"/>
@@ -4137,10 +4147,10 @@
         <v>116</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="7" customFormat="1" ht="21">
@@ -4151,10 +4161,10 @@
         <v>117</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F130" s="23"/>
     </row>
@@ -4166,10 +4176,10 @@
         <v>118</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="21">
@@ -4180,10 +4190,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="21">
@@ -4194,10 +4204,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="21">
@@ -4208,10 +4218,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="21">
@@ -4222,10 +4232,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="21">
@@ -4236,10 +4246,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="21">
@@ -4250,10 +4260,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="21">
@@ -4286,7 +4296,7 @@
         <v>127</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D140" s="17"/>
       <c r="F140" s="23"/>
@@ -4312,10 +4322,10 @@
         <v>129</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="21">
@@ -4326,10 +4336,10 @@
         <v>130</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="21">
@@ -4340,10 +4350,10 @@
         <v>131</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="21">
@@ -4354,10 +4364,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4368,10 +4378,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4433,7 +4443,7 @@
         <v>2</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="21">
@@ -4441,13 +4451,13 @@
         <v>115</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D152" s="20" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4455,10 +4465,10 @@
         <v>115</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C153" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D153" s="32"/>
       <c r="F153" s="32"/>
@@ -4471,27 +4481,27 @@
         <v>139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="155" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A155" s="30" t="s">
+        <v>467</v>
+      </c>
+      <c r="B155" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="C155" s="30" t="s">
         <v>469</v>
       </c>
-      <c r="B155" s="31" t="s">
+      <c r="D155" s="36" t="s">
         <v>470</v>
       </c>
-      <c r="C155" s="30" t="s">
+      <c r="F155" s="38" t="s">
         <v>471</v>
-      </c>
-      <c r="D155" s="36" t="s">
-        <v>472</v>
-      </c>
-      <c r="F155" s="38" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4499,13 +4509,13 @@
         <v>115</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F156" s="32"/>
     </row>
@@ -4514,13 +4524,13 @@
         <v>115</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="21">
@@ -4550,13 +4560,13 @@
         <v>115</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D160" s="34" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F160" s="61"/>
     </row>
@@ -4568,10 +4578,10 @@
         <v>142</v>
       </c>
       <c r="C161" s="35" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D161" s="20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="21">
@@ -4582,10 +4592,10 @@
         <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="21">
@@ -4594,16 +4604,16 @@
     </row>
     <row r="165" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A165" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F165" s="23"/>
     </row>
@@ -4615,10 +4625,10 @@
         <v>145</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="21">
@@ -4626,13 +4636,13 @@
         <v>144</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="21">
@@ -4643,10 +4653,10 @@
         <v>146</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="21">
@@ -4657,10 +4667,10 @@
         <v>147</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="21">
@@ -4671,10 +4681,10 @@
         <v>148</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="21">
@@ -4685,10 +4695,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="21">
@@ -4699,10 +4709,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="21">
@@ -4713,10 +4723,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="21">
@@ -4727,10 +4737,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="21">
@@ -4763,10 +4773,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="21">
@@ -4777,10 +4787,10 @@
         <v>156</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="21">
@@ -4799,13 +4809,13 @@
         <v>144</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F180" s="32"/>
     </row>
@@ -4825,13 +4835,13 @@
         <v>144</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D182" s="20" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="21">
@@ -4853,10 +4863,10 @@
         <v>160</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="21">
@@ -4875,13 +4885,13 @@
         <v>144</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D186" s="20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="21">
@@ -4927,10 +4937,10 @@
         <v>165</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D190" s="20" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="21">
@@ -4973,13 +4983,13 @@
         <v>144</v>
       </c>
       <c r="B194" s="37" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C194" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D194" s="32" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F194" s="32"/>
     </row>
@@ -4999,13 +5009,13 @@
         <v>144</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D196" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F196" s="23"/>
     </row>
@@ -5014,13 +5024,13 @@
         <v>144</v>
       </c>
       <c r="B197" s="39" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="21">
@@ -5073,13 +5083,13 @@
         <v>173</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D203" s="20" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="21">
@@ -5087,13 +5097,13 @@
         <v>173</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D204" s="20" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="21">
@@ -5101,13 +5111,13 @@
         <v>173</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D205" s="20" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="21">
@@ -5129,10 +5139,10 @@
         <v>175</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D207" s="20" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="21">
@@ -5143,10 +5153,10 @@
         <v>176</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D208" s="20" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="21">
@@ -5157,10 +5167,10 @@
         <v>177</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D209" s="20" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="21">
@@ -5182,10 +5192,10 @@
         <v>179</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="21">
@@ -5226,7 +5236,7 @@
         <v>173</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>2</v>
@@ -5242,10 +5252,10 @@
         <v>183</v>
       </c>
       <c r="C216" s="43" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D216" s="44" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F216" s="62"/>
     </row>
@@ -5257,10 +5267,10 @@
         <v>184</v>
       </c>
       <c r="C217" s="48" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D217" s="49" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F217" s="63"/>
     </row>
@@ -5294,10 +5304,10 @@
         <v>187</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D220" s="20" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="21">
@@ -5353,11 +5363,11 @@
         <v>192</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D225" s="23"/>
       <c r="F225" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="21">
@@ -5904,13 +5914,13 @@
         <v>229</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D277" s="22" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F277" s="23"/>
     </row>
@@ -6007,10 +6017,10 @@
         <v>249</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D287" s="16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="21">
@@ -6021,10 +6031,10 @@
         <v>250</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D288" s="16" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="21">
@@ -6035,10 +6045,10 @@
         <v>251</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D289" s="20" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="21">
@@ -6049,35 +6059,37 @@
         <v>252</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="21">
-      <c r="A291" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" s="65" customFormat="1" ht="14.4">
+      <c r="A291" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="B291" s="13" t="s">
+      <c r="B291" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="C291" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C291" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D291" s="66"/>
+      <c r="F291" s="66"/>
     </row>
     <row r="292" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A292" s="6" t="s">
         <v>248</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C292" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D292" s="22" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F292" s="23"/>
     </row>
@@ -6089,10 +6101,10 @@
         <v>254</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="21">
@@ -6103,13 +6115,13 @@
         <v>255</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F294" s="20" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="21">
@@ -6120,10 +6132,10 @@
         <v>256</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D295" s="20" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="296" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6131,13 +6143,13 @@
         <v>248</v>
       </c>
       <c r="B296" s="31" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C296" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D296" s="36" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F296" s="32"/>
     </row>
@@ -6171,10 +6183,10 @@
         <v>259</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D299" s="20" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="300" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6185,10 +6197,10 @@
         <v>260</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D300" s="22" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F300" s="23"/>
     </row>
@@ -6200,10 +6212,10 @@
         <v>261</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D301" s="20" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="21">
@@ -6222,13 +6234,13 @@
         <v>248</v>
       </c>
       <c r="B303" s="31" t="s">
-        <v>573</v>
+        <v>603</v>
       </c>
       <c r="C303" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D303" s="36" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F303" s="32"/>
     </row>
@@ -6251,29 +6263,31 @@
         <v>264</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D305" s="20" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" ht="21">
-      <c r="A306" s="3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A306" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B306" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="C306" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B306" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="C306" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D306" s="23"/>
+      <c r="F306" s="23"/>
     </row>
     <row r="307" spans="1:6" ht="21">
       <c r="A307" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>2</v>
@@ -6284,29 +6298,31 @@
         <v>248</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="21">
-      <c r="A309" s="3" t="s">
+    <row r="309" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A309" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B309" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="C309" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B309" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="C309" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D309" s="23"/>
+      <c r="F309" s="23"/>
     </row>
     <row r="310" spans="1:6" ht="21">
       <c r="A310" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>2</v>
@@ -6317,13 +6333,13 @@
         <v>248</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D311" s="20" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6331,7 +6347,7 @@
         <v>248</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -6342,13 +6358,13 @@
         <v>248</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D313" s="20" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="21">
@@ -6356,13 +6372,13 @@
         <v>248</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="315" spans="1:6" ht="21">
@@ -6370,10 +6386,13 @@
         <v>248</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>2</v>
+        <v>419</v>
+      </c>
+      <c r="D315" s="20" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="316" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6381,7 +6400,7 @@
         <v>248</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C316" s="6" t="s">
         <v>2</v>
@@ -6394,7 +6413,7 @@
         <v>248</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -6405,7 +6424,7 @@
         <v>248</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -6416,13 +6435,13 @@
         <v>248</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="D319" s="23" t="s">
-        <v>582</v>
+        <v>419</v>
+      </c>
+      <c r="D319" s="22" t="s">
+        <v>579</v>
       </c>
       <c r="F319" s="23"/>
     </row>
@@ -6431,7 +6450,7 @@
         <v>248</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6442,7 +6461,7 @@
         <v>248</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -6453,7 +6472,7 @@
         <v>248</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -6464,16 +6483,16 @@
         <v>248</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D323" s="16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="F323" s="57" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="21">
@@ -6481,13 +6500,13 @@
         <v>248</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D324" s="20" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6495,13 +6514,13 @@
         <v>248</v>
       </c>
       <c r="B325" s="31" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C325" s="30" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D325" s="36" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F325" s="32"/>
     </row>
@@ -6515,38 +6534,38 @@
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D328" s="21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="21">
       <c r="A329" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D329" s="16" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A330" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C330" s="6" t="s">
         <v>2</v>
@@ -6556,38 +6575,38 @@
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D331" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="21">
       <c r="A332" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D332" s="16" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A333" s="6" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C333" s="6" t="s">
         <v>2</v>
@@ -6597,10 +6616,10 @@
     </row>
     <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>2</v>
@@ -6608,10 +6627,10 @@
     </row>
     <row r="335" spans="1:6" ht="21">
       <c r="A335" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>2</v>
@@ -6619,50 +6638,52 @@
     </row>
     <row r="336" spans="1:6" ht="21">
       <c r="A336" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D336" s="20" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="337" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A337" s="5" t="s">
-        <v>533</v>
+      <c r="A337" s="6" t="s">
+        <v>531</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D337" s="22" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F337" s="23"/>
     </row>
-    <row r="338" spans="1:6" ht="21">
+    <row r="338" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A338" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="B338" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C338" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="B338" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C338" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D338" s="23"/>
+      <c r="F338" s="23"/>
     </row>
     <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>2</v>
@@ -6670,35 +6691,36 @@
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:6" ht="21">
+    <row r="341" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A341" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="B341" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="C341" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D341" s="20" t="s">
-        <v>523</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="B341" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C341" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="D341" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="F341" s="23"/>
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6706,25 +6728,25 @@
     </row>
     <row r="343" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A343" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C343" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D343" s="52" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F343" s="23"/>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6732,19 +6754,19 @@
     </row>
     <row r="345" spans="1:6" ht="21">
       <c r="A345" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D345" s="20" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F345" s="57" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
@@ -6757,10 +6779,10 @@
     </row>
     <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>2</v>
@@ -6768,10 +6790,10 @@
     </row>
     <row r="349" spans="1:6" ht="21">
       <c r="A349" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B349" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="B349" s="13" t="s">
-        <v>301</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>2</v>
@@ -6779,10 +6801,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6790,10 +6812,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6801,10 +6823,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6812,10 +6834,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6823,10 +6845,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6834,10 +6856,10 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -6845,10 +6867,10 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6856,10 +6878,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6867,10 +6889,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6878,10 +6900,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6889,10 +6911,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6900,10 +6922,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6911,10 +6933,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6922,10 +6944,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6933,10 +6955,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6944,10 +6966,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6955,10 +6977,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6966,10 +6988,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -6977,10 +6999,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -6988,10 +7010,10 @@
     </row>
     <row r="369" spans="1:6" ht="21">
       <c r="A369" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -6999,10 +7021,10 @@
     </row>
     <row r="370" spans="1:6" ht="21">
       <c r="A370" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -7010,10 +7032,10 @@
     </row>
     <row r="371" spans="1:6" ht="21">
       <c r="A371" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -7021,10 +7043,10 @@
     </row>
     <row r="372" spans="1:6" ht="21">
       <c r="A372" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -7032,10 +7054,10 @@
     </row>
     <row r="373" spans="1:6" ht="21">
       <c r="A373" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -7043,10 +7065,10 @@
     </row>
     <row r="374" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A374" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C374" s="6" t="s">
         <v>2</v>
@@ -7056,10 +7078,10 @@
     </row>
     <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -7067,10 +7089,10 @@
     </row>
     <row r="376" spans="1:6" ht="21">
       <c r="A376" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>2</v>
@@ -7078,10 +7100,10 @@
     </row>
     <row r="377" spans="1:6" ht="21">
       <c r="A377" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -7089,10 +7111,10 @@
     </row>
     <row r="378" spans="1:6" ht="21">
       <c r="A378" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -7100,10 +7122,10 @@
     </row>
     <row r="379" spans="1:6" ht="21">
       <c r="A379" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -7111,10 +7133,10 @@
     </row>
     <row r="380" spans="1:6" ht="21">
       <c r="A380" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -7122,10 +7144,10 @@
     </row>
     <row r="381" spans="1:6" ht="21">
       <c r="A381" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -7133,10 +7155,10 @@
     </row>
     <row r="382" spans="1:6" ht="21">
       <c r="A382" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -7144,10 +7166,10 @@
     </row>
     <row r="383" spans="1:6" ht="21">
       <c r="A383" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -7155,10 +7177,10 @@
     </row>
     <row r="384" spans="1:6" ht="21">
       <c r="A384" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -7166,10 +7188,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -7177,10 +7199,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -7188,10 +7210,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -7199,10 +7221,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -7210,10 +7232,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -7221,10 +7243,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -7240,10 +7262,10 @@
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>2</v>
@@ -7251,10 +7273,10 @@
     </row>
     <row r="394" spans="1:3" ht="21">
       <c r="A394" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B394" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="B394" s="13" t="s">
-        <v>345</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>2</v>
@@ -7262,10 +7284,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7273,7 +7295,7 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B396" s="13" t="s">
         <v>77</v>
@@ -7284,10 +7306,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -7295,10 +7317,10 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>2</v>
@@ -7314,21 +7336,21 @@
     </row>
     <row r="401" spans="1:6" ht="21">
       <c r="A401" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B401" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C401" s="35" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="21">
       <c r="A402" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B402" s="13" t="s">
         <v>349</v>
-      </c>
-      <c r="B402" s="13" t="s">
-        <v>351</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>2</v>
@@ -7336,10 +7358,10 @@
     </row>
     <row r="403" spans="1:6" ht="21">
       <c r="A403" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>2</v>
@@ -7347,10 +7369,10 @@
     </row>
     <row r="404" spans="1:6" ht="21">
       <c r="A404" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7358,10 +7380,10 @@
     </row>
     <row r="405" spans="1:6" ht="21">
       <c r="A405" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -7369,21 +7391,21 @@
     </row>
     <row r="406" spans="1:6" ht="21">
       <c r="A406" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="21">
       <c r="A407" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7391,7 +7413,7 @@
     </row>
     <row r="408" spans="1:6" ht="21">
       <c r="A408" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B408" s="13" t="s">
         <v>237</v>
@@ -7402,10 +7424,10 @@
     </row>
     <row r="409" spans="1:6" ht="21">
       <c r="A409" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7413,10 +7435,10 @@
     </row>
     <row r="410" spans="1:6" ht="21">
       <c r="A410" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>2</v>
@@ -7424,10 +7446,10 @@
     </row>
     <row r="411" spans="1:6" ht="21">
       <c r="A411" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7435,10 +7457,10 @@
     </row>
     <row r="412" spans="1:6" ht="21">
       <c r="A412" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7446,10 +7468,10 @@
     </row>
     <row r="413" spans="1:6" ht="21">
       <c r="A413" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7457,10 +7479,10 @@
     </row>
     <row r="414" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A414" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>2</v>
@@ -7470,10 +7492,10 @@
     </row>
     <row r="415" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A415" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B415" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>2</v>
@@ -7483,10 +7505,10 @@
     </row>
     <row r="416" spans="1:6" ht="21">
       <c r="A416" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7494,10 +7516,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7505,10 +7527,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7516,10 +7538,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7527,10 +7549,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7538,10 +7560,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7549,10 +7571,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7560,10 +7582,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7571,10 +7593,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7582,10 +7604,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7593,10 +7615,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7604,10 +7626,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7615,10 +7637,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7626,10 +7648,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7637,10 +7659,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7648,10 +7670,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7659,10 +7681,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7670,10 +7692,10 @@
     </row>
     <row r="433" spans="1:6" ht="21">
       <c r="A433" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7681,10 +7703,10 @@
     </row>
     <row r="434" spans="1:6" ht="21">
       <c r="A434" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7692,10 +7714,10 @@
     </row>
     <row r="435" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A435" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B435" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>2</v>
@@ -7705,10 +7727,10 @@
     </row>
     <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7716,10 +7738,10 @@
     </row>
     <row r="437" spans="1:6" ht="21">
       <c r="A437" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>2</v>
@@ -7727,10 +7749,10 @@
     </row>
     <row r="438" spans="1:6" ht="21">
       <c r="A438" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7738,10 +7760,10 @@
     </row>
     <row r="439" spans="1:6" ht="21">
       <c r="A439" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7749,10 +7771,10 @@
     </row>
     <row r="440" spans="1:6" ht="21">
       <c r="A440" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7760,10 +7782,10 @@
     </row>
     <row r="441" spans="1:6" ht="21">
       <c r="A441" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7771,10 +7793,10 @@
     </row>
     <row r="442" spans="1:6" ht="21">
       <c r="A442" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7782,10 +7804,10 @@
     </row>
     <row r="443" spans="1:6" ht="21">
       <c r="A443" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7793,10 +7815,10 @@
     </row>
     <row r="444" spans="1:6" ht="21">
       <c r="A444" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7804,10 +7826,10 @@
     </row>
     <row r="445" spans="1:6" ht="21">
       <c r="A445" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7815,10 +7837,10 @@
     </row>
     <row r="446" spans="1:6" ht="21">
       <c r="A446" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7826,10 +7848,10 @@
     </row>
     <row r="447" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A447" s="24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B447" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C447" s="24" t="s">
         <v>2</v>
@@ -7839,10 +7861,10 @@
     </row>
     <row r="448" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A448" s="24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B448" s="25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C448" s="24" t="s">
         <v>2</v>
@@ -7852,10 +7874,10 @@
     </row>
     <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>2</v>
@@ -7863,10 +7885,10 @@
     </row>
     <row r="450" spans="1:6" ht="21">
       <c r="A450" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>2</v>
@@ -7874,10 +7896,10 @@
     </row>
     <row r="451" spans="1:6" ht="21">
       <c r="A451" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7885,10 +7907,10 @@
     </row>
     <row r="452" spans="1:6" ht="21">
       <c r="A452" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7896,23 +7918,23 @@
     </row>
     <row r="453" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A453" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D453" s="23"/>
       <c r="F453" s="23"/>
     </row>
     <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7920,10 +7942,10 @@
     </row>
     <row r="455" spans="1:6" ht="21">
       <c r="A455" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C455" s="2" t="s">
         <v>2</v>
@@ -7931,10 +7953,10 @@
     </row>
     <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A456" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>2</v>
@@ -7944,10 +7966,10 @@
     </row>
     <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7955,10 +7977,10 @@
     </row>
     <row r="458" spans="1:6" ht="21">
       <c r="A458" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>2</v>
@@ -7966,10 +7988,10 @@
     </row>
     <row r="459" spans="1:6" ht="21">
       <c r="A459" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -7977,10 +7999,10 @@
     </row>
     <row r="460" spans="1:6" ht="21">
       <c r="A460" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -7997,97 +8019,97 @@
     </row>
     <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C463" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D463" s="16" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="21">
       <c r="A464" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B464" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="B464" s="13" t="s">
-        <v>411</v>
-      </c>
       <c r="C464" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F464" s="57" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="21">
       <c r="A465" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="21">
       <c r="A466" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="21">
       <c r="A467" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="21">
       <c r="A468" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="21">
       <c r="A469" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -8095,44 +8117,44 @@
     </row>
     <row r="470" spans="1:6" ht="21">
       <c r="A470" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D470" s="20" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="471" spans="1:6" ht="21">
       <c r="A471" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D471" s="20" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="472" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A472" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D472" s="22" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F472" s="23"/>
     </row>
@@ -8413,10 +8435,10 @@
     <hyperlink ref="B303" r:id="rId273" display="Largest rectangular Area in Histogram"/>
     <hyperlink ref="B304" r:id="rId274"/>
     <hyperlink ref="B305" r:id="rId275"/>
-    <hyperlink ref="B306" r:id="rId276"/>
+    <hyperlink ref="B306" r:id="rId276" display="Implement Stack using Queue"/>
     <hyperlink ref="B307" r:id="rId277"/>
     <hyperlink ref="B308" r:id="rId278"/>
-    <hyperlink ref="B309" r:id="rId279"/>
+    <hyperlink ref="B309" r:id="rId279" display="Implement Queue using Stack  "/>
     <hyperlink ref="B310" r:id="rId280"/>
     <hyperlink ref="B311" r:id="rId281"/>
     <hyperlink ref="B312" r:id="rId282"/>
@@ -8703,8 +8725,9 @@
     <hyperlink ref="D107" r:id="rId563"/>
     <hyperlink ref="D112" r:id="rId564"/>
     <hyperlink ref="D314" r:id="rId565"/>
+    <hyperlink ref="D315" r:id="rId566"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId566"/>
+  <pageSetup orientation="portrait" r:id="rId567"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
max area of island
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="605">
   <si>
     <t>Topic:</t>
   </si>
@@ -795,9 +795,6 @@
   </si>
   <si>
     <t>Find the next Greater element</t>
-  </si>
-  <si>
-    <t>Arithmetic Expression evaluation</t>
   </si>
   <si>
     <t>Evaluation of Postfix expression</t>
@@ -2139,7 +2136,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2296,13 +2293,6 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
@@ -2622,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F472"/>
+  <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F302" sqref="F302"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C377" sqref="C377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2640,7 +2630,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21">
@@ -2651,10 +2641,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2668,10 +2658,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21">
@@ -2682,10 +2672,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21">
@@ -2696,10 +2686,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21">
@@ -2710,10 +2700,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21">
@@ -2724,10 +2714,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21">
@@ -2738,10 +2728,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
@@ -2752,10 +2742,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>419</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2766,10 +2756,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F12" s="59"/>
     </row>
@@ -2784,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
@@ -2795,10 +2785,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21">
@@ -2809,10 +2799,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="21">
@@ -2823,10 +2813,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F16" s="60"/>
     </row>
@@ -2835,7 +2825,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2849,10 +2839,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2863,13 +2853,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>546</v>
+      </c>
+      <c r="F19" s="57" t="s">
         <v>547</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2880,10 +2870,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F20" s="59"/>
     </row>
@@ -2895,10 +2885,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2909,10 +2899,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2923,10 +2913,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2937,10 +2927,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2951,10 +2941,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2965,10 +2955,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2979,10 +2969,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -3023,13 +3013,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F31" s="26"/>
     </row>
@@ -3038,7 +3028,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -3051,13 +3041,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3065,13 +3055,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F34" s="23"/>
     </row>
@@ -3105,10 +3095,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F37" s="61"/>
     </row>
@@ -3117,13 +3107,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F38" s="29"/>
     </row>
@@ -3132,13 +3122,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
+        <v>531</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="D39" s="53" t="s">
         <v>532</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>533</v>
       </c>
       <c r="F39" s="29"/>
     </row>
@@ -3156,13 +3146,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F42" s="23"/>
     </row>
@@ -3174,10 +3164,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21">
@@ -3199,10 +3189,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -3213,10 +3203,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
@@ -3227,13 +3217,13 @@
         <v>37</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D47" s="36" t="s">
+        <v>573</v>
+      </c>
+      <c r="F47" s="32" t="s">
         <v>574</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -3255,10 +3245,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3269,10 +3259,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3299,10 +3289,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3313,10 +3303,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3327,10 +3317,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3516,7 +3506,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="21">
@@ -3527,10 +3517,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="21">
@@ -3587,10 +3577,10 @@
         <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="21">
@@ -3793,10 +3783,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="21">
@@ -3807,10 +3797,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="21">
@@ -3821,10 +3811,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="21">
@@ -3835,10 +3825,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="21">
@@ -3871,10 +3861,10 @@
         <v>92</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="21">
@@ -3885,10 +3875,10 @@
         <v>93</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="21">
@@ -3910,10 +3900,10 @@
         <v>95</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3924,10 +3914,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F108" s="23"/>
     </row>
@@ -3972,10 +3962,10 @@
         <v>100</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="21">
@@ -4019,7 +4009,7 @@
         <v>104</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="21">
@@ -4041,7 +4031,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D118" s="26"/>
       <c r="F118" s="26"/>
@@ -4054,7 +4044,7 @@
         <v>107</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D119" s="26"/>
       <c r="F119" s="26"/>
@@ -4100,7 +4090,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D123" s="26"/>
       <c r="F123" s="26"/>
@@ -4150,10 +4140,10 @@
         <v>116</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="7" customFormat="1" ht="21">
@@ -4164,10 +4154,10 @@
         <v>117</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F130" s="23"/>
     </row>
@@ -4179,10 +4169,10 @@
         <v>118</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="21">
@@ -4193,10 +4183,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="21">
@@ -4207,10 +4197,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="21">
@@ -4221,10 +4211,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="21">
@@ -4235,10 +4225,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="21">
@@ -4249,10 +4239,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="21">
@@ -4263,10 +4253,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="21">
@@ -4299,7 +4289,7 @@
         <v>127</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D140" s="17"/>
       <c r="F140" s="23"/>
@@ -4325,10 +4315,10 @@
         <v>129</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="21">
@@ -4339,10 +4329,10 @@
         <v>130</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="21">
@@ -4353,10 +4343,10 @@
         <v>131</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="21">
@@ -4367,10 +4357,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4381,10 +4371,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4446,7 +4436,7 @@
         <v>2</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="21">
@@ -4454,13 +4444,13 @@
         <v>115</v>
       </c>
       <c r="B152" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D152" s="20" t="s">
         <v>443</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D152" s="20" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="153" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4468,10 +4458,10 @@
         <v>115</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C153" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D153" s="32"/>
       <c r="F153" s="32"/>
@@ -4484,27 +4474,27 @@
         <v>139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="155" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A155" s="30" t="s">
+        <v>466</v>
+      </c>
+      <c r="B155" s="31" t="s">
         <v>467</v>
       </c>
-      <c r="B155" s="31" t="s">
+      <c r="C155" s="30" t="s">
         <v>468</v>
       </c>
-      <c r="C155" s="30" t="s">
+      <c r="D155" s="36" t="s">
         <v>469</v>
       </c>
-      <c r="D155" s="36" t="s">
+      <c r="F155" s="38" t="s">
         <v>470</v>
-      </c>
-      <c r="F155" s="38" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4512,13 +4502,13 @@
         <v>115</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F156" s="32"/>
     </row>
@@ -4527,13 +4517,13 @@
         <v>115</v>
       </c>
       <c r="B157" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D157" s="20" t="s">
         <v>463</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D157" s="20" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="21">
@@ -4563,13 +4553,13 @@
         <v>115</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D160" s="34" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F160" s="61"/>
     </row>
@@ -4581,10 +4571,10 @@
         <v>142</v>
       </c>
       <c r="C161" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D161" s="20" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="21">
@@ -4595,10 +4585,10 @@
         <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="21">
@@ -4607,16 +4597,16 @@
     </row>
     <row r="165" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A165" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="B165" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="B165" s="7" t="s">
-        <v>484</v>
-      </c>
       <c r="C165" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F165" s="23"/>
     </row>
@@ -4628,10 +4618,10 @@
         <v>145</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="21">
@@ -4639,13 +4629,13 @@
         <v>144</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="21">
@@ -4656,10 +4646,10 @@
         <v>146</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="21">
@@ -4670,10 +4660,10 @@
         <v>147</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="21">
@@ -4684,10 +4674,10 @@
         <v>148</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="21">
@@ -4698,10 +4688,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="21">
@@ -4712,10 +4702,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="21">
@@ -4726,10 +4716,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="21">
@@ -4740,10 +4730,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="21">
@@ -4776,10 +4766,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="21">
@@ -4790,10 +4780,10 @@
         <v>156</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="21">
@@ -4812,13 +4802,13 @@
         <v>144</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F180" s="32"/>
     </row>
@@ -4838,13 +4828,13 @@
         <v>144</v>
       </c>
       <c r="B182" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D182" s="20" t="s">
         <v>494</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D182" s="20" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="21">
@@ -4866,10 +4856,10 @@
         <v>160</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="21">
@@ -4888,13 +4878,13 @@
         <v>144</v>
       </c>
       <c r="B186" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D186" s="20" t="s">
         <v>509</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D186" s="20" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="21">
@@ -4940,10 +4930,10 @@
         <v>165</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D190" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="21">
@@ -4986,13 +4976,13 @@
         <v>144</v>
       </c>
       <c r="B194" s="37" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C194" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D194" s="32" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F194" s="32"/>
     </row>
@@ -5012,13 +5002,13 @@
         <v>144</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D196" s="23" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F196" s="23"/>
     </row>
@@ -5027,13 +5017,13 @@
         <v>144</v>
       </c>
       <c r="B197" s="39" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="21">
@@ -5086,13 +5076,13 @@
         <v>173</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D203" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="204" spans="1:6" ht="21">
@@ -5100,13 +5090,13 @@
         <v>173</v>
       </c>
       <c r="B204" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D204" s="20" t="s">
         <v>502</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D204" s="20" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="21">
@@ -5114,13 +5104,13 @@
         <v>173</v>
       </c>
       <c r="B205" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D205" s="20" t="s">
         <v>504</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D205" s="20" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="21">
@@ -5142,10 +5132,10 @@
         <v>175</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D207" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="21">
@@ -5156,10 +5146,10 @@
         <v>176</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D208" s="20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="21">
@@ -5170,10 +5160,10 @@
         <v>177</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D209" s="20" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="21">
@@ -5195,10 +5185,10 @@
         <v>179</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D211" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="21">
@@ -5239,7 +5229,7 @@
         <v>173</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C215" s="6" t="s">
         <v>2</v>
@@ -5255,10 +5245,10 @@
         <v>183</v>
       </c>
       <c r="C216" s="43" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D216" s="44" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F216" s="62"/>
     </row>
@@ -5270,10 +5260,10 @@
         <v>184</v>
       </c>
       <c r="C217" s="48" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D217" s="49" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F217" s="63"/>
     </row>
@@ -5307,10 +5297,10 @@
         <v>187</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D220" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="21">
@@ -5366,11 +5356,11 @@
         <v>192</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D225" s="23"/>
       <c r="F225" s="23" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="21">
@@ -5917,13 +5907,13 @@
         <v>229</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D277" s="22" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F277" s="23"/>
     </row>
@@ -6020,10 +6010,10 @@
         <v>249</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D287" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="21">
@@ -6034,10 +6024,10 @@
         <v>250</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D288" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="21">
@@ -6048,10 +6038,10 @@
         <v>251</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D289" s="20" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="21">
@@ -6062,37 +6052,37 @@
         <v>252</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" s="65" customFormat="1" ht="14.4">
-      <c r="A291" s="64" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A291" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B291" s="65" t="s">
+      <c r="B291" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="C291" s="64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D291" s="66"/>
-      <c r="F291" s="66"/>
+      <c r="C291" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D291" s="32"/>
+      <c r="F291" s="32"/>
     </row>
     <row r="292" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A292" s="6" t="s">
         <v>248</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C292" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D292" s="22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F292" s="23"/>
     </row>
@@ -6104,10 +6094,10 @@
         <v>254</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D293" s="20" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="294" spans="1:6" ht="21">
@@ -6118,13 +6108,13 @@
         <v>255</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F294" s="20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="21">
@@ -6135,10 +6125,10 @@
         <v>256</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D295" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="296" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6146,13 +6136,13 @@
         <v>248</v>
       </c>
       <c r="B296" s="31" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C296" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D296" s="36" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F296" s="32"/>
     </row>
@@ -6164,7 +6154,10 @@
         <v>257</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D297" s="20" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="298" spans="1:6" ht="21">
@@ -6175,40 +6168,40 @@
         <v>258</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D298" s="20" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6" ht="21">
-      <c r="A299" s="3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A299" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B299" s="13" t="s">
+      <c r="B299" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="C299" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D299" s="20" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A300" s="6" t="s">
+      <c r="C299" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D299" s="22" t="s">
+        <v>563</v>
+      </c>
+      <c r="F299" s="23"/>
+    </row>
+    <row r="300" spans="1:6" ht="21">
+      <c r="A300" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B300" s="58" t="s">
+      <c r="B300" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="C300" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D300" s="22" t="s">
+      <c r="C300" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D300" s="20" t="s">
         <v>564</v>
       </c>
-      <c r="F300" s="23"/>
     </row>
     <row r="301" spans="1:6" ht="21">
       <c r="A301" s="3" t="s">
@@ -6218,37 +6211,34 @@
         <v>261</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D301" s="20" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" ht="21">
-      <c r="A302" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A302" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B302" s="13" t="s">
+      <c r="B302" s="31" t="s">
+        <v>602</v>
+      </c>
+      <c r="C302" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D302" s="36" t="s">
+        <v>570</v>
+      </c>
+      <c r="F302" s="32"/>
+    </row>
+    <row r="303" spans="1:6" ht="21">
+      <c r="A303" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B303" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="C302" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A303" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B303" s="31" t="s">
-        <v>603</v>
-      </c>
-      <c r="C303" s="30" t="s">
-        <v>419</v>
-      </c>
-      <c r="D303" s="36" t="s">
-        <v>571</v>
-      </c>
-      <c r="F303" s="32"/>
+      <c r="C303" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="304" spans="1:6" ht="21">
       <c r="A304" s="3" t="s">
@@ -6258,35 +6248,35 @@
         <v>263</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" ht="21">
-      <c r="A305" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D304" s="20" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A305" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B305" s="13" t="s">
+      <c r="B305" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="C305" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D305" s="23"/>
+      <c r="F305" s="23"/>
+    </row>
+    <row r="306" spans="1:6" ht="21">
+      <c r="A306" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B306" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="C305" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D305" s="20" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A306" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B306" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="C306" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D306" s="23"/>
-      <c r="F306" s="23"/>
+      <c r="C306" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="307" spans="1:6" ht="21">
       <c r="A307" s="3" t="s">
@@ -6299,29 +6289,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="21">
-      <c r="A308" s="3" t="s">
+    <row r="308" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A308" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B308" s="13" t="s">
+      <c r="B308" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="C308" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D308" s="23"/>
+      <c r="F308" s="23"/>
+    </row>
+    <row r="309" spans="1:6" ht="21">
+      <c r="A309" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B309" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="C308" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A309" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B309" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="C309" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D309" s="23"/>
-      <c r="F309" s="23"/>
+      <c r="C309" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="310" spans="1:6" ht="21">
       <c r="A310" s="3" t="s">
@@ -6331,7 +6321,10 @@
         <v>267</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D310" s="20" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="21">
@@ -6342,10 +6335,7 @@
         <v>268</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D311" s="20" t="s">
-        <v>577</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6356,7 +6346,10 @@
         <v>269</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D312" s="20" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="313" spans="1:6" ht="21">
@@ -6367,10 +6360,10 @@
         <v>270</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D313" s="20" t="s">
-        <v>578</v>
+        <v>596</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="21">
@@ -6381,38 +6374,35 @@
         <v>271</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" ht="21">
-      <c r="A315" s="3" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A315" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B315" s="13" t="s">
+      <c r="B315" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="C315" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D315" s="23"/>
+      <c r="F315" s="23"/>
+    </row>
+    <row r="316" spans="1:6" ht="21">
+      <c r="A316" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B316" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C315" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D315" s="20" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A316" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B316" s="7" t="s">
-        <v>600</v>
-      </c>
-      <c r="C316" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D316" s="23"/>
-      <c r="F316" s="23"/>
+      <c r="C316" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="317" spans="1:6" ht="21">
       <c r="A317" s="3" t="s">
@@ -6425,31 +6415,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="21">
-      <c r="A318" s="3" t="s">
+    <row r="318" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A318" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B318" s="13" t="s">
+      <c r="B318" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="C318" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D318" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="F318" s="23"/>
+    </row>
+    <row r="319" spans="1:6" ht="21">
+      <c r="A319" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B319" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="C318" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A319" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B319" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="C319" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D319" s="22" t="s">
-        <v>579</v>
-      </c>
-      <c r="F319" s="23"/>
+      <c r="C319" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="320" spans="1:6" ht="21">
       <c r="A320" s="3" t="s">
@@ -6481,7 +6471,13 @@
         <v>277</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D322" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="F322" s="57" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="21">
@@ -6492,137 +6488,131 @@
         <v>278</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D323" s="16" t="s">
-        <v>599</v>
-      </c>
-      <c r="F323" s="57" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" ht="21">
-      <c r="A324" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D323" s="20" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A324" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B324" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C324" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D324" s="20" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A325" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="B325" s="31" t="s">
+      <c r="B324" s="31" t="s">
+        <v>580</v>
+      </c>
+      <c r="C324" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D324" s="36" t="s">
         <v>581</v>
       </c>
-      <c r="C325" s="30" t="s">
-        <v>419</v>
-      </c>
-      <c r="D325" s="36" t="s">
-        <v>582</v>
-      </c>
-      <c r="F325" s="32"/>
+      <c r="F324" s="32"/>
+    </row>
+    <row r="325" spans="1:6" ht="21">
+      <c r="B325" s="4"/>
+      <c r="C325" s="2"/>
     </row>
     <row r="326" spans="1:6" ht="21">
       <c r="B326" s="4"/>
       <c r="C326" s="2"/>
     </row>
     <row r="327" spans="1:6" ht="21">
-      <c r="B327" s="4"/>
-      <c r="C327" s="2"/>
+      <c r="A327" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B327" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D327" s="21" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B328" s="13" t="s">
         <v>280</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D328" s="21" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="329" spans="1:6" ht="21">
-      <c r="A329" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B329" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="D328" s="16" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A329" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B329" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C329" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D329" s="16" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A330" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B330" s="7" t="s">
+      <c r="C329" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D329" s="23"/>
+      <c r="F329" s="23"/>
+    </row>
+    <row r="330" spans="1:6" ht="21">
+      <c r="A330" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B330" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="C330" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D330" s="23"/>
-      <c r="F330" s="23"/>
+      <c r="C330" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D330" s="20" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B331" s="13" t="s">
         <v>283</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D331" s="20" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" ht="21">
-      <c r="A332" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B332" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="D331" s="16" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A332" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B332" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C332" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D332" s="16" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A333" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B333" s="7" t="s">
+      <c r="C332" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D332" s="23"/>
+      <c r="F332" s="23"/>
+    </row>
+    <row r="333" spans="1:6" ht="21">
+      <c r="A333" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B333" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C333" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D333" s="23"/>
-      <c r="F333" s="23"/>
+      <c r="C333" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B334" s="13" t="s">
         <v>286</v>
@@ -6633,60 +6623,60 @@
     </row>
     <row r="335" spans="1:6" ht="21">
       <c r="A335" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B335" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="B335" s="15" t="s">
         <v>287</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" ht="21">
-      <c r="A336" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B336" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="C336" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D336" s="20" t="s">
-        <v>526</v>
-      </c>
+      <c r="D335" s="20" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A336" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B336" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C336" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D336" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="F336" s="23"/>
     </row>
     <row r="337" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A337" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>523</v>
+        <v>288</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D337" s="22" t="s">
-        <v>522</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D337" s="23"/>
       <c r="F337" s="23"/>
     </row>
-    <row r="338" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A338" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B338" s="7" t="s">
+    <row r="338" spans="1:6" ht="21">
+      <c r="A338" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B338" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="C338" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D338" s="23"/>
-      <c r="F338" s="23"/>
+      <c r="C338" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B339" s="13" t="s">
         <v>290</v>
@@ -6695,97 +6685,97 @@
         <v>2</v>
       </c>
     </row>
-    <row r="340" spans="1:6" ht="21">
-      <c r="A340" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B340" s="13" t="s">
+    <row r="340" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A340" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B340" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="C340" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="341" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A341" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="B341" s="7" t="s">
+      <c r="C340" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D340" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="F340" s="23"/>
+    </row>
+    <row r="341" spans="1:6" ht="21">
+      <c r="A341" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B341" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C341" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D341" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F341" s="23"/>
-    </row>
-    <row r="342" spans="1:6" ht="21">
+      <c r="C341" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A342" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B342" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="B342" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C342" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="C342" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D342" s="52" t="s">
+        <v>518</v>
+      </c>
+      <c r="F342" s="23"/>
+    </row>
+    <row r="343" spans="1:6" ht="21">
       <c r="A343" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B343" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B343" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="C343" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D343" s="52" t="s">
-        <v>519</v>
-      </c>
-      <c r="F343" s="23"/>
+      <c r="C343" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B344" s="13" t="s">
         <v>295</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D344" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="F344" s="57" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="345" spans="1:6" ht="21">
-      <c r="A345" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B345" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="C345" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D345" s="20" t="s">
-        <v>524</v>
-      </c>
-      <c r="F345" s="57" t="s">
-        <v>525</v>
-      </c>
+      <c r="B345" s="4"/>
+      <c r="C345" s="2"/>
     </row>
     <row r="346" spans="1:6" ht="21">
       <c r="B346" s="4"/>
       <c r="C346" s="2"/>
     </row>
     <row r="347" spans="1:6" ht="21">
-      <c r="B347" s="4"/>
-      <c r="C347" s="2"/>
+      <c r="A347" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B347" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B348" s="13" t="s">
         <v>298</v>
@@ -6796,7 +6786,7 @@
     </row>
     <row r="349" spans="1:6" ht="21">
       <c r="A349" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B349" s="13" t="s">
         <v>299</v>
@@ -6807,7 +6797,7 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B350" s="13" t="s">
         <v>300</v>
@@ -6818,7 +6808,7 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B351" s="13" t="s">
         <v>301</v>
@@ -6829,7 +6819,7 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B352" s="13" t="s">
         <v>302</v>
@@ -6840,7 +6830,7 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B353" s="13" t="s">
         <v>303</v>
@@ -6851,18 +6841,18 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B354" s="13" t="s">
         <v>304</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B355" s="13" t="s">
         <v>305</v>
@@ -6873,7 +6863,7 @@
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B356" s="13" t="s">
         <v>306</v>
@@ -6884,7 +6874,7 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B357" s="13" t="s">
         <v>307</v>
@@ -6895,7 +6885,7 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B358" s="13" t="s">
         <v>308</v>
@@ -6906,7 +6896,7 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B359" s="13" t="s">
         <v>309</v>
@@ -6917,7 +6907,7 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B360" s="13" t="s">
         <v>310</v>
@@ -6928,7 +6918,7 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B361" s="13" t="s">
         <v>311</v>
@@ -6939,7 +6929,7 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B362" s="13" t="s">
         <v>312</v>
@@ -6950,7 +6940,7 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B363" s="13" t="s">
         <v>313</v>
@@ -6961,7 +6951,7 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B364" s="13" t="s">
         <v>314</v>
@@ -6972,7 +6962,7 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B365" s="13" t="s">
         <v>315</v>
@@ -6983,7 +6973,7 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B366" s="13" t="s">
         <v>316</v>
@@ -6994,7 +6984,7 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B367" s="13" t="s">
         <v>317</v>
@@ -7005,7 +6995,7 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B368" s="13" t="s">
         <v>318</v>
@@ -7016,7 +7006,7 @@
     </row>
     <row r="369" spans="1:6" ht="21">
       <c r="A369" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B369" s="13" t="s">
         <v>319</v>
@@ -7027,7 +7017,7 @@
     </row>
     <row r="370" spans="1:6" ht="21">
       <c r="A370" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B370" s="13" t="s">
         <v>320</v>
@@ -7038,7 +7028,7 @@
     </row>
     <row r="371" spans="1:6" ht="21">
       <c r="A371" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B371" s="13" t="s">
         <v>321</v>
@@ -7049,7 +7039,7 @@
     </row>
     <row r="372" spans="1:6" ht="21">
       <c r="A372" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B372" s="13" t="s">
         <v>322</v>
@@ -7058,33 +7048,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="21">
-      <c r="A373" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B373" s="13" t="s">
+    <row r="373" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A373" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B373" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C373" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A374" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="B374" s="7" t="s">
+      <c r="C373" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D373" s="23"/>
+      <c r="F373" s="23"/>
+    </row>
+    <row r="374" spans="1:6" ht="21">
+      <c r="A374" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B374" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="C374" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D374" s="23"/>
-      <c r="F374" s="23"/>
+      <c r="C374" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B375" s="13" t="s">
         <v>325</v>
@@ -7095,7 +7085,7 @@
     </row>
     <row r="376" spans="1:6" ht="21">
       <c r="A376" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B376" s="13" t="s">
         <v>326</v>
@@ -7106,7 +7096,7 @@
     </row>
     <row r="377" spans="1:6" ht="21">
       <c r="A377" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B377" s="13" t="s">
         <v>327</v>
@@ -7117,7 +7107,7 @@
     </row>
     <row r="378" spans="1:6" ht="21">
       <c r="A378" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B378" s="13" t="s">
         <v>328</v>
@@ -7128,7 +7118,7 @@
     </row>
     <row r="379" spans="1:6" ht="21">
       <c r="A379" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B379" s="13" t="s">
         <v>329</v>
@@ -7139,7 +7129,7 @@
     </row>
     <row r="380" spans="1:6" ht="21">
       <c r="A380" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B380" s="13" t="s">
         <v>330</v>
@@ -7150,7 +7140,7 @@
     </row>
     <row r="381" spans="1:6" ht="21">
       <c r="A381" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B381" s="13" t="s">
         <v>331</v>
@@ -7161,7 +7151,7 @@
     </row>
     <row r="382" spans="1:6" ht="21">
       <c r="A382" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B382" s="13" t="s">
         <v>332</v>
@@ -7172,7 +7162,7 @@
     </row>
     <row r="383" spans="1:6" ht="21">
       <c r="A383" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B383" s="13" t="s">
         <v>333</v>
@@ -7183,7 +7173,7 @@
     </row>
     <row r="384" spans="1:6" ht="21">
       <c r="A384" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B384" s="13" t="s">
         <v>334</v>
@@ -7194,7 +7184,7 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B385" s="13" t="s">
         <v>335</v>
@@ -7205,7 +7195,7 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B386" s="13" t="s">
         <v>336</v>
@@ -7216,7 +7206,7 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B387" s="13" t="s">
         <v>337</v>
@@ -7227,7 +7217,7 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B388" s="13" t="s">
         <v>338</v>
@@ -7238,7 +7228,7 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B389" s="13" t="s">
         <v>339</v>
@@ -7248,27 +7238,27 @@
       </c>
     </row>
     <row r="390" spans="1:3" ht="21">
-      <c r="A390" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B390" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="C390" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B390" s="4"/>
+      <c r="C390" s="2"/>
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="B391" s="4"/>
       <c r="C391" s="2"/>
     </row>
     <row r="392" spans="1:3" ht="21">
-      <c r="B392" s="4"/>
-      <c r="C392" s="2"/>
+      <c r="A392" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B392" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B393" s="13" t="s">
         <v>342</v>
@@ -7279,7 +7269,7 @@
     </row>
     <row r="394" spans="1:3" ht="21">
       <c r="A394" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B394" s="13" t="s">
         <v>343</v>
@@ -7290,10 +7280,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>344</v>
+        <v>77</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7301,10 +7291,10 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>77</v>
+        <v>344</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -7312,7 +7302,7 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B397" s="13" t="s">
         <v>345</v>
@@ -7322,38 +7312,38 @@
       </c>
     </row>
     <row r="398" spans="1:3" ht="21">
-      <c r="A398" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B398" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C398" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B398" s="4"/>
+      <c r="C398" s="2"/>
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="B399" s="4"/>
       <c r="C399" s="2"/>
     </row>
     <row r="400" spans="1:3" ht="21">
-      <c r="B400" s="4"/>
-      <c r="C400" s="2"/>
+      <c r="A400" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B400" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C400" s="35" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="401" spans="1:6" ht="21">
       <c r="A401" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B401" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C401" s="35" t="s">
-        <v>419</v>
+      <c r="C401" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="21">
       <c r="A402" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B402" s="13" t="s">
         <v>349</v>
@@ -7364,7 +7354,7 @@
     </row>
     <row r="403" spans="1:6" ht="21">
       <c r="A403" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B403" s="13" t="s">
         <v>350</v>
@@ -7375,7 +7365,7 @@
     </row>
     <row r="404" spans="1:6" ht="21">
       <c r="A404" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B404" s="13" t="s">
         <v>351</v>
@@ -7386,32 +7376,32 @@
     </row>
     <row r="405" spans="1:6" ht="21">
       <c r="A405" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B405" s="13" t="s">
         <v>352</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="21">
       <c r="A406" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B406" s="13" t="s">
         <v>353</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>419</v>
+        <v>2</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="21">
       <c r="A407" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>354</v>
+        <v>237</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7419,10 +7409,10 @@
     </row>
     <row r="408" spans="1:6" ht="21">
       <c r="A408" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>237</v>
+        <v>354</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>2</v>
@@ -7430,7 +7420,7 @@
     </row>
     <row r="409" spans="1:6" ht="21">
       <c r="A409" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B409" s="13" t="s">
         <v>355</v>
@@ -7441,7 +7431,7 @@
     </row>
     <row r="410" spans="1:6" ht="21">
       <c r="A410" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B410" s="13" t="s">
         <v>356</v>
@@ -7452,7 +7442,7 @@
     </row>
     <row r="411" spans="1:6" ht="21">
       <c r="A411" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B411" s="13" t="s">
         <v>357</v>
@@ -7463,7 +7453,7 @@
     </row>
     <row r="412" spans="1:6" ht="21">
       <c r="A412" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B412" s="13" t="s">
         <v>358</v>
@@ -7472,20 +7462,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="21">
-      <c r="A413" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B413" s="13" t="s">
+    <row r="413" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A413" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B413" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="C413" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C413" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D413" s="23"/>
+      <c r="F413" s="23"/>
     </row>
     <row r="414" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A414" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B414" s="7" t="s">
         <v>360</v>
@@ -7496,22 +7488,20 @@
       <c r="D414" s="23"/>
       <c r="F414" s="23"/>
     </row>
-    <row r="415" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A415" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B415" s="7" t="s">
+    <row r="415" spans="1:6" ht="21">
+      <c r="A415" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B415" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C415" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D415" s="23"/>
-      <c r="F415" s="23"/>
+      <c r="C415" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="416" spans="1:6" ht="21">
       <c r="A416" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B416" s="13" t="s">
         <v>362</v>
@@ -7522,7 +7512,7 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B417" s="13" t="s">
         <v>363</v>
@@ -7533,7 +7523,7 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B418" s="13" t="s">
         <v>364</v>
@@ -7544,7 +7534,7 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B419" s="13" t="s">
         <v>365</v>
@@ -7555,7 +7545,7 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B420" s="13" t="s">
         <v>366</v>
@@ -7566,7 +7556,7 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B421" s="13" t="s">
         <v>367</v>
@@ -7577,7 +7567,7 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B422" s="13" t="s">
         <v>368</v>
@@ -7588,7 +7578,7 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B423" s="13" t="s">
         <v>369</v>
@@ -7599,7 +7589,7 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B424" s="13" t="s">
         <v>370</v>
@@ -7610,7 +7600,7 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B425" s="13" t="s">
         <v>371</v>
@@ -7621,7 +7611,7 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B426" s="13" t="s">
         <v>372</v>
@@ -7632,7 +7622,7 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B427" s="13" t="s">
         <v>373</v>
@@ -7643,7 +7633,7 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B428" s="13" t="s">
         <v>374</v>
@@ -7654,7 +7644,7 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B429" s="13" t="s">
         <v>375</v>
@@ -7665,7 +7655,7 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B430" s="13" t="s">
         <v>376</v>
@@ -7676,7 +7666,7 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B431" s="13" t="s">
         <v>377</v>
@@ -7687,7 +7677,7 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B432" s="13" t="s">
         <v>378</v>
@@ -7698,7 +7688,7 @@
     </row>
     <row r="433" spans="1:6" ht="21">
       <c r="A433" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B433" s="13" t="s">
         <v>379</v>
@@ -7707,33 +7697,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="21">
-      <c r="A434" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B434" s="13" t="s">
+    <row r="434" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A434" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B434" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="C434" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="435" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A435" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B435" s="7" t="s">
+      <c r="C434" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D434" s="23"/>
+      <c r="F434" s="23"/>
+    </row>
+    <row r="435" spans="1:6" ht="21">
+      <c r="A435" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B435" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="C435" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D435" s="23"/>
-      <c r="F435" s="23"/>
+      <c r="C435" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B436" s="13" t="s">
         <v>382</v>
@@ -7744,7 +7734,7 @@
     </row>
     <row r="437" spans="1:6" ht="21">
       <c r="A437" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B437" s="13" t="s">
         <v>383</v>
@@ -7755,7 +7745,7 @@
     </row>
     <row r="438" spans="1:6" ht="21">
       <c r="A438" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B438" s="13" t="s">
         <v>384</v>
@@ -7766,7 +7756,7 @@
     </row>
     <row r="439" spans="1:6" ht="21">
       <c r="A439" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B439" s="13" t="s">
         <v>385</v>
@@ -7777,7 +7767,7 @@
     </row>
     <row r="440" spans="1:6" ht="21">
       <c r="A440" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B440" s="13" t="s">
         <v>386</v>
@@ -7788,7 +7778,7 @@
     </row>
     <row r="441" spans="1:6" ht="21">
       <c r="A441" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B441" s="13" t="s">
         <v>387</v>
@@ -7799,7 +7789,7 @@
     </row>
     <row r="442" spans="1:6" ht="21">
       <c r="A442" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B442" s="13" t="s">
         <v>388</v>
@@ -7810,7 +7800,7 @@
     </row>
     <row r="443" spans="1:6" ht="21">
       <c r="A443" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B443" s="13" t="s">
         <v>389</v>
@@ -7821,7 +7811,7 @@
     </row>
     <row r="444" spans="1:6" ht="21">
       <c r="A444" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B444" s="13" t="s">
         <v>390</v>
@@ -7832,7 +7822,7 @@
     </row>
     <row r="445" spans="1:6" ht="21">
       <c r="A445" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B445" s="13" t="s">
         <v>391</v>
@@ -7841,20 +7831,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="21">
-      <c r="A446" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B446" s="13" t="s">
+    <row r="446" spans="1:6" s="25" customFormat="1" ht="21">
+      <c r="A446" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B446" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="C446" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C446" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D446" s="26"/>
+      <c r="F446" s="26"/>
     </row>
     <row r="447" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A447" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B447" s="25" t="s">
         <v>393</v>
@@ -7865,22 +7857,20 @@
       <c r="D447" s="26"/>
       <c r="F447" s="26"/>
     </row>
-    <row r="448" spans="1:6" s="25" customFormat="1" ht="21">
-      <c r="A448" s="24" t="s">
-        <v>347</v>
-      </c>
-      <c r="B448" s="25" t="s">
+    <row r="448" spans="1:6" ht="21">
+      <c r="A448" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B448" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="C448" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D448" s="26"/>
-      <c r="F448" s="26"/>
+      <c r="C448" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B449" s="13" t="s">
         <v>395</v>
@@ -7891,7 +7881,7 @@
     </row>
     <row r="450" spans="1:6" ht="21">
       <c r="A450" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B450" s="13" t="s">
         <v>396</v>
@@ -7902,7 +7892,7 @@
     </row>
     <row r="451" spans="1:6" ht="21">
       <c r="A451" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B451" s="13" t="s">
         <v>397</v>
@@ -7911,33 +7901,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="21">
-      <c r="A452" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B452" s="13" t="s">
+    <row r="452" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A452" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B452" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="C452" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="453" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A453" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B453" s="7" t="s">
+      <c r="C452" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D452" s="23"/>
+      <c r="F452" s="23"/>
+    </row>
+    <row r="453" spans="1:6" ht="21">
+      <c r="A453" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B453" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="C453" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D453" s="23"/>
-      <c r="F453" s="23"/>
+      <c r="C453" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B454" s="13" t="s">
         <v>400</v>
@@ -7946,33 +7936,33 @@
         <v>2</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="21">
-      <c r="A455" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B455" s="13" t="s">
+    <row r="455" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A455" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B455" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="C455" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A456" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B456" s="7" t="s">
+      <c r="C455" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D455" s="23"/>
+      <c r="F455" s="23"/>
+    </row>
+    <row r="456" spans="1:6" ht="21">
+      <c r="A456" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B456" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="C456" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D456" s="23"/>
-      <c r="F456" s="23"/>
+      <c r="C456" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B457" s="13" t="s">
         <v>403</v>
@@ -7983,7 +7973,7 @@
     </row>
     <row r="458" spans="1:6" ht="21">
       <c r="A458" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B458" s="13" t="s">
         <v>404</v>
@@ -7994,7 +7984,7 @@
     </row>
     <row r="459" spans="1:6" ht="21">
       <c r="A459" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B459" s="13" t="s">
         <v>405</v>
@@ -8004,79 +7994,82 @@
       </c>
     </row>
     <row r="460" spans="1:6" ht="21">
-      <c r="A460" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="B460" s="13" t="s">
-        <v>406</v>
-      </c>
-      <c r="C460" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B460" s="4"/>
+      <c r="C460" s="2"/>
     </row>
     <row r="461" spans="1:6" ht="21">
+      <c r="A461" s="5"/>
       <c r="B461" s="4"/>
       <c r="C461" s="2"/>
     </row>
     <row r="462" spans="1:6" ht="21">
-      <c r="A462" s="5"/>
-      <c r="B462" s="4"/>
-      <c r="C462" s="2"/>
+      <c r="A462" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B462" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="C462" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D462" s="16" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B463" s="13" t="s">
         <v>408</v>
       </c>
       <c r="C463" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D463" s="16" t="s">
-        <v>519</v>
+        <v>418</v>
+      </c>
+      <c r="D463" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="F463" s="57" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="21">
       <c r="A464" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B464" s="13" t="s">
         <v>409</v>
       </c>
       <c r="C464" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>588</v>
-      </c>
-      <c r="F464" s="57" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="21">
       <c r="A465" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B465" s="13" t="s">
         <v>410</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="21">
       <c r="A466" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B466" s="13" t="s">
         <v>411</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D466" s="20" t="s">
         <v>583</v>
@@ -8084,85 +8077,71 @@
     </row>
     <row r="467" spans="1:6" ht="21">
       <c r="A467" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B467" s="13" t="s">
         <v>412</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="21">
       <c r="A468" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B468" s="13" t="s">
         <v>413</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D468" s="20" t="s">
-        <v>587</v>
+        <v>2</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="21">
       <c r="A469" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B469" s="13" t="s">
         <v>414</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D469" s="20" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="470" spans="1:6" ht="21">
       <c r="A470" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B470" s="13" t="s">
         <v>415</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D470" s="20" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="471" spans="1:6" ht="21">
-      <c r="A471" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="B471" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="C471" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D471" s="20" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="472" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A472" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="B472" s="7" t="s">
-        <v>586</v>
-      </c>
-      <c r="C472" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="D472" s="22" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A471" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="B471" s="7" t="s">
         <v>585</v>
       </c>
-      <c r="F472" s="23"/>
+      <c r="C471" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D471" s="22" t="s">
+        <v>584</v>
+      </c>
+      <c r="F471" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8432,34 +8411,34 @@
     <hyperlink ref="B294" r:id="rId264"/>
     <hyperlink ref="B295" r:id="rId265"/>
     <hyperlink ref="B296" r:id="rId266" display="The celebrity Problem"/>
-    <hyperlink ref="B297" r:id="rId267" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B297" r:id="rId267"/>
     <hyperlink ref="B298" r:id="rId268"/>
     <hyperlink ref="B299" r:id="rId269"/>
     <hyperlink ref="B300" r:id="rId270"/>
     <hyperlink ref="B301" r:id="rId271"/>
-    <hyperlink ref="B302" r:id="rId272"/>
-    <hyperlink ref="B303" r:id="rId273" display="Largest rectangular Area in Histogram"/>
+    <hyperlink ref="B302" r:id="rId272" display="Largest rectangular Area in Histogram"/>
+    <hyperlink ref="B303" r:id="rId273"/>
     <hyperlink ref="B304" r:id="rId274"/>
-    <hyperlink ref="B305" r:id="rId275"/>
-    <hyperlink ref="B306" r:id="rId276" display="Implement Stack using Queue"/>
+    <hyperlink ref="B305" r:id="rId275" display="Implement Stack using Queue"/>
+    <hyperlink ref="B306" r:id="rId276"/>
     <hyperlink ref="B307" r:id="rId277"/>
-    <hyperlink ref="B308" r:id="rId278"/>
-    <hyperlink ref="B309" r:id="rId279" display="Implement Queue using Stack  "/>
+    <hyperlink ref="B308" r:id="rId278" display="Implement Queue using Stack  "/>
+    <hyperlink ref="B309" r:id="rId279"/>
     <hyperlink ref="B310" r:id="rId280"/>
     <hyperlink ref="B311" r:id="rId281"/>
     <hyperlink ref="B312" r:id="rId282"/>
     <hyperlink ref="B313" r:id="rId283"/>
     <hyperlink ref="B314" r:id="rId284"/>
-    <hyperlink ref="B315" r:id="rId285"/>
-    <hyperlink ref="B316" r:id="rId286" display="Find the first circular tour that visits all Petrol Pumps"/>
+    <hyperlink ref="B315" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps"/>
+    <hyperlink ref="B316" r:id="rId286"/>
     <hyperlink ref="B317" r:id="rId287"/>
-    <hyperlink ref="B318" r:id="rId288"/>
-    <hyperlink ref="B319" r:id="rId289" display="First negative integer in every window of size “k”"/>
+    <hyperlink ref="B318" r:id="rId288" display="First negative integer in every window of size “k”"/>
+    <hyperlink ref="B319" r:id="rId289"/>
     <hyperlink ref="B320" r:id="rId290"/>
     <hyperlink ref="B321" r:id="rId291"/>
     <hyperlink ref="B322" r:id="rId292"/>
-    <hyperlink ref="B323" r:id="rId293"/>
-    <hyperlink ref="B325" r:id="rId294" display="Next Smaller Element"/>
+    <hyperlink ref="B324" r:id="rId293" display="Next Smaller Element"/>
+    <hyperlink ref="B327" r:id="rId294"/>
     <hyperlink ref="B328" r:id="rId295"/>
     <hyperlink ref="B329" r:id="rId296"/>
     <hyperlink ref="B330" r:id="rId297"/>
@@ -8468,8 +8447,8 @@
     <hyperlink ref="B333" r:id="rId300"/>
     <hyperlink ref="B334" r:id="rId301"/>
     <hyperlink ref="B335" r:id="rId302"/>
-    <hyperlink ref="B336" r:id="rId303"/>
-    <hyperlink ref="B337" r:id="rId304" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
+    <hyperlink ref="B336" r:id="rId303" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
+    <hyperlink ref="B337" r:id="rId304"/>
     <hyperlink ref="B338" r:id="rId305"/>
     <hyperlink ref="B339" r:id="rId306"/>
     <hyperlink ref="B340" r:id="rId307"/>
@@ -8477,7 +8456,7 @@
     <hyperlink ref="B342" r:id="rId309"/>
     <hyperlink ref="B343" r:id="rId310"/>
     <hyperlink ref="B344" r:id="rId311"/>
-    <hyperlink ref="B345" r:id="rId312"/>
+    <hyperlink ref="B348" r:id="rId312"/>
     <hyperlink ref="B349" r:id="rId313"/>
     <hyperlink ref="B350" r:id="rId314"/>
     <hyperlink ref="B351" r:id="rId315"/>
@@ -8499,8 +8478,8 @@
     <hyperlink ref="B367" r:id="rId331"/>
     <hyperlink ref="B368" r:id="rId332"/>
     <hyperlink ref="B369" r:id="rId333"/>
-    <hyperlink ref="B370" r:id="rId334"/>
-    <hyperlink ref="B371" r:id="rId335" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B370" r:id="rId334" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B371" r:id="rId335"/>
     <hyperlink ref="B372" r:id="rId336"/>
     <hyperlink ref="B373" r:id="rId337"/>
     <hyperlink ref="B374" r:id="rId338"/>
@@ -8514,18 +8493,18 @@
     <hyperlink ref="B382" r:id="rId346"/>
     <hyperlink ref="B383" r:id="rId347"/>
     <hyperlink ref="B384" r:id="rId348"/>
-    <hyperlink ref="B385" r:id="rId349"/>
-    <hyperlink ref="B387" r:id="rId350"/>
-    <hyperlink ref="B386" r:id="rId351"/>
+    <hyperlink ref="B386" r:id="rId349"/>
+    <hyperlink ref="B385" r:id="rId350"/>
+    <hyperlink ref="B387" r:id="rId351"/>
     <hyperlink ref="B388" r:id="rId352"/>
     <hyperlink ref="B389" r:id="rId353"/>
-    <hyperlink ref="B390" r:id="rId354"/>
+    <hyperlink ref="B392" r:id="rId354"/>
     <hyperlink ref="B393" r:id="rId355"/>
     <hyperlink ref="B394" r:id="rId356"/>
     <hyperlink ref="B395" r:id="rId357"/>
     <hyperlink ref="B396" r:id="rId358"/>
     <hyperlink ref="B397" r:id="rId359"/>
-    <hyperlink ref="B398" r:id="rId360"/>
+    <hyperlink ref="B400" r:id="rId360"/>
     <hyperlink ref="B401" r:id="rId361"/>
     <hyperlink ref="B402" r:id="rId362"/>
     <hyperlink ref="B403" r:id="rId363"/>
@@ -8565,9 +8544,9 @@
     <hyperlink ref="B437" r:id="rId397"/>
     <hyperlink ref="B438" r:id="rId398"/>
     <hyperlink ref="B439" r:id="rId399"/>
-    <hyperlink ref="B440" r:id="rId400"/>
-    <hyperlink ref="B442" r:id="rId401"/>
-    <hyperlink ref="B441" r:id="rId402"/>
+    <hyperlink ref="B441" r:id="rId400"/>
+    <hyperlink ref="B440" r:id="rId401"/>
+    <hyperlink ref="B442" r:id="rId402"/>
     <hyperlink ref="B443" r:id="rId403"/>
     <hyperlink ref="B444" r:id="rId404"/>
     <hyperlink ref="B445" r:id="rId405"/>
@@ -8578,163 +8557,162 @@
     <hyperlink ref="B450" r:id="rId410"/>
     <hyperlink ref="B451" r:id="rId411"/>
     <hyperlink ref="B452" r:id="rId412"/>
-    <hyperlink ref="B453" r:id="rId413"/>
-    <hyperlink ref="B460" r:id="rId414"/>
-    <hyperlink ref="B459" r:id="rId415"/>
-    <hyperlink ref="B458" r:id="rId416"/>
-    <hyperlink ref="B457" r:id="rId417"/>
-    <hyperlink ref="B456" r:id="rId418"/>
-    <hyperlink ref="B455" r:id="rId419"/>
-    <hyperlink ref="B454" r:id="rId420"/>
+    <hyperlink ref="B459" r:id="rId413"/>
+    <hyperlink ref="B458" r:id="rId414"/>
+    <hyperlink ref="B457" r:id="rId415"/>
+    <hyperlink ref="B456" r:id="rId416"/>
+    <hyperlink ref="B455" r:id="rId417"/>
+    <hyperlink ref="B454" r:id="rId418"/>
+    <hyperlink ref="B453" r:id="rId419"/>
+    <hyperlink ref="B462" r:id="rId420"/>
     <hyperlink ref="B463" r:id="rId421"/>
     <hyperlink ref="B464" r:id="rId422"/>
     <hyperlink ref="B465" r:id="rId423"/>
     <hyperlink ref="B466" r:id="rId424"/>
     <hyperlink ref="B467" r:id="rId425"/>
     <hyperlink ref="B468" r:id="rId426"/>
-    <hyperlink ref="B469" r:id="rId427"/>
-    <hyperlink ref="B472" r:id="rId428" display="Power Set"/>
-    <hyperlink ref="B470" r:id="rId429"/>
-    <hyperlink ref="B471" r:id="rId430" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B348" r:id="rId431"/>
-    <hyperlink ref="D16" r:id="rId432"/>
-    <hyperlink ref="D5" r:id="rId433"/>
-    <hyperlink ref="D7" r:id="rId434"/>
-    <hyperlink ref="D11" r:id="rId435"/>
-    <hyperlink ref="D6" r:id="rId436"/>
-    <hyperlink ref="D8" r:id="rId437"/>
-    <hyperlink ref="D15" r:id="rId438"/>
-    <hyperlink ref="D14" r:id="rId439"/>
-    <hyperlink ref="D20" r:id="rId440"/>
-    <hyperlink ref="D54" r:id="rId441"/>
-    <hyperlink ref="D13" r:id="rId442"/>
-    <hyperlink ref="D31" r:id="rId443"/>
-    <hyperlink ref="D26" r:id="rId444"/>
-    <hyperlink ref="D21" r:id="rId445"/>
-    <hyperlink ref="D18" r:id="rId446"/>
-    <hyperlink ref="D42" r:id="rId447"/>
-    <hyperlink ref="D55" r:id="rId448"/>
-    <hyperlink ref="D56" r:id="rId449"/>
-    <hyperlink ref="D101" r:id="rId450"/>
-    <hyperlink ref="D98" r:id="rId451"/>
-    <hyperlink ref="D108" r:id="rId452"/>
-    <hyperlink ref="D152" r:id="rId453"/>
-    <hyperlink ref="D146" r:id="rId454"/>
-    <hyperlink ref="D129" r:id="rId455"/>
-    <hyperlink ref="D130" r:id="rId456"/>
-    <hyperlink ref="D131" r:id="rId457"/>
-    <hyperlink ref="D134" r:id="rId458"/>
-    <hyperlink ref="D135" r:id="rId459"/>
-    <hyperlink ref="D137" r:id="rId460"/>
-    <hyperlink ref="D142" r:id="rId461"/>
-    <hyperlink ref="D145" r:id="rId462"/>
-    <hyperlink ref="D143" r:id="rId463"/>
-    <hyperlink ref="D144" r:id="rId464"/>
-    <hyperlink ref="D160" r:id="rId465"/>
-    <hyperlink ref="D161" r:id="rId466"/>
-    <hyperlink ref="D136" r:id="rId467"/>
-    <hyperlink ref="D162" r:id="rId468"/>
-    <hyperlink ref="D154" r:id="rId469"/>
-    <hyperlink ref="B156" r:id="rId470" display="Merge K sorted Linked list"/>
-    <hyperlink ref="D157" r:id="rId471"/>
-    <hyperlink ref="D156" r:id="rId472"/>
-    <hyperlink ref="D155" r:id="rId473"/>
-    <hyperlink ref="D151" r:id="rId474"/>
-    <hyperlink ref="D170" r:id="rId475"/>
-    <hyperlink ref="D172" r:id="rId476"/>
-    <hyperlink ref="D171" r:id="rId477"/>
-    <hyperlink ref="D165" r:id="rId478"/>
-    <hyperlink ref="D167" r:id="rId479"/>
-    <hyperlink ref="D178" r:id="rId480"/>
-    <hyperlink ref="D169" r:id="rId481"/>
-    <hyperlink ref="D168" r:id="rId482"/>
-    <hyperlink ref="D177" r:id="rId483"/>
-    <hyperlink ref="D194" r:id="rId484"/>
-    <hyperlink ref="D180" r:id="rId485"/>
-    <hyperlink ref="D173" r:id="rId486"/>
-    <hyperlink ref="D174" r:id="rId487"/>
-    <hyperlink ref="D197" r:id="rId488"/>
-    <hyperlink ref="B197" r:id="rId489"/>
-    <hyperlink ref="D182" r:id="rId490"/>
-    <hyperlink ref="D203" r:id="rId491"/>
-    <hyperlink ref="D196" r:id="rId492"/>
-    <hyperlink ref="D166" r:id="rId493"/>
-    <hyperlink ref="D184" r:id="rId494"/>
-    <hyperlink ref="D190" r:id="rId495"/>
-    <hyperlink ref="D204" r:id="rId496"/>
-    <hyperlink ref="D217" r:id="rId497"/>
-    <hyperlink ref="D186" r:id="rId498"/>
-    <hyperlink ref="D207" r:id="rId499"/>
-    <hyperlink ref="D25" r:id="rId500"/>
-    <hyperlink ref="D209" r:id="rId501"/>
-    <hyperlink ref="D220" r:id="rId502"/>
-    <hyperlink ref="D211" r:id="rId503"/>
-    <hyperlink ref="D49" r:id="rId504"/>
-    <hyperlink ref="D208" r:id="rId505"/>
-    <hyperlink ref="D331" r:id="rId506"/>
-    <hyperlink ref="D341" r:id="rId507"/>
-    <hyperlink ref="D337" r:id="rId508"/>
-    <hyperlink ref="D345" r:id="rId509"/>
-    <hyperlink ref="D336" r:id="rId510"/>
-    <hyperlink ref="D9" r:id="rId511"/>
-    <hyperlink ref="D38" r:id="rId512"/>
-    <hyperlink ref="D23" r:id="rId513"/>
-    <hyperlink ref="B39" r:id="rId514" display="Median of 2 sorted arrays of equal size"/>
-    <hyperlink ref="D39" r:id="rId515"/>
-    <hyperlink ref="D33" r:id="rId516"/>
-    <hyperlink ref="D43" r:id="rId517"/>
-    <hyperlink ref="D45" r:id="rId518"/>
-    <hyperlink ref="D50" r:id="rId519"/>
-    <hyperlink ref="D277" r:id="rId520"/>
-    <hyperlink ref="D27" r:id="rId521"/>
-    <hyperlink ref="D24" r:id="rId522"/>
-    <hyperlink ref="D37" r:id="rId523"/>
-    <hyperlink ref="D19" r:id="rId524"/>
-    <hyperlink ref="D12" r:id="rId525"/>
-    <hyperlink ref="D34" r:id="rId526"/>
-    <hyperlink ref="D10" r:id="rId527"/>
-    <hyperlink ref="D99" r:id="rId528"/>
-    <hyperlink ref="D22" r:id="rId529"/>
-    <hyperlink ref="D100" r:id="rId530"/>
-    <hyperlink ref="D289" r:id="rId531"/>
-    <hyperlink ref="D293" r:id="rId532"/>
-    <hyperlink ref="D290" r:id="rId533"/>
-    <hyperlink ref="D299" r:id="rId534"/>
-    <hyperlink ref="D301" r:id="rId535"/>
-    <hyperlink ref="D294" r:id="rId536"/>
-    <hyperlink ref="D292" r:id="rId537"/>
-    <hyperlink ref="D300" r:id="rId538"/>
-    <hyperlink ref="D305" r:id="rId539"/>
-    <hyperlink ref="D78" r:id="rId540"/>
-    <hyperlink ref="D73" r:id="rId541"/>
-    <hyperlink ref="D325" r:id="rId542"/>
-    <hyperlink ref="D295" r:id="rId543"/>
-    <hyperlink ref="D303" r:id="rId544"/>
-    <hyperlink ref="D296" r:id="rId545"/>
-    <hyperlink ref="D47" r:id="rId546"/>
-    <hyperlink ref="F294" r:id="rId547"/>
-    <hyperlink ref="D311" r:id="rId548"/>
-    <hyperlink ref="D313" r:id="rId549"/>
-    <hyperlink ref="D319" r:id="rId550"/>
-    <hyperlink ref="B324" r:id="rId551"/>
-    <hyperlink ref="D324" r:id="rId552"/>
+    <hyperlink ref="B471" r:id="rId427" display="Power Set"/>
+    <hyperlink ref="B469" r:id="rId428"/>
+    <hyperlink ref="B470" r:id="rId429" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B347" r:id="rId430"/>
+    <hyperlink ref="D16" r:id="rId431"/>
+    <hyperlink ref="D5" r:id="rId432"/>
+    <hyperlink ref="D7" r:id="rId433"/>
+    <hyperlink ref="D11" r:id="rId434"/>
+    <hyperlink ref="D6" r:id="rId435"/>
+    <hyperlink ref="D8" r:id="rId436"/>
+    <hyperlink ref="D15" r:id="rId437"/>
+    <hyperlink ref="D14" r:id="rId438"/>
+    <hyperlink ref="D20" r:id="rId439"/>
+    <hyperlink ref="D54" r:id="rId440"/>
+    <hyperlink ref="D13" r:id="rId441"/>
+    <hyperlink ref="D31" r:id="rId442"/>
+    <hyperlink ref="D26" r:id="rId443"/>
+    <hyperlink ref="D21" r:id="rId444"/>
+    <hyperlink ref="D18" r:id="rId445"/>
+    <hyperlink ref="D42" r:id="rId446"/>
+    <hyperlink ref="D55" r:id="rId447"/>
+    <hyperlink ref="D56" r:id="rId448"/>
+    <hyperlink ref="D101" r:id="rId449"/>
+    <hyperlink ref="D98" r:id="rId450"/>
+    <hyperlink ref="D108" r:id="rId451"/>
+    <hyperlink ref="D152" r:id="rId452"/>
+    <hyperlink ref="D146" r:id="rId453"/>
+    <hyperlink ref="D129" r:id="rId454"/>
+    <hyperlink ref="D130" r:id="rId455"/>
+    <hyperlink ref="D131" r:id="rId456"/>
+    <hyperlink ref="D134" r:id="rId457"/>
+    <hyperlink ref="D135" r:id="rId458"/>
+    <hyperlink ref="D137" r:id="rId459"/>
+    <hyperlink ref="D142" r:id="rId460"/>
+    <hyperlink ref="D145" r:id="rId461"/>
+    <hyperlink ref="D143" r:id="rId462"/>
+    <hyperlink ref="D144" r:id="rId463"/>
+    <hyperlink ref="D160" r:id="rId464"/>
+    <hyperlink ref="D161" r:id="rId465"/>
+    <hyperlink ref="D136" r:id="rId466"/>
+    <hyperlink ref="D162" r:id="rId467"/>
+    <hyperlink ref="D154" r:id="rId468"/>
+    <hyperlink ref="B156" r:id="rId469" display="Merge K sorted Linked list"/>
+    <hyperlink ref="D157" r:id="rId470"/>
+    <hyperlink ref="D156" r:id="rId471"/>
+    <hyperlink ref="D155" r:id="rId472"/>
+    <hyperlink ref="D151" r:id="rId473"/>
+    <hyperlink ref="D170" r:id="rId474"/>
+    <hyperlink ref="D172" r:id="rId475"/>
+    <hyperlink ref="D171" r:id="rId476"/>
+    <hyperlink ref="D165" r:id="rId477"/>
+    <hyperlink ref="D167" r:id="rId478"/>
+    <hyperlink ref="D178" r:id="rId479"/>
+    <hyperlink ref="D169" r:id="rId480"/>
+    <hyperlink ref="D168" r:id="rId481"/>
+    <hyperlink ref="D177" r:id="rId482"/>
+    <hyperlink ref="D194" r:id="rId483"/>
+    <hyperlink ref="D180" r:id="rId484"/>
+    <hyperlink ref="D173" r:id="rId485"/>
+    <hyperlink ref="D174" r:id="rId486"/>
+    <hyperlink ref="D197" r:id="rId487"/>
+    <hyperlink ref="B197" r:id="rId488"/>
+    <hyperlink ref="D182" r:id="rId489"/>
+    <hyperlink ref="D203" r:id="rId490"/>
+    <hyperlink ref="D196" r:id="rId491"/>
+    <hyperlink ref="D166" r:id="rId492"/>
+    <hyperlink ref="D184" r:id="rId493"/>
+    <hyperlink ref="D190" r:id="rId494"/>
+    <hyperlink ref="D204" r:id="rId495"/>
+    <hyperlink ref="D217" r:id="rId496"/>
+    <hyperlink ref="D186" r:id="rId497"/>
+    <hyperlink ref="D207" r:id="rId498"/>
+    <hyperlink ref="D25" r:id="rId499"/>
+    <hyperlink ref="D209" r:id="rId500"/>
+    <hyperlink ref="D220" r:id="rId501"/>
+    <hyperlink ref="D211" r:id="rId502"/>
+    <hyperlink ref="D49" r:id="rId503"/>
+    <hyperlink ref="D208" r:id="rId504"/>
+    <hyperlink ref="D330" r:id="rId505"/>
+    <hyperlink ref="D340" r:id="rId506"/>
+    <hyperlink ref="D336" r:id="rId507"/>
+    <hyperlink ref="D344" r:id="rId508"/>
+    <hyperlink ref="D335" r:id="rId509"/>
+    <hyperlink ref="D9" r:id="rId510"/>
+    <hyperlink ref="D38" r:id="rId511"/>
+    <hyperlink ref="D23" r:id="rId512"/>
+    <hyperlink ref="B39" r:id="rId513" display="Median of 2 sorted arrays of equal size"/>
+    <hyperlink ref="D39" r:id="rId514"/>
+    <hyperlink ref="D33" r:id="rId515"/>
+    <hyperlink ref="D43" r:id="rId516"/>
+    <hyperlink ref="D45" r:id="rId517"/>
+    <hyperlink ref="D50" r:id="rId518"/>
+    <hyperlink ref="D277" r:id="rId519"/>
+    <hyperlink ref="D27" r:id="rId520"/>
+    <hyperlink ref="D24" r:id="rId521"/>
+    <hyperlink ref="D37" r:id="rId522"/>
+    <hyperlink ref="D19" r:id="rId523"/>
+    <hyperlink ref="D12" r:id="rId524"/>
+    <hyperlink ref="D34" r:id="rId525"/>
+    <hyperlink ref="D10" r:id="rId526"/>
+    <hyperlink ref="D99" r:id="rId527"/>
+    <hyperlink ref="D22" r:id="rId528"/>
+    <hyperlink ref="D100" r:id="rId529"/>
+    <hyperlink ref="D289" r:id="rId530"/>
+    <hyperlink ref="D293" r:id="rId531"/>
+    <hyperlink ref="D290" r:id="rId532"/>
+    <hyperlink ref="D298" r:id="rId533"/>
+    <hyperlink ref="D300" r:id="rId534"/>
+    <hyperlink ref="D294" r:id="rId535"/>
+    <hyperlink ref="D292" r:id="rId536"/>
+    <hyperlink ref="D299" r:id="rId537"/>
+    <hyperlink ref="D304" r:id="rId538"/>
+    <hyperlink ref="D78" r:id="rId539"/>
+    <hyperlink ref="D73" r:id="rId540"/>
+    <hyperlink ref="D324" r:id="rId541"/>
+    <hyperlink ref="D295" r:id="rId542"/>
+    <hyperlink ref="D302" r:id="rId543"/>
+    <hyperlink ref="D296" r:id="rId544"/>
+    <hyperlink ref="D47" r:id="rId545"/>
+    <hyperlink ref="F294" r:id="rId546"/>
+    <hyperlink ref="D310" r:id="rId547"/>
+    <hyperlink ref="D312" r:id="rId548"/>
+    <hyperlink ref="D318" r:id="rId549"/>
+    <hyperlink ref="B323" r:id="rId550"/>
+    <hyperlink ref="D323" r:id="rId551"/>
+    <hyperlink ref="D465" r:id="rId552"/>
     <hyperlink ref="D466" r:id="rId553"/>
-    <hyperlink ref="D467" r:id="rId554"/>
-    <hyperlink ref="D472" r:id="rId555"/>
-    <hyperlink ref="D468" r:id="rId556"/>
+    <hyperlink ref="D471" r:id="rId554"/>
+    <hyperlink ref="D467" r:id="rId555"/>
+    <hyperlink ref="D463" r:id="rId556"/>
     <hyperlink ref="D464" r:id="rId557"/>
-    <hyperlink ref="D465" r:id="rId558"/>
-    <hyperlink ref="D471" r:id="rId559"/>
-    <hyperlink ref="D470" r:id="rId560"/>
-    <hyperlink ref="D105" r:id="rId561"/>
-    <hyperlink ref="D104" r:id="rId562"/>
-    <hyperlink ref="D107" r:id="rId563"/>
-    <hyperlink ref="D112" r:id="rId564"/>
+    <hyperlink ref="D470" r:id="rId558"/>
+    <hyperlink ref="D469" r:id="rId559"/>
+    <hyperlink ref="D105" r:id="rId560"/>
+    <hyperlink ref="D104" r:id="rId561"/>
+    <hyperlink ref="D107" r:id="rId562"/>
+    <hyperlink ref="D112" r:id="rId563"/>
+    <hyperlink ref="D313" r:id="rId564"/>
     <hyperlink ref="D314" r:id="rId565"/>
-    <hyperlink ref="D315" r:id="rId566"/>
-    <hyperlink ref="D298" r:id="rId567"/>
+    <hyperlink ref="D297" r:id="rId566"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId568"/>
+  <pageSetup orientation="portrait" r:id="rId567"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implement stack using queue
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="606">
   <si>
     <t>Topic:</t>
   </si>
@@ -1852,6 +1852,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/evaluate-reverse-polish-notation/submissions/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/learn/card/queue-stack/239/conclusion/1387/</t>
   </si>
 </sst>
 </file>
@@ -2614,8 +2617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C377" sqref="C377"/>
+    <sheetView tabSelected="1" topLeftCell="A291" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F304" sqref="F304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6262,9 +6265,11 @@
         <v>601</v>
       </c>
       <c r="C305" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D305" s="23"/>
+        <v>418</v>
+      </c>
+      <c r="D305" s="22" t="s">
+        <v>605</v>
+      </c>
       <c r="F305" s="23"/>
     </row>
     <row r="306" spans="1:6" ht="21">
@@ -8711,8 +8716,9 @@
     <hyperlink ref="D313" r:id="rId564"/>
     <hyperlink ref="D314" r:id="rId565"/>
     <hyperlink ref="D297" r:id="rId566"/>
+    <hyperlink ref="D305" r:id="rId567"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId567"/>
+  <pageSetup orientation="portrait" r:id="rId568"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merge 2 binary tree
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="608">
   <si>
     <t>Topic:</t>
   </si>
@@ -1855,6 +1855,12 @@
   </si>
   <si>
     <t>https://leetcode.com/explore/learn/card/queue-stack/239/conclusion/1387/</t>
+  </si>
+  <si>
+    <t>Merge 2 Binary tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-two-binary-trees/</t>
   </si>
 </sst>
 </file>
@@ -2615,10 +2621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F471"/>
+  <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F304" sqref="F304"/>
+    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5040,34 +5046,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A199" s="6" t="s">
+    <row r="199" spans="1:6" ht="21">
+      <c r="A199" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B199" s="7" t="s">
+      <c r="B199" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D199" s="16" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A200" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B200" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C199" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D199" s="23"/>
-      <c r="F199" s="23"/>
-    </row>
-    <row r="200" spans="1:6" ht="21">
-      <c r="A200" s="3" t="s">
+      <c r="C200" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D200" s="23"/>
+      <c r="F200" s="23"/>
+    </row>
+    <row r="201" spans="1:6" ht="21">
+      <c r="A201" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B200" s="13" t="s">
+      <c r="B201" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="C200" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="21">
-      <c r="A201" s="5"/>
-      <c r="B201" s="4"/>
-      <c r="C201" s="2"/>
+      <c r="C201" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="202" spans="1:6" ht="21">
       <c r="A202" s="5"/>
@@ -5075,31 +5090,22 @@
       <c r="C202" s="2"/>
     </row>
     <row r="203" spans="1:6" ht="21">
-      <c r="A203" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B203" s="13" t="s">
-        <v>506</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D203" s="20" t="s">
-        <v>495</v>
-      </c>
+      <c r="A203" s="5"/>
+      <c r="B203" s="4"/>
+      <c r="C203" s="2"/>
     </row>
     <row r="204" spans="1:6" ht="21">
       <c r="A204" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D204" s="20" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="21">
@@ -5107,13 +5113,13 @@
         <v>173</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D205" s="20" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="21">
@@ -5121,10 +5127,13 @@
         <v>173</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>174</v>
+        <v>503</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D206" s="20" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="21">
@@ -5132,13 +5141,10 @@
         <v>173</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D207" s="20" t="s">
-        <v>510</v>
+        <v>2</v>
       </c>
     </row>
     <row r="208" spans="1:6" ht="21">
@@ -5146,13 +5152,13 @@
         <v>173</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D208" s="20" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="21">
@@ -5160,13 +5166,13 @@
         <v>173</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D209" s="20" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="21">
@@ -5174,35 +5180,38 @@
         <v>173</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D210" s="20" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="21">
       <c r="A211" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B211" s="15" t="s">
-        <v>179</v>
+      <c r="B211" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D211" s="20" t="s">
-        <v>514</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="21">
       <c r="A212" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B212" s="13" t="s">
-        <v>180</v>
+      <c r="B212" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D212" s="20" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="21">
@@ -5210,7 +5219,7 @@
         <v>173</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>2</v>
@@ -5221,72 +5230,72 @@
         <v>173</v>
       </c>
       <c r="B214" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="21">
+      <c r="A215" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B215" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C214" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A215" s="6" t="s">
+      <c r="C215" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A216" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B216" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="C215" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D215" s="23"/>
-      <c r="F215" s="23"/>
-    </row>
-    <row r="216" spans="1:6" s="45" customFormat="1" ht="21">
-      <c r="A216" s="41" t="s">
+      <c r="C216" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D216" s="23"/>
+      <c r="F216" s="23"/>
+    </row>
+    <row r="217" spans="1:6" s="45" customFormat="1" ht="21">
+      <c r="A217" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="B216" s="42" t="s">
+      <c r="B217" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="C216" s="43" t="s">
-        <v>418</v>
-      </c>
-      <c r="D216" s="44" t="s">
+      <c r="C217" s="43" t="s">
+        <v>418</v>
+      </c>
+      <c r="D217" s="44" t="s">
         <v>507</v>
       </c>
-      <c r="F216" s="62"/>
-    </row>
-    <row r="217" spans="1:6" s="50" customFormat="1" ht="21">
-      <c r="A217" s="46" t="s">
+      <c r="F217" s="62"/>
+    </row>
+    <row r="218" spans="1:6" s="50" customFormat="1" ht="21">
+      <c r="A218" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="B217" s="47" t="s">
+      <c r="B218" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="C217" s="48" t="s">
-        <v>418</v>
-      </c>
-      <c r="D217" s="49" t="s">
+      <c r="C218" s="48" t="s">
+        <v>418</v>
+      </c>
+      <c r="D218" s="49" t="s">
         <v>505</v>
       </c>
-      <c r="F217" s="63"/>
-    </row>
-    <row r="218" spans="1:6" ht="21">
-      <c r="A218" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B218" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F218" s="63"/>
     </row>
     <row r="219" spans="1:6" ht="21">
       <c r="A219" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>2</v>
@@ -5297,13 +5306,10 @@
         <v>173</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D220" s="20" t="s">
-        <v>513</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="21">
@@ -5311,10 +5317,13 @@
         <v>173</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D221" s="20" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="21">
@@ -5322,7 +5331,7 @@
         <v>173</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>2</v>
@@ -5333,75 +5342,75 @@
         <v>173</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D223" s="51"/>
     </row>
     <row r="224" spans="1:6" ht="21">
       <c r="A224" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B224" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D224" s="51"/>
+    </row>
+    <row r="225" spans="1:6" ht="21">
+      <c r="A225" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B225" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="C224" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A225" s="6" t="s">
+      <c r="C225" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A226" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B225" s="7" t="s">
+      <c r="B226" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C225" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D225" s="23"/>
-      <c r="F225" s="23" t="s">
+      <c r="C226" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D226" s="23"/>
+      <c r="F226" s="23" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="21">
-      <c r="A226" s="3" t="s">
+    <row r="227" spans="1:6" ht="21">
+      <c r="A227" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B226" s="13" t="s">
+      <c r="B227" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="C226" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="21">
-      <c r="B227" s="4"/>
-      <c r="C227" s="2"/>
+      <c r="C227" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="228" spans="1:6" ht="21">
       <c r="B228" s="4"/>
       <c r="C228" s="2"/>
     </row>
     <row r="229" spans="1:6" ht="21">
-      <c r="A229" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B229" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B229" s="4"/>
+      <c r="C229" s="2"/>
     </row>
     <row r="230" spans="1:6" ht="21">
       <c r="A230" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>2</v>
@@ -5412,7 +5421,7 @@
         <v>194</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>2</v>
@@ -5423,7 +5432,7 @@
         <v>194</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>2</v>
@@ -5434,7 +5443,7 @@
         <v>194</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>2</v>
@@ -5445,7 +5454,7 @@
         <v>194</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>2</v>
@@ -5456,7 +5465,7 @@
         <v>194</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>2</v>
@@ -5467,7 +5476,7 @@
         <v>194</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>2</v>
@@ -5478,7 +5487,7 @@
         <v>194</v>
       </c>
       <c r="B237" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>2</v>
@@ -5489,7 +5498,7 @@
         <v>194</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>2</v>
@@ -5500,7 +5509,7 @@
         <v>194</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>2</v>
@@ -5511,7 +5520,7 @@
         <v>194</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>2</v>
@@ -5522,7 +5531,7 @@
         <v>194</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>2</v>
@@ -5533,7 +5542,7 @@
         <v>194</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>2</v>
@@ -5544,7 +5553,7 @@
         <v>194</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>2</v>
@@ -5555,7 +5564,7 @@
         <v>194</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>2</v>
@@ -5566,7 +5575,7 @@
         <v>194</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>2</v>
@@ -5577,7 +5586,7 @@
         <v>194</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>2</v>
@@ -5588,7 +5597,7 @@
         <v>194</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>2</v>
@@ -5599,7 +5608,7 @@
         <v>194</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>2</v>
@@ -5610,7 +5619,7 @@
         <v>194</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>2</v>
@@ -5621,7 +5630,7 @@
         <v>194</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>2</v>
@@ -5632,7 +5641,7 @@
         <v>194</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>2</v>
@@ -5643,7 +5652,7 @@
         <v>194</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>2</v>
@@ -5654,7 +5663,7 @@
         <v>194</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>2</v>
@@ -5665,7 +5674,7 @@
         <v>194</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>2</v>
@@ -5676,7 +5685,7 @@
         <v>194</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>2</v>
@@ -5687,7 +5696,7 @@
         <v>194</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>2</v>
@@ -5698,7 +5707,7 @@
         <v>194</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>2</v>
@@ -5709,7 +5718,7 @@
         <v>194</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -5720,7 +5729,7 @@
         <v>194</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -5731,7 +5740,7 @@
         <v>194</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -5742,7 +5751,7 @@
         <v>194</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -5753,7 +5762,7 @@
         <v>194</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>75</v>
+        <v>227</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>2</v>
@@ -5764,50 +5773,50 @@
         <v>194</v>
       </c>
       <c r="B263" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="21">
+      <c r="A264" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B264" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="C263" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="21">
-      <c r="B264" s="4"/>
-      <c r="C264" s="2"/>
+      <c r="C264" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="265" spans="1:6" ht="21">
       <c r="B265" s="4"/>
       <c r="C265" s="2"/>
     </row>
-    <row r="266" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A266" s="6" t="s">
+    <row r="266" spans="1:6" ht="21">
+      <c r="B266" s="4"/>
+      <c r="C266" s="2"/>
+    </row>
+    <row r="267" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A267" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B266" s="7" t="s">
+      <c r="B267" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C266" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D266" s="23"/>
-      <c r="F266" s="23"/>
-    </row>
-    <row r="267" spans="1:6" ht="21">
-      <c r="A267" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B267" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C267" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D267" s="23"/>
+      <c r="F267" s="23"/>
     </row>
     <row r="268" spans="1:6" ht="21">
       <c r="A268" s="3" t="s">
         <v>229</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -5818,31 +5827,29 @@
         <v>229</v>
       </c>
       <c r="B269" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="21">
+      <c r="A270" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B270" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="C269" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A270" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B270" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="C270" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D270" s="23"/>
-      <c r="F270" s="23"/>
+      <c r="C270" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="271" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A271" s="6" t="s">
         <v>229</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C271" s="6" t="s">
         <v>2</v>
@@ -5850,23 +5857,25 @@
       <c r="D271" s="23"/>
       <c r="F271" s="23"/>
     </row>
-    <row r="272" spans="1:6" ht="21">
-      <c r="A272" s="3" t="s">
+    <row r="272" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A272" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B272" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B272" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D272" s="23"/>
+      <c r="F272" s="23"/>
     </row>
     <row r="273" spans="1:6" ht="21">
       <c r="A273" s="3" t="s">
         <v>229</v>
       </c>
       <c r="B273" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>2</v>
@@ -5877,7 +5886,7 @@
         <v>229</v>
       </c>
       <c r="B274" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>2</v>
@@ -5888,7 +5897,7 @@
         <v>229</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C275" s="2" t="s">
         <v>2</v>
@@ -5899,44 +5908,44 @@
         <v>229</v>
       </c>
       <c r="B276" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="21">
+      <c r="A277" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B277" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="C276" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A277" s="6" t="s">
+      <c r="C277" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A278" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="B277" s="7" t="s">
+      <c r="B278" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="C277" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D277" s="22" t="s">
+      <c r="C278" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D278" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="F277" s="23"/>
-    </row>
-    <row r="278" spans="1:6" ht="21">
-      <c r="A278" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B278" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F278" s="23"/>
     </row>
     <row r="279" spans="1:6" ht="21">
       <c r="A279" s="3" t="s">
         <v>229</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>2</v>
@@ -5947,7 +5956,7 @@
         <v>229</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>2</v>
@@ -5958,7 +5967,7 @@
         <v>229</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
@@ -5969,7 +5978,7 @@
         <v>229</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>2</v>
@@ -5980,7 +5989,7 @@
         <v>229</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>2</v>
@@ -5991,40 +6000,37 @@
         <v>229</v>
       </c>
       <c r="B284" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="21">
+      <c r="A285" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B285" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="C284" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" ht="21">
-      <c r="B285" s="4"/>
-      <c r="C285" s="2"/>
+      <c r="C285" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="286" spans="1:6" ht="21">
       <c r="B286" s="4"/>
       <c r="C286" s="2"/>
     </row>
     <row r="287" spans="1:6" ht="21">
-      <c r="A287" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B287" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D287" s="16" t="s">
-        <v>555</v>
-      </c>
+      <c r="B287" s="4"/>
+      <c r="C287" s="2"/>
     </row>
     <row r="288" spans="1:6" ht="21">
       <c r="A288" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>418</v>
@@ -6038,13 +6044,13 @@
         <v>248</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D289" s="20" t="s">
-        <v>556</v>
+      <c r="D289" s="16" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="21">
@@ -6052,72 +6058,69 @@
         <v>248</v>
       </c>
       <c r="B290" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D290" s="20" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="21">
+      <c r="A291" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B291" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="C290" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D290" s="20" t="s">
+      <c r="C291" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D291" s="20" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="291" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A291" s="30" t="s">
+    <row r="292" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A292" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B291" s="31" t="s">
+      <c r="B292" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="C291" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D291" s="32"/>
-      <c r="F291" s="32"/>
-    </row>
-    <row r="292" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A292" s="6" t="s">
+      <c r="C292" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D292" s="32"/>
+      <c r="F292" s="32"/>
+    </row>
+    <row r="293" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A293" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B292" s="7" t="s">
+      <c r="B293" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="C292" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D292" s="22" t="s">
+      <c r="C293" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D293" s="22" t="s">
         <v>562</v>
       </c>
-      <c r="F292" s="23"/>
-    </row>
-    <row r="293" spans="1:6" ht="21">
-      <c r="A293" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B293" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D293" s="20" t="s">
-        <v>557</v>
-      </c>
+      <c r="F293" s="23"/>
     </row>
     <row r="294" spans="1:6" ht="21">
       <c r="A294" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B294" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>561</v>
-      </c>
-      <c r="F294" s="20" t="s">
-        <v>575</v>
+        <v>557</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="21">
@@ -6125,211 +6128,214 @@
         <v>248</v>
       </c>
       <c r="B295" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D295" s="20" t="s">
+        <v>561</v>
+      </c>
+      <c r="F295" s="20" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" ht="21">
+      <c r="A296" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B296" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C295" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D295" s="20" t="s">
+      <c r="C296" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D296" s="20" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="296" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A296" s="30" t="s">
+    <row r="297" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A297" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B296" s="31" t="s">
+      <c r="B297" s="31" t="s">
         <v>572</v>
       </c>
-      <c r="C296" s="30" t="s">
-        <v>418</v>
-      </c>
-      <c r="D296" s="36" t="s">
+      <c r="C297" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D297" s="36" t="s">
         <v>571</v>
       </c>
-      <c r="F296" s="32"/>
-    </row>
-    <row r="297" spans="1:6" ht="21">
-      <c r="A297" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B297" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D297" s="20" t="s">
-        <v>604</v>
-      </c>
+      <c r="F297" s="32"/>
     </row>
     <row r="298" spans="1:6" ht="21">
       <c r="A298" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B298" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D298" s="20" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" ht="21">
+      <c r="A299" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B299" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C298" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D298" s="20" t="s">
+      <c r="C299" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D299" s="20" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="299" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A299" s="6" t="s">
+    <row r="300" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A300" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B299" s="58" t="s">
+      <c r="B300" s="58" t="s">
         <v>259</v>
       </c>
-      <c r="C299" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D299" s="22" t="s">
+      <c r="C300" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D300" s="22" t="s">
         <v>563</v>
       </c>
-      <c r="F299" s="23"/>
-    </row>
-    <row r="300" spans="1:6" ht="21">
-      <c r="A300" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B300" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="C300" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D300" s="20" t="s">
-        <v>564</v>
-      </c>
+      <c r="F300" s="23"/>
     </row>
     <row r="301" spans="1:6" ht="21">
       <c r="A301" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B301" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D301" s="20" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="21">
+      <c r="A302" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B302" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="C301" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A302" s="30" t="s">
+      <c r="C302" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A303" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B302" s="31" t="s">
+      <c r="B303" s="31" t="s">
         <v>602</v>
       </c>
-      <c r="C302" s="30" t="s">
-        <v>418</v>
-      </c>
-      <c r="D302" s="36" t="s">
+      <c r="C303" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D303" s="36" t="s">
         <v>570</v>
       </c>
-      <c r="F302" s="32"/>
-    </row>
-    <row r="303" spans="1:6" ht="21">
-      <c r="A303" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B303" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="C303" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F303" s="32"/>
     </row>
     <row r="304" spans="1:6" ht="21">
       <c r="A304" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B304" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" ht="21">
+      <c r="A305" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B305" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C304" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D304" s="20" t="s">
+      <c r="C305" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D305" s="20" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="305" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A305" s="6" t="s">
+    <row r="306" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A306" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B305" s="7" t="s">
+      <c r="B306" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="C305" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D305" s="22" t="s">
+      <c r="C306" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D306" s="22" t="s">
         <v>605</v>
       </c>
-      <c r="F305" s="23"/>
-    </row>
-    <row r="306" spans="1:6" ht="21">
-      <c r="A306" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B306" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="C306" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F306" s="23"/>
     </row>
     <row r="307" spans="1:6" ht="21">
       <c r="A307" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B307" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C307" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" ht="21">
+      <c r="A308" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B308" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="C307" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A308" s="6" t="s">
+      <c r="C308" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A309" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B308" s="7" t="s">
+      <c r="B309" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="C308" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D308" s="23"/>
-      <c r="F308" s="23"/>
-    </row>
-    <row r="309" spans="1:6" ht="21">
-      <c r="A309" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B309" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="C309" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C309" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D309" s="23"/>
+      <c r="F309" s="23"/>
     </row>
     <row r="310" spans="1:6" ht="21">
       <c r="A310" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D310" s="20" t="s">
-        <v>576</v>
+        <v>2</v>
       </c>
     </row>
     <row r="311" spans="1:6" ht="21">
@@ -6337,10 +6343,13 @@
         <v>248</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D311" s="20" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6348,13 +6357,10 @@
         <v>248</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D312" s="20" t="s">
-        <v>577</v>
+        <v>2</v>
       </c>
     </row>
     <row r="313" spans="1:6" ht="21">
@@ -6362,13 +6368,13 @@
         <v>248</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D313" s="20" t="s">
-        <v>596</v>
+        <v>577</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="21">
@@ -6376,82 +6382,85 @@
         <v>248</v>
       </c>
       <c r="B314" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C314" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D314" s="20" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" ht="21">
+      <c r="A315" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B315" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="C314" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D314" s="20" t="s">
+      <c r="C315" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D315" s="20" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="315" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A315" s="6" t="s">
+    <row r="316" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A316" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B315" s="7" t="s">
+      <c r="B316" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="C315" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D315" s="23"/>
-      <c r="F315" s="23"/>
-    </row>
-    <row r="316" spans="1:6" ht="21">
-      <c r="A316" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B316" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C316" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D316" s="23"/>
+      <c r="F316" s="23"/>
     </row>
     <row r="317" spans="1:6" ht="21">
       <c r="A317" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B317" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" ht="21">
+      <c r="A318" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B318" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="C317" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A318" s="6" t="s">
+      <c r="C318" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A319" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B318" s="7" t="s">
+      <c r="B319" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="C318" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D318" s="22" t="s">
+      <c r="C319" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D319" s="22" t="s">
         <v>578</v>
       </c>
-      <c r="F318" s="23"/>
-    </row>
-    <row r="319" spans="1:6" ht="21">
-      <c r="A319" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B319" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="C319" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="F319" s="23"/>
     </row>
     <row r="320" spans="1:6" ht="21">
       <c r="A320" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6462,7 +6471,7 @@
         <v>248</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>2</v>
@@ -6473,16 +6482,10 @@
         <v>248</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D322" s="16" t="s">
-        <v>598</v>
-      </c>
-      <c r="F322" s="57" t="s">
-        <v>597</v>
+        <v>2</v>
       </c>
     </row>
     <row r="323" spans="1:6" ht="21">
@@ -6490,137 +6493,143 @@
         <v>248</v>
       </c>
       <c r="B323" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D323" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="F323" s="57" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" ht="21">
+      <c r="A324" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B324" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="C323" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D323" s="20" t="s">
+      <c r="C324" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D324" s="20" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="324" spans="1:6" s="31" customFormat="1" ht="21">
-      <c r="A324" s="30" t="s">
+    <row r="325" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A325" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="B324" s="31" t="s">
+      <c r="B325" s="31" t="s">
         <v>580</v>
       </c>
-      <c r="C324" s="30" t="s">
-        <v>418</v>
-      </c>
-      <c r="D324" s="36" t="s">
+      <c r="C325" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="D325" s="36" t="s">
         <v>581</v>
       </c>
-      <c r="F324" s="32"/>
-    </row>
-    <row r="325" spans="1:6" ht="21">
-      <c r="B325" s="4"/>
-      <c r="C325" s="2"/>
+      <c r="F325" s="32"/>
     </row>
     <row r="326" spans="1:6" ht="21">
       <c r="B326" s="4"/>
       <c r="C326" s="2"/>
     </row>
     <row r="327" spans="1:6" ht="21">
-      <c r="A327" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B327" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C327" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D327" s="21" t="s">
-        <v>518</v>
-      </c>
+      <c r="B327" s="4"/>
+      <c r="C327" s="2"/>
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328" s="5" t="s">
         <v>530</v>
       </c>
       <c r="B328" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D328" s="21" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" ht="21">
+      <c r="A329" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B329" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="C328" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D328" s="16" t="s">
+      <c r="C329" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D329" s="16" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="329" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A329" s="6" t="s">
+    <row r="330" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A330" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B329" s="7" t="s">
+      <c r="B330" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C329" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D329" s="23"/>
-      <c r="F329" s="23"/>
-    </row>
-    <row r="330" spans="1:6" ht="21">
-      <c r="A330" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B330" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="C330" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D330" s="20" t="s">
-        <v>421</v>
-      </c>
+      <c r="C330" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D330" s="23"/>
+      <c r="F330" s="23"/>
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
         <v>530</v>
       </c>
       <c r="B331" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D331" s="20" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" ht="21">
+      <c r="A332" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B332" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="C331" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D331" s="16" t="s">
+      <c r="C332" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D332" s="16" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="332" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A332" s="6" t="s">
+    <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A333" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B332" s="7" t="s">
+      <c r="B333" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C332" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D332" s="23"/>
-      <c r="F332" s="23"/>
-    </row>
-    <row r="333" spans="1:6" ht="21">
-      <c r="A333" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B333" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="C333" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C333" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D333" s="23"/>
+      <c r="F333" s="23"/>
     </row>
     <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
         <v>530</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>2</v>
@@ -6630,160 +6639,160 @@
       <c r="A335" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="B335" s="15" t="s">
+      <c r="B335" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C335" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" ht="21">
+      <c r="A336" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B336" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="C335" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D335" s="20" t="s">
+      <c r="C336" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D336" s="20" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="336" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A336" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="B336" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C336" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D336" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F336" s="23"/>
     </row>
     <row r="337" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A337" s="6" t="s">
         <v>530</v>
       </c>
       <c r="B337" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C337" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D337" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="F337" s="23"/>
+    </row>
+    <row r="338" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A338" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B338" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C337" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D337" s="23"/>
-      <c r="F337" s="23"/>
-    </row>
-    <row r="338" spans="1:6" ht="21">
-      <c r="A338" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B338" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="C338" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C338" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D338" s="23"/>
+      <c r="F338" s="23"/>
     </row>
     <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
         <v>530</v>
       </c>
       <c r="B339" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" ht="21">
+      <c r="A340" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B340" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="C339" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="340" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A340" s="6" t="s">
+      <c r="C340" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A341" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B340" s="7" t="s">
+      <c r="B341" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="C340" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D340" s="22" t="s">
+      <c r="C341" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D341" s="22" t="s">
         <v>520</v>
       </c>
-      <c r="F340" s="23"/>
-    </row>
-    <row r="341" spans="1:6" ht="21">
-      <c r="A341" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B341" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="C341" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="342" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="F341" s="23"/>
+    </row>
+    <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="B342" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="C342" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D342" s="52" t="s">
-        <v>518</v>
-      </c>
-      <c r="F342" s="23"/>
-    </row>
-    <row r="343" spans="1:6" ht="21">
+      <c r="B342" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A343" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="B343" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="C343" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B343" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C343" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D343" s="52" t="s">
+        <v>518</v>
+      </c>
+      <c r="F343" s="23"/>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
         <v>530</v>
       </c>
       <c r="B344" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" ht="21">
+      <c r="A345" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B345" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="C344" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D344" s="20" t="s">
+      <c r="C345" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D345" s="20" t="s">
         <v>523</v>
       </c>
-      <c r="F344" s="57" t="s">
+      <c r="F345" s="57" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="345" spans="1:6" ht="21">
-      <c r="B345" s="4"/>
-      <c r="C345" s="2"/>
     </row>
     <row r="346" spans="1:6" ht="21">
       <c r="B346" s="4"/>
       <c r="C346" s="2"/>
     </row>
     <row r="347" spans="1:6" ht="21">
-      <c r="A347" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B347" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="C347" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B347" s="4"/>
+      <c r="C347" s="2"/>
     </row>
     <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
         <v>296</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>2</v>
@@ -6794,7 +6803,7 @@
         <v>296</v>
       </c>
       <c r="B349" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>2</v>
@@ -6805,7 +6814,7 @@
         <v>296</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6816,7 +6825,7 @@
         <v>296</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6827,7 +6836,7 @@
         <v>296</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6838,7 +6847,7 @@
         <v>296</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6849,10 +6858,10 @@
         <v>296</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>418</v>
+        <v>2</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="21">
@@ -6860,10 +6869,10 @@
         <v>296</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="21">
@@ -6871,7 +6880,7 @@
         <v>296</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6882,7 +6891,7 @@
         <v>296</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6893,7 +6902,7 @@
         <v>296</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6904,7 +6913,7 @@
         <v>296</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6915,7 +6924,7 @@
         <v>296</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6926,7 +6935,7 @@
         <v>296</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6937,7 +6946,7 @@
         <v>296</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6948,7 +6957,7 @@
         <v>296</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6959,7 +6968,7 @@
         <v>296</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6970,7 +6979,7 @@
         <v>296</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6981,7 +6990,7 @@
         <v>296</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6992,7 +7001,7 @@
         <v>296</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -7003,7 +7012,7 @@
         <v>296</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -7014,7 +7023,7 @@
         <v>296</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -7025,7 +7034,7 @@
         <v>296</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -7036,7 +7045,7 @@
         <v>296</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -7047,42 +7056,42 @@
         <v>296</v>
       </c>
       <c r="B372" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" ht="21">
+      <c r="A373" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B373" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="C372" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="373" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A373" s="6" t="s">
+      <c r="C373" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A374" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="B373" s="7" t="s">
+      <c r="B374" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C373" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D373" s="23"/>
-      <c r="F373" s="23"/>
-    </row>
-    <row r="374" spans="1:6" ht="21">
-      <c r="A374" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B374" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="C374" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C374" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D374" s="23"/>
+      <c r="F374" s="23"/>
     </row>
     <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
         <v>296</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -7093,7 +7102,7 @@
         <v>296</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>2</v>
@@ -7104,7 +7113,7 @@
         <v>296</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -7115,7 +7124,7 @@
         <v>296</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -7126,7 +7135,7 @@
         <v>296</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -7137,7 +7146,7 @@
         <v>296</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -7148,7 +7157,7 @@
         <v>296</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -7159,7 +7168,7 @@
         <v>296</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -7170,7 +7179,7 @@
         <v>296</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -7181,7 +7190,7 @@
         <v>296</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -7192,7 +7201,7 @@
         <v>296</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -7203,7 +7212,7 @@
         <v>296</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -7214,7 +7223,7 @@
         <v>296</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -7225,7 +7234,7 @@
         <v>296</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -7236,37 +7245,37 @@
         <v>296</v>
       </c>
       <c r="B389" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="21">
+      <c r="A390" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B390" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="C389" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="390" spans="1:3" ht="21">
-      <c r="B390" s="4"/>
-      <c r="C390" s="2"/>
+      <c r="C390" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="391" spans="1:3" ht="21">
       <c r="B391" s="4"/>
       <c r="C391" s="2"/>
     </row>
     <row r="392" spans="1:3" ht="21">
-      <c r="A392" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="B392" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="C392" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B392" s="4"/>
+      <c r="C392" s="2"/>
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
         <v>340</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>2</v>
@@ -7277,7 +7286,7 @@
         <v>340</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>2</v>
@@ -7288,7 +7297,7 @@
         <v>340</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>77</v>
+        <v>343</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7299,7 +7308,7 @@
         <v>340</v>
       </c>
       <c r="B396" s="13" t="s">
-        <v>344</v>
+        <v>77</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -7310,40 +7319,40 @@
         <v>340</v>
       </c>
       <c r="B397" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" ht="21">
+      <c r="A398" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B398" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="C397" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="398" spans="1:3" ht="21">
-      <c r="B398" s="4"/>
-      <c r="C398" s="2"/>
+      <c r="C398" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="399" spans="1:3" ht="21">
       <c r="B399" s="4"/>
       <c r="C399" s="2"/>
     </row>
     <row r="400" spans="1:3" ht="21">
-      <c r="A400" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B400" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C400" s="35" t="s">
-        <v>418</v>
-      </c>
+      <c r="B400" s="4"/>
+      <c r="C400" s="2"/>
     </row>
     <row r="401" spans="1:6" ht="21">
       <c r="A401" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B401" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="C401" s="2" t="s">
-        <v>2</v>
+        <v>347</v>
+      </c>
+      <c r="C401" s="35" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="21">
@@ -7351,7 +7360,7 @@
         <v>346</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>2</v>
@@ -7362,7 +7371,7 @@
         <v>346</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>2</v>
@@ -7373,7 +7382,7 @@
         <v>346</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7384,10 +7393,10 @@
         <v>346</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>418</v>
+        <v>2</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="21">
@@ -7395,10 +7404,10 @@
         <v>346</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="21">
@@ -7406,7 +7415,7 @@
         <v>346</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>237</v>
+        <v>353</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7417,7 +7426,7 @@
         <v>346</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>354</v>
+        <v>237</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>2</v>
@@ -7428,7 +7437,7 @@
         <v>346</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7439,7 +7448,7 @@
         <v>346</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>2</v>
@@ -7450,7 +7459,7 @@
         <v>346</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7461,31 +7470,29 @@
         <v>346</v>
       </c>
       <c r="B412" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" ht="21">
+      <c r="A413" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B413" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="C412" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="413" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A413" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="B413" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="C413" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D413" s="23"/>
-      <c r="F413" s="23"/>
+      <c r="C413" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="414" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A414" s="6" t="s">
         <v>346</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>2</v>
@@ -7493,23 +7500,25 @@
       <c r="D414" s="23"/>
       <c r="F414" s="23"/>
     </row>
-    <row r="415" spans="1:6" ht="21">
-      <c r="A415" s="3" t="s">
+    <row r="415" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A415" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B415" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="C415" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B415" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C415" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D415" s="23"/>
+      <c r="F415" s="23"/>
     </row>
     <row r="416" spans="1:6" ht="21">
       <c r="A416" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7520,7 +7529,7 @@
         <v>346</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7531,7 +7540,7 @@
         <v>346</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7542,7 +7551,7 @@
         <v>346</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7553,7 +7562,7 @@
         <v>346</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7564,7 +7573,7 @@
         <v>346</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7575,7 +7584,7 @@
         <v>346</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7586,7 +7595,7 @@
         <v>346</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7597,7 +7606,7 @@
         <v>346</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7608,7 +7617,7 @@
         <v>346</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7619,7 +7628,7 @@
         <v>346</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7630,7 +7639,7 @@
         <v>346</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7641,7 +7650,7 @@
         <v>346</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7652,7 +7661,7 @@
         <v>346</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7663,7 +7672,7 @@
         <v>346</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7674,7 +7683,7 @@
         <v>346</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7685,7 +7694,7 @@
         <v>346</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7696,42 +7705,42 @@
         <v>346</v>
       </c>
       <c r="B433" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="C433" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" ht="21">
+      <c r="A434" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B434" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="C433" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A434" s="6" t="s">
+      <c r="C434" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A435" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B434" s="7" t="s">
+      <c r="B435" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="C434" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D434" s="23"/>
-      <c r="F434" s="23"/>
-    </row>
-    <row r="435" spans="1:6" ht="21">
-      <c r="A435" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B435" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="C435" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C435" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D435" s="23"/>
+      <c r="F435" s="23"/>
     </row>
     <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7742,7 +7751,7 @@
         <v>346</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>2</v>
@@ -7753,7 +7762,7 @@
         <v>346</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7764,7 +7773,7 @@
         <v>346</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7775,7 +7784,7 @@
         <v>346</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7786,7 +7795,7 @@
         <v>346</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7797,7 +7806,7 @@
         <v>346</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7808,7 +7817,7 @@
         <v>346</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7819,7 +7828,7 @@
         <v>346</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7830,31 +7839,29 @@
         <v>346</v>
       </c>
       <c r="B445" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" ht="21">
+      <c r="A446" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B446" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="C445" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="446" spans="1:6" s="25" customFormat="1" ht="21">
-      <c r="A446" s="24" t="s">
-        <v>346</v>
-      </c>
-      <c r="B446" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="C446" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D446" s="26"/>
-      <c r="F446" s="26"/>
+      <c r="C446" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="447" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A447" s="24" t="s">
         <v>346</v>
       </c>
       <c r="B447" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C447" s="24" t="s">
         <v>2</v>
@@ -7862,23 +7869,25 @@
       <c r="D447" s="26"/>
       <c r="F447" s="26"/>
     </row>
-    <row r="448" spans="1:6" ht="21">
-      <c r="A448" s="3" t="s">
+    <row r="448" spans="1:6" s="25" customFormat="1" ht="21">
+      <c r="A448" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="B448" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="C448" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B448" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C448" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D448" s="26"/>
+      <c r="F448" s="26"/>
     </row>
     <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>2</v>
@@ -7889,7 +7898,7 @@
         <v>346</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>2</v>
@@ -7900,77 +7909,77 @@
         <v>346</v>
       </c>
       <c r="B451" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="C451" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" ht="21">
+      <c r="A452" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B452" s="13" t="s">
         <v>397</v>
       </c>
-      <c r="C451" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="452" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A452" s="6" t="s">
+      <c r="C452" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A453" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B452" s="7" t="s">
+      <c r="B453" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="C452" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D452" s="23"/>
-      <c r="F452" s="23"/>
-    </row>
-    <row r="453" spans="1:6" ht="21">
-      <c r="A453" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B453" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="C453" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C453" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D453" s="23"/>
+      <c r="F453" s="23"/>
     </row>
     <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B454" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="C454" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" ht="21">
+      <c r="A455" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B455" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="C454" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="455" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A455" s="6" t="s">
+      <c r="C455" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A456" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="B455" s="7" t="s">
+      <c r="B456" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="C455" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D455" s="23"/>
-      <c r="F455" s="23"/>
-    </row>
-    <row r="456" spans="1:6" ht="21">
-      <c r="A456" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="B456" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="C456" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C456" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D456" s="23"/>
+      <c r="F456" s="23"/>
     </row>
     <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7981,7 +7990,7 @@
         <v>346</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>2</v>
@@ -7992,50 +8001,44 @@
         <v>346</v>
       </c>
       <c r="B459" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="C459" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" ht="21">
+      <c r="A460" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B460" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="C459" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="460" spans="1:6" ht="21">
-      <c r="B460" s="4"/>
-      <c r="C460" s="2"/>
+      <c r="C460" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="461" spans="1:6" ht="21">
-      <c r="A461" s="5"/>
       <c r="B461" s="4"/>
       <c r="C461" s="2"/>
     </row>
     <row r="462" spans="1:6" ht="21">
-      <c r="A462" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="B462" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="C462" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D462" s="16" t="s">
-        <v>518</v>
-      </c>
+      <c r="A462" s="5"/>
+      <c r="B462" s="4"/>
+      <c r="C462" s="2"/>
     </row>
     <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C463" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D463" s="20" t="s">
-        <v>587</v>
-      </c>
-      <c r="F463" s="57" t="s">
-        <v>588</v>
+      <c r="D463" s="16" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="21">
@@ -8043,13 +8046,16 @@
         <v>406</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C464" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>589</v>
+        <v>587</v>
+      </c>
+      <c r="F464" s="57" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="21">
@@ -8057,13 +8063,13 @@
         <v>406</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="21">
@@ -8071,13 +8077,13 @@
         <v>406</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="21">
@@ -8085,13 +8091,13 @@
         <v>406</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>418</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="21">
@@ -8099,10 +8105,13 @@
         <v>406</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>2</v>
+        <v>418</v>
+      </c>
+      <c r="D468" s="20" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="21">
@@ -8110,13 +8119,10 @@
         <v>406</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D469" s="20" t="s">
-        <v>591</v>
+        <v>2</v>
       </c>
     </row>
     <row r="470" spans="1:6" ht="21">
@@ -8124,29 +8130,43 @@
         <v>406</v>
       </c>
       <c r="B470" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="C470" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D470" s="20" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" ht="21">
+      <c r="A471" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B471" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="C470" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D470" s="20" t="s">
+      <c r="C471" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D471" s="20" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="471" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A471" s="6" t="s">
+    <row r="472" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A472" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="B471" s="7" t="s">
+      <c r="B472" s="7" t="s">
         <v>585</v>
       </c>
-      <c r="C471" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="D471" s="22" t="s">
+      <c r="C472" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="D472" s="22" t="s">
         <v>584</v>
       </c>
-      <c r="F471" s="23"/>
+      <c r="F472" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8328,258 +8348,258 @@
     <hyperlink ref="B195" r:id="rId176"/>
     <hyperlink ref="B196" r:id="rId177" display="Find LCA in a Binary tree"/>
     <hyperlink ref="B198" r:id="rId178"/>
-    <hyperlink ref="B199" r:id="rId179"/>
-    <hyperlink ref="B200" r:id="rId180"/>
-    <hyperlink ref="B203" r:id="rId181" display="Fina a value in a BST"/>
-    <hyperlink ref="B206" r:id="rId182"/>
-    <hyperlink ref="B207" r:id="rId183"/>
-    <hyperlink ref="B208" r:id="rId184"/>
-    <hyperlink ref="B209" r:id="rId185"/>
-    <hyperlink ref="B210" r:id="rId186"/>
-    <hyperlink ref="B211" r:id="rId187"/>
-    <hyperlink ref="B212" r:id="rId188"/>
-    <hyperlink ref="B213" r:id="rId189"/>
-    <hyperlink ref="B214" r:id="rId190"/>
-    <hyperlink ref="B215" r:id="rId191" display="Merge two BST [ V.V.V&gt;IMP ]"/>
-    <hyperlink ref="B216" r:id="rId192"/>
-    <hyperlink ref="B217" r:id="rId193"/>
-    <hyperlink ref="B218" r:id="rId194"/>
-    <hyperlink ref="B219" r:id="rId195"/>
-    <hyperlink ref="B220" r:id="rId196"/>
-    <hyperlink ref="B221" r:id="rId197"/>
-    <hyperlink ref="B222" r:id="rId198"/>
-    <hyperlink ref="B223" r:id="rId199"/>
-    <hyperlink ref="B224" r:id="rId200"/>
-    <hyperlink ref="B225" r:id="rId201"/>
-    <hyperlink ref="B226" r:id="rId202"/>
-    <hyperlink ref="B229" r:id="rId203"/>
-    <hyperlink ref="B230" r:id="rId204"/>
-    <hyperlink ref="B231" r:id="rId205"/>
-    <hyperlink ref="B232" r:id="rId206"/>
-    <hyperlink ref="B233" r:id="rId207"/>
-    <hyperlink ref="B234" r:id="rId208"/>
-    <hyperlink ref="B235" r:id="rId209"/>
-    <hyperlink ref="B236" r:id="rId210"/>
-    <hyperlink ref="B237" r:id="rId211"/>
-    <hyperlink ref="B238" r:id="rId212"/>
-    <hyperlink ref="B239" r:id="rId213"/>
-    <hyperlink ref="B240" r:id="rId214"/>
-    <hyperlink ref="B241" r:id="rId215"/>
-    <hyperlink ref="B242" r:id="rId216"/>
-    <hyperlink ref="B243" r:id="rId217"/>
-    <hyperlink ref="B244" r:id="rId218"/>
-    <hyperlink ref="B245" r:id="rId219"/>
-    <hyperlink ref="B246" r:id="rId220"/>
-    <hyperlink ref="B247" r:id="rId221"/>
-    <hyperlink ref="B248" r:id="rId222" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B249" r:id="rId223"/>
-    <hyperlink ref="B250" r:id="rId224"/>
-    <hyperlink ref="B251" r:id="rId225"/>
-    <hyperlink ref="B252" r:id="rId226"/>
-    <hyperlink ref="B253" r:id="rId227"/>
-    <hyperlink ref="B254" r:id="rId228"/>
-    <hyperlink ref="B255" r:id="rId229"/>
-    <hyperlink ref="B256" r:id="rId230"/>
-    <hyperlink ref="B257" r:id="rId231"/>
-    <hyperlink ref="B258" r:id="rId232"/>
-    <hyperlink ref="B259" r:id="rId233"/>
-    <hyperlink ref="B260" r:id="rId234"/>
-    <hyperlink ref="B261" r:id="rId235"/>
-    <hyperlink ref="B262" r:id="rId236"/>
-    <hyperlink ref="B263" r:id="rId237"/>
-    <hyperlink ref="B266" r:id="rId238"/>
-    <hyperlink ref="B267" r:id="rId239"/>
-    <hyperlink ref="B268" r:id="rId240"/>
-    <hyperlink ref="B269" r:id="rId241"/>
-    <hyperlink ref="B270" r:id="rId242"/>
-    <hyperlink ref="B271" r:id="rId243"/>
-    <hyperlink ref="B272" r:id="rId244"/>
-    <hyperlink ref="B273" r:id="rId245"/>
-    <hyperlink ref="B274" r:id="rId246"/>
-    <hyperlink ref="B275" r:id="rId247"/>
-    <hyperlink ref="B276" r:id="rId248"/>
-    <hyperlink ref="B277" r:id="rId249" display="Combinational Sum"/>
-    <hyperlink ref="B278" r:id="rId250"/>
-    <hyperlink ref="B279" r:id="rId251"/>
-    <hyperlink ref="B280" r:id="rId252"/>
-    <hyperlink ref="B281" r:id="rId253"/>
-    <hyperlink ref="B282" r:id="rId254"/>
-    <hyperlink ref="B283" r:id="rId255"/>
-    <hyperlink ref="B284" r:id="rId256"/>
-    <hyperlink ref="B287" r:id="rId257"/>
-    <hyperlink ref="B288" r:id="rId258"/>
-    <hyperlink ref="B289" r:id="rId259"/>
-    <hyperlink ref="B290" r:id="rId260"/>
-    <hyperlink ref="B291" r:id="rId261"/>
-    <hyperlink ref="B292" r:id="rId262" display="Check the expression has valid or Balanced parenthesis or not."/>
-    <hyperlink ref="B293" r:id="rId263"/>
-    <hyperlink ref="B294" r:id="rId264"/>
-    <hyperlink ref="B295" r:id="rId265"/>
-    <hyperlink ref="B296" r:id="rId266" display="The celebrity Problem"/>
-    <hyperlink ref="B297" r:id="rId267"/>
-    <hyperlink ref="B298" r:id="rId268"/>
-    <hyperlink ref="B299" r:id="rId269"/>
-    <hyperlink ref="B300" r:id="rId270"/>
-    <hyperlink ref="B301" r:id="rId271"/>
-    <hyperlink ref="B302" r:id="rId272" display="Largest rectangular Area in Histogram"/>
-    <hyperlink ref="B303" r:id="rId273"/>
-    <hyperlink ref="B304" r:id="rId274"/>
-    <hyperlink ref="B305" r:id="rId275" display="Implement Stack using Queue"/>
-    <hyperlink ref="B306" r:id="rId276"/>
-    <hyperlink ref="B307" r:id="rId277"/>
-    <hyperlink ref="B308" r:id="rId278" display="Implement Queue using Stack  "/>
-    <hyperlink ref="B309" r:id="rId279"/>
-    <hyperlink ref="B310" r:id="rId280"/>
-    <hyperlink ref="B311" r:id="rId281"/>
-    <hyperlink ref="B312" r:id="rId282"/>
-    <hyperlink ref="B313" r:id="rId283"/>
-    <hyperlink ref="B314" r:id="rId284"/>
-    <hyperlink ref="B315" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps"/>
-    <hyperlink ref="B316" r:id="rId286"/>
-    <hyperlink ref="B317" r:id="rId287"/>
-    <hyperlink ref="B318" r:id="rId288" display="First negative integer in every window of size “k”"/>
-    <hyperlink ref="B319" r:id="rId289"/>
-    <hyperlink ref="B320" r:id="rId290"/>
-    <hyperlink ref="B321" r:id="rId291"/>
-    <hyperlink ref="B322" r:id="rId292"/>
-    <hyperlink ref="B324" r:id="rId293" display="Next Smaller Element"/>
-    <hyperlink ref="B327" r:id="rId294"/>
-    <hyperlink ref="B328" r:id="rId295"/>
-    <hyperlink ref="B329" r:id="rId296"/>
-    <hyperlink ref="B330" r:id="rId297"/>
-    <hyperlink ref="B331" r:id="rId298"/>
-    <hyperlink ref="B332" r:id="rId299"/>
-    <hyperlink ref="B333" r:id="rId300"/>
-    <hyperlink ref="B334" r:id="rId301"/>
-    <hyperlink ref="B335" r:id="rId302"/>
-    <hyperlink ref="B336" r:id="rId303" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
-    <hyperlink ref="B337" r:id="rId304"/>
-    <hyperlink ref="B338" r:id="rId305"/>
-    <hyperlink ref="B339" r:id="rId306"/>
-    <hyperlink ref="B340" r:id="rId307"/>
-    <hyperlink ref="B341" r:id="rId308"/>
-    <hyperlink ref="B342" r:id="rId309"/>
-    <hyperlink ref="B343" r:id="rId310"/>
-    <hyperlink ref="B344" r:id="rId311"/>
-    <hyperlink ref="B348" r:id="rId312"/>
-    <hyperlink ref="B349" r:id="rId313"/>
-    <hyperlink ref="B350" r:id="rId314"/>
-    <hyperlink ref="B351" r:id="rId315"/>
-    <hyperlink ref="B352" r:id="rId316"/>
-    <hyperlink ref="B353" r:id="rId317"/>
-    <hyperlink ref="B354" r:id="rId318"/>
-    <hyperlink ref="B355" r:id="rId319"/>
-    <hyperlink ref="B356" r:id="rId320"/>
-    <hyperlink ref="B357" r:id="rId321"/>
-    <hyperlink ref="B358" r:id="rId322"/>
-    <hyperlink ref="B359" r:id="rId323"/>
-    <hyperlink ref="B360" r:id="rId324"/>
-    <hyperlink ref="B361" r:id="rId325"/>
-    <hyperlink ref="B362" r:id="rId326"/>
-    <hyperlink ref="B363" r:id="rId327"/>
-    <hyperlink ref="B364" r:id="rId328"/>
-    <hyperlink ref="B365" r:id="rId329"/>
-    <hyperlink ref="B366" r:id="rId330"/>
-    <hyperlink ref="B367" r:id="rId331"/>
-    <hyperlink ref="B368" r:id="rId332"/>
-    <hyperlink ref="B369" r:id="rId333"/>
-    <hyperlink ref="B370" r:id="rId334" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B371" r:id="rId335"/>
-    <hyperlink ref="B372" r:id="rId336"/>
-    <hyperlink ref="B373" r:id="rId337"/>
-    <hyperlink ref="B374" r:id="rId338"/>
-    <hyperlink ref="B375" r:id="rId339"/>
-    <hyperlink ref="B376" r:id="rId340"/>
-    <hyperlink ref="B377" r:id="rId341"/>
-    <hyperlink ref="B378" r:id="rId342"/>
-    <hyperlink ref="B379" r:id="rId343"/>
-    <hyperlink ref="B380" r:id="rId344"/>
-    <hyperlink ref="B381" r:id="rId345"/>
-    <hyperlink ref="B382" r:id="rId346"/>
-    <hyperlink ref="B383" r:id="rId347"/>
-    <hyperlink ref="B384" r:id="rId348"/>
-    <hyperlink ref="B386" r:id="rId349"/>
-    <hyperlink ref="B385" r:id="rId350"/>
-    <hyperlink ref="B387" r:id="rId351"/>
-    <hyperlink ref="B388" r:id="rId352"/>
-    <hyperlink ref="B389" r:id="rId353"/>
-    <hyperlink ref="B392" r:id="rId354"/>
-    <hyperlink ref="B393" r:id="rId355"/>
-    <hyperlink ref="B394" r:id="rId356"/>
-    <hyperlink ref="B395" r:id="rId357"/>
-    <hyperlink ref="B396" r:id="rId358"/>
-    <hyperlink ref="B397" r:id="rId359"/>
-    <hyperlink ref="B400" r:id="rId360"/>
-    <hyperlink ref="B401" r:id="rId361"/>
-    <hyperlink ref="B402" r:id="rId362"/>
-    <hyperlink ref="B403" r:id="rId363"/>
-    <hyperlink ref="B404" r:id="rId364"/>
-    <hyperlink ref="B405" r:id="rId365"/>
-    <hyperlink ref="B406" r:id="rId366"/>
-    <hyperlink ref="B407" r:id="rId367"/>
-    <hyperlink ref="B408" r:id="rId368"/>
-    <hyperlink ref="B409" r:id="rId369"/>
-    <hyperlink ref="B410" r:id="rId370"/>
-    <hyperlink ref="B411" r:id="rId371"/>
-    <hyperlink ref="B412" r:id="rId372"/>
-    <hyperlink ref="B413" r:id="rId373"/>
-    <hyperlink ref="B414" r:id="rId374"/>
-    <hyperlink ref="B415" r:id="rId375"/>
-    <hyperlink ref="B416" r:id="rId376"/>
-    <hyperlink ref="B417" r:id="rId377"/>
-    <hyperlink ref="B418" r:id="rId378"/>
-    <hyperlink ref="B419" r:id="rId379"/>
-    <hyperlink ref="B420" r:id="rId380"/>
-    <hyperlink ref="B421" r:id="rId381"/>
-    <hyperlink ref="B422" r:id="rId382"/>
-    <hyperlink ref="B423" r:id="rId383"/>
-    <hyperlink ref="B424" r:id="rId384"/>
-    <hyperlink ref="B425" r:id="rId385"/>
-    <hyperlink ref="B426" r:id="rId386"/>
-    <hyperlink ref="B427" r:id="rId387"/>
-    <hyperlink ref="B428" r:id="rId388"/>
-    <hyperlink ref="B429" r:id="rId389"/>
-    <hyperlink ref="B430" r:id="rId390"/>
-    <hyperlink ref="B431" r:id="rId391"/>
-    <hyperlink ref="B432" r:id="rId392"/>
-    <hyperlink ref="B433" r:id="rId393"/>
-    <hyperlink ref="B434" r:id="rId394"/>
-    <hyperlink ref="B435" r:id="rId395"/>
-    <hyperlink ref="B436" r:id="rId396"/>
-    <hyperlink ref="B437" r:id="rId397"/>
-    <hyperlink ref="B438" r:id="rId398"/>
-    <hyperlink ref="B439" r:id="rId399"/>
-    <hyperlink ref="B441" r:id="rId400"/>
-    <hyperlink ref="B440" r:id="rId401"/>
-    <hyperlink ref="B442" r:id="rId402"/>
-    <hyperlink ref="B443" r:id="rId403"/>
-    <hyperlink ref="B444" r:id="rId404"/>
-    <hyperlink ref="B445" r:id="rId405"/>
-    <hyperlink ref="B446" r:id="rId406"/>
-    <hyperlink ref="B447" r:id="rId407"/>
-    <hyperlink ref="B448" r:id="rId408"/>
-    <hyperlink ref="B449" r:id="rId409"/>
-    <hyperlink ref="B450" r:id="rId410"/>
-    <hyperlink ref="B451" r:id="rId411"/>
-    <hyperlink ref="B452" r:id="rId412"/>
-    <hyperlink ref="B459" r:id="rId413"/>
-    <hyperlink ref="B458" r:id="rId414"/>
-    <hyperlink ref="B457" r:id="rId415"/>
-    <hyperlink ref="B456" r:id="rId416"/>
-    <hyperlink ref="B455" r:id="rId417"/>
-    <hyperlink ref="B454" r:id="rId418"/>
-    <hyperlink ref="B453" r:id="rId419"/>
-    <hyperlink ref="B462" r:id="rId420"/>
-    <hyperlink ref="B463" r:id="rId421"/>
-    <hyperlink ref="B464" r:id="rId422"/>
-    <hyperlink ref="B465" r:id="rId423"/>
-    <hyperlink ref="B466" r:id="rId424"/>
-    <hyperlink ref="B467" r:id="rId425"/>
-    <hyperlink ref="B468" r:id="rId426"/>
-    <hyperlink ref="B471" r:id="rId427" display="Power Set"/>
-    <hyperlink ref="B469" r:id="rId428"/>
-    <hyperlink ref="B470" r:id="rId429" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B347" r:id="rId430"/>
+    <hyperlink ref="B200" r:id="rId179"/>
+    <hyperlink ref="B201" r:id="rId180"/>
+    <hyperlink ref="B204" r:id="rId181" display="Fina a value in a BST"/>
+    <hyperlink ref="B207" r:id="rId182"/>
+    <hyperlink ref="B208" r:id="rId183"/>
+    <hyperlink ref="B209" r:id="rId184"/>
+    <hyperlink ref="B210" r:id="rId185"/>
+    <hyperlink ref="B211" r:id="rId186"/>
+    <hyperlink ref="B212" r:id="rId187"/>
+    <hyperlink ref="B213" r:id="rId188"/>
+    <hyperlink ref="B214" r:id="rId189"/>
+    <hyperlink ref="B215" r:id="rId190"/>
+    <hyperlink ref="B216" r:id="rId191" display="Merge two BST [ V.V.V&gt;IMP ]"/>
+    <hyperlink ref="B217" r:id="rId192"/>
+    <hyperlink ref="B218" r:id="rId193"/>
+    <hyperlink ref="B219" r:id="rId194"/>
+    <hyperlink ref="B220" r:id="rId195"/>
+    <hyperlink ref="B221" r:id="rId196"/>
+    <hyperlink ref="B222" r:id="rId197"/>
+    <hyperlink ref="B223" r:id="rId198"/>
+    <hyperlink ref="B224" r:id="rId199"/>
+    <hyperlink ref="B225" r:id="rId200"/>
+    <hyperlink ref="B226" r:id="rId201"/>
+    <hyperlink ref="B227" r:id="rId202"/>
+    <hyperlink ref="B230" r:id="rId203"/>
+    <hyperlink ref="B231" r:id="rId204"/>
+    <hyperlink ref="B232" r:id="rId205"/>
+    <hyperlink ref="B233" r:id="rId206"/>
+    <hyperlink ref="B234" r:id="rId207"/>
+    <hyperlink ref="B235" r:id="rId208"/>
+    <hyperlink ref="B236" r:id="rId209"/>
+    <hyperlink ref="B237" r:id="rId210"/>
+    <hyperlink ref="B238" r:id="rId211"/>
+    <hyperlink ref="B239" r:id="rId212"/>
+    <hyperlink ref="B240" r:id="rId213"/>
+    <hyperlink ref="B241" r:id="rId214"/>
+    <hyperlink ref="B242" r:id="rId215"/>
+    <hyperlink ref="B243" r:id="rId216"/>
+    <hyperlink ref="B244" r:id="rId217"/>
+    <hyperlink ref="B245" r:id="rId218"/>
+    <hyperlink ref="B246" r:id="rId219"/>
+    <hyperlink ref="B247" r:id="rId220"/>
+    <hyperlink ref="B248" r:id="rId221"/>
+    <hyperlink ref="B249" r:id="rId222" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B250" r:id="rId223"/>
+    <hyperlink ref="B251" r:id="rId224"/>
+    <hyperlink ref="B252" r:id="rId225"/>
+    <hyperlink ref="B253" r:id="rId226"/>
+    <hyperlink ref="B254" r:id="rId227"/>
+    <hyperlink ref="B255" r:id="rId228"/>
+    <hyperlink ref="B256" r:id="rId229"/>
+    <hyperlink ref="B257" r:id="rId230"/>
+    <hyperlink ref="B258" r:id="rId231"/>
+    <hyperlink ref="B259" r:id="rId232"/>
+    <hyperlink ref="B260" r:id="rId233"/>
+    <hyperlink ref="B261" r:id="rId234"/>
+    <hyperlink ref="B262" r:id="rId235"/>
+    <hyperlink ref="B263" r:id="rId236"/>
+    <hyperlink ref="B264" r:id="rId237"/>
+    <hyperlink ref="B267" r:id="rId238"/>
+    <hyperlink ref="B268" r:id="rId239"/>
+    <hyperlink ref="B269" r:id="rId240"/>
+    <hyperlink ref="B270" r:id="rId241"/>
+    <hyperlink ref="B271" r:id="rId242"/>
+    <hyperlink ref="B272" r:id="rId243"/>
+    <hyperlink ref="B273" r:id="rId244"/>
+    <hyperlink ref="B274" r:id="rId245"/>
+    <hyperlink ref="B275" r:id="rId246"/>
+    <hyperlink ref="B276" r:id="rId247"/>
+    <hyperlink ref="B277" r:id="rId248"/>
+    <hyperlink ref="B278" r:id="rId249" display="Combinational Sum"/>
+    <hyperlink ref="B279" r:id="rId250"/>
+    <hyperlink ref="B280" r:id="rId251"/>
+    <hyperlink ref="B281" r:id="rId252"/>
+    <hyperlink ref="B282" r:id="rId253"/>
+    <hyperlink ref="B283" r:id="rId254"/>
+    <hyperlink ref="B284" r:id="rId255"/>
+    <hyperlink ref="B285" r:id="rId256"/>
+    <hyperlink ref="B288" r:id="rId257"/>
+    <hyperlink ref="B289" r:id="rId258"/>
+    <hyperlink ref="B290" r:id="rId259"/>
+    <hyperlink ref="B291" r:id="rId260"/>
+    <hyperlink ref="B292" r:id="rId261"/>
+    <hyperlink ref="B293" r:id="rId262" display="Check the expression has valid or Balanced parenthesis or not."/>
+    <hyperlink ref="B294" r:id="rId263"/>
+    <hyperlink ref="B295" r:id="rId264"/>
+    <hyperlink ref="B296" r:id="rId265"/>
+    <hyperlink ref="B297" r:id="rId266" display="The celebrity Problem"/>
+    <hyperlink ref="B298" r:id="rId267"/>
+    <hyperlink ref="B299" r:id="rId268"/>
+    <hyperlink ref="B300" r:id="rId269"/>
+    <hyperlink ref="B301" r:id="rId270"/>
+    <hyperlink ref="B302" r:id="rId271"/>
+    <hyperlink ref="B303" r:id="rId272" display="Largest rectangular Area in Histogram"/>
+    <hyperlink ref="B304" r:id="rId273"/>
+    <hyperlink ref="B305" r:id="rId274"/>
+    <hyperlink ref="B306" r:id="rId275" display="Implement Stack using Queue"/>
+    <hyperlink ref="B307" r:id="rId276"/>
+    <hyperlink ref="B308" r:id="rId277"/>
+    <hyperlink ref="B309" r:id="rId278" display="Implement Queue using Stack  "/>
+    <hyperlink ref="B310" r:id="rId279"/>
+    <hyperlink ref="B311" r:id="rId280"/>
+    <hyperlink ref="B312" r:id="rId281"/>
+    <hyperlink ref="B313" r:id="rId282"/>
+    <hyperlink ref="B314" r:id="rId283"/>
+    <hyperlink ref="B315" r:id="rId284"/>
+    <hyperlink ref="B316" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps"/>
+    <hyperlink ref="B317" r:id="rId286"/>
+    <hyperlink ref="B318" r:id="rId287"/>
+    <hyperlink ref="B319" r:id="rId288" display="First negative integer in every window of size “k”"/>
+    <hyperlink ref="B320" r:id="rId289"/>
+    <hyperlink ref="B321" r:id="rId290"/>
+    <hyperlink ref="B322" r:id="rId291"/>
+    <hyperlink ref="B323" r:id="rId292"/>
+    <hyperlink ref="B325" r:id="rId293" display="Next Smaller Element"/>
+    <hyperlink ref="B328" r:id="rId294"/>
+    <hyperlink ref="B329" r:id="rId295"/>
+    <hyperlink ref="B330" r:id="rId296"/>
+    <hyperlink ref="B331" r:id="rId297"/>
+    <hyperlink ref="B332" r:id="rId298"/>
+    <hyperlink ref="B333" r:id="rId299"/>
+    <hyperlink ref="B334" r:id="rId300"/>
+    <hyperlink ref="B335" r:id="rId301"/>
+    <hyperlink ref="B336" r:id="rId302"/>
+    <hyperlink ref="B337" r:id="rId303" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
+    <hyperlink ref="B338" r:id="rId304"/>
+    <hyperlink ref="B339" r:id="rId305"/>
+    <hyperlink ref="B340" r:id="rId306"/>
+    <hyperlink ref="B341" r:id="rId307"/>
+    <hyperlink ref="B342" r:id="rId308"/>
+    <hyperlink ref="B343" r:id="rId309"/>
+    <hyperlink ref="B344" r:id="rId310"/>
+    <hyperlink ref="B345" r:id="rId311"/>
+    <hyperlink ref="B349" r:id="rId312"/>
+    <hyperlink ref="B350" r:id="rId313"/>
+    <hyperlink ref="B351" r:id="rId314"/>
+    <hyperlink ref="B352" r:id="rId315"/>
+    <hyperlink ref="B353" r:id="rId316"/>
+    <hyperlink ref="B354" r:id="rId317"/>
+    <hyperlink ref="B355" r:id="rId318"/>
+    <hyperlink ref="B356" r:id="rId319"/>
+    <hyperlink ref="B357" r:id="rId320"/>
+    <hyperlink ref="B358" r:id="rId321"/>
+    <hyperlink ref="B359" r:id="rId322"/>
+    <hyperlink ref="B360" r:id="rId323"/>
+    <hyperlink ref="B361" r:id="rId324"/>
+    <hyperlink ref="B362" r:id="rId325"/>
+    <hyperlink ref="B363" r:id="rId326"/>
+    <hyperlink ref="B364" r:id="rId327"/>
+    <hyperlink ref="B365" r:id="rId328"/>
+    <hyperlink ref="B366" r:id="rId329"/>
+    <hyperlink ref="B367" r:id="rId330"/>
+    <hyperlink ref="B368" r:id="rId331"/>
+    <hyperlink ref="B369" r:id="rId332"/>
+    <hyperlink ref="B370" r:id="rId333"/>
+    <hyperlink ref="B371" r:id="rId334" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B372" r:id="rId335"/>
+    <hyperlink ref="B373" r:id="rId336"/>
+    <hyperlink ref="B374" r:id="rId337"/>
+    <hyperlink ref="B375" r:id="rId338"/>
+    <hyperlink ref="B376" r:id="rId339"/>
+    <hyperlink ref="B377" r:id="rId340"/>
+    <hyperlink ref="B378" r:id="rId341"/>
+    <hyperlink ref="B379" r:id="rId342"/>
+    <hyperlink ref="B380" r:id="rId343"/>
+    <hyperlink ref="B381" r:id="rId344"/>
+    <hyperlink ref="B382" r:id="rId345"/>
+    <hyperlink ref="B383" r:id="rId346"/>
+    <hyperlink ref="B384" r:id="rId347"/>
+    <hyperlink ref="B385" r:id="rId348"/>
+    <hyperlink ref="B387" r:id="rId349"/>
+    <hyperlink ref="B386" r:id="rId350"/>
+    <hyperlink ref="B388" r:id="rId351"/>
+    <hyperlink ref="B389" r:id="rId352"/>
+    <hyperlink ref="B390" r:id="rId353"/>
+    <hyperlink ref="B393" r:id="rId354"/>
+    <hyperlink ref="B394" r:id="rId355"/>
+    <hyperlink ref="B395" r:id="rId356"/>
+    <hyperlink ref="B396" r:id="rId357"/>
+    <hyperlink ref="B397" r:id="rId358"/>
+    <hyperlink ref="B398" r:id="rId359"/>
+    <hyperlink ref="B401" r:id="rId360"/>
+    <hyperlink ref="B402" r:id="rId361"/>
+    <hyperlink ref="B403" r:id="rId362"/>
+    <hyperlink ref="B404" r:id="rId363"/>
+    <hyperlink ref="B405" r:id="rId364"/>
+    <hyperlink ref="B406" r:id="rId365"/>
+    <hyperlink ref="B407" r:id="rId366"/>
+    <hyperlink ref="B408" r:id="rId367"/>
+    <hyperlink ref="B409" r:id="rId368"/>
+    <hyperlink ref="B410" r:id="rId369"/>
+    <hyperlink ref="B411" r:id="rId370"/>
+    <hyperlink ref="B412" r:id="rId371"/>
+    <hyperlink ref="B413" r:id="rId372"/>
+    <hyperlink ref="B414" r:id="rId373"/>
+    <hyperlink ref="B415" r:id="rId374"/>
+    <hyperlink ref="B416" r:id="rId375"/>
+    <hyperlink ref="B417" r:id="rId376"/>
+    <hyperlink ref="B418" r:id="rId377"/>
+    <hyperlink ref="B419" r:id="rId378"/>
+    <hyperlink ref="B420" r:id="rId379"/>
+    <hyperlink ref="B421" r:id="rId380"/>
+    <hyperlink ref="B422" r:id="rId381"/>
+    <hyperlink ref="B423" r:id="rId382"/>
+    <hyperlink ref="B424" r:id="rId383"/>
+    <hyperlink ref="B425" r:id="rId384"/>
+    <hyperlink ref="B426" r:id="rId385"/>
+    <hyperlink ref="B427" r:id="rId386"/>
+    <hyperlink ref="B428" r:id="rId387"/>
+    <hyperlink ref="B429" r:id="rId388"/>
+    <hyperlink ref="B430" r:id="rId389"/>
+    <hyperlink ref="B431" r:id="rId390"/>
+    <hyperlink ref="B432" r:id="rId391"/>
+    <hyperlink ref="B433" r:id="rId392"/>
+    <hyperlink ref="B434" r:id="rId393"/>
+    <hyperlink ref="B435" r:id="rId394"/>
+    <hyperlink ref="B436" r:id="rId395"/>
+    <hyperlink ref="B437" r:id="rId396"/>
+    <hyperlink ref="B438" r:id="rId397"/>
+    <hyperlink ref="B439" r:id="rId398"/>
+    <hyperlink ref="B440" r:id="rId399"/>
+    <hyperlink ref="B442" r:id="rId400"/>
+    <hyperlink ref="B441" r:id="rId401"/>
+    <hyperlink ref="B443" r:id="rId402"/>
+    <hyperlink ref="B444" r:id="rId403"/>
+    <hyperlink ref="B445" r:id="rId404"/>
+    <hyperlink ref="B446" r:id="rId405"/>
+    <hyperlink ref="B447" r:id="rId406"/>
+    <hyperlink ref="B448" r:id="rId407"/>
+    <hyperlink ref="B449" r:id="rId408"/>
+    <hyperlink ref="B450" r:id="rId409"/>
+    <hyperlink ref="B451" r:id="rId410"/>
+    <hyperlink ref="B452" r:id="rId411"/>
+    <hyperlink ref="B453" r:id="rId412"/>
+    <hyperlink ref="B460" r:id="rId413"/>
+    <hyperlink ref="B459" r:id="rId414"/>
+    <hyperlink ref="B458" r:id="rId415"/>
+    <hyperlink ref="B457" r:id="rId416"/>
+    <hyperlink ref="B456" r:id="rId417"/>
+    <hyperlink ref="B455" r:id="rId418"/>
+    <hyperlink ref="B454" r:id="rId419"/>
+    <hyperlink ref="B463" r:id="rId420"/>
+    <hyperlink ref="B464" r:id="rId421"/>
+    <hyperlink ref="B465" r:id="rId422"/>
+    <hyperlink ref="B466" r:id="rId423"/>
+    <hyperlink ref="B467" r:id="rId424"/>
+    <hyperlink ref="B468" r:id="rId425"/>
+    <hyperlink ref="B469" r:id="rId426"/>
+    <hyperlink ref="B472" r:id="rId427" display="Power Set"/>
+    <hyperlink ref="B470" r:id="rId428"/>
+    <hyperlink ref="B471" r:id="rId429" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B348" r:id="rId430"/>
     <hyperlink ref="D16" r:id="rId431"/>
     <hyperlink ref="D5" r:id="rId432"/>
     <hyperlink ref="D7" r:id="rId433"/>
@@ -8639,26 +8659,26 @@
     <hyperlink ref="D197" r:id="rId487"/>
     <hyperlink ref="B197" r:id="rId488"/>
     <hyperlink ref="D182" r:id="rId489"/>
-    <hyperlink ref="D203" r:id="rId490"/>
+    <hyperlink ref="D204" r:id="rId490"/>
     <hyperlink ref="D196" r:id="rId491"/>
     <hyperlink ref="D166" r:id="rId492"/>
     <hyperlink ref="D184" r:id="rId493"/>
     <hyperlink ref="D190" r:id="rId494"/>
-    <hyperlink ref="D204" r:id="rId495"/>
-    <hyperlink ref="D217" r:id="rId496"/>
+    <hyperlink ref="D205" r:id="rId495"/>
+    <hyperlink ref="D218" r:id="rId496"/>
     <hyperlink ref="D186" r:id="rId497"/>
-    <hyperlink ref="D207" r:id="rId498"/>
+    <hyperlink ref="D208" r:id="rId498"/>
     <hyperlink ref="D25" r:id="rId499"/>
-    <hyperlink ref="D209" r:id="rId500"/>
-    <hyperlink ref="D220" r:id="rId501"/>
-    <hyperlink ref="D211" r:id="rId502"/>
+    <hyperlink ref="D210" r:id="rId500"/>
+    <hyperlink ref="D221" r:id="rId501"/>
+    <hyperlink ref="D212" r:id="rId502"/>
     <hyperlink ref="D49" r:id="rId503"/>
-    <hyperlink ref="D208" r:id="rId504"/>
-    <hyperlink ref="D330" r:id="rId505"/>
-    <hyperlink ref="D340" r:id="rId506"/>
-    <hyperlink ref="D336" r:id="rId507"/>
-    <hyperlink ref="D344" r:id="rId508"/>
-    <hyperlink ref="D335" r:id="rId509"/>
+    <hyperlink ref="D209" r:id="rId504"/>
+    <hyperlink ref="D331" r:id="rId505"/>
+    <hyperlink ref="D341" r:id="rId506"/>
+    <hyperlink ref="D337" r:id="rId507"/>
+    <hyperlink ref="D345" r:id="rId508"/>
+    <hyperlink ref="D336" r:id="rId509"/>
     <hyperlink ref="D9" r:id="rId510"/>
     <hyperlink ref="D38" r:id="rId511"/>
     <hyperlink ref="D23" r:id="rId512"/>
@@ -8668,7 +8688,7 @@
     <hyperlink ref="D43" r:id="rId516"/>
     <hyperlink ref="D45" r:id="rId517"/>
     <hyperlink ref="D50" r:id="rId518"/>
-    <hyperlink ref="D277" r:id="rId519"/>
+    <hyperlink ref="D278" r:id="rId519"/>
     <hyperlink ref="D27" r:id="rId520"/>
     <hyperlink ref="D24" r:id="rId521"/>
     <hyperlink ref="D37" r:id="rId522"/>
@@ -8679,46 +8699,47 @@
     <hyperlink ref="D99" r:id="rId527"/>
     <hyperlink ref="D22" r:id="rId528"/>
     <hyperlink ref="D100" r:id="rId529"/>
-    <hyperlink ref="D289" r:id="rId530"/>
-    <hyperlink ref="D293" r:id="rId531"/>
-    <hyperlink ref="D290" r:id="rId532"/>
-    <hyperlink ref="D298" r:id="rId533"/>
-    <hyperlink ref="D300" r:id="rId534"/>
-    <hyperlink ref="D294" r:id="rId535"/>
-    <hyperlink ref="D292" r:id="rId536"/>
-    <hyperlink ref="D299" r:id="rId537"/>
-    <hyperlink ref="D304" r:id="rId538"/>
+    <hyperlink ref="D290" r:id="rId530"/>
+    <hyperlink ref="D294" r:id="rId531"/>
+    <hyperlink ref="D291" r:id="rId532"/>
+    <hyperlink ref="D299" r:id="rId533"/>
+    <hyperlink ref="D301" r:id="rId534"/>
+    <hyperlink ref="D295" r:id="rId535"/>
+    <hyperlink ref="D293" r:id="rId536"/>
+    <hyperlink ref="D300" r:id="rId537"/>
+    <hyperlink ref="D305" r:id="rId538"/>
     <hyperlink ref="D78" r:id="rId539"/>
     <hyperlink ref="D73" r:id="rId540"/>
-    <hyperlink ref="D324" r:id="rId541"/>
-    <hyperlink ref="D295" r:id="rId542"/>
-    <hyperlink ref="D302" r:id="rId543"/>
-    <hyperlink ref="D296" r:id="rId544"/>
+    <hyperlink ref="D325" r:id="rId541"/>
+    <hyperlink ref="D296" r:id="rId542"/>
+    <hyperlink ref="D303" r:id="rId543"/>
+    <hyperlink ref="D297" r:id="rId544"/>
     <hyperlink ref="D47" r:id="rId545"/>
-    <hyperlink ref="F294" r:id="rId546"/>
-    <hyperlink ref="D310" r:id="rId547"/>
-    <hyperlink ref="D312" r:id="rId548"/>
-    <hyperlink ref="D318" r:id="rId549"/>
-    <hyperlink ref="B323" r:id="rId550"/>
-    <hyperlink ref="D323" r:id="rId551"/>
-    <hyperlink ref="D465" r:id="rId552"/>
-    <hyperlink ref="D466" r:id="rId553"/>
-    <hyperlink ref="D471" r:id="rId554"/>
-    <hyperlink ref="D467" r:id="rId555"/>
-    <hyperlink ref="D463" r:id="rId556"/>
-    <hyperlink ref="D464" r:id="rId557"/>
-    <hyperlink ref="D470" r:id="rId558"/>
-    <hyperlink ref="D469" r:id="rId559"/>
+    <hyperlink ref="F295" r:id="rId546"/>
+    <hyperlink ref="D311" r:id="rId547"/>
+    <hyperlink ref="D313" r:id="rId548"/>
+    <hyperlink ref="D319" r:id="rId549"/>
+    <hyperlink ref="B324" r:id="rId550"/>
+    <hyperlink ref="D324" r:id="rId551"/>
+    <hyperlink ref="D466" r:id="rId552"/>
+    <hyperlink ref="D467" r:id="rId553"/>
+    <hyperlink ref="D472" r:id="rId554"/>
+    <hyperlink ref="D468" r:id="rId555"/>
+    <hyperlink ref="D464" r:id="rId556"/>
+    <hyperlink ref="D465" r:id="rId557"/>
+    <hyperlink ref="D471" r:id="rId558"/>
+    <hyperlink ref="D470" r:id="rId559"/>
     <hyperlink ref="D105" r:id="rId560"/>
     <hyperlink ref="D104" r:id="rId561"/>
     <hyperlink ref="D107" r:id="rId562"/>
     <hyperlink ref="D112" r:id="rId563"/>
-    <hyperlink ref="D313" r:id="rId564"/>
-    <hyperlink ref="D314" r:id="rId565"/>
-    <hyperlink ref="D297" r:id="rId566"/>
-    <hyperlink ref="D305" r:id="rId567"/>
+    <hyperlink ref="D314" r:id="rId564"/>
+    <hyperlink ref="D315" r:id="rId565"/>
+    <hyperlink ref="D298" r:id="rId566"/>
+    <hyperlink ref="D306" r:id="rId567"/>
+    <hyperlink ref="B199" r:id="rId568" display="Kth Ancestor of node in a Binary tree"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId568"/>
+  <pageSetup orientation="portrait" r:id="rId569"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
circular tour of Gas Station
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="610">
   <si>
     <t>Topic:</t>
   </si>
@@ -837,12 +837,6 @@
   </si>
   <si>
     <t>Reverse the first “K” elements of a queue</t>
-  </si>
-  <si>
-    <t>Interleave the first half of the queue with second half</t>
-  </si>
-  <si>
-    <t>Minimum time required to rot all oranges</t>
   </si>
   <si>
     <t>Distance of nearest cell having 1 in a binary matrix</t>
@@ -1861,6 +1855,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/merge-two-binary-trees/</t>
+  </si>
+  <si>
+    <t>Minimum time required to rot all oranges IMP</t>
+  </si>
+  <si>
+    <t>if asked to only use stack as auxiliary space then we have to go through a very weird procedure</t>
+  </si>
+  <si>
+    <t>Interleave the first half of the queue with second half   [weird approach for stack]</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/gas-station/</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2151,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2304,6 +2310,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2623,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+    <sheetView tabSelected="1" topLeftCell="A302" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E317" sqref="E317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -2639,7 +2649,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24.6">
       <c r="B1" s="10" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21">
@@ -2650,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2667,10 +2677,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>418</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="21">
@@ -2681,10 +2691,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21">
@@ -2695,10 +2705,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21">
@@ -2709,10 +2719,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="21">
@@ -2723,10 +2733,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="21">
@@ -2737,10 +2747,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="21">
@@ -2751,10 +2761,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2765,10 +2775,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F12" s="59"/>
     </row>
@@ -2783,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="21">
@@ -2794,10 +2804,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="21">
@@ -2808,10 +2818,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" ht="21">
@@ -2822,10 +2832,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F16" s="60"/>
     </row>
@@ -2834,7 +2844,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>2</v>
@@ -2848,10 +2858,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21">
@@ -2862,13 +2872,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="19.8">
@@ -2879,10 +2889,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F20" s="59"/>
     </row>
@@ -2894,10 +2904,10 @@
         <v>19</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21">
@@ -2908,10 +2918,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="21">
@@ -2922,10 +2932,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="21">
@@ -2936,10 +2946,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="21">
@@ -2950,10 +2960,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="21">
@@ -2964,10 +2974,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21">
@@ -2978,10 +2988,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="21">
@@ -3022,13 +3032,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F31" s="26"/>
     </row>
@@ -3037,7 +3047,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>2</v>
@@ -3050,13 +3060,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3064,13 +3074,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F34" s="23"/>
     </row>
@@ -3104,10 +3114,10 @@
         <v>31</v>
       </c>
       <c r="C37" s="55" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F37" s="61"/>
     </row>
@@ -3116,13 +3126,13 @@
         <v>3</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F38" s="29"/>
     </row>
@@ -3131,13 +3141,13 @@
         <v>3</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F39" s="29"/>
     </row>
@@ -3155,13 +3165,13 @@
         <v>32</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F42" s="23"/>
     </row>
@@ -3173,10 +3183,10 @@
         <v>33</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21">
@@ -3198,10 +3208,10 @@
         <v>35</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="21">
@@ -3212,10 +3222,10 @@
         <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="31" customFormat="1" ht="21">
@@ -3226,13 +3236,13 @@
         <v>37</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21">
@@ -3254,10 +3264,10 @@
         <v>39</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21">
@@ -3268,10 +3278,10 @@
         <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21">
@@ -3298,10 +3308,10 @@
         <v>43</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>418</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="21">
@@ -3312,10 +3322,10 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="21">
@@ -3326,10 +3336,10 @@
         <v>45</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21">
@@ -3515,7 +3525,7 @@
         <v>61</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="21">
@@ -3526,10 +3536,10 @@
         <v>62</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="21">
@@ -3586,10 +3596,10 @@
         <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="21">
@@ -3792,10 +3802,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D98" s="20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="21">
@@ -3806,10 +3816,10 @@
         <v>87</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D99" s="20" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="21">
@@ -3820,10 +3830,10 @@
         <v>88</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D100" s="20" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="21">
@@ -3834,10 +3844,10 @@
         <v>89</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="21">
@@ -3870,10 +3880,10 @@
         <v>92</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="21">
@@ -3884,10 +3894,10 @@
         <v>93</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="21">
@@ -3909,10 +3919,10 @@
         <v>95</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="7" customFormat="1" ht="21">
@@ -3923,10 +3933,10 @@
         <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D108" s="22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F108" s="23"/>
     </row>
@@ -3971,10 +3981,10 @@
         <v>100</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D112" s="20" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="21">
@@ -4018,7 +4028,7 @@
         <v>104</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="21">
@@ -4040,7 +4050,7 @@
         <v>106</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D118" s="26"/>
       <c r="F118" s="26"/>
@@ -4053,7 +4063,7 @@
         <v>107</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D119" s="26"/>
       <c r="F119" s="26"/>
@@ -4099,7 +4109,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D123" s="26"/>
       <c r="F123" s="26"/>
@@ -4149,10 +4159,10 @@
         <v>116</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="130" spans="1:6" s="7" customFormat="1" ht="21">
@@ -4163,10 +4173,10 @@
         <v>117</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F130" s="23"/>
     </row>
@@ -4178,10 +4188,10 @@
         <v>118</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D131" s="20" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="21">
@@ -4192,10 +4202,10 @@
         <v>119</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D132" s="16" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="21">
@@ -4206,10 +4216,10 @@
         <v>120</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D133" s="16" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="21">
@@ -4220,10 +4230,10 @@
         <v>121</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D134" s="20" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="21">
@@ -4234,10 +4244,10 @@
         <v>122</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D135" s="20" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="21">
@@ -4248,10 +4258,10 @@
         <v>123</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D136" s="20" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="21">
@@ -4262,10 +4272,10 @@
         <v>124</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D137" s="20" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="21">
@@ -4298,7 +4308,7 @@
         <v>127</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D140" s="17"/>
       <c r="F140" s="23"/>
@@ -4324,10 +4334,10 @@
         <v>129</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D142" s="20" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="21">
@@ -4338,10 +4348,10 @@
         <v>130</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D143" s="20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="21">
@@ -4352,10 +4362,10 @@
         <v>131</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D144" s="20" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="21">
@@ -4366,10 +4376,10 @@
         <v>132</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D145" s="20" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="21">
@@ -4380,10 +4390,10 @@
         <v>133</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D146" s="20" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="21">
@@ -4445,7 +4455,7 @@
         <v>2</v>
       </c>
       <c r="D151" s="20" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="21">
@@ -4453,13 +4463,13 @@
         <v>115</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D152" s="20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="153" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4467,10 +4477,10 @@
         <v>115</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C153" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D153" s="32"/>
       <c r="F153" s="32"/>
@@ -4483,27 +4493,27 @@
         <v>139</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D154" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="155" spans="1:6" s="31" customFormat="1" ht="21">
       <c r="A155" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="B155" s="31" t="s">
+        <v>465</v>
+      </c>
+      <c r="C155" s="30" t="s">
         <v>466</v>
       </c>
-      <c r="B155" s="31" t="s">
+      <c r="D155" s="36" t="s">
         <v>467</v>
       </c>
-      <c r="C155" s="30" t="s">
+      <c r="F155" s="38" t="s">
         <v>468</v>
-      </c>
-      <c r="D155" s="36" t="s">
-        <v>469</v>
-      </c>
-      <c r="F155" s="38" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="156" spans="1:6" s="31" customFormat="1" ht="21">
@@ -4511,13 +4521,13 @@
         <v>115</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C156" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D156" s="36" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F156" s="32"/>
     </row>
@@ -4526,13 +4536,13 @@
         <v>115</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D157" s="20" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="21">
@@ -4562,13 +4572,13 @@
         <v>115</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D160" s="34" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F160" s="61"/>
     </row>
@@ -4580,10 +4590,10 @@
         <v>142</v>
       </c>
       <c r="C161" s="35" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D161" s="20" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="21">
@@ -4594,10 +4604,10 @@
         <v>143</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="21">
@@ -4606,16 +4616,16 @@
     </row>
     <row r="165" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A165" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F165" s="23"/>
     </row>
@@ -4627,10 +4637,10 @@
         <v>145</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="21">
@@ -4638,13 +4648,13 @@
         <v>144</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="21">
@@ -4655,10 +4665,10 @@
         <v>146</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D168" s="20" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="21">
@@ -4669,10 +4679,10 @@
         <v>147</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D169" s="20" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="21">
@@ -4683,10 +4693,10 @@
         <v>148</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="21">
@@ -4697,10 +4707,10 @@
         <v>149</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D171" s="20" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="21">
@@ -4711,10 +4721,10 @@
         <v>150</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D172" s="20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="21">
@@ -4725,10 +4735,10 @@
         <v>151</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="21">
@@ -4739,10 +4749,10 @@
         <v>152</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="21">
@@ -4775,10 +4785,10 @@
         <v>155</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="21">
@@ -4789,10 +4799,10 @@
         <v>156</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="21">
@@ -4811,13 +4821,13 @@
         <v>144</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C180" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D180" s="38" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F180" s="32"/>
     </row>
@@ -4837,13 +4847,13 @@
         <v>144</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D182" s="20" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="21">
@@ -4865,10 +4875,10 @@
         <v>160</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D184" s="20" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="21">
@@ -4887,13 +4897,13 @@
         <v>144</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D186" s="20" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="21">
@@ -4939,10 +4949,10 @@
         <v>165</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D190" s="20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="21">
@@ -4985,13 +4995,13 @@
         <v>144</v>
       </c>
       <c r="B194" s="37" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C194" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D194" s="32" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F194" s="32"/>
     </row>
@@ -5011,13 +5021,13 @@
         <v>144</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D196" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F196" s="23"/>
     </row>
@@ -5026,13 +5036,13 @@
         <v>144</v>
       </c>
       <c r="B197" s="39" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D197" s="20" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="21">
@@ -5051,13 +5061,13 @@
         <v>144</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D199" s="16" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="200" spans="1:6" s="7" customFormat="1" ht="21">
@@ -5099,13 +5109,13 @@
         <v>173</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D204" s="20" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="21">
@@ -5113,13 +5123,13 @@
         <v>173</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D205" s="20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="206" spans="1:6" ht="21">
@@ -5127,13 +5137,13 @@
         <v>173</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D206" s="20" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="21">
@@ -5155,10 +5165,10 @@
         <v>175</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D208" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="209" spans="1:6" ht="21">
@@ -5169,10 +5179,10 @@
         <v>176</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D209" s="20" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="210" spans="1:6" ht="21">
@@ -5183,10 +5193,10 @@
         <v>177</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D210" s="20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="21">
@@ -5208,10 +5218,10 @@
         <v>179</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D212" s="20" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="21">
@@ -5252,7 +5262,7 @@
         <v>173</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C216" s="6" t="s">
         <v>2</v>
@@ -5268,10 +5278,10 @@
         <v>183</v>
       </c>
       <c r="C217" s="43" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D217" s="44" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F217" s="62"/>
     </row>
@@ -5283,10 +5293,10 @@
         <v>184</v>
       </c>
       <c r="C218" s="48" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D218" s="49" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F218" s="63"/>
     </row>
@@ -5320,10 +5330,10 @@
         <v>187</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D221" s="20" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="222" spans="1:6" ht="21">
@@ -5379,11 +5389,11 @@
         <v>192</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D226" s="23"/>
       <c r="F226" s="23" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="21">
@@ -5806,7 +5816,7 @@
         <v>230</v>
       </c>
       <c r="C267" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D267" s="23"/>
       <c r="F267" s="23"/>
@@ -5930,13 +5940,13 @@
         <v>229</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C278" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D278" s="22" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F278" s="23"/>
     </row>
@@ -6033,10 +6043,10 @@
         <v>249</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D288" s="16" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="289" spans="1:6" ht="21">
@@ -6047,10 +6057,10 @@
         <v>250</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D289" s="16" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="290" spans="1:6" ht="21">
@@ -6061,10 +6071,10 @@
         <v>251</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D290" s="20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="291" spans="1:6" ht="21">
@@ -6075,10 +6085,10 @@
         <v>252</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D291" s="20" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="292" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6099,13 +6109,13 @@
         <v>248</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C293" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D293" s="22" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F293" s="23"/>
     </row>
@@ -6117,10 +6127,10 @@
         <v>254</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D294" s="20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="295" spans="1:6" ht="21">
@@ -6131,13 +6141,13 @@
         <v>255</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D295" s="20" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F295" s="20" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="296" spans="1:6" ht="21">
@@ -6148,10 +6158,10 @@
         <v>256</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D296" s="20" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="297" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6159,13 +6169,13 @@
         <v>248</v>
       </c>
       <c r="B297" s="31" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C297" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D297" s="36" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F297" s="32"/>
     </row>
@@ -6177,10 +6187,10 @@
         <v>257</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D298" s="20" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="21">
@@ -6191,10 +6201,10 @@
         <v>258</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D299" s="20" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="300" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6205,10 +6215,10 @@
         <v>259</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D300" s="22" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F300" s="23"/>
     </row>
@@ -6220,10 +6230,10 @@
         <v>260</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D301" s="20" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="302" spans="1:6" ht="21">
@@ -6242,13 +6252,13 @@
         <v>248</v>
       </c>
       <c r="B303" s="31" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C303" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D303" s="36" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F303" s="32"/>
     </row>
@@ -6271,10 +6281,10 @@
         <v>263</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D305" s="20" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="306" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6282,13 +6292,13 @@
         <v>248</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D306" s="22" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F306" s="23"/>
     </row>
@@ -6319,7 +6329,7 @@
         <v>248</v>
       </c>
       <c r="B309" s="7" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C309" s="6" t="s">
         <v>2</v>
@@ -6346,10 +6356,10 @@
         <v>267</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D311" s="20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="312" spans="1:6" ht="21">
@@ -6371,10 +6381,10 @@
         <v>269</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D313" s="20" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="314" spans="1:6" ht="21">
@@ -6385,24 +6395,27 @@
         <v>270</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D314" s="20" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" ht="21">
-      <c r="A315" s="3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" s="65" customFormat="1">
+      <c r="A315" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="B315" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D315" s="20" t="s">
-        <v>603</v>
+      <c r="B315" s="65" t="s">
+        <v>608</v>
+      </c>
+      <c r="C315" s="64" t="s">
+        <v>416</v>
+      </c>
+      <c r="D315" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="F315" s="17" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="316" spans="1:6" s="7" customFormat="1" ht="21">
@@ -6410,31 +6423,35 @@
         <v>248</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D316" s="23"/>
+        <v>416</v>
+      </c>
+      <c r="D316" s="22" t="s">
+        <v>609</v>
+      </c>
       <c r="F316" s="23"/>
     </row>
-    <row r="317" spans="1:6" ht="21">
-      <c r="A317" s="3" t="s">
+    <row r="317" spans="1:6" s="7" customFormat="1" ht="21">
+      <c r="A317" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B317" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B317" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C317" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D317" s="23"/>
+      <c r="F317" s="23"/>
     </row>
     <row r="318" spans="1:6" ht="21">
       <c r="A318" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -6445,13 +6462,13 @@
         <v>248</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D319" s="22" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F319" s="23"/>
     </row>
@@ -6460,7 +6477,7 @@
         <v>248</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -6471,10 +6488,10 @@
         <v>248</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>2</v>
+        <v>416</v>
       </c>
     </row>
     <row r="322" spans="1:6" ht="21">
@@ -6482,7 +6499,7 @@
         <v>248</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>2</v>
@@ -6493,16 +6510,16 @@
         <v>248</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D323" s="16" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F323" s="57" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="324" spans="1:6" ht="21">
@@ -6510,13 +6527,13 @@
         <v>248</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D324" s="20" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="325" spans="1:6" s="31" customFormat="1" ht="21">
@@ -6524,13 +6541,13 @@
         <v>248</v>
       </c>
       <c r="B325" s="31" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C325" s="30" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D325" s="36" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F325" s="32"/>
     </row>
@@ -6544,38 +6561,38 @@
     </row>
     <row r="328" spans="1:6" ht="21">
       <c r="A328" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D328" s="21" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="329" spans="1:6" ht="21">
       <c r="A329" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C329" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D329" s="16" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="330" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A330" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C330" s="6" t="s">
         <v>2</v>
@@ -6585,38 +6602,38 @@
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B331" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C331" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D331" s="20" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="332" spans="1:6" ht="21">
       <c r="A332" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B332" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C332" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D332" s="16" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="333" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A333" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C333" s="6" t="s">
         <v>2</v>
@@ -6626,10 +6643,10 @@
     </row>
     <row r="334" spans="1:6" ht="21">
       <c r="A334" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B334" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>2</v>
@@ -6637,10 +6654,10 @@
     </row>
     <row r="335" spans="1:6" ht="21">
       <c r="A335" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B335" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>2</v>
@@ -6648,39 +6665,39 @@
     </row>
     <row r="336" spans="1:6" ht="21">
       <c r="A336" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B336" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D336" s="20" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="337" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A337" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D337" s="22" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F337" s="23"/>
     </row>
     <row r="338" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A338" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C338" s="6" t="s">
         <v>2</v>
@@ -6690,10 +6707,10 @@
     </row>
     <row r="339" spans="1:6" ht="21">
       <c r="A339" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B339" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>2</v>
@@ -6701,10 +6718,10 @@
     </row>
     <row r="340" spans="1:6" ht="21">
       <c r="A340" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B340" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -6712,25 +6729,25 @@
     </row>
     <row r="341" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A341" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B341" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D341" s="22" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F341" s="23"/>
     </row>
     <row r="342" spans="1:6" ht="21">
       <c r="A342" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B342" s="13" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>2</v>
@@ -6738,25 +6755,25 @@
     </row>
     <row r="343" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A343" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C343" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D343" s="52" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F343" s="23"/>
     </row>
     <row r="344" spans="1:6" ht="21">
       <c r="A344" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B344" s="13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>2</v>
@@ -6764,19 +6781,19 @@
     </row>
     <row r="345" spans="1:6" ht="21">
       <c r="A345" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B345" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D345" s="20" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F345" s="57" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
@@ -6789,10 +6806,10 @@
     </row>
     <row r="348" spans="1:6" ht="21">
       <c r="A348" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B348" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>2</v>
@@ -6800,10 +6817,10 @@
     </row>
     <row r="349" spans="1:6" ht="21">
       <c r="A349" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B349" s="13" t="s">
         <v>296</v>
-      </c>
-      <c r="B349" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>2</v>
@@ -6811,10 +6828,10 @@
     </row>
     <row r="350" spans="1:6" ht="21">
       <c r="A350" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B350" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
@@ -6822,10 +6839,10 @@
     </row>
     <row r="351" spans="1:6" ht="21">
       <c r="A351" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B351" s="13" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -6833,10 +6850,10 @@
     </row>
     <row r="352" spans="1:6" ht="21">
       <c r="A352" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B352" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>2</v>
@@ -6844,10 +6861,10 @@
     </row>
     <row r="353" spans="1:3" ht="21">
       <c r="A353" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -6855,10 +6872,10 @@
     </row>
     <row r="354" spans="1:3" ht="21">
       <c r="A354" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -6866,21 +6883,21 @@
     </row>
     <row r="355" spans="1:3" ht="21">
       <c r="A355" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="21">
       <c r="A356" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -6888,10 +6905,10 @@
     </row>
     <row r="357" spans="1:3" ht="21">
       <c r="A357" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B357" s="13" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -6899,10 +6916,10 @@
     </row>
     <row r="358" spans="1:3" ht="21">
       <c r="A358" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B358" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -6910,10 +6927,10 @@
     </row>
     <row r="359" spans="1:3" ht="21">
       <c r="A359" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B359" s="13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>2</v>
@@ -6921,10 +6938,10 @@
     </row>
     <row r="360" spans="1:3" ht="21">
       <c r="A360" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B360" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>2</v>
@@ -6932,10 +6949,10 @@
     </row>
     <row r="361" spans="1:3" ht="21">
       <c r="A361" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B361" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>2</v>
@@ -6943,10 +6960,10 @@
     </row>
     <row r="362" spans="1:3" ht="21">
       <c r="A362" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B362" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -6954,10 +6971,10 @@
     </row>
     <row r="363" spans="1:3" ht="21">
       <c r="A363" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B363" s="13" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -6965,10 +6982,10 @@
     </row>
     <row r="364" spans="1:3" ht="21">
       <c r="A364" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -6976,10 +6993,10 @@
     </row>
     <row r="365" spans="1:3" ht="21">
       <c r="A365" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>2</v>
@@ -6987,10 +7004,10 @@
     </row>
     <row r="366" spans="1:3" ht="21">
       <c r="A366" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>2</v>
@@ -6998,10 +7015,10 @@
     </row>
     <row r="367" spans="1:3" ht="21">
       <c r="A367" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>2</v>
@@ -7009,10 +7026,10 @@
     </row>
     <row r="368" spans="1:3" ht="21">
       <c r="A368" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>2</v>
@@ -7020,10 +7037,10 @@
     </row>
     <row r="369" spans="1:6" ht="21">
       <c r="A369" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>2</v>
@@ -7031,10 +7048,10 @@
     </row>
     <row r="370" spans="1:6" ht="21">
       <c r="A370" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B370" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>2</v>
@@ -7042,10 +7059,10 @@
     </row>
     <row r="371" spans="1:6" ht="21">
       <c r="A371" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>2</v>
@@ -7053,10 +7070,10 @@
     </row>
     <row r="372" spans="1:6" ht="21">
       <c r="A372" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>2</v>
@@ -7064,10 +7081,10 @@
     </row>
     <row r="373" spans="1:6" ht="21">
       <c r="A373" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>2</v>
@@ -7075,10 +7092,10 @@
     </row>
     <row r="374" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A374" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C374" s="6" t="s">
         <v>2</v>
@@ -7088,10 +7105,10 @@
     </row>
     <row r="375" spans="1:6" ht="21">
       <c r="A375" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>2</v>
@@ -7099,10 +7116,10 @@
     </row>
     <row r="376" spans="1:6" ht="21">
       <c r="A376" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>2</v>
@@ -7110,10 +7127,10 @@
     </row>
     <row r="377" spans="1:6" ht="21">
       <c r="A377" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>2</v>
@@ -7121,10 +7138,10 @@
     </row>
     <row r="378" spans="1:6" ht="21">
       <c r="A378" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -7132,10 +7149,10 @@
     </row>
     <row r="379" spans="1:6" ht="21">
       <c r="A379" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>2</v>
@@ -7143,10 +7160,10 @@
     </row>
     <row r="380" spans="1:6" ht="21">
       <c r="A380" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>2</v>
@@ -7154,10 +7171,10 @@
     </row>
     <row r="381" spans="1:6" ht="21">
       <c r="A381" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>2</v>
@@ -7165,10 +7182,10 @@
     </row>
     <row r="382" spans="1:6" ht="21">
       <c r="A382" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>2</v>
@@ -7176,10 +7193,10 @@
     </row>
     <row r="383" spans="1:6" ht="21">
       <c r="A383" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B383" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>2</v>
@@ -7187,10 +7204,10 @@
     </row>
     <row r="384" spans="1:6" ht="21">
       <c r="A384" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B384" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>2</v>
@@ -7198,10 +7215,10 @@
     </row>
     <row r="385" spans="1:3" ht="21">
       <c r="A385" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>2</v>
@@ -7209,10 +7226,10 @@
     </row>
     <row r="386" spans="1:3" ht="21">
       <c r="A386" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>2</v>
@@ -7220,10 +7237,10 @@
     </row>
     <row r="387" spans="1:3" ht="21">
       <c r="A387" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>2</v>
@@ -7231,10 +7248,10 @@
     </row>
     <row r="388" spans="1:3" ht="21">
       <c r="A388" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>2</v>
@@ -7242,10 +7259,10 @@
     </row>
     <row r="389" spans="1:3" ht="21">
       <c r="A389" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -7253,10 +7270,10 @@
     </row>
     <row r="390" spans="1:3" ht="21">
       <c r="A390" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>2</v>
@@ -7272,10 +7289,10 @@
     </row>
     <row r="393" spans="1:3" ht="21">
       <c r="A393" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>2</v>
@@ -7283,10 +7300,10 @@
     </row>
     <row r="394" spans="1:3" ht="21">
       <c r="A394" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B394" s="13" t="s">
         <v>340</v>
-      </c>
-      <c r="B394" s="13" t="s">
-        <v>342</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>2</v>
@@ -7294,10 +7311,10 @@
     </row>
     <row r="395" spans="1:3" ht="21">
       <c r="A395" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>2</v>
@@ -7305,7 +7322,7 @@
     </row>
     <row r="396" spans="1:3" ht="21">
       <c r="A396" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B396" s="13" t="s">
         <v>77</v>
@@ -7316,10 +7333,10 @@
     </row>
     <row r="397" spans="1:3" ht="21">
       <c r="A397" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B397" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -7327,10 +7344,10 @@
     </row>
     <row r="398" spans="1:3" ht="21">
       <c r="A398" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>2</v>
@@ -7346,21 +7363,21 @@
     </row>
     <row r="401" spans="1:6" ht="21">
       <c r="A401" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B401" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C401" s="35" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="21">
       <c r="A402" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B402" s="13" t="s">
         <v>346</v>
-      </c>
-      <c r="B402" s="13" t="s">
-        <v>348</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>2</v>
@@ -7368,10 +7385,10 @@
     </row>
     <row r="403" spans="1:6" ht="21">
       <c r="A403" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>2</v>
@@ -7379,10 +7396,10 @@
     </row>
     <row r="404" spans="1:6" ht="21">
       <c r="A404" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>2</v>
@@ -7390,10 +7407,10 @@
     </row>
     <row r="405" spans="1:6" ht="21">
       <c r="A405" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>2</v>
@@ -7401,21 +7418,21 @@
     </row>
     <row r="406" spans="1:6" ht="21">
       <c r="A406" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="21">
       <c r="A407" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
@@ -7423,7 +7440,7 @@
     </row>
     <row r="408" spans="1:6" ht="21">
       <c r="A408" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B408" s="13" t="s">
         <v>237</v>
@@ -7434,10 +7451,10 @@
     </row>
     <row r="409" spans="1:6" ht="21">
       <c r="A409" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -7445,10 +7462,10 @@
     </row>
     <row r="410" spans="1:6" ht="21">
       <c r="A410" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>2</v>
@@ -7456,10 +7473,10 @@
     </row>
     <row r="411" spans="1:6" ht="21">
       <c r="A411" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -7467,10 +7484,10 @@
     </row>
     <row r="412" spans="1:6" ht="21">
       <c r="A412" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -7478,10 +7495,10 @@
     </row>
     <row r="413" spans="1:6" ht="21">
       <c r="A413" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -7489,10 +7506,10 @@
     </row>
     <row r="414" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A414" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>2</v>
@@ -7502,10 +7519,10 @@
     </row>
     <row r="415" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A415" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B415" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>2</v>
@@ -7515,10 +7532,10 @@
     </row>
     <row r="416" spans="1:6" ht="21">
       <c r="A416" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -7526,10 +7543,10 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -7537,10 +7554,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -7548,10 +7565,10 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -7559,10 +7576,10 @@
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
@@ -7570,10 +7587,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -7581,10 +7598,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>2</v>
@@ -7592,10 +7609,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>2</v>
@@ -7603,10 +7620,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>2</v>
@@ -7614,10 +7631,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>2</v>
@@ -7625,10 +7642,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>2</v>
@@ -7636,10 +7653,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>2</v>
@@ -7647,10 +7664,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>2</v>
@@ -7658,10 +7675,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>2</v>
@@ -7669,10 +7686,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>2</v>
@@ -7680,10 +7697,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -7691,10 +7708,10 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -7702,10 +7719,10 @@
     </row>
     <row r="433" spans="1:6" ht="21">
       <c r="A433" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -7713,10 +7730,10 @@
     </row>
     <row r="434" spans="1:6" ht="21">
       <c r="A434" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -7724,10 +7741,10 @@
     </row>
     <row r="435" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A435" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B435" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>2</v>
@@ -7737,10 +7754,10 @@
     </row>
     <row r="436" spans="1:6" ht="21">
       <c r="A436" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -7748,10 +7765,10 @@
     </row>
     <row r="437" spans="1:6" ht="21">
       <c r="A437" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>2</v>
@@ -7759,10 +7776,10 @@
     </row>
     <row r="438" spans="1:6" ht="21">
       <c r="A438" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -7770,10 +7787,10 @@
     </row>
     <row r="439" spans="1:6" ht="21">
       <c r="A439" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -7781,10 +7798,10 @@
     </row>
     <row r="440" spans="1:6" ht="21">
       <c r="A440" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B440" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>2</v>
@@ -7792,10 +7809,10 @@
     </row>
     <row r="441" spans="1:6" ht="21">
       <c r="A441" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>2</v>
@@ -7803,10 +7820,10 @@
     </row>
     <row r="442" spans="1:6" ht="21">
       <c r="A442" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>2</v>
@@ -7814,10 +7831,10 @@
     </row>
     <row r="443" spans="1:6" ht="21">
       <c r="A443" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C443" s="2" t="s">
         <v>2</v>
@@ -7825,10 +7842,10 @@
     </row>
     <row r="444" spans="1:6" ht="21">
       <c r="A444" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>2</v>
@@ -7836,10 +7853,10 @@
     </row>
     <row r="445" spans="1:6" ht="21">
       <c r="A445" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>2</v>
@@ -7847,10 +7864,10 @@
     </row>
     <row r="446" spans="1:6" ht="21">
       <c r="A446" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>2</v>
@@ -7858,10 +7875,10 @@
     </row>
     <row r="447" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A447" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B447" s="25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C447" s="24" t="s">
         <v>2</v>
@@ -7871,10 +7888,10 @@
     </row>
     <row r="448" spans="1:6" s="25" customFormat="1" ht="21">
       <c r="A448" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B448" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C448" s="24" t="s">
         <v>2</v>
@@ -7884,10 +7901,10 @@
     </row>
     <row r="449" spans="1:6" ht="21">
       <c r="A449" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>2</v>
@@ -7895,10 +7912,10 @@
     </row>
     <row r="450" spans="1:6" ht="21">
       <c r="A450" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>2</v>
@@ -7906,10 +7923,10 @@
     </row>
     <row r="451" spans="1:6" ht="21">
       <c r="A451" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C451" s="2" t="s">
         <v>2</v>
@@ -7917,10 +7934,10 @@
     </row>
     <row r="452" spans="1:6" ht="21">
       <c r="A452" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>2</v>
@@ -7928,23 +7945,23 @@
     </row>
     <row r="453" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A453" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D453" s="23"/>
       <c r="F453" s="23"/>
     </row>
     <row r="454" spans="1:6" ht="21">
       <c r="A454" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>2</v>
@@ -7952,10 +7969,10 @@
     </row>
     <row r="455" spans="1:6" ht="21">
       <c r="A455" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C455" s="2" t="s">
         <v>2</v>
@@ -7963,10 +7980,10 @@
     </row>
     <row r="456" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A456" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>2</v>
@@ -7976,10 +7993,10 @@
     </row>
     <row r="457" spans="1:6" ht="21">
       <c r="A457" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>2</v>
@@ -7987,10 +8004,10 @@
     </row>
     <row r="458" spans="1:6" ht="21">
       <c r="A458" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>2</v>
@@ -7998,10 +8015,10 @@
     </row>
     <row r="459" spans="1:6" ht="21">
       <c r="A459" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>2</v>
@@ -8009,10 +8026,10 @@
     </row>
     <row r="460" spans="1:6" ht="21">
       <c r="A460" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>2</v>
@@ -8029,97 +8046,97 @@
     </row>
     <row r="463" spans="1:6" ht="21">
       <c r="A463" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C463" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D463" s="16" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="464" spans="1:6" ht="21">
       <c r="A464" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B464" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="B464" s="13" t="s">
-        <v>408</v>
-      </c>
       <c r="C464" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D464" s="20" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F464" s="57" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="465" spans="1:6" ht="21">
       <c r="A465" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D465" s="20" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="466" spans="1:6" ht="21">
       <c r="A466" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D466" s="20" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="21">
       <c r="A467" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D467" s="20" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="468" spans="1:6" ht="21">
       <c r="A468" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D468" s="20" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="21">
       <c r="A469" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>2</v>
@@ -8127,44 +8144,44 @@
     </row>
     <row r="470" spans="1:6" ht="21">
       <c r="A470" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D470" s="20" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="471" spans="1:6" ht="21">
       <c r="A471" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D471" s="20" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="472" spans="1:6" s="7" customFormat="1" ht="21">
       <c r="A472" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D472" s="22" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F472" s="23"/>
     </row>
@@ -8453,9 +8470,9 @@
     <hyperlink ref="B312" r:id="rId281"/>
     <hyperlink ref="B313" r:id="rId282"/>
     <hyperlink ref="B314" r:id="rId283"/>
-    <hyperlink ref="B315" r:id="rId284"/>
+    <hyperlink ref="B315" r:id="rId284" display="Interleave the first half of the queue with second half"/>
     <hyperlink ref="B316" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps"/>
-    <hyperlink ref="B317" r:id="rId286"/>
+    <hyperlink ref="B317" r:id="rId286" display="Minimum time required to rot all oranges"/>
     <hyperlink ref="B318" r:id="rId287"/>
     <hyperlink ref="B319" r:id="rId288" display="First negative integer in every window of size “k”"/>
     <hyperlink ref="B320" r:id="rId289"/>
@@ -8738,8 +8755,9 @@
     <hyperlink ref="D298" r:id="rId566"/>
     <hyperlink ref="D306" r:id="rId567"/>
     <hyperlink ref="B199" r:id="rId568" display="Kth Ancestor of node in a Binary tree"/>
+    <hyperlink ref="D316" r:id="rId569"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId569"/>
+  <pageSetup orientation="portrait" r:id="rId570"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bfs traversal of graph
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46397E-522E-4A56-9866-32D1D30D6296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="613">
   <si>
     <t>Topic:</t>
   </si>
@@ -1874,11 +1875,14 @@
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/n-queue-using-array_1170053?leftPanelTab=1</t>
   </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/create-a-graph-and-print-it_1214551?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=0&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Lovebabbar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24">
     <font>
       <sz val="12"/>
@@ -2636,11 +2640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F311" sqref="F311"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F349" sqref="F349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6825,7 +6829,10 @@
         <v>294</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D348" s="20" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="349" spans="1:6" ht="21">
@@ -8200,578 +8207,579 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17" r:id="rId13" display="Merge Intervals"/>
-    <hyperlink ref="B18" r:id="rId14"/>
-    <hyperlink ref="B19" r:id="rId15"/>
-    <hyperlink ref="B20" r:id="rId16"/>
-    <hyperlink ref="B21" r:id="rId17"/>
-    <hyperlink ref="B22" r:id="rId18"/>
-    <hyperlink ref="B23" r:id="rId19"/>
-    <hyperlink ref="B24" r:id="rId20"/>
-    <hyperlink ref="B25" r:id="rId21"/>
-    <hyperlink ref="B26" r:id="rId22"/>
-    <hyperlink ref="B27" r:id="rId23"/>
-    <hyperlink ref="B28" r:id="rId24"/>
-    <hyperlink ref="B29" r:id="rId25"/>
-    <hyperlink ref="B30" r:id="rId26"/>
-    <hyperlink ref="B31" r:id="rId27" display="Find the triplet that sum to a given value"/>
-    <hyperlink ref="B32" r:id="rId28" display="Trapping Rain water problem"/>
-    <hyperlink ref="B33" r:id="rId29" display="Chocolate Distribution problem"/>
-    <hyperlink ref="B34" r:id="rId30" display="Smallest Subarray with sum greater than a given value"/>
-    <hyperlink ref="B35" r:id="rId31"/>
-    <hyperlink ref="B36" r:id="rId32"/>
-    <hyperlink ref="B37" r:id="rId33"/>
-    <hyperlink ref="B38" r:id="rId34" display="Median of 2 sorted arrays of equal size"/>
-    <hyperlink ref="B42" r:id="rId35" display="Spiral traversal on a Matrix"/>
-    <hyperlink ref="B43" r:id="rId36"/>
-    <hyperlink ref="B44" r:id="rId37"/>
-    <hyperlink ref="B45" r:id="rId38"/>
-    <hyperlink ref="B46" r:id="rId39"/>
-    <hyperlink ref="B47" r:id="rId40"/>
-    <hyperlink ref="B48" r:id="rId41"/>
-    <hyperlink ref="B49" r:id="rId42"/>
-    <hyperlink ref="B50" r:id="rId43"/>
-    <hyperlink ref="B51" r:id="rId44"/>
-    <hyperlink ref="B54" r:id="rId45"/>
-    <hyperlink ref="B55" r:id="rId46"/>
-    <hyperlink ref="B56" r:id="rId47"/>
-    <hyperlink ref="B57" r:id="rId48"/>
-    <hyperlink ref="B58" r:id="rId49"/>
-    <hyperlink ref="B59" r:id="rId50"/>
-    <hyperlink ref="B60" r:id="rId51"/>
-    <hyperlink ref="B61" r:id="rId52"/>
-    <hyperlink ref="B62" r:id="rId53"/>
-    <hyperlink ref="B63" r:id="rId54"/>
-    <hyperlink ref="B64" r:id="rId55"/>
-    <hyperlink ref="B65" r:id="rId56"/>
-    <hyperlink ref="B66" r:id="rId57"/>
-    <hyperlink ref="B67" r:id="rId58"/>
-    <hyperlink ref="B68" r:id="rId59"/>
-    <hyperlink ref="B69" r:id="rId60"/>
-    <hyperlink ref="B70" r:id="rId61"/>
-    <hyperlink ref="B71" r:id="rId62"/>
-    <hyperlink ref="B72" r:id="rId63"/>
-    <hyperlink ref="B73" r:id="rId64"/>
-    <hyperlink ref="B74" r:id="rId65"/>
-    <hyperlink ref="B75" r:id="rId66"/>
-    <hyperlink ref="B76" r:id="rId67"/>
-    <hyperlink ref="B77" r:id="rId68"/>
-    <hyperlink ref="B78" r:id="rId69"/>
-    <hyperlink ref="B79" r:id="rId70"/>
-    <hyperlink ref="B80" r:id="rId71"/>
-    <hyperlink ref="B81" r:id="rId72"/>
-    <hyperlink ref="B82" r:id="rId73"/>
-    <hyperlink ref="B83" r:id="rId74"/>
-    <hyperlink ref="B84" r:id="rId75"/>
-    <hyperlink ref="B85" r:id="rId76"/>
-    <hyperlink ref="B86" r:id="rId77"/>
-    <hyperlink ref="B87" r:id="rId78"/>
-    <hyperlink ref="B88" r:id="rId79"/>
-    <hyperlink ref="B89" r:id="rId80"/>
-    <hyperlink ref="B90" r:id="rId81"/>
-    <hyperlink ref="B91" r:id="rId82"/>
-    <hyperlink ref="B92" r:id="rId83"/>
-    <hyperlink ref="B93" r:id="rId84"/>
-    <hyperlink ref="B94" r:id="rId85"/>
-    <hyperlink ref="B95" r:id="rId86"/>
-    <hyperlink ref="B98" r:id="rId87"/>
-    <hyperlink ref="B99" r:id="rId88"/>
-    <hyperlink ref="B100" r:id="rId89"/>
-    <hyperlink ref="B101" r:id="rId90"/>
-    <hyperlink ref="B103" r:id="rId91" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
-    <hyperlink ref="B104" r:id="rId92"/>
-    <hyperlink ref="B105" r:id="rId93"/>
-    <hyperlink ref="B106" r:id="rId94"/>
-    <hyperlink ref="B107" r:id="rId95"/>
-    <hyperlink ref="B108" r:id="rId96"/>
-    <hyperlink ref="B110" r:id="rId97"/>
-    <hyperlink ref="B111" r:id="rId98"/>
-    <hyperlink ref="B112" r:id="rId99"/>
-    <hyperlink ref="B113" r:id="rId100"/>
-    <hyperlink ref="B114" r:id="rId101"/>
-    <hyperlink ref="B115" r:id="rId102"/>
-    <hyperlink ref="B116" r:id="rId103"/>
-    <hyperlink ref="B117" r:id="rId104"/>
-    <hyperlink ref="B118" r:id="rId105"/>
-    <hyperlink ref="B119" r:id="rId106"/>
-    <hyperlink ref="B120" r:id="rId107"/>
-    <hyperlink ref="B121" r:id="rId108"/>
-    <hyperlink ref="B122" r:id="rId109"/>
-    <hyperlink ref="B123" r:id="rId110"/>
-    <hyperlink ref="B124" r:id="rId111"/>
-    <hyperlink ref="B125" r:id="rId112"/>
-    <hyperlink ref="B126" r:id="rId113"/>
-    <hyperlink ref="B102" r:id="rId114"/>
-    <hyperlink ref="B109" r:id="rId115"/>
-    <hyperlink ref="B129" r:id="rId116"/>
-    <hyperlink ref="B130" r:id="rId117"/>
-    <hyperlink ref="B131" r:id="rId118"/>
-    <hyperlink ref="B132" r:id="rId119"/>
-    <hyperlink ref="B133" r:id="rId120"/>
-    <hyperlink ref="B134" r:id="rId121"/>
-    <hyperlink ref="B135" r:id="rId122"/>
-    <hyperlink ref="B136" r:id="rId123"/>
-    <hyperlink ref="B137" r:id="rId124"/>
-    <hyperlink ref="B138" r:id="rId125"/>
-    <hyperlink ref="B139" r:id="rId126"/>
-    <hyperlink ref="B140" r:id="rId127"/>
-    <hyperlink ref="B141" r:id="rId128"/>
-    <hyperlink ref="B142" r:id="rId129"/>
-    <hyperlink ref="B143" r:id="rId130"/>
-    <hyperlink ref="B144" r:id="rId131"/>
-    <hyperlink ref="B145" r:id="rId132"/>
-    <hyperlink ref="B146" r:id="rId133"/>
-    <hyperlink ref="B147" r:id="rId134"/>
-    <hyperlink ref="B148" r:id="rId135"/>
-    <hyperlink ref="B149" r:id="rId136"/>
-    <hyperlink ref="B150" r:id="rId137"/>
-    <hyperlink ref="B153" r:id="rId138" display="Flatten a Linked List"/>
-    <hyperlink ref="B154" r:id="rId139"/>
-    <hyperlink ref="B155" r:id="rId140" display="Clone a linked list with next and random pointer"/>
-    <hyperlink ref="B157" r:id="rId141" display="Merge K sorted Linked list"/>
-    <hyperlink ref="B158" r:id="rId142"/>
-    <hyperlink ref="B159" r:id="rId143"/>
-    <hyperlink ref="B160" r:id="rId144"/>
-    <hyperlink ref="B161" r:id="rId145"/>
-    <hyperlink ref="B162" r:id="rId146"/>
-    <hyperlink ref="B165" r:id="rId147" display="level order traversal"/>
-    <hyperlink ref="B166" r:id="rId148"/>
-    <hyperlink ref="B167" r:id="rId149" display="Height of a tree"/>
-    <hyperlink ref="B168" r:id="rId150"/>
-    <hyperlink ref="B169" r:id="rId151"/>
-    <hyperlink ref="B170" r:id="rId152"/>
-    <hyperlink ref="B171" r:id="rId153"/>
-    <hyperlink ref="B172" r:id="rId154"/>
-    <hyperlink ref="B173" r:id="rId155"/>
-    <hyperlink ref="B174" r:id="rId156"/>
-    <hyperlink ref="B175" r:id="rId157"/>
-    <hyperlink ref="B176" r:id="rId158"/>
-    <hyperlink ref="B177" r:id="rId159"/>
-    <hyperlink ref="B178" r:id="rId160"/>
-    <hyperlink ref="B179" r:id="rId161"/>
-    <hyperlink ref="B180" r:id="rId162" display="Boundary traversal of a Binary tree"/>
-    <hyperlink ref="B181" r:id="rId163"/>
-    <hyperlink ref="B182" r:id="rId164" display="Convert Binary tree into Doubly Linked List"/>
-    <hyperlink ref="B183" r:id="rId165"/>
-    <hyperlink ref="B184" r:id="rId166"/>
-    <hyperlink ref="B185" r:id="rId167" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B187" r:id="rId168"/>
-    <hyperlink ref="B188" r:id="rId169"/>
-    <hyperlink ref="B189" r:id="rId170"/>
-    <hyperlink ref="B190" r:id="rId171"/>
-    <hyperlink ref="B191" r:id="rId172"/>
-    <hyperlink ref="B192" r:id="rId173" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B193" r:id="rId174"/>
-    <hyperlink ref="B194" r:id="rId175"/>
-    <hyperlink ref="B195" r:id="rId176"/>
-    <hyperlink ref="B196" r:id="rId177" display="Find LCA in a Binary tree"/>
-    <hyperlink ref="B198" r:id="rId178"/>
-    <hyperlink ref="B200" r:id="rId179"/>
-    <hyperlink ref="B201" r:id="rId180"/>
-    <hyperlink ref="B204" r:id="rId181" display="Fina a value in a BST"/>
-    <hyperlink ref="B207" r:id="rId182"/>
-    <hyperlink ref="B208" r:id="rId183"/>
-    <hyperlink ref="B209" r:id="rId184"/>
-    <hyperlink ref="B210" r:id="rId185"/>
-    <hyperlink ref="B211" r:id="rId186"/>
-    <hyperlink ref="B212" r:id="rId187"/>
-    <hyperlink ref="B213" r:id="rId188"/>
-    <hyperlink ref="B214" r:id="rId189"/>
-    <hyperlink ref="B215" r:id="rId190"/>
-    <hyperlink ref="B216" r:id="rId191" display="Merge two BST [ V.V.V&gt;IMP ]"/>
-    <hyperlink ref="B217" r:id="rId192"/>
-    <hyperlink ref="B218" r:id="rId193"/>
-    <hyperlink ref="B219" r:id="rId194"/>
-    <hyperlink ref="B220" r:id="rId195"/>
-    <hyperlink ref="B221" r:id="rId196"/>
-    <hyperlink ref="B222" r:id="rId197"/>
-    <hyperlink ref="B223" r:id="rId198"/>
-    <hyperlink ref="B224" r:id="rId199"/>
-    <hyperlink ref="B225" r:id="rId200"/>
-    <hyperlink ref="B226" r:id="rId201"/>
-    <hyperlink ref="B227" r:id="rId202"/>
-    <hyperlink ref="B230" r:id="rId203"/>
-    <hyperlink ref="B231" r:id="rId204"/>
-    <hyperlink ref="B232" r:id="rId205"/>
-    <hyperlink ref="B233" r:id="rId206"/>
-    <hyperlink ref="B234" r:id="rId207"/>
-    <hyperlink ref="B235" r:id="rId208"/>
-    <hyperlink ref="B236" r:id="rId209"/>
-    <hyperlink ref="B237" r:id="rId210"/>
-    <hyperlink ref="B238" r:id="rId211"/>
-    <hyperlink ref="B239" r:id="rId212"/>
-    <hyperlink ref="B240" r:id="rId213"/>
-    <hyperlink ref="B241" r:id="rId214"/>
-    <hyperlink ref="B242" r:id="rId215"/>
-    <hyperlink ref="B243" r:id="rId216"/>
-    <hyperlink ref="B244" r:id="rId217"/>
-    <hyperlink ref="B245" r:id="rId218"/>
-    <hyperlink ref="B246" r:id="rId219"/>
-    <hyperlink ref="B247" r:id="rId220"/>
-    <hyperlink ref="B248" r:id="rId221"/>
-    <hyperlink ref="B249" r:id="rId222" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B250" r:id="rId223"/>
-    <hyperlink ref="B251" r:id="rId224"/>
-    <hyperlink ref="B252" r:id="rId225"/>
-    <hyperlink ref="B253" r:id="rId226"/>
-    <hyperlink ref="B254" r:id="rId227"/>
-    <hyperlink ref="B255" r:id="rId228"/>
-    <hyperlink ref="B256" r:id="rId229"/>
-    <hyperlink ref="B257" r:id="rId230"/>
-    <hyperlink ref="B258" r:id="rId231"/>
-    <hyperlink ref="B259" r:id="rId232"/>
-    <hyperlink ref="B260" r:id="rId233"/>
-    <hyperlink ref="B261" r:id="rId234"/>
-    <hyperlink ref="B262" r:id="rId235"/>
-    <hyperlink ref="B263" r:id="rId236"/>
-    <hyperlink ref="B264" r:id="rId237"/>
-    <hyperlink ref="B267" r:id="rId238"/>
-    <hyperlink ref="B268" r:id="rId239"/>
-    <hyperlink ref="B269" r:id="rId240"/>
-    <hyperlink ref="B270" r:id="rId241"/>
-    <hyperlink ref="B271" r:id="rId242"/>
-    <hyperlink ref="B272" r:id="rId243"/>
-    <hyperlink ref="B273" r:id="rId244"/>
-    <hyperlink ref="B274" r:id="rId245"/>
-    <hyperlink ref="B275" r:id="rId246"/>
-    <hyperlink ref="B276" r:id="rId247"/>
-    <hyperlink ref="B277" r:id="rId248"/>
-    <hyperlink ref="B278" r:id="rId249" display="Combinational Sum"/>
-    <hyperlink ref="B279" r:id="rId250"/>
-    <hyperlink ref="B280" r:id="rId251"/>
-    <hyperlink ref="B281" r:id="rId252"/>
-    <hyperlink ref="B282" r:id="rId253"/>
-    <hyperlink ref="B283" r:id="rId254"/>
-    <hyperlink ref="B284" r:id="rId255"/>
-    <hyperlink ref="B285" r:id="rId256"/>
-    <hyperlink ref="B288" r:id="rId257"/>
-    <hyperlink ref="B289" r:id="rId258"/>
-    <hyperlink ref="B290" r:id="rId259"/>
-    <hyperlink ref="B291" r:id="rId260"/>
-    <hyperlink ref="B292" r:id="rId261"/>
-    <hyperlink ref="B293" r:id="rId262" display="Check the expression has valid or Balanced parenthesis or not."/>
-    <hyperlink ref="B294" r:id="rId263"/>
-    <hyperlink ref="B295" r:id="rId264"/>
-    <hyperlink ref="B296" r:id="rId265"/>
-    <hyperlink ref="B297" r:id="rId266" display="The celebrity Problem"/>
-    <hyperlink ref="B298" r:id="rId267"/>
-    <hyperlink ref="B299" r:id="rId268"/>
-    <hyperlink ref="B300" r:id="rId269"/>
-    <hyperlink ref="B301" r:id="rId270"/>
-    <hyperlink ref="B302" r:id="rId271"/>
-    <hyperlink ref="B303" r:id="rId272" display="Largest rectangular Area in Histogram"/>
-    <hyperlink ref="B304" r:id="rId273"/>
-    <hyperlink ref="B305" r:id="rId274"/>
-    <hyperlink ref="B306" r:id="rId275" display="Implement Stack using Queue"/>
-    <hyperlink ref="B307" r:id="rId276"/>
-    <hyperlink ref="B308" r:id="rId277"/>
-    <hyperlink ref="B309" r:id="rId278" display="Implement Queue using Stack  "/>
-    <hyperlink ref="B310" r:id="rId279"/>
-    <hyperlink ref="B311" r:id="rId280"/>
-    <hyperlink ref="B312" r:id="rId281"/>
-    <hyperlink ref="B313" r:id="rId282"/>
-    <hyperlink ref="B314" r:id="rId283"/>
-    <hyperlink ref="B315" r:id="rId284" display="Interleave the first half of the queue with second half"/>
-    <hyperlink ref="B316" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps"/>
-    <hyperlink ref="B317" r:id="rId286" display="Minimum time required to rot all oranges"/>
-    <hyperlink ref="B318" r:id="rId287"/>
-    <hyperlink ref="B319" r:id="rId288" display="First negative integer in every window of size “k”"/>
-    <hyperlink ref="B320" r:id="rId289"/>
-    <hyperlink ref="B321" r:id="rId290" display="Sum of minimum and maximum elements of all subarrays of size “k”."/>
-    <hyperlink ref="B322" r:id="rId291"/>
-    <hyperlink ref="B323" r:id="rId292"/>
-    <hyperlink ref="B325" r:id="rId293" display="Next Smaller Element"/>
-    <hyperlink ref="B328" r:id="rId294"/>
-    <hyperlink ref="B329" r:id="rId295"/>
-    <hyperlink ref="B330" r:id="rId296"/>
-    <hyperlink ref="B331" r:id="rId297"/>
-    <hyperlink ref="B332" r:id="rId298"/>
-    <hyperlink ref="B333" r:id="rId299"/>
-    <hyperlink ref="B334" r:id="rId300"/>
-    <hyperlink ref="B335" r:id="rId301"/>
-    <hyperlink ref="B336" r:id="rId302"/>
-    <hyperlink ref="B337" r:id="rId303" display="Merge “K” Sorted Linked Lists [V.IMP]"/>
-    <hyperlink ref="B338" r:id="rId304"/>
-    <hyperlink ref="B339" r:id="rId305"/>
-    <hyperlink ref="B340" r:id="rId306"/>
-    <hyperlink ref="B341" r:id="rId307"/>
-    <hyperlink ref="B342" r:id="rId308"/>
-    <hyperlink ref="B343" r:id="rId309"/>
-    <hyperlink ref="B344" r:id="rId310"/>
-    <hyperlink ref="B345" r:id="rId311"/>
-    <hyperlink ref="B349" r:id="rId312"/>
-    <hyperlink ref="B350" r:id="rId313"/>
-    <hyperlink ref="B351" r:id="rId314"/>
-    <hyperlink ref="B352" r:id="rId315"/>
-    <hyperlink ref="B353" r:id="rId316"/>
-    <hyperlink ref="B354" r:id="rId317"/>
-    <hyperlink ref="B355" r:id="rId318"/>
-    <hyperlink ref="B356" r:id="rId319"/>
-    <hyperlink ref="B357" r:id="rId320"/>
-    <hyperlink ref="B358" r:id="rId321"/>
-    <hyperlink ref="B359" r:id="rId322"/>
-    <hyperlink ref="B360" r:id="rId323"/>
-    <hyperlink ref="B361" r:id="rId324"/>
-    <hyperlink ref="B362" r:id="rId325"/>
-    <hyperlink ref="B363" r:id="rId326"/>
-    <hyperlink ref="B364" r:id="rId327"/>
-    <hyperlink ref="B365" r:id="rId328"/>
-    <hyperlink ref="B366" r:id="rId329"/>
-    <hyperlink ref="B367" r:id="rId330"/>
-    <hyperlink ref="B368" r:id="rId331"/>
-    <hyperlink ref="B369" r:id="rId332"/>
-    <hyperlink ref="B370" r:id="rId333"/>
-    <hyperlink ref="B371" r:id="rId334" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B372" r:id="rId335"/>
-    <hyperlink ref="B373" r:id="rId336"/>
-    <hyperlink ref="B374" r:id="rId337"/>
-    <hyperlink ref="B375" r:id="rId338"/>
-    <hyperlink ref="B376" r:id="rId339"/>
-    <hyperlink ref="B377" r:id="rId340"/>
-    <hyperlink ref="B378" r:id="rId341"/>
-    <hyperlink ref="B379" r:id="rId342"/>
-    <hyperlink ref="B380" r:id="rId343"/>
-    <hyperlink ref="B381" r:id="rId344"/>
-    <hyperlink ref="B382" r:id="rId345"/>
-    <hyperlink ref="B383" r:id="rId346"/>
-    <hyperlink ref="B384" r:id="rId347"/>
-    <hyperlink ref="B385" r:id="rId348"/>
-    <hyperlink ref="B387" r:id="rId349"/>
-    <hyperlink ref="B386" r:id="rId350"/>
-    <hyperlink ref="B388" r:id="rId351"/>
-    <hyperlink ref="B389" r:id="rId352"/>
-    <hyperlink ref="B390" r:id="rId353"/>
-    <hyperlink ref="B393" r:id="rId354"/>
-    <hyperlink ref="B394" r:id="rId355"/>
-    <hyperlink ref="B395" r:id="rId356"/>
-    <hyperlink ref="B396" r:id="rId357"/>
-    <hyperlink ref="B397" r:id="rId358"/>
-    <hyperlink ref="B398" r:id="rId359"/>
-    <hyperlink ref="B401" r:id="rId360"/>
-    <hyperlink ref="B402" r:id="rId361"/>
-    <hyperlink ref="B403" r:id="rId362"/>
-    <hyperlink ref="B404" r:id="rId363"/>
-    <hyperlink ref="B405" r:id="rId364"/>
-    <hyperlink ref="B406" r:id="rId365"/>
-    <hyperlink ref="B407" r:id="rId366"/>
-    <hyperlink ref="B408" r:id="rId367"/>
-    <hyperlink ref="B409" r:id="rId368"/>
-    <hyperlink ref="B410" r:id="rId369"/>
-    <hyperlink ref="B411" r:id="rId370"/>
-    <hyperlink ref="B412" r:id="rId371"/>
-    <hyperlink ref="B413" r:id="rId372"/>
-    <hyperlink ref="B414" r:id="rId373"/>
-    <hyperlink ref="B415" r:id="rId374"/>
-    <hyperlink ref="B416" r:id="rId375"/>
-    <hyperlink ref="B417" r:id="rId376"/>
-    <hyperlink ref="B418" r:id="rId377"/>
-    <hyperlink ref="B419" r:id="rId378"/>
-    <hyperlink ref="B420" r:id="rId379"/>
-    <hyperlink ref="B421" r:id="rId380"/>
-    <hyperlink ref="B422" r:id="rId381"/>
-    <hyperlink ref="B423" r:id="rId382"/>
-    <hyperlink ref="B424" r:id="rId383"/>
-    <hyperlink ref="B425" r:id="rId384"/>
-    <hyperlink ref="B426" r:id="rId385"/>
-    <hyperlink ref="B427" r:id="rId386"/>
-    <hyperlink ref="B428" r:id="rId387"/>
-    <hyperlink ref="B429" r:id="rId388"/>
-    <hyperlink ref="B430" r:id="rId389"/>
-    <hyperlink ref="B431" r:id="rId390"/>
-    <hyperlink ref="B432" r:id="rId391"/>
-    <hyperlink ref="B433" r:id="rId392"/>
-    <hyperlink ref="B434" r:id="rId393"/>
-    <hyperlink ref="B435" r:id="rId394"/>
-    <hyperlink ref="B436" r:id="rId395"/>
-    <hyperlink ref="B437" r:id="rId396"/>
-    <hyperlink ref="B438" r:id="rId397"/>
-    <hyperlink ref="B439" r:id="rId398"/>
-    <hyperlink ref="B440" r:id="rId399"/>
-    <hyperlink ref="B442" r:id="rId400"/>
-    <hyperlink ref="B441" r:id="rId401"/>
-    <hyperlink ref="B443" r:id="rId402"/>
-    <hyperlink ref="B444" r:id="rId403"/>
-    <hyperlink ref="B445" r:id="rId404"/>
-    <hyperlink ref="B446" r:id="rId405"/>
-    <hyperlink ref="B447" r:id="rId406"/>
-    <hyperlink ref="B448" r:id="rId407"/>
-    <hyperlink ref="B449" r:id="rId408"/>
-    <hyperlink ref="B450" r:id="rId409"/>
-    <hyperlink ref="B451" r:id="rId410"/>
-    <hyperlink ref="B452" r:id="rId411"/>
-    <hyperlink ref="B453" r:id="rId412"/>
-    <hyperlink ref="B460" r:id="rId413"/>
-    <hyperlink ref="B459" r:id="rId414"/>
-    <hyperlink ref="B458" r:id="rId415"/>
-    <hyperlink ref="B457" r:id="rId416"/>
-    <hyperlink ref="B456" r:id="rId417"/>
-    <hyperlink ref="B455" r:id="rId418"/>
-    <hyperlink ref="B454" r:id="rId419"/>
-    <hyperlink ref="B463" r:id="rId420"/>
-    <hyperlink ref="B464" r:id="rId421"/>
-    <hyperlink ref="B465" r:id="rId422"/>
-    <hyperlink ref="B466" r:id="rId423"/>
-    <hyperlink ref="B467" r:id="rId424"/>
-    <hyperlink ref="B468" r:id="rId425"/>
-    <hyperlink ref="B469" r:id="rId426"/>
-    <hyperlink ref="B472" r:id="rId427" display="Power Set"/>
-    <hyperlink ref="B470" r:id="rId428"/>
-    <hyperlink ref="B471" r:id="rId429" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B348" r:id="rId430"/>
-    <hyperlink ref="D16" r:id="rId431"/>
-    <hyperlink ref="D5" r:id="rId432"/>
-    <hyperlink ref="D7" r:id="rId433"/>
-    <hyperlink ref="D11" r:id="rId434"/>
-    <hyperlink ref="D6" r:id="rId435"/>
-    <hyperlink ref="D8" r:id="rId436"/>
-    <hyperlink ref="D15" r:id="rId437"/>
-    <hyperlink ref="D14" r:id="rId438"/>
-    <hyperlink ref="D20" r:id="rId439"/>
-    <hyperlink ref="D54" r:id="rId440"/>
-    <hyperlink ref="D13" r:id="rId441"/>
-    <hyperlink ref="D31" r:id="rId442"/>
-    <hyperlink ref="D26" r:id="rId443"/>
-    <hyperlink ref="D21" r:id="rId444"/>
-    <hyperlink ref="D18" r:id="rId445"/>
-    <hyperlink ref="D42" r:id="rId446"/>
-    <hyperlink ref="D55" r:id="rId447"/>
-    <hyperlink ref="D56" r:id="rId448"/>
-    <hyperlink ref="D101" r:id="rId449"/>
-    <hyperlink ref="D98" r:id="rId450"/>
-    <hyperlink ref="D108" r:id="rId451"/>
-    <hyperlink ref="D152" r:id="rId452"/>
-    <hyperlink ref="D146" r:id="rId453"/>
-    <hyperlink ref="D129" r:id="rId454"/>
-    <hyperlink ref="D130" r:id="rId455"/>
-    <hyperlink ref="D131" r:id="rId456"/>
-    <hyperlink ref="D134" r:id="rId457"/>
-    <hyperlink ref="D135" r:id="rId458"/>
-    <hyperlink ref="D137" r:id="rId459"/>
-    <hyperlink ref="D142" r:id="rId460"/>
-    <hyperlink ref="D145" r:id="rId461"/>
-    <hyperlink ref="D143" r:id="rId462"/>
-    <hyperlink ref="D144" r:id="rId463"/>
-    <hyperlink ref="D160" r:id="rId464"/>
-    <hyperlink ref="D161" r:id="rId465"/>
-    <hyperlink ref="D136" r:id="rId466"/>
-    <hyperlink ref="D162" r:id="rId467"/>
-    <hyperlink ref="D154" r:id="rId468"/>
-    <hyperlink ref="B156" r:id="rId469" display="Merge K sorted Linked list"/>
-    <hyperlink ref="D157" r:id="rId470"/>
-    <hyperlink ref="D156" r:id="rId471"/>
-    <hyperlink ref="D155" r:id="rId472"/>
-    <hyperlink ref="D151" r:id="rId473"/>
-    <hyperlink ref="D170" r:id="rId474"/>
-    <hyperlink ref="D172" r:id="rId475"/>
-    <hyperlink ref="D171" r:id="rId476"/>
-    <hyperlink ref="D165" r:id="rId477"/>
-    <hyperlink ref="D167" r:id="rId478"/>
-    <hyperlink ref="D178" r:id="rId479"/>
-    <hyperlink ref="D169" r:id="rId480"/>
-    <hyperlink ref="D168" r:id="rId481"/>
-    <hyperlink ref="D177" r:id="rId482"/>
-    <hyperlink ref="D194" r:id="rId483"/>
-    <hyperlink ref="D180" r:id="rId484"/>
-    <hyperlink ref="D173" r:id="rId485"/>
-    <hyperlink ref="D174" r:id="rId486"/>
-    <hyperlink ref="D197" r:id="rId487"/>
-    <hyperlink ref="B197" r:id="rId488"/>
-    <hyperlink ref="D182" r:id="rId489"/>
-    <hyperlink ref="D204" r:id="rId490"/>
-    <hyperlink ref="D196" r:id="rId491"/>
-    <hyperlink ref="D166" r:id="rId492"/>
-    <hyperlink ref="D184" r:id="rId493"/>
-    <hyperlink ref="D190" r:id="rId494"/>
-    <hyperlink ref="D205" r:id="rId495"/>
-    <hyperlink ref="D218" r:id="rId496"/>
-    <hyperlink ref="D186" r:id="rId497"/>
-    <hyperlink ref="D208" r:id="rId498"/>
-    <hyperlink ref="D25" r:id="rId499"/>
-    <hyperlink ref="D210" r:id="rId500"/>
-    <hyperlink ref="D221" r:id="rId501"/>
-    <hyperlink ref="D212" r:id="rId502"/>
-    <hyperlink ref="D49" r:id="rId503"/>
-    <hyperlink ref="D209" r:id="rId504"/>
-    <hyperlink ref="D331" r:id="rId505"/>
-    <hyperlink ref="D341" r:id="rId506"/>
-    <hyperlink ref="D337" r:id="rId507"/>
-    <hyperlink ref="D345" r:id="rId508"/>
-    <hyperlink ref="D336" r:id="rId509"/>
-    <hyperlink ref="D9" r:id="rId510"/>
-    <hyperlink ref="D38" r:id="rId511"/>
-    <hyperlink ref="D23" r:id="rId512"/>
-    <hyperlink ref="B39" r:id="rId513" display="Median of 2 sorted arrays of equal size"/>
-    <hyperlink ref="D39" r:id="rId514"/>
-    <hyperlink ref="D33" r:id="rId515"/>
-    <hyperlink ref="D43" r:id="rId516"/>
-    <hyperlink ref="D45" r:id="rId517"/>
-    <hyperlink ref="D50" r:id="rId518"/>
-    <hyperlink ref="D278" r:id="rId519"/>
-    <hyperlink ref="D27" r:id="rId520"/>
-    <hyperlink ref="D24" r:id="rId521"/>
-    <hyperlink ref="D37" r:id="rId522"/>
-    <hyperlink ref="D19" r:id="rId523"/>
-    <hyperlink ref="D12" r:id="rId524"/>
-    <hyperlink ref="D34" r:id="rId525"/>
-    <hyperlink ref="D10" r:id="rId526"/>
-    <hyperlink ref="D99" r:id="rId527"/>
-    <hyperlink ref="D22" r:id="rId528"/>
-    <hyperlink ref="D100" r:id="rId529"/>
-    <hyperlink ref="D290" r:id="rId530"/>
-    <hyperlink ref="D294" r:id="rId531"/>
-    <hyperlink ref="D291" r:id="rId532"/>
-    <hyperlink ref="D299" r:id="rId533"/>
-    <hyperlink ref="D301" r:id="rId534"/>
-    <hyperlink ref="D295" r:id="rId535"/>
-    <hyperlink ref="D293" r:id="rId536"/>
-    <hyperlink ref="D300" r:id="rId537"/>
-    <hyperlink ref="D305" r:id="rId538"/>
-    <hyperlink ref="D78" r:id="rId539"/>
-    <hyperlink ref="D73" r:id="rId540"/>
-    <hyperlink ref="D325" r:id="rId541"/>
-    <hyperlink ref="D296" r:id="rId542"/>
-    <hyperlink ref="D303" r:id="rId543"/>
-    <hyperlink ref="D297" r:id="rId544"/>
-    <hyperlink ref="D47" r:id="rId545"/>
-    <hyperlink ref="F295" r:id="rId546"/>
-    <hyperlink ref="D311" r:id="rId547"/>
-    <hyperlink ref="D313" r:id="rId548"/>
-    <hyperlink ref="D319" r:id="rId549"/>
-    <hyperlink ref="B324" r:id="rId550"/>
-    <hyperlink ref="D324" r:id="rId551"/>
-    <hyperlink ref="D466" r:id="rId552"/>
-    <hyperlink ref="D467" r:id="rId553"/>
-    <hyperlink ref="D472" r:id="rId554"/>
-    <hyperlink ref="D468" r:id="rId555"/>
-    <hyperlink ref="D464" r:id="rId556"/>
-    <hyperlink ref="D465" r:id="rId557"/>
-    <hyperlink ref="D471" r:id="rId558"/>
-    <hyperlink ref="D470" r:id="rId559"/>
-    <hyperlink ref="D105" r:id="rId560"/>
-    <hyperlink ref="D104" r:id="rId561"/>
-    <hyperlink ref="D107" r:id="rId562"/>
-    <hyperlink ref="D112" r:id="rId563"/>
-    <hyperlink ref="D314" r:id="rId564"/>
-    <hyperlink ref="D315" r:id="rId565"/>
-    <hyperlink ref="D298" r:id="rId566"/>
-    <hyperlink ref="D306" r:id="rId567"/>
-    <hyperlink ref="B199" r:id="rId568" display="Kth Ancestor of node in a Binary tree"/>
-    <hyperlink ref="D316" r:id="rId569"/>
-    <hyperlink ref="D310" r:id="rId570"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" display="Merge Intervals" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B31" r:id="rId27" display="Find the triplet that sum to a given value" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B32" r:id="rId28" display="Trapping Rain water problem" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B33" r:id="rId29" display="Chocolate Distribution problem" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B34" r:id="rId30" display="Smallest Subarray with sum greater than a given value" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B36" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B38" r:id="rId34" display="Median of 2 sorted arrays of equal size" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B42" r:id="rId35" display="Spiral traversal on a Matrix" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B43" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B44" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B45" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B46" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B47" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B49" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B50" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B51" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B54" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B55" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B56" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B57" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B58" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B59" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B60" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B61" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B62" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B63" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B64" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B65" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B66" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B67" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B68" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B69" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B70" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B71" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B72" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B73" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B74" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B75" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B76" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B77" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B78" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B79" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B80" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B81" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B82" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B83" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B84" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B85" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B86" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B87" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B88" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B89" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B90" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B91" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B92" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B93" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B94" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B95" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B98" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B99" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B100" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B101" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B103" r:id="rId91" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B104" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B105" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B106" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B107" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B108" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B110" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B111" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B112" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B113" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B114" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B115" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B116" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B117" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B118" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B119" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B120" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B121" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B122" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B123" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B124" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B125" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B126" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B102" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B109" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B129" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B130" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B131" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B132" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B133" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B134" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B135" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B136" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B137" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B138" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B139" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B140" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B141" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B142" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B143" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B144" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B145" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B146" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B147" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B148" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B149" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B150" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B153" r:id="rId138" display="Flatten a Linked List" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B154" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B155" r:id="rId140" display="Clone a linked list with next and random pointer" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B157" r:id="rId141" display="Merge K sorted Linked list" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B158" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B159" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B160" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B161" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B162" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B165" r:id="rId147" display="level order traversal" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B166" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B167" r:id="rId149" display="Height of a tree" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B168" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B169" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B170" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B171" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B172" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B173" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B174" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B175" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B176" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B177" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="B178" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B179" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B180" r:id="rId162" display="Boundary traversal of a Binary tree" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B181" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B182" r:id="rId164" display="Convert Binary tree into Doubly Linked List" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B183" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B184" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B185" r:id="rId167" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B187" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B188" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B189" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B190" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B191" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B192" r:id="rId173" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B193" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B194" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B195" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B196" r:id="rId177" display="Find LCA in a Binary tree" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B198" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B200" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B201" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B204" r:id="rId181" display="Fina a value in a BST" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B207" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B208" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B209" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B210" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B211" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B212" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="B213" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B214" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="B215" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="B216" r:id="rId191" display="Merge two BST [ V.V.V&gt;IMP ]" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="B217" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="B218" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="B219" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B220" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="B221" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B222" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="B223" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B224" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="B225" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B226" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="B227" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B230" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="B231" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B232" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="B233" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B234" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="B235" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B236" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="B237" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B238" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="B239" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B240" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="B241" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B242" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B243" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B244" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B245" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B246" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B247" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B248" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B249" r:id="rId222" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B250" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B251" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B252" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B253" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B254" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B255" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B256" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B257" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B258" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B259" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B260" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B261" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B262" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B263" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B264" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="B267" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B268" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B269" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="B270" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B271" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B272" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="B273" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B274" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B275" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B276" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B277" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B278" r:id="rId249" display="Combinational Sum" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B279" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B280" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="B281" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B282" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B283" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B284" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B285" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B288" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B289" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B290" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B291" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B292" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B293" r:id="rId262" display="Check the expression has valid or Balanced parenthesis or not." xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B294" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B295" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B296" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B297" r:id="rId266" display="The celebrity Problem" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B298" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B299" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B300" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B301" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B302" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B303" r:id="rId272" display="Largest rectangular Area in Histogram" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B304" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B305" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B306" r:id="rId275" display="Implement Stack using Queue" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B307" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B308" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B309" r:id="rId278" display="Implement Queue using Stack  " xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B310" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B311" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B312" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B313" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B314" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B315" r:id="rId284" display="Interleave the first half of the queue with second half" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B316" r:id="rId285" display="Find the first circular tour that visits all Petrol Pumps" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B317" r:id="rId286" display="Minimum time required to rot all oranges" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B318" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B319" r:id="rId288" display="First negative integer in every window of size “k”" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B320" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B321" r:id="rId290" display="Sum of minimum and maximum elements of all subarrays of size “k”." xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B322" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B323" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B325" r:id="rId293" display="Next Smaller Element" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B328" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B329" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B330" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B331" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B332" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B333" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B334" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="B335" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="B336" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="B337" r:id="rId303" display="Merge “K” Sorted Linked Lists [V.IMP]" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="B338" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="B339" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="B340" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="B341" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="B342" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="B343" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="B344" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="B345" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="B349" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="B350" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="B351" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B352" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="B353" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="B354" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="B355" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="B356" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="B357" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="B358" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="B359" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="B360" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="B361" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="B362" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="B363" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="B364" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="B365" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="B366" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="B367" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="B368" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="B369" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="B370" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="B371" r:id="rId334" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="B372" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="B373" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="B374" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="B375" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="B376" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="B377" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="B378" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="B379" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="B380" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="B381" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="B382" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="B383" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="B384" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="B385" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="B387" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="B386" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="B388" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="B389" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="B390" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="B393" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="B394" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="B395" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="B396" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="B397" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="B398" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="B401" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="B402" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="B403" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="B404" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="B405" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="B406" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="B407" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="B408" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="B409" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="B410" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="B411" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="B412" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="B413" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="B414" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="B415" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="B416" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="B417" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="B418" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="B419" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="B420" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="B421" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="B422" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="B423" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="B424" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="B425" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="B426" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="B427" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="B428" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="B429" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="B430" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="B431" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="B432" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="B433" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="B434" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="B435" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="B436" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="B437" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="B438" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="B439" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="B440" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="B442" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="B441" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="B443" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="B444" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="B445" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="B446" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="B447" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="B448" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="B449" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="B450" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="B451" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="B452" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="B453" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="B460" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="B459" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="B458" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="B457" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="B456" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="B455" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="B454" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="B463" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="B464" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
+    <hyperlink ref="B465" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
+    <hyperlink ref="B466" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
+    <hyperlink ref="B467" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
+    <hyperlink ref="B468" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
+    <hyperlink ref="B469" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
+    <hyperlink ref="B472" r:id="rId427" display="Power Set" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
+    <hyperlink ref="B470" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
+    <hyperlink ref="B471" r:id="rId429" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
+    <hyperlink ref="B348" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
+    <hyperlink ref="D16" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
+    <hyperlink ref="D5" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
+    <hyperlink ref="D7" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
+    <hyperlink ref="D11" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
+    <hyperlink ref="D6" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
+    <hyperlink ref="D8" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
+    <hyperlink ref="D15" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
+    <hyperlink ref="D14" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
+    <hyperlink ref="D20" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
+    <hyperlink ref="D54" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
+    <hyperlink ref="D13" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
+    <hyperlink ref="D31" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
+    <hyperlink ref="D26" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
+    <hyperlink ref="D21" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
+    <hyperlink ref="D18" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
+    <hyperlink ref="D42" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
+    <hyperlink ref="D55" r:id="rId447" xr:uid="{00000000-0004-0000-0000-0000BE010000}"/>
+    <hyperlink ref="D56" r:id="rId448" xr:uid="{00000000-0004-0000-0000-0000BF010000}"/>
+    <hyperlink ref="D101" r:id="rId449" xr:uid="{00000000-0004-0000-0000-0000C0010000}"/>
+    <hyperlink ref="D98" r:id="rId450" xr:uid="{00000000-0004-0000-0000-0000C1010000}"/>
+    <hyperlink ref="D108" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
+    <hyperlink ref="D152" r:id="rId452" xr:uid="{00000000-0004-0000-0000-0000C3010000}"/>
+    <hyperlink ref="D146" r:id="rId453" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
+    <hyperlink ref="D129" r:id="rId454" xr:uid="{00000000-0004-0000-0000-0000C5010000}"/>
+    <hyperlink ref="D130" r:id="rId455" xr:uid="{00000000-0004-0000-0000-0000C6010000}"/>
+    <hyperlink ref="D131" r:id="rId456" xr:uid="{00000000-0004-0000-0000-0000C7010000}"/>
+    <hyperlink ref="D134" r:id="rId457" xr:uid="{00000000-0004-0000-0000-0000C8010000}"/>
+    <hyperlink ref="D135" r:id="rId458" xr:uid="{00000000-0004-0000-0000-0000C9010000}"/>
+    <hyperlink ref="D137" r:id="rId459" xr:uid="{00000000-0004-0000-0000-0000CA010000}"/>
+    <hyperlink ref="D142" r:id="rId460" xr:uid="{00000000-0004-0000-0000-0000CB010000}"/>
+    <hyperlink ref="D145" r:id="rId461" xr:uid="{00000000-0004-0000-0000-0000CC010000}"/>
+    <hyperlink ref="D143" r:id="rId462" xr:uid="{00000000-0004-0000-0000-0000CD010000}"/>
+    <hyperlink ref="D144" r:id="rId463" xr:uid="{00000000-0004-0000-0000-0000CE010000}"/>
+    <hyperlink ref="D160" r:id="rId464" xr:uid="{00000000-0004-0000-0000-0000CF010000}"/>
+    <hyperlink ref="D161" r:id="rId465" xr:uid="{00000000-0004-0000-0000-0000D0010000}"/>
+    <hyperlink ref="D136" r:id="rId466" xr:uid="{00000000-0004-0000-0000-0000D1010000}"/>
+    <hyperlink ref="D162" r:id="rId467" xr:uid="{00000000-0004-0000-0000-0000D2010000}"/>
+    <hyperlink ref="D154" r:id="rId468" xr:uid="{00000000-0004-0000-0000-0000D3010000}"/>
+    <hyperlink ref="B156" r:id="rId469" display="Merge K sorted Linked list" xr:uid="{00000000-0004-0000-0000-0000D4010000}"/>
+    <hyperlink ref="D157" r:id="rId470" xr:uid="{00000000-0004-0000-0000-0000D5010000}"/>
+    <hyperlink ref="D156" r:id="rId471" xr:uid="{00000000-0004-0000-0000-0000D6010000}"/>
+    <hyperlink ref="D155" r:id="rId472" xr:uid="{00000000-0004-0000-0000-0000D7010000}"/>
+    <hyperlink ref="D151" r:id="rId473" xr:uid="{00000000-0004-0000-0000-0000D8010000}"/>
+    <hyperlink ref="D170" r:id="rId474" xr:uid="{00000000-0004-0000-0000-0000D9010000}"/>
+    <hyperlink ref="D172" r:id="rId475" xr:uid="{00000000-0004-0000-0000-0000DA010000}"/>
+    <hyperlink ref="D171" r:id="rId476" xr:uid="{00000000-0004-0000-0000-0000DB010000}"/>
+    <hyperlink ref="D165" r:id="rId477" xr:uid="{00000000-0004-0000-0000-0000DC010000}"/>
+    <hyperlink ref="D167" r:id="rId478" xr:uid="{00000000-0004-0000-0000-0000DD010000}"/>
+    <hyperlink ref="D178" r:id="rId479" xr:uid="{00000000-0004-0000-0000-0000DE010000}"/>
+    <hyperlink ref="D169" r:id="rId480" xr:uid="{00000000-0004-0000-0000-0000DF010000}"/>
+    <hyperlink ref="D168" r:id="rId481" xr:uid="{00000000-0004-0000-0000-0000E0010000}"/>
+    <hyperlink ref="D177" r:id="rId482" xr:uid="{00000000-0004-0000-0000-0000E1010000}"/>
+    <hyperlink ref="D194" r:id="rId483" xr:uid="{00000000-0004-0000-0000-0000E2010000}"/>
+    <hyperlink ref="D180" r:id="rId484" xr:uid="{00000000-0004-0000-0000-0000E3010000}"/>
+    <hyperlink ref="D173" r:id="rId485" xr:uid="{00000000-0004-0000-0000-0000E4010000}"/>
+    <hyperlink ref="D174" r:id="rId486" xr:uid="{00000000-0004-0000-0000-0000E5010000}"/>
+    <hyperlink ref="D197" r:id="rId487" xr:uid="{00000000-0004-0000-0000-0000E6010000}"/>
+    <hyperlink ref="B197" r:id="rId488" xr:uid="{00000000-0004-0000-0000-0000E7010000}"/>
+    <hyperlink ref="D182" r:id="rId489" xr:uid="{00000000-0004-0000-0000-0000E8010000}"/>
+    <hyperlink ref="D204" r:id="rId490" xr:uid="{00000000-0004-0000-0000-0000E9010000}"/>
+    <hyperlink ref="D196" r:id="rId491" xr:uid="{00000000-0004-0000-0000-0000EA010000}"/>
+    <hyperlink ref="D166" r:id="rId492" xr:uid="{00000000-0004-0000-0000-0000EB010000}"/>
+    <hyperlink ref="D184" r:id="rId493" xr:uid="{00000000-0004-0000-0000-0000EC010000}"/>
+    <hyperlink ref="D190" r:id="rId494" xr:uid="{00000000-0004-0000-0000-0000ED010000}"/>
+    <hyperlink ref="D205" r:id="rId495" xr:uid="{00000000-0004-0000-0000-0000EE010000}"/>
+    <hyperlink ref="D218" r:id="rId496" xr:uid="{00000000-0004-0000-0000-0000EF010000}"/>
+    <hyperlink ref="D186" r:id="rId497" xr:uid="{00000000-0004-0000-0000-0000F0010000}"/>
+    <hyperlink ref="D208" r:id="rId498" xr:uid="{00000000-0004-0000-0000-0000F1010000}"/>
+    <hyperlink ref="D25" r:id="rId499" xr:uid="{00000000-0004-0000-0000-0000F2010000}"/>
+    <hyperlink ref="D210" r:id="rId500" xr:uid="{00000000-0004-0000-0000-0000F3010000}"/>
+    <hyperlink ref="D221" r:id="rId501" xr:uid="{00000000-0004-0000-0000-0000F4010000}"/>
+    <hyperlink ref="D212" r:id="rId502" xr:uid="{00000000-0004-0000-0000-0000F5010000}"/>
+    <hyperlink ref="D49" r:id="rId503" xr:uid="{00000000-0004-0000-0000-0000F6010000}"/>
+    <hyperlink ref="D209" r:id="rId504" xr:uid="{00000000-0004-0000-0000-0000F7010000}"/>
+    <hyperlink ref="D331" r:id="rId505" xr:uid="{00000000-0004-0000-0000-0000F8010000}"/>
+    <hyperlink ref="D341" r:id="rId506" xr:uid="{00000000-0004-0000-0000-0000F9010000}"/>
+    <hyperlink ref="D337" r:id="rId507" xr:uid="{00000000-0004-0000-0000-0000FA010000}"/>
+    <hyperlink ref="D345" r:id="rId508" xr:uid="{00000000-0004-0000-0000-0000FB010000}"/>
+    <hyperlink ref="D336" r:id="rId509" xr:uid="{00000000-0004-0000-0000-0000FC010000}"/>
+    <hyperlink ref="D9" r:id="rId510" xr:uid="{00000000-0004-0000-0000-0000FD010000}"/>
+    <hyperlink ref="D38" r:id="rId511" xr:uid="{00000000-0004-0000-0000-0000FE010000}"/>
+    <hyperlink ref="D23" r:id="rId512" xr:uid="{00000000-0004-0000-0000-0000FF010000}"/>
+    <hyperlink ref="B39" r:id="rId513" display="Median of 2 sorted arrays of equal size" xr:uid="{00000000-0004-0000-0000-000000020000}"/>
+    <hyperlink ref="D39" r:id="rId514" xr:uid="{00000000-0004-0000-0000-000001020000}"/>
+    <hyperlink ref="D33" r:id="rId515" xr:uid="{00000000-0004-0000-0000-000002020000}"/>
+    <hyperlink ref="D43" r:id="rId516" xr:uid="{00000000-0004-0000-0000-000003020000}"/>
+    <hyperlink ref="D45" r:id="rId517" xr:uid="{00000000-0004-0000-0000-000004020000}"/>
+    <hyperlink ref="D50" r:id="rId518" xr:uid="{00000000-0004-0000-0000-000005020000}"/>
+    <hyperlink ref="D278" r:id="rId519" xr:uid="{00000000-0004-0000-0000-000006020000}"/>
+    <hyperlink ref="D27" r:id="rId520" xr:uid="{00000000-0004-0000-0000-000007020000}"/>
+    <hyperlink ref="D24" r:id="rId521" xr:uid="{00000000-0004-0000-0000-000008020000}"/>
+    <hyperlink ref="D37" r:id="rId522" xr:uid="{00000000-0004-0000-0000-000009020000}"/>
+    <hyperlink ref="D19" r:id="rId523" xr:uid="{00000000-0004-0000-0000-00000A020000}"/>
+    <hyperlink ref="D12" r:id="rId524" xr:uid="{00000000-0004-0000-0000-00000B020000}"/>
+    <hyperlink ref="D34" r:id="rId525" xr:uid="{00000000-0004-0000-0000-00000C020000}"/>
+    <hyperlink ref="D10" r:id="rId526" xr:uid="{00000000-0004-0000-0000-00000D020000}"/>
+    <hyperlink ref="D99" r:id="rId527" xr:uid="{00000000-0004-0000-0000-00000E020000}"/>
+    <hyperlink ref="D22" r:id="rId528" xr:uid="{00000000-0004-0000-0000-00000F020000}"/>
+    <hyperlink ref="D100" r:id="rId529" xr:uid="{00000000-0004-0000-0000-000010020000}"/>
+    <hyperlink ref="D290" r:id="rId530" xr:uid="{00000000-0004-0000-0000-000011020000}"/>
+    <hyperlink ref="D294" r:id="rId531" xr:uid="{00000000-0004-0000-0000-000012020000}"/>
+    <hyperlink ref="D291" r:id="rId532" xr:uid="{00000000-0004-0000-0000-000013020000}"/>
+    <hyperlink ref="D299" r:id="rId533" xr:uid="{00000000-0004-0000-0000-000014020000}"/>
+    <hyperlink ref="D301" r:id="rId534" xr:uid="{00000000-0004-0000-0000-000015020000}"/>
+    <hyperlink ref="D295" r:id="rId535" xr:uid="{00000000-0004-0000-0000-000016020000}"/>
+    <hyperlink ref="D293" r:id="rId536" xr:uid="{00000000-0004-0000-0000-000017020000}"/>
+    <hyperlink ref="D300" r:id="rId537" xr:uid="{00000000-0004-0000-0000-000018020000}"/>
+    <hyperlink ref="D305" r:id="rId538" xr:uid="{00000000-0004-0000-0000-000019020000}"/>
+    <hyperlink ref="D78" r:id="rId539" xr:uid="{00000000-0004-0000-0000-00001A020000}"/>
+    <hyperlink ref="D73" r:id="rId540" xr:uid="{00000000-0004-0000-0000-00001B020000}"/>
+    <hyperlink ref="D325" r:id="rId541" xr:uid="{00000000-0004-0000-0000-00001C020000}"/>
+    <hyperlink ref="D296" r:id="rId542" xr:uid="{00000000-0004-0000-0000-00001D020000}"/>
+    <hyperlink ref="D303" r:id="rId543" xr:uid="{00000000-0004-0000-0000-00001E020000}"/>
+    <hyperlink ref="D297" r:id="rId544" xr:uid="{00000000-0004-0000-0000-00001F020000}"/>
+    <hyperlink ref="D47" r:id="rId545" xr:uid="{00000000-0004-0000-0000-000020020000}"/>
+    <hyperlink ref="F295" r:id="rId546" xr:uid="{00000000-0004-0000-0000-000021020000}"/>
+    <hyperlink ref="D311" r:id="rId547" xr:uid="{00000000-0004-0000-0000-000022020000}"/>
+    <hyperlink ref="D313" r:id="rId548" xr:uid="{00000000-0004-0000-0000-000023020000}"/>
+    <hyperlink ref="D319" r:id="rId549" xr:uid="{00000000-0004-0000-0000-000024020000}"/>
+    <hyperlink ref="B324" r:id="rId550" xr:uid="{00000000-0004-0000-0000-000025020000}"/>
+    <hyperlink ref="D324" r:id="rId551" xr:uid="{00000000-0004-0000-0000-000026020000}"/>
+    <hyperlink ref="D466" r:id="rId552" xr:uid="{00000000-0004-0000-0000-000027020000}"/>
+    <hyperlink ref="D467" r:id="rId553" xr:uid="{00000000-0004-0000-0000-000028020000}"/>
+    <hyperlink ref="D472" r:id="rId554" xr:uid="{00000000-0004-0000-0000-000029020000}"/>
+    <hyperlink ref="D468" r:id="rId555" xr:uid="{00000000-0004-0000-0000-00002A020000}"/>
+    <hyperlink ref="D464" r:id="rId556" xr:uid="{00000000-0004-0000-0000-00002B020000}"/>
+    <hyperlink ref="D465" r:id="rId557" xr:uid="{00000000-0004-0000-0000-00002C020000}"/>
+    <hyperlink ref="D471" r:id="rId558" xr:uid="{00000000-0004-0000-0000-00002D020000}"/>
+    <hyperlink ref="D470" r:id="rId559" xr:uid="{00000000-0004-0000-0000-00002E020000}"/>
+    <hyperlink ref="D105" r:id="rId560" xr:uid="{00000000-0004-0000-0000-00002F020000}"/>
+    <hyperlink ref="D104" r:id="rId561" xr:uid="{00000000-0004-0000-0000-000030020000}"/>
+    <hyperlink ref="D107" r:id="rId562" xr:uid="{00000000-0004-0000-0000-000031020000}"/>
+    <hyperlink ref="D112" r:id="rId563" xr:uid="{00000000-0004-0000-0000-000032020000}"/>
+    <hyperlink ref="D314" r:id="rId564" xr:uid="{00000000-0004-0000-0000-000033020000}"/>
+    <hyperlink ref="D315" r:id="rId565" xr:uid="{00000000-0004-0000-0000-000034020000}"/>
+    <hyperlink ref="D298" r:id="rId566" xr:uid="{00000000-0004-0000-0000-000035020000}"/>
+    <hyperlink ref="D306" r:id="rId567" xr:uid="{00000000-0004-0000-0000-000036020000}"/>
+    <hyperlink ref="B199" r:id="rId568" display="Kth Ancestor of node in a Binary tree" xr:uid="{00000000-0004-0000-0000-000037020000}"/>
+    <hyperlink ref="D316" r:id="rId569" xr:uid="{00000000-0004-0000-0000-000038020000}"/>
+    <hyperlink ref="D310" r:id="rId570" xr:uid="{00000000-0004-0000-0000-000039020000}"/>
+    <hyperlink ref="D348" r:id="rId571" xr:uid="{2A5AD221-FC32-4636-AAB6-ADB337165D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId571"/>
+  <pageSetup orientation="portrait" r:id="rId572"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sudoku solver and palindromic partitioning
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C46397E-522E-4A56-9866-32D1D30D6296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6D032D-822C-4F89-907E-733383939D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="621">
   <si>
     <t>Topic:</t>
   </si>
@@ -1877,6 +1877,30 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/create-a-graph-and-print-it_1214551?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=0&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Lovebabbar</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sudoku-solver/submissions/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/n-queen</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutations/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/permutation-sequence/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-partitioning/</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/subset-sums2234/1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flower-planting-with-no-adjacent/</t>
   </si>
 </sst>
 </file>
@@ -2643,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F349" sqref="F349"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F271" sqref="F271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5839,7 +5863,10 @@
         <v>231</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D268" s="20" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="269" spans="1:6" ht="21">
@@ -5872,9 +5899,11 @@
         <v>234</v>
       </c>
       <c r="C271" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D271" s="23"/>
+        <v>415</v>
+      </c>
+      <c r="D271" s="22" t="s">
+        <v>613</v>
+      </c>
       <c r="F271" s="23"/>
     </row>
     <row r="272" spans="1:6" s="7" customFormat="1" ht="21">
@@ -5885,9 +5914,11 @@
         <v>235</v>
       </c>
       <c r="C272" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D272" s="23"/>
+        <v>415</v>
+      </c>
+      <c r="D272" s="22" t="s">
+        <v>620</v>
+      </c>
       <c r="F272" s="23"/>
     </row>
     <row r="273" spans="1:6" ht="21">
@@ -5898,7 +5929,10 @@
         <v>236</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D273" s="20" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="21">
@@ -5909,7 +5943,10 @@
         <v>237</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D274" s="20" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="275" spans="1:6" ht="21">
@@ -5979,7 +6016,10 @@
         <v>242</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D280" s="20" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="281" spans="1:6" ht="21">
@@ -6012,7 +6052,10 @@
         <v>245</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D283" s="20" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="284" spans="1:6" ht="21">
@@ -6034,7 +6077,10 @@
         <v>247</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>2</v>
+        <v>415</v>
+      </c>
+      <c r="D285" s="20" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="21">
@@ -8778,8 +8824,16 @@
     <hyperlink ref="D316" r:id="rId569" xr:uid="{00000000-0004-0000-0000-000038020000}"/>
     <hyperlink ref="D310" r:id="rId570" xr:uid="{00000000-0004-0000-0000-000039020000}"/>
     <hyperlink ref="D348" r:id="rId571" xr:uid="{2A5AD221-FC32-4636-AAB6-ADB337165D7C}"/>
+    <hyperlink ref="D271" r:id="rId572" xr:uid="{07F30169-3EC5-4F07-A0DB-5A3206D92C0A}"/>
+    <hyperlink ref="D268" r:id="rId573" xr:uid="{3283DA81-46FF-424B-8090-30D283898FC3}"/>
+    <hyperlink ref="D280" r:id="rId574" xr:uid="{BACC2442-61AB-4071-B92F-AA3F9073FA3D}"/>
+    <hyperlink ref="D285" r:id="rId575" xr:uid="{B48BE9C4-EE8D-40EE-BB42-D914B06F63F7}"/>
+    <hyperlink ref="D283" r:id="rId576" xr:uid="{3395A06C-5B35-4560-9992-76F2961E580C}"/>
+    <hyperlink ref="D273" r:id="rId577" xr:uid="{4211F5F0-08D6-4447-8E7E-150B380A8DAD}"/>
+    <hyperlink ref="D274" r:id="rId578" xr:uid="{1B16E747-A583-45DF-A54B-6907513F0E18}"/>
+    <hyperlink ref="D272" r:id="rId579" xr:uid="{933B32DB-C051-4BC9-ABC7-B1199BA2C3B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId572"/>
+  <pageSetup orientation="portrait" r:id="rId580"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
top and bottom view of binary tree
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468F798C-F35E-40A6-BB09-094F756E402D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F0358-951F-4614-AB7D-665DE895662E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="623">
   <si>
     <t>Topic:</t>
   </si>
@@ -1901,6 +1901,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/linked-list-cycle-ii/</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/893110?topList=striver-sde-sheet-problems&amp;utm_source=striver&amp;utm_medium=website&amp;leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/top-view-of-the-tree_799401?topList=striver-sde-sheet-problems&amp;leftPanelTab=1</t>
   </si>
 </sst>
 </file>
@@ -2668,7 +2674,7 @@
   <dimension ref="A1:F464"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A172" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -4806,7 +4812,10 @@
         <v>151</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
+      </c>
+      <c r="D174" s="20" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="21">
@@ -4817,7 +4826,10 @@
         <v>152</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
+      </c>
+      <c r="D175" s="20" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="21">
@@ -8764,8 +8776,10 @@
     <hyperlink ref="D120" r:id="rId577" xr:uid="{BC3816F3-63CF-454F-A309-FDC77C099B17}"/>
     <hyperlink ref="D123" r:id="rId578" xr:uid="{637DC126-7F73-4B54-902F-7BFB02285785}"/>
     <hyperlink ref="D132" r:id="rId579" xr:uid="{F613950A-3D69-4F21-84A7-926EA067ECFD}"/>
+    <hyperlink ref="D175" r:id="rId580" xr:uid="{74F40F06-3413-446D-A4B8-70062A59FD80}"/>
+    <hyperlink ref="D174" r:id="rId581" xr:uid="{84A74533-FE49-4B04-8D2E-21E0D7D88EDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId580"/>
+  <pageSetup orientation="portrait" r:id="rId582"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
largest bst in binary tree
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA69618-3B34-46AD-BC88-04555C201418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08E751B-16BE-4C15-B362-8F934AC3EDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="630">
   <si>
     <t>Topic:</t>
   </si>
@@ -1916,6 +1916,18 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/flatten-a-linked-list_1112655?source=youtube&amp;campaign=YouTube_CodestudioLovebabbar5thfeb&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=YouTube_CodestudioLovebabbar5thfeb</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/893103?topList=striver-sde-sheet-problems&amp;utm_source=striver&amp;utm_medium=website&amp;leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/h_920474?leftPanelTab=0&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Lovebabbar</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/brothers-from-different-root/1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-binary-search-tree-from-preorder-traversal/</t>
   </si>
 </sst>
 </file>
@@ -2682,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A362" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C384" sqref="C384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -5300,7 +5312,10 @@
         <v>178</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
+      </c>
+      <c r="D212" s="20" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="21">
@@ -5311,7 +5326,7 @@
         <v>179</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="21">
@@ -5333,9 +5348,11 @@
         <v>469</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D215" s="23"/>
+        <v>406</v>
+      </c>
+      <c r="D215" s="22" t="s">
+        <v>627</v>
+      </c>
       <c r="F215" s="23"/>
     </row>
     <row r="216" spans="1:6" s="45" customFormat="1" ht="21">
@@ -5376,7 +5393,10 @@
         <v>183</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
+      </c>
+      <c r="D218" s="20" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="219" spans="1:6" ht="21">
@@ -5434,7 +5454,7 @@
         <v>188</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
       <c r="D223" s="51"/>
     </row>
@@ -5459,7 +5479,9 @@
       <c r="C225" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="D225" s="23"/>
+      <c r="D225" s="22" t="s">
+        <v>626</v>
+      </c>
       <c r="F225" s="23" t="s">
         <v>505</v>
       </c>
@@ -5472,7 +5494,10 @@
         <v>191</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
+      </c>
+      <c r="D226" s="20" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="21">
@@ -6848,7 +6873,7 @@
         <v>286</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="342" spans="1:6" ht="21">
@@ -6859,7 +6884,7 @@
         <v>287</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="343" spans="1:6" ht="21">
@@ -6892,7 +6917,7 @@
         <v>290</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="346" spans="1:6" ht="21">
@@ -6925,7 +6950,7 @@
         <v>293</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="349" spans="1:6" ht="21">
@@ -6958,7 +6983,7 @@
         <v>296</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="352" spans="1:6" ht="21">
@@ -7024,7 +7049,7 @@
         <v>302</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="358" spans="1:6" ht="21">
@@ -7035,7 +7060,7 @@
         <v>303</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="359" spans="1:6" ht="21">
@@ -7057,7 +7082,7 @@
         <v>305</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="361" spans="1:6" ht="21">
@@ -7068,7 +7093,7 @@
         <v>306</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>2</v>
+        <v>406</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="21">
@@ -8796,8 +8821,13 @@
     <hyperlink ref="D284" r:id="rId582" xr:uid="{BDE3BFDA-898C-4F79-A756-4CB03DE25326}"/>
     <hyperlink ref="D139" r:id="rId583" xr:uid="{11201B28-1E53-4645-8D2D-04E91DA92827}"/>
     <hyperlink ref="D152" r:id="rId584" xr:uid="{D0E4C4E1-FB63-420C-84A4-A7D2B81DD342}"/>
+    <hyperlink ref="D226" r:id="rId585" xr:uid="{B9391A48-F316-4ACB-B7A4-D1DACAF6DF9C}"/>
+    <hyperlink ref="D225" r:id="rId586" xr:uid="{15BE91D7-2E51-474E-821B-B84A7A267231}"/>
+    <hyperlink ref="D215" r:id="rId587" xr:uid="{48E69F75-57C7-43A3-94BE-B782F9630295}"/>
+    <hyperlink ref="D218" r:id="rId588" xr:uid="{82EFE91A-29ED-4A71-8D94-B3A19F47C5FE}"/>
+    <hyperlink ref="D212" r:id="rId589" xr:uid="{9A39CD08-6279-481A-8523-66667804FF43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId585"/>
+  <pageSetup orientation="portrait" r:id="rId590"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Median of Data Stream
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AD7D75-8D68-4004-B4A8-AEA8E0F7FAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04850855-AA63-487D-BFAA-73C8D85B5F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="633">
   <si>
     <t>Topic:</t>
   </si>
@@ -1928,6 +1928,15 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/is-binary-heap-tree_893136</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/merge-two-binary-max-heaps_1170049?leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/convert-bst-to-min-heap_920498?leftPanelTab=3</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/k-th-largest-sum-contiguous-subarray_920398?leftPanelTab=0&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Lovebabbar</t>
   </si>
 </sst>
 </file>
@@ -2694,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F323" sqref="F323"/>
+    <sheetView tabSelected="1" topLeftCell="A373" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D386" sqref="D386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6669,9 +6678,11 @@
         <v>271</v>
       </c>
       <c r="C324" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D324" s="23"/>
+        <v>405</v>
+      </c>
+      <c r="D324" s="22" t="s">
+        <v>411</v>
+      </c>
       <c r="F324" s="23"/>
     </row>
     <row r="325" spans="1:6" ht="21">
@@ -6682,7 +6693,10 @@
         <v>272</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>2</v>
+        <v>405</v>
+      </c>
+      <c r="D325" s="20" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="326" spans="1:6" ht="21">
@@ -6693,7 +6707,10 @@
         <v>273</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>2</v>
+        <v>405</v>
+      </c>
+      <c r="D326" s="20" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="327" spans="1:6" ht="21">
@@ -6725,32 +6742,33 @@
       </c>
       <c r="F328" s="23"/>
     </row>
-    <row r="329" spans="1:6" s="7" customFormat="1" ht="21">
-      <c r="A329" s="6" t="s">
+    <row r="329" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A329" s="30" t="s">
         <v>516</v>
       </c>
-      <c r="B329" s="7" t="s">
+      <c r="B329" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="C329" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D329" s="23"/>
-      <c r="F329" s="23"/>
-    </row>
-    <row r="330" spans="1:6" ht="21">
-      <c r="A330" s="5" t="s">
+      <c r="C329" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D329" s="32"/>
+      <c r="F329" s="32"/>
+    </row>
+    <row r="330" spans="1:6" s="31" customFormat="1" ht="21">
+      <c r="A330" s="30" t="s">
         <v>516</v>
       </c>
-      <c r="B330" s="13" t="s">
+      <c r="B330" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="C330" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D330" s="20" t="s">
+      <c r="C330" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="D330" s="32" t="s">
         <v>628</v>
       </c>
+      <c r="F330" s="32"/>
     </row>
     <row r="331" spans="1:6" ht="21">
       <c r="A331" s="5" t="s">
@@ -6789,7 +6807,10 @@
         <v>279</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>2</v>
+        <v>405</v>
+      </c>
+      <c r="D333" s="20" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="334" spans="1:6" s="7" customFormat="1" ht="21">
@@ -7337,7 +7358,7 @@
         <v>328</v>
       </c>
       <c r="C384" s="2" t="s">
-        <v>2</v>
+        <v>405</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="21">
@@ -7381,7 +7402,7 @@
         <v>331</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>2</v>
+        <v>405</v>
       </c>
     </row>
     <row r="389" spans="1:3" ht="21">
@@ -8819,8 +8840,12 @@
     <hyperlink ref="D323" r:id="rId588" xr:uid="{7F399674-A8E5-43A0-BEFD-3BEC339F9A6F}"/>
     <hyperlink ref="D330" r:id="rId589" xr:uid="{5F432E30-5183-423C-9F77-A58C590D2B01}"/>
     <hyperlink ref="D331" r:id="rId590" xr:uid="{A09FC207-0BFF-4605-ACE9-D73FA388FF6E}"/>
+    <hyperlink ref="D324" r:id="rId591" xr:uid="{5079FA9C-19D6-4DB2-867F-B8B2A9C2B02F}"/>
+    <hyperlink ref="D325" r:id="rId592" xr:uid="{2230611B-4601-46C3-BD2F-D9B097DF0CB0}"/>
+    <hyperlink ref="D333" r:id="rId593" xr:uid="{6334817C-4572-41DF-9A29-87030EF93249}"/>
+    <hyperlink ref="D326" r:id="rId594" xr:uid="{DC6DA814-F01B-4F59-AFB0-25D9D05A91D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId591"/>
+  <pageSetup orientation="portrait" r:id="rId595"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cycle in undirected graph
</commit_message>
<xml_diff>
--- a/450-QuestionSeries/FINAL450.xlsx
+++ b/450-QuestionSeries/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS&amp;algo\babbar DSA Series\450-QuestionSeries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4B374-690F-4C03-A269-46139E352BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C8EA7-8022-4782-ADD2-3E2BE9D89BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2995" uniqueCount="649">
   <si>
     <t>Topic:</t>
   </si>
@@ -1934,6 +1934,57 @@
   </si>
   <si>
     <t>https://www.codingninjas.com/codestudio/problems/implement-a-phone-directory_1062666?topList=love-babbar-dsa-sheet-problems&amp;leftPanelTab=0&amp;utm_source=youtube&amp;utm_medium=affiliate&amp;utm_campaign=Lovebabbar</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/dfs-traversal_630462?topList=striver-sde-sheet-problems&amp;leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/bfs-in-graph_973002?topList=striver-sde-sheet-problems&amp;leftPanelTab=0</t>
+  </si>
+  <si>
+    <t>https://www.codingninjas.com/codestudio/problems/1062670?topList=striver-sde-sheet-problems&amp;utm_source=striver&amp;utm_medium=website&amp;leftPanelTab=1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcose.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcomi.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcofl.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcocl.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcoma.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcowo.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcodi.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcoim.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcofi.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcogi.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcoto.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcotr.com/problems/course-schedule/</t>
+  </si>
+  <si>
+    <t>https://leetcogr.com/problems/course-schedule/</t>
   </si>
 </sst>
 </file>
@@ -2700,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F461"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D387" sqref="D387"/>
+    <sheetView tabSelected="1" topLeftCell="A338" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D346" sqref="D346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.296875" defaultRowHeight="18"/>
@@ -6874,6 +6925,9 @@
       <c r="C339" s="2" t="s">
         <v>403</v>
       </c>
+      <c r="D339" s="20" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="340" spans="1:4" ht="21">
       <c r="A340" s="5" t="s">
@@ -6885,6 +6939,9 @@
       <c r="C340" s="2" t="s">
         <v>403</v>
       </c>
+      <c r="D340" s="20" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="341" spans="1:4" ht="21">
       <c r="A341" s="5" t="s">
@@ -6894,7 +6951,10 @@
         <v>286</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
+      </c>
+      <c r="D341" s="20" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="21">
@@ -6905,7 +6965,10 @@
         <v>287</v>
       </c>
       <c r="C342" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
+      </c>
+      <c r="D342" s="20" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="21">
@@ -6993,7 +7056,7 @@
         <v>295</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="21">
@@ -7026,7 +7089,7 @@
         <v>298</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
       </c>
     </row>
     <row r="354" spans="1:6" ht="21">
@@ -7114,7 +7177,7 @@
         <v>306</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
       </c>
     </row>
     <row r="362" spans="1:6" ht="21">
@@ -7248,7 +7311,7 @@
         <v>318</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>2</v>
+        <v>403</v>
       </c>
     </row>
     <row r="374" spans="1:4" ht="21">
@@ -8827,8 +8890,12 @@
     <hyperlink ref="D332" r:id="rId591" xr:uid="{6334817C-4572-41DF-9A29-87030EF93249}"/>
     <hyperlink ref="D325" r:id="rId592" xr:uid="{DC6DA814-F01B-4F59-AFB0-25D9D05A91D0}"/>
     <hyperlink ref="D387" r:id="rId593" xr:uid="{98D865FE-E1B3-4F5D-926F-5C97169A9F69}"/>
+    <hyperlink ref="D340" r:id="rId594" xr:uid="{F1FCB126-2C06-4061-A4F9-1DE7952F6BF0}"/>
+    <hyperlink ref="D339" r:id="rId595" xr:uid="{D5AA24C8-D8EE-4F6E-8A8C-3FE4B14F08B0}"/>
+    <hyperlink ref="D342" r:id="rId596" xr:uid="{1DB5F5CB-1594-4759-9FE9-FBC070581FB0}"/>
+    <hyperlink ref="D341" r:id="rId597" xr:uid="{393B6990-6ADA-49F4-B04F-6BECD2617FBC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId594"/>
+  <pageSetup orientation="portrait" r:id="rId598"/>
 </worksheet>
 </file>
</xml_diff>